<commit_message>
fix SyntheticDataPipeline and regenerate
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -531,7 +531,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BSD</t>
+          <t>BSD License</t>
         </is>
       </c>
     </row>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1459,7 +1459,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1498,7 +1498,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>If you have any information that can contribute to identifying or locating the rights-holder(s), please notify the organization that has made the Item available.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>If you have any information that can contribute to identifying or locating the rights-holder(s) please notify the organization that has made the Item available.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1614,7 +1614,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1691,7 +1691,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy, or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1730,7 +1730,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1807,7 +1807,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -5004,7 +5004,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 0 image 0 rights holder</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -5051,7 +5051,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 0 image 1 rights holder</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -5098,7 +5098,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 1 image 0 rights holder</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -5145,7 +5145,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 1 image 1 rights holder</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -5192,7 +5192,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 2 image 0 rights holder</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -5239,7 +5239,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 2 image 1 rights holder</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -5286,7 +5286,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 3 image 0 rights holder</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 3 image 1 rights holder</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -5380,7 +5380,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 4 image 0 rights holder</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -5427,7 +5427,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 4 image 1 rights holder</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -5474,7 +5474,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 5 image 0 rights holder</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -5521,7 +5521,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 5 image 1 rights holder</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -5568,7 +5568,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 6 image 0 rights holder</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -5615,7 +5615,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 6 image 1 rights holder</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -5662,7 +5662,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 7 image 0 rights holder</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -5709,7 +5709,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 7 image 1 rights holder</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -5756,7 +5756,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 8 image 0 rights holder</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -5803,7 +5803,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 8 image 1 rights holder</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -5850,7 +5850,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 9 image 0 rights holder</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -5897,7 +5897,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Cultural context 9 image 1 rights holder</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -5944,7 +5944,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 0 image 0 rights holder</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -5991,7 +5991,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 0 image 1 rights holder</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -6038,7 +6038,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 1 image 0 rights holder</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -6085,7 +6085,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 1 image 1 rights holder</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -6132,7 +6132,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 2 image 0 rights holder</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -6179,7 +6179,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 2 image 1 rights holder</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -6226,7 +6226,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 3 image 0 rights holder</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -6273,7 +6273,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 3 image 1 rights holder</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -6320,7 +6320,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 4 image 0 rights holder</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -6367,7 +6367,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 4 image 1 rights holder</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -6414,7 +6414,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 5 image 0 rights holder</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -6461,7 +6461,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 5 image 1 rights holder</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -6508,7 +6508,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 6 image 0 rights holder</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -6555,7 +6555,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 6 image 1 rights holder</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -6602,7 +6602,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 7 image 0 rights holder</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -6649,7 +6649,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 7 image 1 rights holder</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -6696,7 +6696,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 8 image 0 rights holder</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -6743,7 +6743,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 8 image 1 rights holder</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -6790,7 +6790,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 9 image 0 rights holder</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -6837,7 +6837,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Extent 9 image 1 rights holder</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -6884,7 +6884,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 0 image 0 rights holder</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -6931,7 +6931,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 0 image 1 rights holder</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -6978,7 +6978,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 1 image 0 rights holder</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -7025,7 +7025,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 1 image 1 rights holder</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -7072,7 +7072,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 2 image 0 rights holder</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -7119,7 +7119,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 2 image 1 rights holder</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -7166,7 +7166,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 3 image 0 rights holder</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -7213,7 +7213,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 3 image 1 rights holder</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -7260,7 +7260,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 4 image 0 rights holder</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -7307,7 +7307,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 4 image 1 rights holder</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -7354,7 +7354,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 5 image 0 rights holder</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
@@ -7401,7 +7401,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 5 image 1 rights holder</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -7448,7 +7448,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 6 image 0 rights holder</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
@@ -7495,7 +7495,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 6 image 1 rights holder</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
@@ -7542,7 +7542,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 7 image 0 rights holder</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -7589,7 +7589,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 7 image 1 rights holder</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -7636,7 +7636,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 8 image 0 rights holder</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
@@ -7683,7 +7683,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 8 image 1 rights holder</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
@@ -7730,7 +7730,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 9 image 0 rights holder</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
@@ -7777,7 +7777,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Language 9 image 1 rights holder</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
@@ -7824,7 +7824,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 0 image 0 rights holder</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -7871,7 +7871,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 0 image 1 rights holder</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
@@ -7918,7 +7918,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 1 image 0 rights holder</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
@@ -7965,7 +7965,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 1 image 1 rights holder</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
@@ -8012,7 +8012,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 2 image 0 rights holder</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -8059,7 +8059,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 2 image 1 rights holder</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
@@ -8106,7 +8106,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 3 image 0 rights holder</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
@@ -8153,7 +8153,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 3 image 1 rights holder</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
@@ -8200,7 +8200,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 4 image 0 rights holder</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -8247,7 +8247,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 4 image 1 rights holder</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
@@ -8294,7 +8294,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 5 image 0 rights holder</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
@@ -8341,7 +8341,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 5 image 1 rights holder</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
@@ -8388,7 +8388,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 6 image 0 rights holder</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
@@ -8435,7 +8435,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 6 image 1 rights holder</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
@@ -8482,7 +8482,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 7 image 0 rights holder</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -8529,7 +8529,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 7 image 1 rights holder</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
@@ -8576,7 +8576,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 8 image 0 rights holder</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
@@ -8623,7 +8623,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 8 image 1 rights holder</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
@@ -8670,7 +8670,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 9 image 0 rights holder</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
@@ -8717,7 +8717,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Material 9 image 1 rights holder</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
@@ -8764,7 +8764,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 0 image 0 rights holder</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
@@ -8811,7 +8811,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 0 image 1 rights holder</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
@@ -8858,7 +8858,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 1 image 0 rights holder</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
@@ -8905,7 +8905,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 1 image 1 rights holder</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
@@ -8952,7 +8952,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 2 image 0 rights holder</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
@@ -8999,7 +8999,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 2 image 1 rights holder</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
@@ -9046,7 +9046,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 3 image 0 rights holder</t>
         </is>
       </c>
       <c r="I88" t="inlineStr">
@@ -9093,7 +9093,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 3 image 1 rights holder</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
@@ -9140,7 +9140,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 4 image 0 rights holder</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
@@ -9187,7 +9187,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 4 image 1 rights holder</t>
         </is>
       </c>
       <c r="I91" t="inlineStr">
@@ -9234,7 +9234,7 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 5 image 0 rights holder</t>
         </is>
       </c>
       <c r="I92" t="inlineStr">
@@ -9281,7 +9281,7 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 5 image 1 rights holder</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
@@ -9328,7 +9328,7 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 6 image 0 rights holder</t>
         </is>
       </c>
       <c r="I94" t="inlineStr">
@@ -9375,7 +9375,7 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 6 image 1 rights holder</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
@@ -9422,7 +9422,7 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 7 image 0 rights holder</t>
         </is>
       </c>
       <c r="I96" t="inlineStr">
@@ -9469,7 +9469,7 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 7 image 1 rights holder</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
@@ -9516,7 +9516,7 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 8 image 0 rights holder</t>
         </is>
       </c>
       <c r="I98" t="inlineStr">
@@ -9563,7 +9563,7 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 8 image 1 rights holder</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
@@ -9610,7 +9610,7 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 9 image 0 rights holder</t>
         </is>
       </c>
       <c r="I100" t="inlineStr">
@@ -9657,7 +9657,7 @@
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Medium 9 image 1 rights holder</t>
         </is>
       </c>
       <c r="I101" t="inlineStr">
@@ -9704,7 +9704,7 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 0 image 0 rights holder</t>
         </is>
       </c>
       <c r="I102" t="inlineStr">
@@ -9751,7 +9751,7 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 0 image 1 rights holder</t>
         </is>
       </c>
       <c r="I103" t="inlineStr">
@@ -9798,7 +9798,7 @@
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 1 image 0 rights holder</t>
         </is>
       </c>
       <c r="I104" t="inlineStr">
@@ -9845,7 +9845,7 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 1 image 1 rights holder</t>
         </is>
       </c>
       <c r="I105" t="inlineStr">
@@ -9892,7 +9892,7 @@
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 2 image 0 rights holder</t>
         </is>
       </c>
       <c r="I106" t="inlineStr">
@@ -9939,7 +9939,7 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 2 image 1 rights holder</t>
         </is>
       </c>
       <c r="I107" t="inlineStr">
@@ -9986,7 +9986,7 @@
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 3 image 0 rights holder</t>
         </is>
       </c>
       <c r="I108" t="inlineStr">
@@ -10033,7 +10033,7 @@
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 3 image 1 rights holder</t>
         </is>
       </c>
       <c r="I109" t="inlineStr">
@@ -10080,7 +10080,7 @@
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 4 image 0 rights holder</t>
         </is>
       </c>
       <c r="I110" t="inlineStr">
@@ -10127,7 +10127,7 @@
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 4 image 1 rights holder</t>
         </is>
       </c>
       <c r="I111" t="inlineStr">
@@ -10174,7 +10174,7 @@
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 5 image 0 rights holder</t>
         </is>
       </c>
       <c r="I112" t="inlineStr">
@@ -10221,7 +10221,7 @@
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 5 image 1 rights holder</t>
         </is>
       </c>
       <c r="I113" t="inlineStr">
@@ -10268,7 +10268,7 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 6 image 0 rights holder</t>
         </is>
       </c>
       <c r="I114" t="inlineStr">
@@ -10315,7 +10315,7 @@
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 6 image 1 rights holder</t>
         </is>
       </c>
       <c r="I115" t="inlineStr">
@@ -10362,7 +10362,7 @@
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 7 image 0 rights holder</t>
         </is>
       </c>
       <c r="I116" t="inlineStr">
@@ -10409,7 +10409,7 @@
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 7 image 1 rights holder</t>
         </is>
       </c>
       <c r="I117" t="inlineStr">
@@ -10456,7 +10456,7 @@
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 8 image 0 rights holder</t>
         </is>
       </c>
       <c r="I118" t="inlineStr">
@@ -10503,7 +10503,7 @@
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 8 image 1 rights holder</t>
         </is>
       </c>
       <c r="I119" t="inlineStr">
@@ -10550,7 +10550,7 @@
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 9 image 0 rights holder</t>
         </is>
       </c>
       <c r="I120" t="inlineStr">
@@ -10597,7 +10597,7 @@
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Publisher 9 image 1 rights holder</t>
         </is>
       </c>
       <c r="I121" t="inlineStr">
@@ -10644,7 +10644,7 @@
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 0 image 0 rights holder</t>
         </is>
       </c>
       <c r="I122" t="inlineStr">
@@ -10691,7 +10691,7 @@
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 0 image 1 rights holder</t>
         </is>
       </c>
       <c r="I123" t="inlineStr">
@@ -10738,7 +10738,7 @@
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 1 image 0 rights holder</t>
         </is>
       </c>
       <c r="I124" t="inlineStr">
@@ -10785,7 +10785,7 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 1 image 1 rights holder</t>
         </is>
       </c>
       <c r="I125" t="inlineStr">
@@ -10832,7 +10832,7 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 2 image 0 rights holder</t>
         </is>
       </c>
       <c r="I126" t="inlineStr">
@@ -10879,7 +10879,7 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 2 image 1 rights holder</t>
         </is>
       </c>
       <c r="I127" t="inlineStr">
@@ -10926,7 +10926,7 @@
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 3 image 0 rights holder</t>
         </is>
       </c>
       <c r="I128" t="inlineStr">
@@ -10973,7 +10973,7 @@
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 3 image 1 rights holder</t>
         </is>
       </c>
       <c r="I129" t="inlineStr">
@@ -11020,7 +11020,7 @@
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 4 image 0 rights holder</t>
         </is>
       </c>
       <c r="I130" t="inlineStr">
@@ -11067,7 +11067,7 @@
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 4 image 1 rights holder</t>
         </is>
       </c>
       <c r="I131" t="inlineStr">
@@ -11114,7 +11114,7 @@
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 5 image 0 rights holder</t>
         </is>
       </c>
       <c r="I132" t="inlineStr">
@@ -11161,7 +11161,7 @@
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 5 image 1 rights holder</t>
         </is>
       </c>
       <c r="I133" t="inlineStr">
@@ -11208,7 +11208,7 @@
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 6 image 0 rights holder</t>
         </is>
       </c>
       <c r="I134" t="inlineStr">
@@ -11255,7 +11255,7 @@
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 6 image 1 rights holder</t>
         </is>
       </c>
       <c r="I135" t="inlineStr">
@@ -11302,7 +11302,7 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 7 image 0 rights holder</t>
         </is>
       </c>
       <c r="I136" t="inlineStr">
@@ -11349,7 +11349,7 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 7 image 1 rights holder</t>
         </is>
       </c>
       <c r="I137" t="inlineStr">
@@ -11396,7 +11396,7 @@
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 8 image 0 rights holder</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
@@ -11443,7 +11443,7 @@
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 8 image 1 rights holder</t>
         </is>
       </c>
       <c r="I139" t="inlineStr">
@@ -11490,7 +11490,7 @@
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 9 image 0 rights holder</t>
         </is>
       </c>
       <c r="I140" t="inlineStr">
@@ -11537,7 +11537,7 @@
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Source 9 image 1 rights holder</t>
         </is>
       </c>
       <c r="I141" t="inlineStr">
@@ -11584,7 +11584,7 @@
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 0 image 0 rights holder</t>
         </is>
       </c>
       <c r="I142" t="inlineStr">
@@ -11631,7 +11631,7 @@
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 0 image 1 rights holder</t>
         </is>
       </c>
       <c r="I143" t="inlineStr">
@@ -11678,7 +11678,7 @@
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 1 image 0 rights holder</t>
         </is>
       </c>
       <c r="I144" t="inlineStr">
@@ -11725,7 +11725,7 @@
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 1 image 1 rights holder</t>
         </is>
       </c>
       <c r="I145" t="inlineStr">
@@ -11772,7 +11772,7 @@
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 2 image 0 rights holder</t>
         </is>
       </c>
       <c r="I146" t="inlineStr">
@@ -11819,7 +11819,7 @@
       </c>
       <c r="H147" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 2 image 1 rights holder</t>
         </is>
       </c>
       <c r="I147" t="inlineStr">
@@ -11866,7 +11866,7 @@
       </c>
       <c r="H148" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 3 image 0 rights holder</t>
         </is>
       </c>
       <c r="I148" t="inlineStr">
@@ -11913,7 +11913,7 @@
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 3 image 1 rights holder</t>
         </is>
       </c>
       <c r="I149" t="inlineStr">
@@ -11960,7 +11960,7 @@
       </c>
       <c r="H150" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 4 image 0 rights holder</t>
         </is>
       </c>
       <c r="I150" t="inlineStr">
@@ -12007,7 +12007,7 @@
       </c>
       <c r="H151" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 4 image 1 rights holder</t>
         </is>
       </c>
       <c r="I151" t="inlineStr">
@@ -12054,7 +12054,7 @@
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 5 image 0 rights holder</t>
         </is>
       </c>
       <c r="I152" t="inlineStr">
@@ -12101,7 +12101,7 @@
       </c>
       <c r="H153" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 5 image 1 rights holder</t>
         </is>
       </c>
       <c r="I153" t="inlineStr">
@@ -12148,7 +12148,7 @@
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 6 image 0 rights holder</t>
         </is>
       </c>
       <c r="I154" t="inlineStr">
@@ -12195,7 +12195,7 @@
       </c>
       <c r="H155" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 6 image 1 rights holder</t>
         </is>
       </c>
       <c r="I155" t="inlineStr">
@@ -12242,7 +12242,7 @@
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 7 image 0 rights holder</t>
         </is>
       </c>
       <c r="I156" t="inlineStr">
@@ -12289,7 +12289,7 @@
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 7 image 1 rights holder</t>
         </is>
       </c>
       <c r="I157" t="inlineStr">
@@ -12336,7 +12336,7 @@
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 8 image 0 rights holder</t>
         </is>
       </c>
       <c r="I158" t="inlineStr">
@@ -12383,7 +12383,7 @@
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 8 image 1 rights holder</t>
         </is>
       </c>
       <c r="I159" t="inlineStr">
@@ -12430,7 +12430,7 @@
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 9 image 0 rights holder</t>
         </is>
       </c>
       <c r="I160" t="inlineStr">
@@ -12477,7 +12477,7 @@
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Spatial 9 image 1 rights holder</t>
         </is>
       </c>
       <c r="I161" t="inlineStr">
@@ -12524,7 +12524,7 @@
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 0 image 0 rights holder</t>
         </is>
       </c>
       <c r="I162" t="inlineStr">
@@ -12571,7 +12571,7 @@
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 0 image 1 rights holder</t>
         </is>
       </c>
       <c r="I163" t="inlineStr">
@@ -12618,7 +12618,7 @@
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 1 image 0 rights holder</t>
         </is>
       </c>
       <c r="I164" t="inlineStr">
@@ -12665,7 +12665,7 @@
       </c>
       <c r="H165" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 1 image 1 rights holder</t>
         </is>
       </c>
       <c r="I165" t="inlineStr">
@@ -12712,7 +12712,7 @@
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 2 image 0 rights holder</t>
         </is>
       </c>
       <c r="I166" t="inlineStr">
@@ -12759,7 +12759,7 @@
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 2 image 1 rights holder</t>
         </is>
       </c>
       <c r="I167" t="inlineStr">
@@ -12806,7 +12806,7 @@
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 3 image 0 rights holder</t>
         </is>
       </c>
       <c r="I168" t="inlineStr">
@@ -12853,7 +12853,7 @@
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 3 image 1 rights holder</t>
         </is>
       </c>
       <c r="I169" t="inlineStr">
@@ -12900,7 +12900,7 @@
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 4 image 0 rights holder</t>
         </is>
       </c>
       <c r="I170" t="inlineStr">
@@ -12947,7 +12947,7 @@
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 4 image 1 rights holder</t>
         </is>
       </c>
       <c r="I171" t="inlineStr">
@@ -12994,7 +12994,7 @@
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 5 image 0 rights holder</t>
         </is>
       </c>
       <c r="I172" t="inlineStr">
@@ -13041,7 +13041,7 @@
       </c>
       <c r="H173" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 5 image 1 rights holder</t>
         </is>
       </c>
       <c r="I173" t="inlineStr">
@@ -13088,7 +13088,7 @@
       </c>
       <c r="H174" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 6 image 0 rights holder</t>
         </is>
       </c>
       <c r="I174" t="inlineStr">
@@ -13135,7 +13135,7 @@
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 6 image 1 rights holder</t>
         </is>
       </c>
       <c r="I175" t="inlineStr">
@@ -13182,7 +13182,7 @@
       </c>
       <c r="H176" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 7 image 0 rights holder</t>
         </is>
       </c>
       <c r="I176" t="inlineStr">
@@ -13229,7 +13229,7 @@
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 7 image 1 rights holder</t>
         </is>
       </c>
       <c r="I177" t="inlineStr">
@@ -13276,7 +13276,7 @@
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 8 image 0 rights holder</t>
         </is>
       </c>
       <c r="I178" t="inlineStr">
@@ -13323,7 +13323,7 @@
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 8 image 1 rights holder</t>
         </is>
       </c>
       <c r="I179" t="inlineStr">
@@ -13370,7 +13370,7 @@
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 9 image 0 rights holder</t>
         </is>
       </c>
       <c r="I180" t="inlineStr">
@@ -13417,7 +13417,7 @@
       </c>
       <c r="H181" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Subject 9 image 1 rights holder</t>
         </is>
       </c>
       <c r="I181" t="inlineStr">
@@ -13464,7 +13464,7 @@
       </c>
       <c r="H182" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 0 image 0 rights holder</t>
         </is>
       </c>
       <c r="I182" t="inlineStr">
@@ -13511,7 +13511,7 @@
       </c>
       <c r="H183" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 0 image 1 rights holder</t>
         </is>
       </c>
       <c r="I183" t="inlineStr">
@@ -13558,7 +13558,7 @@
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 1 image 0 rights holder</t>
         </is>
       </c>
       <c r="I184" t="inlineStr">
@@ -13605,7 +13605,7 @@
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 1 image 1 rights holder</t>
         </is>
       </c>
       <c r="I185" t="inlineStr">
@@ -13652,7 +13652,7 @@
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 2 image 0 rights holder</t>
         </is>
       </c>
       <c r="I186" t="inlineStr">
@@ -13699,7 +13699,7 @@
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 2 image 1 rights holder</t>
         </is>
       </c>
       <c r="I187" t="inlineStr">
@@ -13746,7 +13746,7 @@
       </c>
       <c r="H188" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 3 image 0 rights holder</t>
         </is>
       </c>
       <c r="I188" t="inlineStr">
@@ -13793,7 +13793,7 @@
       </c>
       <c r="H189" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 3 image 1 rights holder</t>
         </is>
       </c>
       <c r="I189" t="inlineStr">
@@ -13840,7 +13840,7 @@
       </c>
       <c r="H190" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 4 image 0 rights holder</t>
         </is>
       </c>
       <c r="I190" t="inlineStr">
@@ -13887,7 +13887,7 @@
       </c>
       <c r="H191" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 4 image 1 rights holder</t>
         </is>
       </c>
       <c r="I191" t="inlineStr">
@@ -13934,7 +13934,7 @@
       </c>
       <c r="H192" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 5 image 0 rights holder</t>
         </is>
       </c>
       <c r="I192" t="inlineStr">
@@ -13981,7 +13981,7 @@
       </c>
       <c r="H193" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 5 image 1 rights holder</t>
         </is>
       </c>
       <c r="I193" t="inlineStr">
@@ -14028,7 +14028,7 @@
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 6 image 0 rights holder</t>
         </is>
       </c>
       <c r="I194" t="inlineStr">
@@ -14075,7 +14075,7 @@
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 6 image 1 rights holder</t>
         </is>
       </c>
       <c r="I195" t="inlineStr">
@@ -14122,7 +14122,7 @@
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 7 image 0 rights holder</t>
         </is>
       </c>
       <c r="I196" t="inlineStr">
@@ -14169,7 +14169,7 @@
       </c>
       <c r="H197" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 7 image 1 rights holder</t>
         </is>
       </c>
       <c r="I197" t="inlineStr">
@@ -14216,7 +14216,7 @@
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 8 image 0 rights holder</t>
         </is>
       </c>
       <c r="I198" t="inlineStr">
@@ -14263,7 +14263,7 @@
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 8 image 1 rights holder</t>
         </is>
       </c>
       <c r="I199" t="inlineStr">
@@ -14310,7 +14310,7 @@
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 9 image 0 rights holder</t>
         </is>
       </c>
       <c r="I200" t="inlineStr">
@@ -14357,7 +14357,7 @@
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Technique 9 image 1 rights holder</t>
         </is>
       </c>
       <c r="I201" t="inlineStr">
@@ -14404,7 +14404,7 @@
       </c>
       <c r="H202" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 0 image 0 rights holder</t>
         </is>
       </c>
       <c r="I202" t="inlineStr">
@@ -14451,7 +14451,7 @@
       </c>
       <c r="H203" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 0 image 1 rights holder</t>
         </is>
       </c>
       <c r="I203" t="inlineStr">
@@ -14498,7 +14498,7 @@
       </c>
       <c r="H204" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 1 image 0 rights holder</t>
         </is>
       </c>
       <c r="I204" t="inlineStr">
@@ -14545,7 +14545,7 @@
       </c>
       <c r="H205" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 1 image 1 rights holder</t>
         </is>
       </c>
       <c r="I205" t="inlineStr">
@@ -14592,7 +14592,7 @@
       </c>
       <c r="H206" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 2 image 0 rights holder</t>
         </is>
       </c>
       <c r="I206" t="inlineStr">
@@ -14639,7 +14639,7 @@
       </c>
       <c r="H207" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 2 image 1 rights holder</t>
         </is>
       </c>
       <c r="I207" t="inlineStr">
@@ -14686,7 +14686,7 @@
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 3 image 0 rights holder</t>
         </is>
       </c>
       <c r="I208" t="inlineStr">
@@ -14733,7 +14733,7 @@
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 3 image 1 rights holder</t>
         </is>
       </c>
       <c r="I209" t="inlineStr">
@@ -14780,7 +14780,7 @@
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 4 image 0 rights holder</t>
         </is>
       </c>
       <c r="I210" t="inlineStr">
@@ -14827,7 +14827,7 @@
       </c>
       <c r="H211" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 4 image 1 rights holder</t>
         </is>
       </c>
       <c r="I211" t="inlineStr">
@@ -14874,7 +14874,7 @@
       </c>
       <c r="H212" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 5 image 0 rights holder</t>
         </is>
       </c>
       <c r="I212" t="inlineStr">
@@ -14921,7 +14921,7 @@
       </c>
       <c r="H213" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 5 image 1 rights holder</t>
         </is>
       </c>
       <c r="I213" t="inlineStr">
@@ -14968,7 +14968,7 @@
       </c>
       <c r="H214" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 6 image 0 rights holder</t>
         </is>
       </c>
       <c r="I214" t="inlineStr">
@@ -15015,7 +15015,7 @@
       </c>
       <c r="H215" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 6 image 1 rights holder</t>
         </is>
       </c>
       <c r="I215" t="inlineStr">
@@ -15062,7 +15062,7 @@
       </c>
       <c r="H216" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 7 image 0 rights holder</t>
         </is>
       </c>
       <c r="I216" t="inlineStr">
@@ -15109,7 +15109,7 @@
       </c>
       <c r="H217" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 7 image 1 rights holder</t>
         </is>
       </c>
       <c r="I217" t="inlineStr">
@@ -15156,7 +15156,7 @@
       </c>
       <c r="H218" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 8 image 0 rights holder</t>
         </is>
       </c>
       <c r="I218" t="inlineStr">
@@ -15203,7 +15203,7 @@
       </c>
       <c r="H219" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 8 image 1 rights holder</t>
         </is>
       </c>
       <c r="I219" t="inlineStr">
@@ -15250,7 +15250,7 @@
       </c>
       <c r="H220" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 9 image 0 rights holder</t>
         </is>
       </c>
       <c r="I220" t="inlineStr">
@@ -15297,7 +15297,7 @@
       </c>
       <c r="H221" t="inlineStr">
         <is>
-          <t>Property definition rights holder</t>
+          <t>Type 9 image 1 rights holder</t>
         </is>
       </c>
       <c r="I221" t="inlineStr">
@@ -15814,7 +15814,7 @@
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>Institution0 rights holder</t>
+          <t>Institution0 image 0 rights holder</t>
         </is>
       </c>
       <c r="I232" t="inlineStr">
@@ -15861,7 +15861,7 @@
       </c>
       <c r="H233" t="inlineStr">
         <is>
-          <t>Institution0 rights holder</t>
+          <t>Institution0 image 1 rights holder</t>
         </is>
       </c>
       <c r="I233" t="inlineStr">
@@ -15908,7 +15908,7 @@
       </c>
       <c r="H234" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work0 rights holder</t>
+          <t>Institution0Collection0Work0 image 0 rights holder</t>
         </is>
       </c>
       <c r="I234" t="inlineStr">
@@ -15955,7 +15955,7 @@
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work0 rights holder</t>
+          <t>Institution0Collection0Work0 image 1 rights holder</t>
         </is>
       </c>
       <c r="I235" t="inlineStr">
@@ -16002,7 +16002,7 @@
       </c>
       <c r="H236" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work1 rights holder</t>
+          <t>Institution0Collection0Work1 image 0 rights holder</t>
         </is>
       </c>
       <c r="I236" t="inlineStr">
@@ -16049,7 +16049,7 @@
       </c>
       <c r="H237" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work1 rights holder</t>
+          <t>Institution0Collection0Work1 image 1 rights holder</t>
         </is>
       </c>
       <c r="I237" t="inlineStr">
@@ -16096,7 +16096,7 @@
       </c>
       <c r="H238" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work2 rights holder</t>
+          <t>Institution0Collection0Work2 image 0 rights holder</t>
         </is>
       </c>
       <c r="I238" t="inlineStr">
@@ -16143,7 +16143,7 @@
       </c>
       <c r="H239" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work2 rights holder</t>
+          <t>Institution0Collection0Work2 image 1 rights holder</t>
         </is>
       </c>
       <c r="I239" t="inlineStr">
@@ -16190,7 +16190,7 @@
       </c>
       <c r="H240" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work3 rights holder</t>
+          <t>Institution0Collection0Work3 image 0 rights holder</t>
         </is>
       </c>
       <c r="I240" t="inlineStr">
@@ -16237,7 +16237,7 @@
       </c>
       <c r="H241" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work3 rights holder</t>
+          <t>Institution0Collection0Work3 image 1 rights holder</t>
         </is>
       </c>
       <c r="I241" t="inlineStr">
@@ -16284,7 +16284,7 @@
       </c>
       <c r="H242" t="inlineStr">
         <is>
-          <t>Institution0SharedWork4 rights holder</t>
+          <t>Institution0SharedWork4 image 0 rights holder</t>
         </is>
       </c>
       <c r="I242" t="inlineStr">
@@ -16331,7 +16331,7 @@
       </c>
       <c r="H243" t="inlineStr">
         <is>
-          <t>Institution0SharedWork4 rights holder</t>
+          <t>Institution0SharedWork4 image 1 rights holder</t>
         </is>
       </c>
       <c r="I243" t="inlineStr">
@@ -16378,7 +16378,7 @@
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>Institution0SharedWork5 rights holder</t>
+          <t>Institution0SharedWork5 image 0 rights holder</t>
         </is>
       </c>
       <c r="I244" t="inlineStr">
@@ -16425,7 +16425,7 @@
       </c>
       <c r="H245" t="inlineStr">
         <is>
-          <t>Institution0SharedWork5 rights holder</t>
+          <t>Institution0SharedWork5 image 1 rights holder</t>
         </is>
       </c>
       <c r="I245" t="inlineStr">
@@ -16472,7 +16472,7 @@
       </c>
       <c r="H246" t="inlineStr">
         <is>
-          <t>Institution0SharedWork6 rights holder</t>
+          <t>Institution0SharedWork6 image 0 rights holder</t>
         </is>
       </c>
       <c r="I246" t="inlineStr">
@@ -16519,7 +16519,7 @@
       </c>
       <c r="H247" t="inlineStr">
         <is>
-          <t>Institution0SharedWork6 rights holder</t>
+          <t>Institution0SharedWork6 image 1 rights holder</t>
         </is>
       </c>
       <c r="I247" t="inlineStr">
@@ -16566,7 +16566,7 @@
       </c>
       <c r="H248" t="inlineStr">
         <is>
-          <t>Institution0SharedWork7 rights holder</t>
+          <t>Institution0SharedWork7 image 0 rights holder</t>
         </is>
       </c>
       <c r="I248" t="inlineStr">
@@ -16613,7 +16613,7 @@
       </c>
       <c r="H249" t="inlineStr">
         <is>
-          <t>Institution0SharedWork7 rights holder</t>
+          <t>Institution0SharedWork7 image 1 rights holder</t>
         </is>
       </c>
       <c r="I249" t="inlineStr">
@@ -16660,7 +16660,7 @@
       </c>
       <c r="H250" t="inlineStr">
         <is>
-          <t>Institution1 rights holder</t>
+          <t>Institution1 image 0 rights holder</t>
         </is>
       </c>
       <c r="I250" t="inlineStr">
@@ -16707,7 +16707,7 @@
       </c>
       <c r="H251" t="inlineStr">
         <is>
-          <t>Institution1 rights holder</t>
+          <t>Institution1 image 1 rights holder</t>
         </is>
       </c>
       <c r="I251" t="inlineStr">
@@ -16754,7 +16754,7 @@
       </c>
       <c r="H252" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work8 rights holder</t>
+          <t>Institution1Collection0Work8 image 0 rights holder</t>
         </is>
       </c>
       <c r="I252" t="inlineStr">
@@ -16801,7 +16801,7 @@
       </c>
       <c r="H253" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work8 rights holder</t>
+          <t>Institution1Collection0Work8 image 1 rights holder</t>
         </is>
       </c>
       <c r="I253" t="inlineStr">
@@ -16848,7 +16848,7 @@
       </c>
       <c r="H254" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work9 rights holder</t>
+          <t>Institution1Collection0Work9 image 0 rights holder</t>
         </is>
       </c>
       <c r="I254" t="inlineStr">
@@ -16895,7 +16895,7 @@
       </c>
       <c r="H255" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work9 rights holder</t>
+          <t>Institution1Collection0Work9 image 1 rights holder</t>
         </is>
       </c>
       <c r="I255" t="inlineStr">
@@ -16942,7 +16942,7 @@
       </c>
       <c r="H256" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work10 rights holder</t>
+          <t>Institution1Collection0Work10 image 0 rights holder</t>
         </is>
       </c>
       <c r="I256" t="inlineStr">
@@ -16989,7 +16989,7 @@
       </c>
       <c r="H257" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work10 rights holder</t>
+          <t>Institution1Collection0Work10 image 1 rights holder</t>
         </is>
       </c>
       <c r="I257" t="inlineStr">
@@ -17036,7 +17036,7 @@
       </c>
       <c r="H258" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work11 rights holder</t>
+          <t>Institution1Collection0Work11 image 0 rights holder</t>
         </is>
       </c>
       <c r="I258" t="inlineStr">
@@ -17083,7 +17083,7 @@
       </c>
       <c r="H259" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work11 rights holder</t>
+          <t>Institution1Collection0Work11 image 1 rights holder</t>
         </is>
       </c>
       <c r="I259" t="inlineStr">
@@ -17130,7 +17130,7 @@
       </c>
       <c r="H260" t="inlineStr">
         <is>
-          <t>Institution1SharedWork12 rights holder</t>
+          <t>Institution1SharedWork12 image 0 rights holder</t>
         </is>
       </c>
       <c r="I260" t="inlineStr">
@@ -17177,7 +17177,7 @@
       </c>
       <c r="H261" t="inlineStr">
         <is>
-          <t>Institution1SharedWork12 rights holder</t>
+          <t>Institution1SharedWork12 image 1 rights holder</t>
         </is>
       </c>
       <c r="I261" t="inlineStr">
@@ -17224,7 +17224,7 @@
       </c>
       <c r="H262" t="inlineStr">
         <is>
-          <t>Institution1SharedWork13 rights holder</t>
+          <t>Institution1SharedWork13 image 0 rights holder</t>
         </is>
       </c>
       <c r="I262" t="inlineStr">
@@ -17271,7 +17271,7 @@
       </c>
       <c r="H263" t="inlineStr">
         <is>
-          <t>Institution1SharedWork13 rights holder</t>
+          <t>Institution1SharedWork13 image 1 rights holder</t>
         </is>
       </c>
       <c r="I263" t="inlineStr">
@@ -17318,7 +17318,7 @@
       </c>
       <c r="H264" t="inlineStr">
         <is>
-          <t>Institution1SharedWork14 rights holder</t>
+          <t>Institution1SharedWork14 image 0 rights holder</t>
         </is>
       </c>
       <c r="I264" t="inlineStr">
@@ -17365,7 +17365,7 @@
       </c>
       <c r="H265" t="inlineStr">
         <is>
-          <t>Institution1SharedWork14 rights holder</t>
+          <t>Institution1SharedWork14 image 1 rights holder</t>
         </is>
       </c>
       <c r="I265" t="inlineStr">
@@ -17412,7 +17412,7 @@
       </c>
       <c r="H266" t="inlineStr">
         <is>
-          <t>Institution1SharedWork15 rights holder</t>
+          <t>Institution1SharedWork15 image 0 rights holder</t>
         </is>
       </c>
       <c r="I266" t="inlineStr">
@@ -17459,7 +17459,7 @@
       </c>
       <c r="H267" t="inlineStr">
         <is>
-          <t>Institution1SharedWork15 rights holder</t>
+          <t>Institution1SharedWork15 image 1 rights holder</t>
         </is>
       </c>
       <c r="I267" t="inlineStr">
@@ -17506,7 +17506,7 @@
       </c>
       <c r="H268" t="inlineStr">
         <is>
-          <t>FreestandingWork16 rights holder</t>
+          <t>FreestandingWork16 image 0 rights holder</t>
         </is>
       </c>
       <c r="I268" t="inlineStr">
@@ -17553,7 +17553,7 @@
       </c>
       <c r="H269" t="inlineStr">
         <is>
-          <t>FreestandingWork16 rights holder</t>
+          <t>FreestandingWork16 image 1 rights holder</t>
         </is>
       </c>
       <c r="I269" t="inlineStr">
@@ -17600,7 +17600,7 @@
       </c>
       <c r="H270" t="inlineStr">
         <is>
-          <t>FreestandingWork17 rights holder</t>
+          <t>FreestandingWork17 image 0 rights holder</t>
         </is>
       </c>
       <c r="I270" t="inlineStr">
@@ -17647,7 +17647,7 @@
       </c>
       <c r="H271" t="inlineStr">
         <is>
-          <t>FreestandingWork17 rights holder</t>
+          <t>FreestandingWork17 image 1 rights holder</t>
         </is>
       </c>
       <c r="I271" t="inlineStr">
@@ -17694,7 +17694,7 @@
       </c>
       <c r="H272" t="inlineStr">
         <is>
-          <t>FreestandingWork18 rights holder</t>
+          <t>FreestandingWork18 image 0 rights holder</t>
         </is>
       </c>
       <c r="I272" t="inlineStr">
@@ -17741,7 +17741,7 @@
       </c>
       <c r="H273" t="inlineStr">
         <is>
-          <t>FreestandingWork18 rights holder</t>
+          <t>FreestandingWork18 image 1 rights holder</t>
         </is>
       </c>
       <c r="I273" t="inlineStr">
@@ -17788,7 +17788,7 @@
       </c>
       <c r="H274" t="inlineStr">
         <is>
-          <t>FreestandingWork19 rights holder</t>
+          <t>FreestandingWork19 image 0 rights holder</t>
         </is>
       </c>
       <c r="I274" t="inlineStr">
@@ -17835,7 +17835,7 @@
       </c>
       <c r="H275" t="inlineStr">
         <is>
-          <t>FreestandingWork19 rights holder</t>
+          <t>FreestandingWork19 image 1 rights holder</t>
         </is>
       </c>
       <c r="I275" t="inlineStr">
@@ -18157,7 +18157,7 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -18177,7 +18177,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18193,22 +18193,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>license</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
           <t>name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>rights</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>rightsHolderLiteral</t>
         </is>
       </c>
     </row>
@@ -18220,22 +18205,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
           <t>Institution0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Institution0 rights holder</t>
         </is>
       </c>
     </row>
@@ -18247,22 +18217,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
           <t>Institution1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Institution1 rights holder</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ensure the synthetic data pipeline runs
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -531,7 +531,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BSD License</t>
+          <t>BSD</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>MIT</t>
+          <t>MIT License</t>
         </is>
       </c>
     </row>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1420,7 +1420,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1459,7 +1459,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1614,7 +1614,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1653,7 +1653,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1691,7 +1691,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy, or moral rights may limit how you may use the material.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -18157,7 +18157,7 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">

</xml_diff>

<commit_message>
SyntheticDataPipeline: don't generate Work dcterms:created, dcterms:date, and other date predicates; generate WorkClosing and WorkOpening in addition to WorkCreation events
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -17,7 +17,9 @@
     <sheet name="Institution" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Collection" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="Work" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="WorkCreation" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="WorkClosing" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="WorkCreation" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="WorkOpening" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -487,13 +489,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,15 +506,87 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>@graph</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>@graph</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>@id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>cc:legalcode</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>cc:licenseClass</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>cc:permits</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>cc:requires</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
@@ -524,14 +598,18 @@
           <t>http://creativecommons.org/licenses/BSD/</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
         <is>
           <t>BSD</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>BSD</t>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>BSD License</t>
         </is>
       </c>
     </row>
@@ -541,12 +619,16 @@
           <t>http://creativecommons.org/licenses/by/1.0/</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
         <is>
           <t>by</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Attribution 1.0 Generic</t>
         </is>
@@ -558,12 +640,16 @@
           <t>http://creativecommons.org/licenses/by/2.0/</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
         <is>
           <t>by</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Attribution 2.0 Generic</t>
         </is>
@@ -575,12 +661,16 @@
           <t>http://creativecommons.org/licenses/by/2.5/</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
         <is>
           <t>by</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Attribution 2.5 Generic</t>
         </is>
@@ -592,12 +682,16 @@
           <t>http://creativecommons.org/licenses/by/3.0/</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
         <is>
           <t>by</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Attribution 3.0 Unported</t>
         </is>
@@ -609,12 +703,16 @@
           <t>http://creativecommons.org/licenses/by/4.0/</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
         <is>
           <t>by</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>Attribution 4.0 International</t>
         </is>
@@ -626,12 +724,16 @@
           <t>http://creativecommons.org/licenses/by-nc/1.0/</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
         <is>
           <t>by-nc</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>Attribution-NonCommercial 1.0 Generic</t>
         </is>
@@ -643,12 +745,16 @@
           <t>http://creativecommons.org/licenses/by-nc/2.0/</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
         <is>
           <t>by-nc</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>Attribution-NonCommercial 2.0 Generic</t>
         </is>
@@ -660,12 +766,16 @@
           <t>http://creativecommons.org/licenses/by-nc/2.5/</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
         <is>
           <t>by-nc</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>Attribution-NonCommercial 2.5 Generic</t>
         </is>
@@ -677,12 +787,16 @@
           <t>http://creativecommons.org/licenses/by-nc/3.0/</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
         <is>
           <t>by-nc</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>Attribution-NonCommercial 3.0 Unported</t>
         </is>
@@ -694,12 +808,16 @@
           <t>http://creativecommons.org/licenses/by-nc/4.0/</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
         <is>
           <t>by-nc</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>Attribution-NonCommercial 4.0 International</t>
         </is>
@@ -711,12 +829,16 @@
           <t>http://creativecommons.org/licenses/by-nc-nd/2.0/</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
         <is>
           <t>by-nc-nd</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>Attribution-NonCommercial-NoDerivs 2.0 Generic</t>
         </is>
@@ -728,12 +850,16 @@
           <t>http://creativecommons.org/licenses/by-nc-nd/2.5/</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
         <is>
           <t>by-nc-nd</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>Attribution-NonCommercial-NoDerivs 2.5 Generic</t>
         </is>
@@ -745,12 +871,16 @@
           <t>http://creativecommons.org/licenses/by-nc-nd/3.0/</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
         <is>
           <t>by-nc-nd</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>Attribution-NonCommercial-NoDerivs 3.0 Unported</t>
         </is>
@@ -762,12 +892,16 @@
           <t>http://creativecommons.org/licenses/by-nc-nd/4.0/</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
         <is>
           <t>by-nc-nd</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>Attribution-NonCommercial-NoDerivatives 4.0 International</t>
         </is>
@@ -779,12 +913,16 @@
           <t>http://creativecommons.org/licenses/by-nc-sa/1.0/</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
         <is>
           <t>by-nc-sa</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>Attribution-NonCommercial-ShareAlike 1.0 Generic</t>
         </is>
@@ -796,12 +934,16 @@
           <t>http://creativecommons.org/licenses/by-nc-sa/2.0/</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
         <is>
           <t>by-nc-sa</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>Attribution-NonCommercial-ShareAlike 2.0 Generic</t>
         </is>
@@ -813,12 +955,16 @@
           <t>http://creativecommons.org/licenses/by-nc-sa/2.5/</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
         <is>
           <t>by-nc-sa</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>Attribution-NonCommercial-ShareAlike 2.5 Generic</t>
         </is>
@@ -830,12 +976,16 @@
           <t>http://creativecommons.org/licenses/by-nc-sa/3.0/</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
         <is>
           <t>by-nc-sa</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>Attribution-NonCommercial-ShareAlike 3.0 Unported</t>
         </is>
@@ -847,12 +997,16 @@
           <t>http://creativecommons.org/licenses/by-nc-sa/4.0/</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
         <is>
           <t>by-nc-sa</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>Attribution-NonCommercial-ShareAlike 4.0 International</t>
         </is>
@@ -864,12 +1018,16 @@
           <t>http://creativecommons.org/licenses/by-nd/1.0/</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
         <is>
           <t>by-nd</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>Attribution-NoDerivs 1.0 Generic</t>
         </is>
@@ -881,12 +1039,16 @@
           <t>http://creativecommons.org/licenses/by-nd/2.0/</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
         <is>
           <t>by-nd</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>Attribution-NoDerivs 2.0 Generic</t>
         </is>
@@ -898,12 +1060,16 @@
           <t>http://creativecommons.org/licenses/by-nd/2.5/</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
         <is>
           <t>by-nd</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>Attribution-NoDerivs 2.5 Generic</t>
         </is>
@@ -915,12 +1081,16 @@
           <t>http://creativecommons.org/licenses/by-nd/3.0/</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
         <is>
           <t>by-nd</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>Attribution-NoDerivs 3.0 Unported</t>
         </is>
@@ -932,12 +1102,16 @@
           <t>http://creativecommons.org/licenses/by-nd/4.0/</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
         <is>
           <t>by-nd</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>Attribution-NoDerivatives 4.0 International</t>
         </is>
@@ -949,12 +1123,16 @@
           <t>http://creativecommons.org/licenses/by-nd-nc/1.0/</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
         <is>
           <t>by-nd-nc</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>Attribution-NoDerivs-NonCommercial 1.0 Generic</t>
         </is>
@@ -966,12 +1144,16 @@
           <t>http://creativecommons.org/licenses/by-sa/1.0/</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
         <is>
           <t>by-sa</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="G28" t="inlineStr">
         <is>
           <t>Attribution-ShareAlike 1.0 Generic</t>
         </is>
@@ -983,12 +1165,16 @@
           <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
         <is>
           <t>by-sa</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>Attribution-ShareAlike 2.0 Generic</t>
         </is>
@@ -1000,12 +1186,16 @@
           <t>http://creativecommons.org/licenses/by-sa/2.5/</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr">
         <is>
           <t>by-sa</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="G30" t="inlineStr">
         <is>
           <t>Attribution-ShareAlike 2.5 Generic</t>
         </is>
@@ -1017,12 +1207,16 @@
           <t>http://creativecommons.org/licenses/by-sa/3.0/</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
         <is>
           <t>by-sa</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="G31" t="inlineStr">
         <is>
           <t>Attribution-ShareAlike 3.0 Unported</t>
         </is>
@@ -1034,12 +1228,16 @@
           <t>http://creativecommons.org/licenses/by-sa/4.0/</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr">
         <is>
           <t>by-sa</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="G32" t="inlineStr">
         <is>
           <t>Attribution-ShareAlike 4.0 International</t>
         </is>
@@ -1051,12 +1249,16 @@
           <t>http://creativecommons.org/publicdomain/zero/1.0/</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
         <is>
           <t>CC0</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="G33" t="inlineStr">
         <is>
           <t>CC0 1.0 Universal</t>
         </is>
@@ -1068,12 +1270,16 @@
           <t>http://creativecommons.org/licenses/devnations/2.0/</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr">
         <is>
           <t>devnations</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="G34" t="inlineStr">
         <is>
           <t>Developing Nations License</t>
         </is>
@@ -1085,12 +1291,16 @@
           <t>http://creativecommons.org/licenses/GPL/2.0/</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
         <is>
           <t>GPL</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="G35" t="inlineStr">
         <is>
           <t>GNU General Public License</t>
         </is>
@@ -1102,12 +1312,16 @@
           <t>http://creativecommons.org/licenses/LGPL/2.1/</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr">
         <is>
           <t>LGPL</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="G36" t="inlineStr">
         <is>
           <t>GNU Lesser General Public License</t>
         </is>
@@ -1119,12 +1333,16 @@
           <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr">
         <is>
           <t>mark</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="G37" t="inlineStr">
         <is>
           <t>Public Domain Mark 1.0</t>
         </is>
@@ -1136,14 +1354,18 @@
           <t>http://creativecommons.org/licenses/MIT/</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr">
         <is>
           <t>MIT</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>MIT License</t>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>MIT</t>
         </is>
       </c>
     </row>
@@ -1153,12 +1375,16 @@
           <t>http://creativecommons.org/licenses/nc/1.0/</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr">
         <is>
           <t>nc</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="G39" t="inlineStr">
         <is>
           <t>NonCommercial 1.0 Generic</t>
         </is>
@@ -1170,12 +1396,16 @@
           <t>http://creativecommons.org/licenses/nc-sampling+/1.0/</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr">
         <is>
           <t>nc-sampling+</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="G40" t="inlineStr">
         <is>
           <t>NonCommercial Sampling Plus 1.0</t>
         </is>
@@ -1187,12 +1417,16 @@
           <t>http://creativecommons.org/licenses/nc-sa/1.0/</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr">
         <is>
           <t>nc-sa</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="G41" t="inlineStr">
         <is>
           <t>NonCommercial-ShareAlike 1.0 Generic</t>
         </is>
@@ -1204,12 +1438,16 @@
           <t>http://creativecommons.org/licenses/nd/1.0/</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr">
         <is>
           <t>nd</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="G42" t="inlineStr">
         <is>
           <t>NoDerivs 1.0 Generic</t>
         </is>
@@ -1221,12 +1459,16 @@
           <t>http://creativecommons.org/licenses/nd-nc/1.0/</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr">
         <is>
           <t>nd-nc</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="G43" t="inlineStr">
         <is>
           <t>NoDerivs-NonCommercial 1.0 Generic</t>
         </is>
@@ -1238,12 +1480,16 @@
           <t>http://creativecommons.org/licenses/publicdomain/</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr">
         <is>
           <t>publicdomain</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="G44" t="inlineStr">
         <is>
           <t>Public Domain</t>
         </is>
@@ -1255,12 +1501,16 @@
           <t>http://creativecommons.org/licenses/sampling/1.0/</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr">
         <is>
           <t>sampling</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="G45" t="inlineStr">
         <is>
           <t>Sampling 1.0</t>
         </is>
@@ -1272,12 +1522,16 @@
           <t>http://creativecommons.org/licenses/sampling+/1.0/</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr">
         <is>
           <t>sampling+</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="G46" t="inlineStr">
         <is>
           <t>Sampling Plus 1.0</t>
         </is>
@@ -1289,12 +1543,16 @@
           <t>http://creativecommons.org/licenses/sa/1.0/</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr">
         <is>
           <t>sa</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="G47" t="inlineStr">
         <is>
           <t>ShareAlike 1.0 Generic</t>
         </is>
@@ -1420,7 +1678,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1498,7 +1756,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1537,7 +1795,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1614,7 +1872,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1653,7 +1911,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1730,7 +1988,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1807,7 +2065,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -18025,7 +18283,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -18091,7 +18349,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -18157,7 +18415,7 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">

</xml_diff>

<commit_message>
remove institution from SyntheticDataPipeline
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -14,12 +14,11 @@
     <sheet name="Image" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Organization" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Person" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Institution" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Collection" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Work" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="WorkClosing" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="WorkCreation" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="WorkOpening" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Collection" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Work" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="WorkClosing" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="WorkCreation" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="WorkOpening" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -515,32 +514,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>@graph</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -609,7 +582,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>BSD</t>
+          <t>BSD License</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1338,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>MIT</t>
+          <t>MIT License</t>
         </is>
       </c>
     </row>
@@ -1678,7 +1651,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1717,7 +1690,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1795,7 +1768,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>If you have any information that can contribute to identifying or locating the rights-holder(s), please notify the organization that has made the Item available.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1833,7 +1806,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>If you have any information that can contribute to identifying or locating the rights-holder(s) please notify the organization that has made the Item available.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1872,7 +1845,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1911,7 +1884,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1988,7 +1961,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -5169,7 +5142,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I275"/>
+  <dimension ref="A1:I257"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16037,7 +16010,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0Image0</t>
+          <t>https://place-hold.it/1000x1000?text=Collection0Work0Image0</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -16047,12 +16020,12 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>Institution0 image 0</t>
+          <t>Collection0Work0 image 0</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>http://example.com/institution0</t>
+          <t>http://example.com/collection0/work0</t>
         </is>
       </c>
       <c r="E232" t="inlineStr">
@@ -16072,7 +16045,7 @@
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>Institution0 image 0 rights holder</t>
+          <t>Collection0Work0 image 0 rights holder</t>
         </is>
       </c>
       <c r="I232" t="inlineStr">
@@ -16084,7 +16057,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0Image1</t>
+          <t>https://place-hold.it/1000x1000?text=Collection0Work0Image1</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
@@ -16094,12 +16067,12 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>Institution0 image 1</t>
+          <t>Collection0Work0 image 1</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>http://example.com/institution0</t>
+          <t>http://example.com/collection0/work0</t>
         </is>
       </c>
       <c r="E233" t="inlineStr">
@@ -16119,7 +16092,7 @@
       </c>
       <c r="H233" t="inlineStr">
         <is>
-          <t>Institution0 image 1 rights holder</t>
+          <t>Collection0Work0 image 1 rights holder</t>
         </is>
       </c>
       <c r="I233" t="inlineStr">
@@ -16131,7 +16104,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0Collection0Work0Image0</t>
+          <t>https://place-hold.it/1000x1000?text=Collection0Work1Image0</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -16141,12 +16114,12 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work0 image 0</t>
+          <t>Collection0Work1 image 0</t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>http://example.com/institution0/collection0/work0</t>
+          <t>http://example.com/collection0/work1</t>
         </is>
       </c>
       <c r="E234" t="inlineStr">
@@ -16166,7 +16139,7 @@
       </c>
       <c r="H234" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work0 image 0 rights holder</t>
+          <t>Collection0Work1 image 0 rights holder</t>
         </is>
       </c>
       <c r="I234" t="inlineStr">
@@ -16178,7 +16151,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0Collection0Work0Image1</t>
+          <t>https://place-hold.it/1000x1000?text=Collection0Work1Image1</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -16188,12 +16161,12 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work0 image 1</t>
+          <t>Collection0Work1 image 1</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>http://example.com/institution0/collection0/work0</t>
+          <t>http://example.com/collection0/work1</t>
         </is>
       </c>
       <c r="E235" t="inlineStr">
@@ -16213,7 +16186,7 @@
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work0 image 1 rights holder</t>
+          <t>Collection0Work1 image 1 rights holder</t>
         </is>
       </c>
       <c r="I235" t="inlineStr">
@@ -16225,7 +16198,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0Collection0Work1Image0</t>
+          <t>https://place-hold.it/1000x1000?text=Collection0Work2Image0</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -16235,12 +16208,12 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work1 image 0</t>
+          <t>Collection0Work2 image 0</t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>http://example.com/institution0/collection0/work1</t>
+          <t>http://example.com/collection0/work2</t>
         </is>
       </c>
       <c r="E236" t="inlineStr">
@@ -16260,7 +16233,7 @@
       </c>
       <c r="H236" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work1 image 0 rights holder</t>
+          <t>Collection0Work2 image 0 rights holder</t>
         </is>
       </c>
       <c r="I236" t="inlineStr">
@@ -16272,7 +16245,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0Collection0Work1Image1</t>
+          <t>https://place-hold.it/1000x1000?text=Collection0Work2Image1</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -16282,12 +16255,12 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work1 image 1</t>
+          <t>Collection0Work2 image 1</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>http://example.com/institution0/collection0/work1</t>
+          <t>http://example.com/collection0/work2</t>
         </is>
       </c>
       <c r="E237" t="inlineStr">
@@ -16307,7 +16280,7 @@
       </c>
       <c r="H237" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work1 image 1 rights holder</t>
+          <t>Collection0Work2 image 1 rights holder</t>
         </is>
       </c>
       <c r="I237" t="inlineStr">
@@ -16319,7 +16292,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0Collection0Work2Image0</t>
+          <t>https://place-hold.it/1000x1000?text=Collection0Work3Image0</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -16329,12 +16302,12 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work2 image 0</t>
+          <t>Collection0Work3 image 0</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>http://example.com/institution0/collection0/work2</t>
+          <t>http://example.com/collection0/work3</t>
         </is>
       </c>
       <c r="E238" t="inlineStr">
@@ -16354,7 +16327,7 @@
       </c>
       <c r="H238" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work2 image 0 rights holder</t>
+          <t>Collection0Work3 image 0 rights holder</t>
         </is>
       </c>
       <c r="I238" t="inlineStr">
@@ -16366,7 +16339,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0Collection0Work2Image1</t>
+          <t>https://place-hold.it/1000x1000?text=Collection0Work3Image1</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -16376,12 +16349,12 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work2 image 1</t>
+          <t>Collection0Work3 image 1</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>http://example.com/institution0/collection0/work2</t>
+          <t>http://example.com/collection0/work3</t>
         </is>
       </c>
       <c r="E239" t="inlineStr">
@@ -16401,7 +16374,7 @@
       </c>
       <c r="H239" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work2 image 1 rights holder</t>
+          <t>Collection0Work3 image 1 rights holder</t>
         </is>
       </c>
       <c r="I239" t="inlineStr">
@@ -16413,7 +16386,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0Collection0Work3Image0</t>
+          <t>https://place-hold.it/1000x1000?text=Collection1Image0</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -16423,12 +16396,12 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work3 image 0</t>
+          <t>Collection1 image 0</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>http://example.com/institution0/collection0/work3</t>
+          <t>http://example.com/collection1</t>
         </is>
       </c>
       <c r="E240" t="inlineStr">
@@ -16448,7 +16421,7 @@
       </c>
       <c r="H240" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work3 image 0 rights holder</t>
+          <t>Collection1 image 0 rights holder</t>
         </is>
       </c>
       <c r="I240" t="inlineStr">
@@ -16460,7 +16433,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0Collection0Work3Image1</t>
+          <t>https://place-hold.it/1000x1000?text=Collection1Image1</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -16470,12 +16443,12 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work3 image 1</t>
+          <t>Collection1 image 1</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>http://example.com/institution0/collection0/work3</t>
+          <t>http://example.com/collection1</t>
         </is>
       </c>
       <c r="E241" t="inlineStr">
@@ -16495,7 +16468,7 @@
       </c>
       <c r="H241" t="inlineStr">
         <is>
-          <t>Institution0Collection0Work3 image 1 rights holder</t>
+          <t>Collection1 image 1 rights holder</t>
         </is>
       </c>
       <c r="I241" t="inlineStr">
@@ -16507,7 +16480,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0SharedWork4Image0</t>
+          <t>https://place-hold.it/1000x1000?text=Collection1Work4Image0</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -16517,12 +16490,12 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>Institution0SharedWork4 image 0</t>
+          <t>Collection1Work4 image 0</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>http://example.com/institution0/shared/work4</t>
+          <t>http://example.com/collection1/work4</t>
         </is>
       </c>
       <c r="E242" t="inlineStr">
@@ -16542,7 +16515,7 @@
       </c>
       <c r="H242" t="inlineStr">
         <is>
-          <t>Institution0SharedWork4 image 0 rights holder</t>
+          <t>Collection1Work4 image 0 rights holder</t>
         </is>
       </c>
       <c r="I242" t="inlineStr">
@@ -16554,7 +16527,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0SharedWork4Image1</t>
+          <t>https://place-hold.it/1000x1000?text=Collection1Work4Image1</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -16564,12 +16537,12 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>Institution0SharedWork4 image 1</t>
+          <t>Collection1Work4 image 1</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>http://example.com/institution0/shared/work4</t>
+          <t>http://example.com/collection1/work4</t>
         </is>
       </c>
       <c r="E243" t="inlineStr">
@@ -16589,7 +16562,7 @@
       </c>
       <c r="H243" t="inlineStr">
         <is>
-          <t>Institution0SharedWork4 image 1 rights holder</t>
+          <t>Collection1Work4 image 1 rights holder</t>
         </is>
       </c>
       <c r="I243" t="inlineStr">
@@ -16601,7 +16574,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0SharedWork5Image0</t>
+          <t>https://place-hold.it/1000x1000?text=Collection1Work5Image0</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -16611,12 +16584,12 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>Institution0SharedWork5 image 0</t>
+          <t>Collection1Work5 image 0</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>http://example.com/institution0/shared/work5</t>
+          <t>http://example.com/collection1/work5</t>
         </is>
       </c>
       <c r="E244" t="inlineStr">
@@ -16636,7 +16609,7 @@
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>Institution0SharedWork5 image 0 rights holder</t>
+          <t>Collection1Work5 image 0 rights holder</t>
         </is>
       </c>
       <c r="I244" t="inlineStr">
@@ -16648,7 +16621,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0SharedWork5Image1</t>
+          <t>https://place-hold.it/1000x1000?text=Collection1Work5Image1</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -16658,12 +16631,12 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>Institution0SharedWork5 image 1</t>
+          <t>Collection1Work5 image 1</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>http://example.com/institution0/shared/work5</t>
+          <t>http://example.com/collection1/work5</t>
         </is>
       </c>
       <c r="E245" t="inlineStr">
@@ -16683,7 +16656,7 @@
       </c>
       <c r="H245" t="inlineStr">
         <is>
-          <t>Institution0SharedWork5 image 1 rights holder</t>
+          <t>Collection1Work5 image 1 rights holder</t>
         </is>
       </c>
       <c r="I245" t="inlineStr">
@@ -16695,7 +16668,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0SharedWork6Image0</t>
+          <t>https://place-hold.it/1000x1000?text=Collection1Work6Image0</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -16705,12 +16678,12 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>Institution0SharedWork6 image 0</t>
+          <t>Collection1Work6 image 0</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>http://example.com/institution0/shared/work6</t>
+          <t>http://example.com/collection1/work6</t>
         </is>
       </c>
       <c r="E246" t="inlineStr">
@@ -16730,7 +16703,7 @@
       </c>
       <c r="H246" t="inlineStr">
         <is>
-          <t>Institution0SharedWork6 image 0 rights holder</t>
+          <t>Collection1Work6 image 0 rights holder</t>
         </is>
       </c>
       <c r="I246" t="inlineStr">
@@ -16742,7 +16715,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0SharedWork6Image1</t>
+          <t>https://place-hold.it/1000x1000?text=Collection1Work6Image1</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
@@ -16752,12 +16725,12 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>Institution0SharedWork6 image 1</t>
+          <t>Collection1Work6 image 1</t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>http://example.com/institution0/shared/work6</t>
+          <t>http://example.com/collection1/work6</t>
         </is>
       </c>
       <c r="E247" t="inlineStr">
@@ -16777,7 +16750,7 @@
       </c>
       <c r="H247" t="inlineStr">
         <is>
-          <t>Institution0SharedWork6 image 1 rights holder</t>
+          <t>Collection1Work6 image 1 rights holder</t>
         </is>
       </c>
       <c r="I247" t="inlineStr">
@@ -16789,7 +16762,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0SharedWork7Image0</t>
+          <t>https://place-hold.it/1000x1000?text=Collection1Work7Image0</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -16799,12 +16772,12 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>Institution0SharedWork7 image 0</t>
+          <t>Collection1Work7 image 0</t>
         </is>
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>http://example.com/institution0/shared/work7</t>
+          <t>http://example.com/collection1/work7</t>
         </is>
       </c>
       <c r="E248" t="inlineStr">
@@ -16824,7 +16797,7 @@
       </c>
       <c r="H248" t="inlineStr">
         <is>
-          <t>Institution0SharedWork7 image 0 rights holder</t>
+          <t>Collection1Work7 image 0 rights holder</t>
         </is>
       </c>
       <c r="I248" t="inlineStr">
@@ -16836,7 +16809,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution0SharedWork7Image1</t>
+          <t>https://place-hold.it/1000x1000?text=Collection1Work7Image1</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -16846,12 +16819,12 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>Institution0SharedWork7 image 1</t>
+          <t>Collection1Work7 image 1</t>
         </is>
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>http://example.com/institution0/shared/work7</t>
+          <t>http://example.com/collection1/work7</t>
         </is>
       </c>
       <c r="E249" t="inlineStr">
@@ -16871,7 +16844,7 @@
       </c>
       <c r="H249" t="inlineStr">
         <is>
-          <t>Institution0SharedWork7 image 1 rights holder</t>
+          <t>Collection1Work7 image 1 rights holder</t>
         </is>
       </c>
       <c r="I249" t="inlineStr">
@@ -16883,7 +16856,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1Image0</t>
+          <t>https://place-hold.it/1000x1000?text=FreestandingWork8Image0</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -16893,12 +16866,12 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>Institution1 image 0</t>
+          <t>FreestandingWork8 image 0</t>
         </is>
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>http://example.com/institution1</t>
+          <t>http://example.com/freestandingwork8</t>
         </is>
       </c>
       <c r="E250" t="inlineStr">
@@ -16918,7 +16891,7 @@
       </c>
       <c r="H250" t="inlineStr">
         <is>
-          <t>Institution1 image 0 rights holder</t>
+          <t>FreestandingWork8 image 0 rights holder</t>
         </is>
       </c>
       <c r="I250" t="inlineStr">
@@ -16930,7 +16903,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1Image1</t>
+          <t>https://place-hold.it/1000x1000?text=FreestandingWork8Image1</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -16940,12 +16913,12 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>Institution1 image 1</t>
+          <t>FreestandingWork8 image 1</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>http://example.com/institution1</t>
+          <t>http://example.com/freestandingwork8</t>
         </is>
       </c>
       <c r="E251" t="inlineStr">
@@ -16965,7 +16938,7 @@
       </c>
       <c r="H251" t="inlineStr">
         <is>
-          <t>Institution1 image 1 rights holder</t>
+          <t>FreestandingWork8 image 1 rights holder</t>
         </is>
       </c>
       <c r="I251" t="inlineStr">
@@ -16977,7 +16950,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1Collection0Work8Image0</t>
+          <t>https://place-hold.it/1000x1000?text=FreestandingWork9Image0</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -16987,12 +16960,12 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work8 image 0</t>
+          <t>FreestandingWork9 image 0</t>
         </is>
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>http://example.com/institution1/collection0/work8</t>
+          <t>http://example.com/freestandingwork9</t>
         </is>
       </c>
       <c r="E252" t="inlineStr">
@@ -17012,7 +16985,7 @@
       </c>
       <c r="H252" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work8 image 0 rights holder</t>
+          <t>FreestandingWork9 image 0 rights holder</t>
         </is>
       </c>
       <c r="I252" t="inlineStr">
@@ -17024,7 +16997,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1Collection0Work8Image1</t>
+          <t>https://place-hold.it/1000x1000?text=FreestandingWork9Image1</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -17034,12 +17007,12 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work8 image 1</t>
+          <t>FreestandingWork9 image 1</t>
         </is>
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>http://example.com/institution1/collection0/work8</t>
+          <t>http://example.com/freestandingwork9</t>
         </is>
       </c>
       <c r="E253" t="inlineStr">
@@ -17059,7 +17032,7 @@
       </c>
       <c r="H253" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work8 image 1 rights holder</t>
+          <t>FreestandingWork9 image 1 rights holder</t>
         </is>
       </c>
       <c r="I253" t="inlineStr">
@@ -17071,7 +17044,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1Collection0Work9Image0</t>
+          <t>https://place-hold.it/1000x1000?text=FreestandingWork10Image0</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
@@ -17081,12 +17054,12 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work9 image 0</t>
+          <t>FreestandingWork10 image 0</t>
         </is>
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>http://example.com/institution1/collection0/work9</t>
+          <t>http://example.com/freestandingwork10</t>
         </is>
       </c>
       <c r="E254" t="inlineStr">
@@ -17106,7 +17079,7 @@
       </c>
       <c r="H254" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work9 image 0 rights holder</t>
+          <t>FreestandingWork10 image 0 rights holder</t>
         </is>
       </c>
       <c r="I254" t="inlineStr">
@@ -17118,7 +17091,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1Collection0Work9Image1</t>
+          <t>https://place-hold.it/1000x1000?text=FreestandingWork10Image1</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
@@ -17128,12 +17101,12 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work9 image 1</t>
+          <t>FreestandingWork10 image 1</t>
         </is>
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>http://example.com/institution1/collection0/work9</t>
+          <t>http://example.com/freestandingwork10</t>
         </is>
       </c>
       <c r="E255" t="inlineStr">
@@ -17153,7 +17126,7 @@
       </c>
       <c r="H255" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work9 image 1 rights holder</t>
+          <t>FreestandingWork10 image 1 rights holder</t>
         </is>
       </c>
       <c r="I255" t="inlineStr">
@@ -17165,7 +17138,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1Collection0Work10Image0</t>
+          <t>https://place-hold.it/1000x1000?text=FreestandingWork11Image0</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -17175,12 +17148,12 @@
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work10 image 0</t>
+          <t>FreestandingWork11 image 0</t>
         </is>
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>http://example.com/institution1/collection0/work10</t>
+          <t>http://example.com/freestandingwork11</t>
         </is>
       </c>
       <c r="E256" t="inlineStr">
@@ -17200,7 +17173,7 @@
       </c>
       <c r="H256" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work10 image 0 rights holder</t>
+          <t>FreestandingWork11 image 0 rights holder</t>
         </is>
       </c>
       <c r="I256" t="inlineStr">
@@ -17212,7 +17185,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1Collection0Work10Image1</t>
+          <t>https://place-hold.it/1000x1000?text=FreestandingWork11Image1</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -17222,12 +17195,12 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work10 image 1</t>
+          <t>FreestandingWork11 image 1</t>
         </is>
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>http://example.com/institution1/collection0/work10</t>
+          <t>http://example.com/freestandingwork11</t>
         </is>
       </c>
       <c r="E257" t="inlineStr">
@@ -17247,856 +17220,10 @@
       </c>
       <c r="H257" t="inlineStr">
         <is>
-          <t>Institution1Collection0Work10 image 1 rights holder</t>
+          <t>FreestandingWork11 image 1 rights holder</t>
         </is>
       </c>
       <c r="I257" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="258">
-      <c r="A258" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1Collection0Work11Image0</t>
-        </is>
-      </c>
-      <c r="B258" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C258" t="inlineStr">
-        <is>
-          <t>Institution1Collection0Work11 image 0</t>
-        </is>
-      </c>
-      <c r="D258" t="inlineStr">
-        <is>
-          <t>http://example.com/institution1/collection0/work11</t>
-        </is>
-      </c>
-      <c r="E258" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F258" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G258" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H258" t="inlineStr">
-        <is>
-          <t>Institution1Collection0Work11 image 0 rights holder</t>
-        </is>
-      </c>
-      <c r="I258" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="259">
-      <c r="A259" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1Collection0Work11Image1</t>
-        </is>
-      </c>
-      <c r="B259" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C259" t="inlineStr">
-        <is>
-          <t>Institution1Collection0Work11 image 1</t>
-        </is>
-      </c>
-      <c r="D259" t="inlineStr">
-        <is>
-          <t>http://example.com/institution1/collection0/work11</t>
-        </is>
-      </c>
-      <c r="E259" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F259" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G259" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H259" t="inlineStr">
-        <is>
-          <t>Institution1Collection0Work11 image 1 rights holder</t>
-        </is>
-      </c>
-      <c r="I259" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="260">
-      <c r="A260" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1SharedWork12Image0</t>
-        </is>
-      </c>
-      <c r="B260" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C260" t="inlineStr">
-        <is>
-          <t>Institution1SharedWork12 image 0</t>
-        </is>
-      </c>
-      <c r="D260" t="inlineStr">
-        <is>
-          <t>http://example.com/institution1/shared/work12</t>
-        </is>
-      </c>
-      <c r="E260" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F260" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G260" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H260" t="inlineStr">
-        <is>
-          <t>Institution1SharedWork12 image 0 rights holder</t>
-        </is>
-      </c>
-      <c r="I260" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="261">
-      <c r="A261" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1SharedWork12Image1</t>
-        </is>
-      </c>
-      <c r="B261" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C261" t="inlineStr">
-        <is>
-          <t>Institution1SharedWork12 image 1</t>
-        </is>
-      </c>
-      <c r="D261" t="inlineStr">
-        <is>
-          <t>http://example.com/institution1/shared/work12</t>
-        </is>
-      </c>
-      <c r="E261" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F261" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G261" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H261" t="inlineStr">
-        <is>
-          <t>Institution1SharedWork12 image 1 rights holder</t>
-        </is>
-      </c>
-      <c r="I261" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="262">
-      <c r="A262" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1SharedWork13Image0</t>
-        </is>
-      </c>
-      <c r="B262" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C262" t="inlineStr">
-        <is>
-          <t>Institution1SharedWork13 image 0</t>
-        </is>
-      </c>
-      <c r="D262" t="inlineStr">
-        <is>
-          <t>http://example.com/institution1/shared/work13</t>
-        </is>
-      </c>
-      <c r="E262" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F262" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G262" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H262" t="inlineStr">
-        <is>
-          <t>Institution1SharedWork13 image 0 rights holder</t>
-        </is>
-      </c>
-      <c r="I262" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="263">
-      <c r="A263" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1SharedWork13Image1</t>
-        </is>
-      </c>
-      <c r="B263" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C263" t="inlineStr">
-        <is>
-          <t>Institution1SharedWork13 image 1</t>
-        </is>
-      </c>
-      <c r="D263" t="inlineStr">
-        <is>
-          <t>http://example.com/institution1/shared/work13</t>
-        </is>
-      </c>
-      <c r="E263" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F263" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G263" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H263" t="inlineStr">
-        <is>
-          <t>Institution1SharedWork13 image 1 rights holder</t>
-        </is>
-      </c>
-      <c r="I263" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="264">
-      <c r="A264" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1SharedWork14Image0</t>
-        </is>
-      </c>
-      <c r="B264" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C264" t="inlineStr">
-        <is>
-          <t>Institution1SharedWork14 image 0</t>
-        </is>
-      </c>
-      <c r="D264" t="inlineStr">
-        <is>
-          <t>http://example.com/institution1/shared/work14</t>
-        </is>
-      </c>
-      <c r="E264" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F264" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G264" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H264" t="inlineStr">
-        <is>
-          <t>Institution1SharedWork14 image 0 rights holder</t>
-        </is>
-      </c>
-      <c r="I264" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="265">
-      <c r="A265" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1SharedWork14Image1</t>
-        </is>
-      </c>
-      <c r="B265" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C265" t="inlineStr">
-        <is>
-          <t>Institution1SharedWork14 image 1</t>
-        </is>
-      </c>
-      <c r="D265" t="inlineStr">
-        <is>
-          <t>http://example.com/institution1/shared/work14</t>
-        </is>
-      </c>
-      <c r="E265" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F265" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G265" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H265" t="inlineStr">
-        <is>
-          <t>Institution1SharedWork14 image 1 rights holder</t>
-        </is>
-      </c>
-      <c r="I265" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="266">
-      <c r="A266" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1SharedWork15Image0</t>
-        </is>
-      </c>
-      <c r="B266" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C266" t="inlineStr">
-        <is>
-          <t>Institution1SharedWork15 image 0</t>
-        </is>
-      </c>
-      <c r="D266" t="inlineStr">
-        <is>
-          <t>http://example.com/institution1/shared/work15</t>
-        </is>
-      </c>
-      <c r="E266" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F266" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G266" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H266" t="inlineStr">
-        <is>
-          <t>Institution1SharedWork15 image 0 rights holder</t>
-        </is>
-      </c>
-      <c r="I266" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="267">
-      <c r="A267" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=Institution1SharedWork15Image1</t>
-        </is>
-      </c>
-      <c r="B267" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C267" t="inlineStr">
-        <is>
-          <t>Institution1SharedWork15 image 1</t>
-        </is>
-      </c>
-      <c r="D267" t="inlineStr">
-        <is>
-          <t>http://example.com/institution1/shared/work15</t>
-        </is>
-      </c>
-      <c r="E267" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F267" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G267" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H267" t="inlineStr">
-        <is>
-          <t>Institution1SharedWork15 image 1 rights holder</t>
-        </is>
-      </c>
-      <c r="I267" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="268">
-      <c r="A268" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=FreestandingWork16Image0</t>
-        </is>
-      </c>
-      <c r="B268" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C268" t="inlineStr">
-        <is>
-          <t>FreestandingWork16 image 0</t>
-        </is>
-      </c>
-      <c r="D268" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork16</t>
-        </is>
-      </c>
-      <c r="E268" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F268" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G268" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H268" t="inlineStr">
-        <is>
-          <t>FreestandingWork16 image 0 rights holder</t>
-        </is>
-      </c>
-      <c r="I268" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="269">
-      <c r="A269" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=FreestandingWork16Image1</t>
-        </is>
-      </c>
-      <c r="B269" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C269" t="inlineStr">
-        <is>
-          <t>FreestandingWork16 image 1</t>
-        </is>
-      </c>
-      <c r="D269" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork16</t>
-        </is>
-      </c>
-      <c r="E269" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F269" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G269" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H269" t="inlineStr">
-        <is>
-          <t>FreestandingWork16 image 1 rights holder</t>
-        </is>
-      </c>
-      <c r="I269" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="270">
-      <c r="A270" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=FreestandingWork17Image0</t>
-        </is>
-      </c>
-      <c r="B270" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C270" t="inlineStr">
-        <is>
-          <t>FreestandingWork17 image 0</t>
-        </is>
-      </c>
-      <c r="D270" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork17</t>
-        </is>
-      </c>
-      <c r="E270" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F270" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G270" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H270" t="inlineStr">
-        <is>
-          <t>FreestandingWork17 image 0 rights holder</t>
-        </is>
-      </c>
-      <c r="I270" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="271">
-      <c r="A271" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=FreestandingWork17Image1</t>
-        </is>
-      </c>
-      <c r="B271" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C271" t="inlineStr">
-        <is>
-          <t>FreestandingWork17 image 1</t>
-        </is>
-      </c>
-      <c r="D271" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork17</t>
-        </is>
-      </c>
-      <c r="E271" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F271" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G271" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H271" t="inlineStr">
-        <is>
-          <t>FreestandingWork17 image 1 rights holder</t>
-        </is>
-      </c>
-      <c r="I271" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="272">
-      <c r="A272" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=FreestandingWork18Image0</t>
-        </is>
-      </c>
-      <c r="B272" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C272" t="inlineStr">
-        <is>
-          <t>FreestandingWork18 image 0</t>
-        </is>
-      </c>
-      <c r="D272" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork18</t>
-        </is>
-      </c>
-      <c r="E272" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F272" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G272" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H272" t="inlineStr">
-        <is>
-          <t>FreestandingWork18 image 0 rights holder</t>
-        </is>
-      </c>
-      <c r="I272" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="273">
-      <c r="A273" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=FreestandingWork18Image1</t>
-        </is>
-      </c>
-      <c r="B273" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C273" t="inlineStr">
-        <is>
-          <t>FreestandingWork18 image 1</t>
-        </is>
-      </c>
-      <c r="D273" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork18</t>
-        </is>
-      </c>
-      <c r="E273" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F273" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G273" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H273" t="inlineStr">
-        <is>
-          <t>FreestandingWork18 image 1 rights holder</t>
-        </is>
-      </c>
-      <c r="I273" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="274">
-      <c r="A274" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=FreestandingWork19Image0</t>
-        </is>
-      </c>
-      <c r="B274" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C274" t="inlineStr">
-        <is>
-          <t>FreestandingWork19 image 0</t>
-        </is>
-      </c>
-      <c r="D274" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork19</t>
-        </is>
-      </c>
-      <c r="E274" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F274" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G274" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H274" t="inlineStr">
-        <is>
-          <t>FreestandingWork19 image 0 rights holder</t>
-        </is>
-      </c>
-      <c r="I274" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="275">
-      <c r="A275" t="inlineStr">
-        <is>
-          <t>https://place-hold.it/1000x1000?text=FreestandingWork19Image1</t>
-        </is>
-      </c>
-      <c r="B275" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="C275" t="inlineStr">
-        <is>
-          <t>FreestandingWork19 image 1</t>
-        </is>
-      </c>
-      <c r="D275" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork19</t>
-        </is>
-      </c>
-      <c r="E275" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F275" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="G275" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="H275" t="inlineStr">
-        <is>
-          <t>FreestandingWork19 image 1 rights holder</t>
-        </is>
-      </c>
-      <c r="I275" t="inlineStr">
         <is>
           <t>1000</t>
         </is>
@@ -18283,7 +17410,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -18316,7 +17443,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -18349,7 +17476,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -18382,7 +17509,7 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -18435,7 +17562,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18446,36 +17573,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>@id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>http://example.com/institution0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Institution0</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>http://example.com/institution1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Institution1</t>
+          <t>@graph</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
py: regenerate synthetic data
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="NamedValue" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Concept" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Image" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Organization" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Person" sheetId="5" state="visible" r:id="rId5"/>
@@ -674,7 +674,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E111"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -700,11 +700,6 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
           <t>value</t>
         </is>
       </c>
@@ -712,7 +707,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -722,15 +717,10 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Named value 0</t>
+          <t>Concept 0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
-        <is>
-          <t>Named value 0</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
         <is>
           <t>Cultural context 0</t>
         </is>
@@ -739,7 +729,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -749,15 +739,10 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Named value 1</t>
+          <t>Concept 1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
-        <is>
-          <t>Named value 1</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
         <is>
           <t>Cultural context 1</t>
         </is>
@@ -766,7 +751,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:2</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -776,15 +761,10 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Named value 2</t>
+          <t>Concept 2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
-        <is>
-          <t>Named value 2</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
         <is>
           <t>Cultural context 2</t>
         </is>
@@ -793,7 +773,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:3</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -803,15 +783,10 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Named value 3</t>
+          <t>Concept 3</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
-        <is>
-          <t>Named value 3</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
         <is>
           <t>Cultural context 3</t>
         </is>
@@ -820,7 +795,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:4</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -830,15 +805,10 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Named value 4</t>
+          <t>Concept 4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
-        <is>
-          <t>Named value 4</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
         <is>
           <t>Cultural context 4</t>
         </is>
@@ -847,7 +817,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:5</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -857,15 +827,10 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Named value 5</t>
+          <t>Concept 5</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
-        <is>
-          <t>Named value 5</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
         <is>
           <t>Cultural context 5</t>
         </is>
@@ -874,7 +839,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:6</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -884,15 +849,10 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Named value 6</t>
+          <t>Concept 6</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
-        <is>
-          <t>Named value 6</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
         <is>
           <t>Cultural context 6</t>
         </is>
@@ -901,7 +861,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:7</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -911,15 +871,10 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Named value 7</t>
+          <t>Concept 7</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
-        <is>
-          <t>Named value 7</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
         <is>
           <t>Cultural context 7</t>
         </is>
@@ -928,7 +883,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:8</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -938,15 +893,10 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Named value 8</t>
+          <t>Concept 8</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
-        <is>
-          <t>Named value 8</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
         <is>
           <t>Cultural context 8</t>
         </is>
@@ -955,7 +905,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:9</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -965,15 +915,10 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Named value 9</t>
+          <t>Concept 9</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
-        <is>
-          <t>Named value 9</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
         <is>
           <t>Cultural context 9</t>
         </is>
@@ -982,7 +927,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:10</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -992,15 +937,10 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Named value 10</t>
+          <t>Concept 10</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
-        <is>
-          <t>Named value 10</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
         <is>
           <t>Extent 0</t>
         </is>
@@ -1009,7 +949,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:11</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1019,15 +959,10 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Named value 11</t>
+          <t>Concept 11</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
-        <is>
-          <t>Named value 11</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
         <is>
           <t>Extent 1</t>
         </is>
@@ -1036,7 +971,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:12</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1046,15 +981,10 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Named value 12</t>
+          <t>Concept 12</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
-        <is>
-          <t>Named value 12</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
         <is>
           <t>Extent 2</t>
         </is>
@@ -1063,7 +993,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:13</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1073,15 +1003,10 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Named value 13</t>
+          <t>Concept 13</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
-        <is>
-          <t>Named value 13</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
         <is>
           <t>Extent 3</t>
         </is>
@@ -1090,7 +1015,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:14</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1100,15 +1025,10 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Named value 14</t>
+          <t>Concept 14</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
-        <is>
-          <t>Named value 14</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
         <is>
           <t>Extent 4</t>
         </is>
@@ -1117,7 +1037,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:15</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1127,15 +1047,10 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Named value 15</t>
+          <t>Concept 15</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
-        <is>
-          <t>Named value 15</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
         <is>
           <t>Extent 5</t>
         </is>
@@ -1144,7 +1059,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:16</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1154,15 +1069,10 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Named value 16</t>
+          <t>Concept 16</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
-        <is>
-          <t>Named value 16</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
         <is>
           <t>Extent 6</t>
         </is>
@@ -1171,7 +1081,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:17</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1181,15 +1091,10 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Named value 17</t>
+          <t>Concept 17</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
-        <is>
-          <t>Named value 17</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
         <is>
           <t>Extent 7</t>
         </is>
@@ -1198,7 +1103,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:18</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1208,15 +1113,10 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Named value 18</t>
+          <t>Concept 18</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
-        <is>
-          <t>Named value 18</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
         <is>
           <t>Extent 8</t>
         </is>
@@ -1225,7 +1125,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:19</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1235,15 +1135,10 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Named value 19</t>
+          <t>Concept 19</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
-        <is>
-          <t>Named value 19</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
         <is>
           <t>Extent 9</t>
         </is>
@@ -1252,7 +1147,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:20</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1262,15 +1157,10 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Named value 20</t>
+          <t>Concept 20</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
-        <is>
-          <t>Named value 20</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
         <is>
           <t>Language 0</t>
         </is>
@@ -1279,7 +1169,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:21</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1289,15 +1179,10 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Named value 21</t>
+          <t>Concept 21</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
-        <is>
-          <t>Named value 21</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
         <is>
           <t>Language 1</t>
         </is>
@@ -1306,7 +1191,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:22</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1316,15 +1201,10 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Named value 22</t>
+          <t>Concept 22</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
-        <is>
-          <t>Named value 22</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
         <is>
           <t>Language 2</t>
         </is>
@@ -1333,7 +1213,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:23</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1343,15 +1223,10 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Named value 23</t>
+          <t>Concept 23</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
-        <is>
-          <t>Named value 23</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
         <is>
           <t>Language 3</t>
         </is>
@@ -1360,7 +1235,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:24</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1370,15 +1245,10 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Named value 24</t>
+          <t>Concept 24</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
-        <is>
-          <t>Named value 24</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
         <is>
           <t>Language 4</t>
         </is>
@@ -1387,7 +1257,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:25</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1397,15 +1267,10 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Named value 25</t>
+          <t>Concept 25</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
-        <is>
-          <t>Named value 25</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
         <is>
           <t>Language 5</t>
         </is>
@@ -1414,7 +1279,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:26</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1424,15 +1289,10 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Named value 26</t>
+          <t>Concept 26</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
-        <is>
-          <t>Named value 26</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
         <is>
           <t>Language 6</t>
         </is>
@@ -1441,7 +1301,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:27</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1451,15 +1311,10 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Named value 27</t>
+          <t>Concept 27</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
-        <is>
-          <t>Named value 27</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
         <is>
           <t>Language 7</t>
         </is>
@@ -1468,7 +1323,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:28</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1478,15 +1333,10 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Named value 28</t>
+          <t>Concept 28</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
-        <is>
-          <t>Named value 28</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
         <is>
           <t>Language 8</t>
         </is>
@@ -1495,7 +1345,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:29</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1505,15 +1355,10 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Named value 29</t>
+          <t>Concept 29</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
-        <is>
-          <t>Named value 29</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
         <is>
           <t>Language 9</t>
         </is>
@@ -1522,7 +1367,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:30</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1532,15 +1377,10 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Named value 30</t>
+          <t>Concept 30</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
-        <is>
-          <t>Named value 30</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
         <is>
           <t>Material 0</t>
         </is>
@@ -1549,7 +1389,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:31</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1559,15 +1399,10 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Named value 31</t>
+          <t>Concept 31</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
-        <is>
-          <t>Named value 31</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
         <is>
           <t>Material 1</t>
         </is>
@@ -1576,7 +1411,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:32</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1586,15 +1421,10 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Named value 32</t>
+          <t>Concept 32</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
-        <is>
-          <t>Named value 32</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
         <is>
           <t>Material 2</t>
         </is>
@@ -1603,7 +1433,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:33</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1613,15 +1443,10 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Named value 33</t>
+          <t>Concept 33</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
-        <is>
-          <t>Named value 33</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
         <is>
           <t>Material 3</t>
         </is>
@@ -1630,7 +1455,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:34</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1640,15 +1465,10 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Named value 34</t>
+          <t>Concept 34</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
-        <is>
-          <t>Named value 34</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
         <is>
           <t>Material 4</t>
         </is>
@@ -1657,7 +1477,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:35</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1667,15 +1487,10 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Named value 35</t>
+          <t>Concept 35</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
-        <is>
-          <t>Named value 35</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
         <is>
           <t>Material 5</t>
         </is>
@@ -1684,7 +1499,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:36</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1694,15 +1509,10 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Named value 36</t>
+          <t>Concept 36</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
-        <is>
-          <t>Named value 36</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
         <is>
           <t>Material 6</t>
         </is>
@@ -1711,7 +1521,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:37</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1721,15 +1531,10 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Named value 37</t>
+          <t>Concept 37</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
-        <is>
-          <t>Named value 37</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
         <is>
           <t>Material 7</t>
         </is>
@@ -1738,7 +1543,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:38</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1748,15 +1553,10 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Named value 38</t>
+          <t>Concept 38</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
-        <is>
-          <t>Named value 38</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
         <is>
           <t>Material 8</t>
         </is>
@@ -1765,7 +1565,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:39</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1775,15 +1575,10 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Named value 39</t>
+          <t>Concept 39</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
-        <is>
-          <t>Named value 39</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
         <is>
           <t>Material 9</t>
         </is>
@@ -1792,7 +1587,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:40</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1802,15 +1597,10 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Named value 40</t>
+          <t>Concept 40</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
-        <is>
-          <t>Named value 40</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
         <is>
           <t>Medium 0</t>
         </is>
@@ -1819,7 +1609,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:41</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1829,15 +1619,10 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Named value 41</t>
+          <t>Concept 41</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
-        <is>
-          <t>Named value 41</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
         <is>
           <t>Medium 1</t>
         </is>
@@ -1846,7 +1631,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:42</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1856,15 +1641,10 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Named value 42</t>
+          <t>Concept 42</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
-        <is>
-          <t>Named value 42</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
         <is>
           <t>Medium 2</t>
         </is>
@@ -1873,7 +1653,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:43</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1883,15 +1663,10 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Named value 43</t>
+          <t>Concept 43</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
-        <is>
-          <t>Named value 43</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
         <is>
           <t>Medium 3</t>
         </is>
@@ -1900,7 +1675,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:44</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1910,15 +1685,10 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Named value 44</t>
+          <t>Concept 44</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
-        <is>
-          <t>Named value 44</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
         <is>
           <t>Medium 4</t>
         </is>
@@ -1927,7 +1697,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:45</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1937,15 +1707,10 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Named value 45</t>
+          <t>Concept 45</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
-        <is>
-          <t>Named value 45</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
         <is>
           <t>Medium 5</t>
         </is>
@@ -1954,7 +1719,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:46</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1964,15 +1729,10 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Named value 46</t>
+          <t>Concept 46</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
-        <is>
-          <t>Named value 46</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
         <is>
           <t>Medium 6</t>
         </is>
@@ -1981,7 +1741,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:47</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1991,15 +1751,10 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Named value 47</t>
+          <t>Concept 47</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
-        <is>
-          <t>Named value 47</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
         <is>
           <t>Medium 7</t>
         </is>
@@ -2008,7 +1763,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:48</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2018,15 +1773,10 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Named value 48</t>
+          <t>Concept 48</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
-        <is>
-          <t>Named value 48</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
         <is>
           <t>Medium 8</t>
         </is>
@@ -2035,7 +1785,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:49</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2045,15 +1795,10 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Named value 49</t>
+          <t>Concept 49</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
-        <is>
-          <t>Named value 49</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
         <is>
           <t>Medium 9</t>
         </is>
@@ -2062,7 +1807,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:50</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2072,15 +1817,10 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Named value 50</t>
+          <t>Concept 50</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
-        <is>
-          <t>Named value 50</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
         <is>
           <t>Publisher 0</t>
         </is>
@@ -2089,7 +1829,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:51</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2099,15 +1839,10 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Named value 51</t>
+          <t>Concept 51</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
-        <is>
-          <t>Named value 51</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
         <is>
           <t>Publisher 1</t>
         </is>
@@ -2116,7 +1851,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:52</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2126,15 +1861,10 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Named value 52</t>
+          <t>Concept 52</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
-        <is>
-          <t>Named value 52</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
         <is>
           <t>Publisher 2</t>
         </is>
@@ -2143,7 +1873,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:53</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2153,15 +1883,10 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Named value 53</t>
+          <t>Concept 53</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
-        <is>
-          <t>Named value 53</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
         <is>
           <t>Publisher 3</t>
         </is>
@@ -2170,7 +1895,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:54</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2180,15 +1905,10 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Named value 54</t>
+          <t>Concept 54</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
-        <is>
-          <t>Named value 54</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
         <is>
           <t>Publisher 4</t>
         </is>
@@ -2197,7 +1917,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:55</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2207,15 +1927,10 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Named value 55</t>
+          <t>Concept 55</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
-        <is>
-          <t>Named value 55</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
         <is>
           <t>Publisher 5</t>
         </is>
@@ -2224,7 +1939,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:56</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2234,15 +1949,10 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Named value 56</t>
+          <t>Concept 56</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
-        <is>
-          <t>Named value 56</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
         <is>
           <t>Publisher 6</t>
         </is>
@@ -2251,7 +1961,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:57</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2261,15 +1971,10 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Named value 57</t>
+          <t>Concept 57</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
-        <is>
-          <t>Named value 57</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
         <is>
           <t>Publisher 7</t>
         </is>
@@ -2278,7 +1983,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:58</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2288,15 +1993,10 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Named value 58</t>
+          <t>Concept 58</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
-        <is>
-          <t>Named value 58</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
         <is>
           <t>Publisher 8</t>
         </is>
@@ -2305,7 +2005,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:59</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2315,15 +2015,10 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Named value 59</t>
+          <t>Concept 59</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
-        <is>
-          <t>Named value 59</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
         <is>
           <t>Publisher 9</t>
         </is>
@@ -2332,7 +2027,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:60</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2342,15 +2037,10 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Named value 60</t>
+          <t>Concept 60</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
-        <is>
-          <t>Named value 60</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
         <is>
           <t>Source 0</t>
         </is>
@@ -2359,7 +2049,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:61</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2369,15 +2059,10 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Named value 61</t>
+          <t>Concept 61</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
-        <is>
-          <t>Named value 61</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
         <is>
           <t>Source 1</t>
         </is>
@@ -2386,7 +2071,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:62</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2396,15 +2081,10 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Named value 62</t>
+          <t>Concept 62</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
-        <is>
-          <t>Named value 62</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
         <is>
           <t>Source 2</t>
         </is>
@@ -2413,7 +2093,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:63</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2423,15 +2103,10 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Named value 63</t>
+          <t>Concept 63</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
-        <is>
-          <t>Named value 63</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
         <is>
           <t>Source 3</t>
         </is>
@@ -2440,7 +2115,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:64</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2450,15 +2125,10 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Named value 64</t>
+          <t>Concept 64</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
-        <is>
-          <t>Named value 64</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
         <is>
           <t>Source 4</t>
         </is>
@@ -2467,7 +2137,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:65</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2477,15 +2147,10 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Named value 65</t>
+          <t>Concept 65</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
-        <is>
-          <t>Named value 65</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
         <is>
           <t>Source 5</t>
         </is>
@@ -2494,7 +2159,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:66</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2504,15 +2169,10 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Named value 66</t>
+          <t>Concept 66</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
-        <is>
-          <t>Named value 66</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
         <is>
           <t>Source 6</t>
         </is>
@@ -2521,7 +2181,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:67</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2531,15 +2191,10 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Named value 67</t>
+          <t>Concept 67</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
-        <is>
-          <t>Named value 67</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
         <is>
           <t>Source 7</t>
         </is>
@@ -2548,7 +2203,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:68</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2558,15 +2213,10 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Named value 68</t>
+          <t>Concept 68</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
-        <is>
-          <t>Named value 68</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
         <is>
           <t>Source 8</t>
         </is>
@@ -2575,7 +2225,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:69</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2585,15 +2235,10 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Named value 69</t>
+          <t>Concept 69</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
-        <is>
-          <t>Named value 69</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
         <is>
           <t>Source 9</t>
         </is>
@@ -2602,7 +2247,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:70</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2612,15 +2257,10 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Named value 70</t>
+          <t>Concept 70</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
-        <is>
-          <t>Named value 70</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
         <is>
           <t>Spatial 0</t>
         </is>
@@ -2629,7 +2269,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:71</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2639,15 +2279,10 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Named value 71</t>
+          <t>Concept 71</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
-        <is>
-          <t>Named value 71</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
         <is>
           <t>Spatial 1</t>
         </is>
@@ -2656,7 +2291,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:72</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2666,15 +2301,10 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Named value 72</t>
+          <t>Concept 72</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
-        <is>
-          <t>Named value 72</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
         <is>
           <t>Spatial 2</t>
         </is>
@@ -2683,7 +2313,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:73</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2693,15 +2323,10 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Named value 73</t>
+          <t>Concept 73</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
-        <is>
-          <t>Named value 73</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
         <is>
           <t>Spatial 3</t>
         </is>
@@ -2710,7 +2335,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:74</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2720,15 +2345,10 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Named value 74</t>
+          <t>Concept 74</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
-        <is>
-          <t>Named value 74</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
         <is>
           <t>Spatial 4</t>
         </is>
@@ -2737,7 +2357,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:75</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2747,15 +2367,10 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Named value 75</t>
+          <t>Concept 75</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
-        <is>
-          <t>Named value 75</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
         <is>
           <t>Spatial 5</t>
         </is>
@@ -2764,7 +2379,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:76</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2774,15 +2389,10 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Named value 76</t>
+          <t>Concept 76</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
-        <is>
-          <t>Named value 76</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
         <is>
           <t>Spatial 6</t>
         </is>
@@ -2791,7 +2401,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:77</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2801,15 +2411,10 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Named value 77</t>
+          <t>Concept 77</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
-        <is>
-          <t>Named value 77</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
         <is>
           <t>Spatial 7</t>
         </is>
@@ -2818,7 +2423,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:78</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2828,15 +2433,10 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Named value 78</t>
+          <t>Concept 78</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
-        <is>
-          <t>Named value 78</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
         <is>
           <t>Spatial 8</t>
         </is>
@@ -2845,7 +2445,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:79</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2855,15 +2455,10 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Named value 79</t>
+          <t>Concept 79</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
-        <is>
-          <t>Named value 79</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
         <is>
           <t>Spatial 9</t>
         </is>
@@ -2872,7 +2467,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:80</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2882,15 +2477,10 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Named value 80</t>
+          <t>Concept 80</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
-        <is>
-          <t>Named value 80</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
         <is>
           <t>Subject 0</t>
         </is>
@@ -2899,7 +2489,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:81</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2909,15 +2499,10 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Named value 81</t>
+          <t>Concept 81</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
-        <is>
-          <t>Named value 81</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
         <is>
           <t>Subject 1</t>
         </is>
@@ -2926,7 +2511,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:82</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2936,15 +2521,10 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Named value 82</t>
+          <t>Concept 82</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
-        <is>
-          <t>Named value 82</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
         <is>
           <t>Subject 2</t>
         </is>
@@ -2953,7 +2533,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:83</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2963,15 +2543,10 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Named value 83</t>
+          <t>Concept 83</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
-        <is>
-          <t>Named value 83</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
         <is>
           <t>Subject 3</t>
         </is>
@@ -2980,7 +2555,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:84</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2990,15 +2565,10 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Named value 84</t>
+          <t>Concept 84</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
-        <is>
-          <t>Named value 84</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
         <is>
           <t>Subject 4</t>
         </is>
@@ -3007,7 +2577,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:85</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -3017,15 +2587,10 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Named value 85</t>
+          <t>Concept 85</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
-        <is>
-          <t>Named value 85</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
         <is>
           <t>Subject 5</t>
         </is>
@@ -3034,7 +2599,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:86</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -3044,15 +2609,10 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Named value 86</t>
+          <t>Concept 86</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
-        <is>
-          <t>Named value 86</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
         <is>
           <t>Subject 6</t>
         </is>
@@ -3061,7 +2621,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:87</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -3071,15 +2631,10 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Named value 87</t>
+          <t>Concept 87</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
-        <is>
-          <t>Named value 87</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
         <is>
           <t>Subject 7</t>
         </is>
@@ -3088,7 +2643,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:88</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -3098,15 +2653,10 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Named value 88</t>
+          <t>Concept 88</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
-        <is>
-          <t>Named value 88</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
         <is>
           <t>Subject 8</t>
         </is>
@@ -3115,7 +2665,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:89</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -3125,15 +2675,10 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Named value 89</t>
+          <t>Concept 89</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
-        <is>
-          <t>Named value 89</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
         <is>
           <t>Subject 9</t>
         </is>
@@ -3142,7 +2687,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:90</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -3152,15 +2697,10 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Named value 90</t>
+          <t>Concept 90</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
-        <is>
-          <t>Named value 90</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
         <is>
           <t>Technique 0</t>
         </is>
@@ -3169,7 +2709,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:91</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -3179,15 +2719,10 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Named value 91</t>
+          <t>Concept 91</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
-        <is>
-          <t>Named value 91</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr">
         <is>
           <t>Technique 1</t>
         </is>
@@ -3196,7 +2731,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:92</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -3206,15 +2741,10 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Named value 92</t>
+          <t>Concept 92</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
-        <is>
-          <t>Named value 92</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr">
         <is>
           <t>Technique 2</t>
         </is>
@@ -3223,7 +2753,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:93</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -3233,15 +2763,10 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Named value 93</t>
+          <t>Concept 93</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
-        <is>
-          <t>Named value 93</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr">
         <is>
           <t>Technique 3</t>
         </is>
@@ -3250,7 +2775,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:94</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -3260,15 +2785,10 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Named value 94</t>
+          <t>Concept 94</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
-        <is>
-          <t>Named value 94</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
         <is>
           <t>Technique 4</t>
         </is>
@@ -3277,7 +2797,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:95</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -3287,15 +2807,10 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Named value 95</t>
+          <t>Concept 95</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
-        <is>
-          <t>Named value 95</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr">
         <is>
           <t>Technique 5</t>
         </is>
@@ -3304,7 +2819,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:96</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -3314,15 +2829,10 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Named value 96</t>
+          <t>Concept 96</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
-        <is>
-          <t>Named value 96</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr">
         <is>
           <t>Technique 6</t>
         </is>
@@ -3331,7 +2841,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:97</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -3341,15 +2851,10 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Named value 97</t>
+          <t>Concept 97</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
-        <is>
-          <t>Named value 97</t>
-        </is>
-      </c>
-      <c r="E99" t="inlineStr">
         <is>
           <t>Technique 7</t>
         </is>
@@ -3358,7 +2863,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:98</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -3368,15 +2873,10 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Named value 98</t>
+          <t>Concept 98</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
-        <is>
-          <t>Named value 98</t>
-        </is>
-      </c>
-      <c r="E100" t="inlineStr">
         <is>
           <t>Technique 8</t>
         </is>
@@ -3385,7 +2885,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:99</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -3395,15 +2895,10 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Named value 99</t>
+          <t>Concept 99</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
-        <is>
-          <t>Named value 99</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr">
         <is>
           <t>Technique 9</t>
         </is>
@@ -3412,7 +2907,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:100</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -3422,15 +2917,10 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Named value 100</t>
+          <t>Concept 100</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
-        <is>
-          <t>Named value 100</t>
-        </is>
-      </c>
-      <c r="E102" t="inlineStr">
         <is>
           <t>Type 0</t>
         </is>
@@ -3439,7 +2929,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:101</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -3449,15 +2939,10 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Named value 101</t>
+          <t>Concept 101</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
-        <is>
-          <t>Named value 101</t>
-        </is>
-      </c>
-      <c r="E103" t="inlineStr">
         <is>
           <t>Type 1</t>
         </is>
@@ -3466,7 +2951,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:102</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -3476,15 +2961,10 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Named value 102</t>
+          <t>Concept 102</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
-        <is>
-          <t>Named value 102</t>
-        </is>
-      </c>
-      <c r="E104" t="inlineStr">
         <is>
           <t>Type 2</t>
         </is>
@@ -3493,7 +2973,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:103</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -3503,15 +2983,10 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Named value 103</t>
+          <t>Concept 103</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
-        <is>
-          <t>Named value 103</t>
-        </is>
-      </c>
-      <c r="E105" t="inlineStr">
         <is>
           <t>Type 3</t>
         </is>
@@ -3520,7 +2995,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:104</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -3530,15 +3005,10 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Named value 104</t>
+          <t>Concept 104</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
-        <is>
-          <t>Named value 104</t>
-        </is>
-      </c>
-      <c r="E106" t="inlineStr">
         <is>
           <t>Type 4</t>
         </is>
@@ -3547,7 +3017,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:105</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3557,15 +3027,10 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Named value 105</t>
+          <t>Concept 105</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
-        <is>
-          <t>Named value 105</t>
-        </is>
-      </c>
-      <c r="E107" t="inlineStr">
         <is>
           <t>Type 5</t>
         </is>
@@ -3574,7 +3039,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:106</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3584,15 +3049,10 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Named value 106</t>
+          <t>Concept 106</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
-        <is>
-          <t>Named value 106</t>
-        </is>
-      </c>
-      <c r="E108" t="inlineStr">
         <is>
           <t>Type 6</t>
         </is>
@@ -3601,7 +3061,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:107</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3611,15 +3071,10 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Named value 107</t>
+          <t>Concept 107</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
-        <is>
-          <t>Named value 107</t>
-        </is>
-      </c>
-      <c r="E109" t="inlineStr">
         <is>
           <t>Type 7</t>
         </is>
@@ -3628,7 +3083,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:108</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3638,15 +3093,10 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Named value 108</t>
+          <t>Concept 108</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
-        <is>
-          <t>Named value 108</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr">
         <is>
           <t>Type 8</t>
         </is>
@@ -3655,7 +3105,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:109</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3665,15 +3115,10 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Named value 109</t>
+          <t>Concept 109</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
-        <is>
-          <t>Named value 109</t>
-        </is>
-      </c>
-      <c r="E111" t="inlineStr">
         <is>
           <t>Type 9</t>
         </is>
@@ -3763,7 +3208,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -3810,7 +3255,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -3857,7 +3302,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -3904,7 +3349,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -3951,7 +3396,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:2</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -3998,7 +3443,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:2</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -4045,7 +3490,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:3</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -4092,7 +3537,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:3</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -4139,7 +3584,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:4</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -4186,7 +3631,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:4</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -4233,7 +3678,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:5</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -4280,7 +3725,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:5</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -4327,7 +3772,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:6</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -4374,7 +3819,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:6</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -4421,7 +3866,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:7</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -4468,7 +3913,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:7</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -4515,7 +3960,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:8</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -4562,7 +4007,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:8</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -4609,7 +4054,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:9</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -4656,7 +4101,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:9</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -4703,7 +4148,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:10</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -4750,7 +4195,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:10</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -4797,7 +4242,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:11</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -4844,7 +4289,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:11</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -4891,7 +4336,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:12</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -4938,7 +4383,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:12</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -4985,7 +4430,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:13</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -5032,7 +4477,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:13</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -5079,7 +4524,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:14</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -5126,7 +4571,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:14</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -5173,7 +4618,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:15</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -5220,7 +4665,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:15</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -5267,7 +4712,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:16</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -5314,7 +4759,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:16</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -5361,7 +4806,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:17</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -5408,7 +4853,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:17</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -5455,7 +4900,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:18</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -5502,7 +4947,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:18</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -5549,7 +4994,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:19</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -5596,7 +5041,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:19</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -5643,7 +5088,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:20</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -5690,7 +5135,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:20</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -5737,7 +5182,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:21</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -5784,7 +5229,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:21</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -5831,7 +5276,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:22</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -5878,7 +5323,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:22</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -5925,7 +5370,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:23</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -5972,7 +5417,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:23</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -6019,7 +5464,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:24</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -6066,7 +5511,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:24</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -6113,7 +5558,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:25</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -6160,7 +5605,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:25</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -6207,7 +5652,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:26</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -6254,7 +5699,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:26</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -6301,7 +5746,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:27</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -6348,7 +5793,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:27</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -6395,7 +5840,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:28</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -6442,7 +5887,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:28</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -6489,7 +5934,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:29</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -6536,7 +5981,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:29</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -6583,7 +6028,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:30</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -6630,7 +6075,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:30</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -6677,7 +6122,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:31</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -6724,7 +6169,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:31</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -6771,7 +6216,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:32</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -6818,7 +6263,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:32</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -6865,7 +6310,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:33</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -6912,7 +6357,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:33</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -6959,7 +6404,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:34</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -7006,7 +6451,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:34</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -7053,7 +6498,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:35</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -7100,7 +6545,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:35</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -7147,7 +6592,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:36</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -7194,7 +6639,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:36</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -7241,7 +6686,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:37</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -7288,7 +6733,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:37</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -7335,7 +6780,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:38</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -7382,7 +6827,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:38</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -7429,7 +6874,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:39</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -7476,7 +6921,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:39</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -7523,7 +6968,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:40</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -7570,7 +7015,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:40</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -7617,7 +7062,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:41</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -7664,7 +7109,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:41</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -7711,7 +7156,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:42</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -7758,7 +7203,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:42</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -7805,7 +7250,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:43</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -7852,7 +7297,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:43</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -7899,7 +7344,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:44</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -7946,7 +7391,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:44</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -7993,7 +7438,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:45</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -8040,7 +7485,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:45</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -8087,7 +7532,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:46</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -8134,7 +7579,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:46</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -8181,7 +7626,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:47</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -8228,7 +7673,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:47</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -8275,7 +7720,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:48</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -8322,7 +7767,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:48</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -8369,7 +7814,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:49</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -8416,7 +7861,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:49</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -8463,7 +7908,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:50</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -8510,7 +7955,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:50</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -8557,7 +8002,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:51</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -8604,7 +8049,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:51</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -8651,7 +8096,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:52</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -8698,7 +8143,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:52</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -8745,7 +8190,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:53</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -8792,7 +8237,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:53</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -8839,7 +8284,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:54</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
@@ -8886,7 +8331,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:54</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -8933,7 +8378,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:55</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -8980,7 +8425,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:55</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -9027,7 +8472,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:56</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -9074,7 +8519,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:56</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -9121,7 +8566,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:57</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -9168,7 +8613,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:57</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -9215,7 +8660,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:58</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
@@ -9262,7 +8707,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:58</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -9309,7 +8754,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:59</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
@@ -9356,7 +8801,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:59</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
@@ -9403,7 +8848,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:60</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
@@ -9450,7 +8895,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:60</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -9497,7 +8942,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:61</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -9544,7 +8989,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:61</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
@@ -9591,7 +9036,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:62</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -9638,7 +9083,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:62</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
@@ -9685,7 +9130,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:63</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
@@ -9732,7 +9177,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:63</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
@@ -9779,7 +9224,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:64</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -9826,7 +9271,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:64</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
@@ -9873,7 +9318,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:65</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -9920,7 +9365,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:65</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -9967,7 +9412,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:66</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -10014,7 +9459,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:66</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -10061,7 +9506,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:67</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -10108,7 +9553,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:67</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -10155,7 +9600,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:68</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -10202,7 +9647,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:68</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -10249,7 +9694,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:69</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
@@ -10296,7 +9741,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:69</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
@@ -10343,7 +9788,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:70</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
@@ -10390,7 +9835,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:70</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
@@ -10437,7 +9882,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:71</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
@@ -10484,7 +9929,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:71</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
@@ -10531,7 +9976,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:72</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
@@ -10578,7 +10023,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:72</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
@@ -10625,7 +10070,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:73</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
@@ -10672,7 +10117,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:73</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
@@ -10719,7 +10164,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:74</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
@@ -10766,7 +10211,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:74</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
@@ -10813,7 +10258,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:75</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
@@ -10860,7 +10305,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:75</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -10907,7 +10352,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:76</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
@@ -10954,7 +10399,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:76</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
@@ -11001,7 +10446,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:77</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
@@ -11048,7 +10493,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:77</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
@@ -11095,7 +10540,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:78</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
@@ -11142,7 +10587,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:78</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
@@ -11189,7 +10634,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:79</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
@@ -11236,7 +10681,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:79</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
@@ -11283,7 +10728,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:80</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
@@ -11330,7 +10775,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:80</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
@@ -11377,7 +10822,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:81</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
@@ -11424,7 +10869,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:81</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
@@ -11471,7 +10916,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:82</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
@@ -11518,7 +10963,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:82</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
@@ -11565,7 +11010,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:83</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
@@ -11612,7 +11057,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:83</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
@@ -11659,7 +11104,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:84</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
@@ -11706,7 +11151,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:84</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
@@ -11753,7 +11198,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:85</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
@@ -11800,7 +11245,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:85</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
@@ -11847,7 +11292,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:86</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
@@ -11894,7 +11339,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:86</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
@@ -11941,7 +11386,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:87</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
@@ -11988,7 +11433,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:87</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
@@ -12035,7 +11480,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:88</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
@@ -12082,7 +11527,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:88</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
@@ -12129,7 +11574,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:89</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
@@ -12176,7 +11621,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:89</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
@@ -12223,7 +11668,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:90</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
@@ -12270,7 +11715,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:90</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90</t>
         </is>
       </c>
       <c r="E183" t="inlineStr">
@@ -12317,7 +11762,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:91</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
@@ -12364,7 +11809,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:91</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
@@ -12411,7 +11856,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:92</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
@@ -12458,7 +11903,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:92</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
@@ -12505,7 +11950,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:93</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93</t>
         </is>
       </c>
       <c r="E188" t="inlineStr">
@@ -12552,7 +11997,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:93</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
@@ -12599,7 +12044,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:94</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
@@ -12646,7 +12091,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:94</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
@@ -12693,7 +12138,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:95</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95</t>
         </is>
       </c>
       <c r="E192" t="inlineStr">
@@ -12740,7 +12185,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:95</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
@@ -12787,7 +12232,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:96</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
@@ -12834,7 +12279,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:96</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
@@ -12881,7 +12326,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:97</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
@@ -12928,7 +12373,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:97</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
@@ -12975,7 +12420,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:98</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
@@ -13022,7 +12467,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:98</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
@@ -13069,7 +12514,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:99</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99</t>
         </is>
       </c>
       <c r="E200" t="inlineStr">
@@ -13116,7 +12561,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:99</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">
@@ -13163,7 +12608,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:100</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100</t>
         </is>
       </c>
       <c r="E202" t="inlineStr">
@@ -13210,7 +12655,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:100</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100</t>
         </is>
       </c>
       <c r="E203" t="inlineStr">
@@ -13257,7 +12702,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:101</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
         </is>
       </c>
       <c r="E204" t="inlineStr">
@@ -13304,7 +12749,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:101</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
         </is>
       </c>
       <c r="E205" t="inlineStr">
@@ -13351,7 +12796,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:102</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
         </is>
       </c>
       <c r="E206" t="inlineStr">
@@ -13398,7 +12843,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:102</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
         </is>
       </c>
       <c r="E207" t="inlineStr">
@@ -13445,7 +12890,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:103</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103</t>
         </is>
       </c>
       <c r="E208" t="inlineStr">
@@ -13492,7 +12937,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:103</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103</t>
         </is>
       </c>
       <c r="E209" t="inlineStr">
@@ -13539,7 +12984,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:104</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104</t>
         </is>
       </c>
       <c r="E210" t="inlineStr">
@@ -13586,7 +13031,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:104</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104</t>
         </is>
       </c>
       <c r="E211" t="inlineStr">
@@ -13633,7 +13078,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:105</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105</t>
         </is>
       </c>
       <c r="E212" t="inlineStr">
@@ -13680,7 +13125,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:105</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105</t>
         </is>
       </c>
       <c r="E213" t="inlineStr">
@@ -13727,7 +13172,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:106</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106</t>
         </is>
       </c>
       <c r="E214" t="inlineStr">
@@ -13774,7 +13219,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:106</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106</t>
         </is>
       </c>
       <c r="E215" t="inlineStr">
@@ -13821,7 +13266,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:107</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107</t>
         </is>
       </c>
       <c r="E216" t="inlineStr">
@@ -13868,7 +13313,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:107</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107</t>
         </is>
       </c>
       <c r="E217" t="inlineStr">
@@ -13915,7 +13360,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:108</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108</t>
         </is>
       </c>
       <c r="E218" t="inlineStr">
@@ -13962,7 +13407,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:108</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108</t>
         </is>
       </c>
       <c r="E219" t="inlineStr">
@@ -14009,7 +13454,7 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:109</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109</t>
         </is>
       </c>
       <c r="E220" t="inlineStr">
@@ -14056,7 +13501,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:named_value:109</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109</t>
         </is>
       </c>
       <c r="E221" t="inlineStr">
@@ -16024,7 +15469,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">

</xml_diff>

<commit_message>
integrate properties and property groups into synthetic data
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -8,16 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Concept" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Image" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Organization" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Person" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Collection" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Work" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="WorkClosing" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="WorkCreation" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="License" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="RightsStatement" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="PropertyGroup" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Property" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Concept" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Image" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Organization" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Person" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Collection" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Work" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="WorkClosing" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="WorkCreation" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="License" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="RightsStatement" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -441,6 +443,58 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>@graph</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>@graph</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -546,7 +600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -622,7 +676,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -647,7 +701,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -663,2437 +717,19 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>prefLabel</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>property</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>value</t>
+          <t>label</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Concept 0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>vra:culturalContext</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Cultural context 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Concept 1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>vra:culturalContext</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Cultural context 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Concept 2</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>vra:culturalContext</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Cultural context 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Concept 3</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>vra:culturalContext</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Cultural context 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Concept 4</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>vra:culturalContext</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Cultural context 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Concept 5</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>vra:culturalContext</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Cultural context 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Concept 6</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>vra:culturalContext</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Cultural context 6</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Concept 7</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>vra:culturalContext</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Cultural context 7</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Concept 8</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>vra:culturalContext</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Cultural context 8</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Concept 9</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>vra:culturalContext</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Cultural context 9</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Concept 10</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>dcterms:extent</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Extent 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Concept 11</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>dcterms:extent</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Extent 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Concept 12</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>dcterms:extent</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Extent 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Concept 13</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>dcterms:extent</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Extent 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Concept 14</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>dcterms:extent</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Extent 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Concept 15</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>dcterms:extent</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Extent 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Concept 16</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>dcterms:extent</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Extent 6</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Concept 17</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>dcterms:extent</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Extent 7</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Concept 18</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>dcterms:extent</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Extent 8</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Concept 19</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>dcterms:extent</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Extent 9</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Concept 20</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>dcterms:language</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Language 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Concept 21</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>dcterms:language</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Language 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Concept 22</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>dcterms:language</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Language 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Concept 23</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>dcterms:language</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Language 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Concept 24</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>dcterms:language</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Language 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Concept 25</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>dcterms:language</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Language 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Concept 26</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>dcterms:language</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Language 6</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Concept 27</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>dcterms:language</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Language 7</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Concept 28</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>dcterms:language</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Language 8</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Concept 29</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>dcterms:language</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Language 9</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Concept 30</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>vra:material</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Material 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Concept 31</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>vra:material</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Material 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Concept 32</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>vra:material</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Material 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Concept 33</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>vra:material</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Material 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Concept 34</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>vra:material</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Material 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Concept 35</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>vra:material</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Material 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Concept 36</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>vra:material</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Material 6</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Concept 37</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>vra:material</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Material 7</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Concept 38</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>vra:material</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Material 8</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Concept 39</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>vra:material</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Material 9</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Concept 40</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>dcterms:medium</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Medium 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Concept 41</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>dcterms:medium</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Medium 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Concept 42</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>dcterms:medium</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Medium 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Concept 43</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>dcterms:medium</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Medium 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Concept 44</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>dcterms:medium</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Medium 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Concept 45</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>dcterms:medium</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Medium 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Concept 46</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>dcterms:medium</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Medium 6</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Concept 47</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>dcterms:medium</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Medium 7</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Concept 48</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>dcterms:medium</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Medium 8</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Concept 49</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>dcterms:medium</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Medium 9</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Concept 50</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>dcterms:publisher</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Publisher 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Concept 51</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>dcterms:publisher</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Publisher 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Concept 52</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>dcterms:publisher</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Publisher 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Concept 53</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>dcterms:publisher</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>Publisher 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Concept 54</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>dcterms:publisher</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Publisher 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Concept 55</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>dcterms:publisher</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Publisher 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>Concept 56</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>dcterms:publisher</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Publisher 6</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Concept 57</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>dcterms:publisher</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>Publisher 7</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>Concept 58</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>dcterms:publisher</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Publisher 8</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>Concept 59</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>dcterms:publisher</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>Publisher 9</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Concept 60</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>dcterms:source</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Source 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Concept 61</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>dcterms:source</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Source 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Concept 62</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>dcterms:source</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Source 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Concept 63</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>dcterms:source</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Source 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Concept 64</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>dcterms:source</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>Source 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Concept 65</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>dcterms:source</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>Source 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Concept 66</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>dcterms:source</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>Source 6</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Concept 67</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>dcterms:source</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>Source 7</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Concept 68</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>dcterms:source</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>Source 8</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Concept 69</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>dcterms:source</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>Source 9</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Concept 70</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>dcterms:spatial</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>Spatial 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>Concept 71</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>dcterms:spatial</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>Spatial 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Concept 72</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>dcterms:spatial</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>Spatial 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>Concept 73</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>dcterms:spatial</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>Spatial 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Concept 74</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>dcterms:spatial</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>Spatial 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>Concept 75</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>dcterms:spatial</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>Spatial 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>Concept 76</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>dcterms:spatial</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>Spatial 6</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Concept 77</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>dcterms:spatial</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>Spatial 7</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>Concept 78</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>dcterms:spatial</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>Spatial 8</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Concept 79</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>dcterms:spatial</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>Spatial 9</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>Concept 80</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>dcterms:subject</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>Subject 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>Concept 81</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>dcterms:subject</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>Subject 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>Concept 82</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>dcterms:subject</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>Subject 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>Concept 83</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>dcterms:subject</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>Subject 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>Concept 84</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>dcterms:subject</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>Subject 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>Concept 85</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>dcterms:subject</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>Subject 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>Concept 86</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>dcterms:subject</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>Subject 6</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>Concept 87</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>dcterms:subject</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>Subject 7</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>Concept 88</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>dcterms:subject</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>Subject 8</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>Concept 89</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>dcterms:subject</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>Subject 9</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>Concept 90</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>vra:technique</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>Technique 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Concept 91</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>vra:technique</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>Technique 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>Concept 92</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>vra:technique</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>Technique 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>Concept 93</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>vra:technique</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>Technique 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>Concept 94</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>vra:technique</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>Technique 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>Concept 95</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>vra:technique</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>Technique 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>Concept 96</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>vra:technique</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>Technique 6</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>Concept 97</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>vra:technique</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>Technique 7</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>Concept 98</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>vra:technique</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>Technique 8</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>Concept 99</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>vra:technique</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>Technique 9</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>Concept 100</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>dcterms:type</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>Type 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>Concept 101</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>dcterms:type</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>Type 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>Concept 102</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>dcterms:type</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>Type 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>Concept 103</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>dcterms:type</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>Type 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>Concept 104</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>dcterms:type</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>Type 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>Concept 105</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>dcterms:type</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>Type 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>Concept 106</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>dcterms:type</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>Type 6</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>Concept 107</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>dcterms:type</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>Type 7</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>Concept 108</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>dcterms:type</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>Type 8</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>Concept 109</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>dcterms:type</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>Type 9</t>
+          <t>Synthetic data properties</t>
         </is>
       </c>
     </row>
@@ -3103,6 +739,2195 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>@id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>group</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>range</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>vra:culturalContext</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cultural context</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Cultural%20context</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>dcterms:extent</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Extent</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Extent</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>dcterms:language</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Language</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Language</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>vra:material</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Material</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Material</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>dcterms:medium</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>dcterms:publisher</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Publisher</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Publisher</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>dcterms:source</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Source</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>dcterms:spatial</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Spatial</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Spatial</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>dcterms:subject</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Subject</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Subject</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>vra:technique</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Technique</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Technique</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>dcterms:type</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C111"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>@id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>prefLabel</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Concept 0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cultural context 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Concept 1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Cultural context 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Concept 2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Cultural context 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Concept 3</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Cultural context 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Concept 4</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cultural context 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Concept 5</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Cultural context 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Concept 6</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Cultural context 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Concept 7</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Cultural context 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Concept 8</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Cultural context 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Concept 9</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Cultural context 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Concept 10</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Extent 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Concept 11</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Extent 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Concept 12</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Extent 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Concept 13</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Extent 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Concept 14</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Extent 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Concept 15</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Extent 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Concept 16</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Extent 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Concept 17</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Extent 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Concept 18</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Extent 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Concept 19</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Extent 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Concept 20</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Language 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Concept 21</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Language 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Concept 22</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Language 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Concept 23</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Language 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Concept 24</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Language 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Concept 25</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Language 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Concept 26</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Language 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Concept 27</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Language 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Concept 28</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Language 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Concept 29</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Language 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Concept 30</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Material 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Concept 31</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Material 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Concept 32</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Material 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Concept 33</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Material 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Concept 34</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Material 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Concept 35</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Material 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Concept 36</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Material 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Concept 37</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Material 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Concept 38</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Material 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Concept 39</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Material 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Concept 40</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Medium 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Concept 41</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Medium 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Concept 42</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Medium 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Concept 43</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Medium 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Concept 44</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Medium 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Concept 45</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Medium 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Concept 46</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Medium 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Concept 47</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Medium 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Concept 48</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Medium 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Concept 49</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Medium 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Concept 50</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Publisher 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Concept 51</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Publisher 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Concept 52</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Publisher 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Concept 53</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Publisher 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Concept 54</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Publisher 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Concept 55</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Publisher 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Concept 56</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Publisher 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Concept 57</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Publisher 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Concept 58</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Publisher 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Concept 59</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Publisher 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Concept 60</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Source 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Concept 61</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Source 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Concept 62</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Source 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Concept 63</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Source 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Concept 64</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Source 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Concept 65</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Source 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Concept 66</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Source 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Concept 67</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Source 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Concept 68</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Source 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Concept 69</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Source 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Concept 70</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Spatial 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Concept 71</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Spatial 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Concept 72</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Spatial 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Concept 73</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Spatial 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Concept 74</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Spatial 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Concept 75</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Spatial 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Concept 76</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Spatial 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Concept 77</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Spatial 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Concept 78</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Spatial 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Concept 79</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Spatial 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Concept 80</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Subject 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Concept 81</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Subject 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Concept 82</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Subject 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Concept 83</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Subject 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Concept 84</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Subject 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Concept 85</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Subject 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Concept 86</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Subject 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Concept 87</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Subject 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Concept 88</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Subject 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Concept 89</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Subject 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Concept 90</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Technique 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Concept 91</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Technique 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Concept 92</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Technique 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Concept 93</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Technique 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Concept 94</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Technique 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Concept 95</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Technique 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Concept 96</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Technique 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Concept 97</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Technique 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Concept 98</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Technique 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Concept 99</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Technique 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Concept 100</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Type 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Concept 101</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Type 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Concept 102</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Concept 103</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Type 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Concept 104</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Type 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Concept 105</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Type 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Concept 106</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Type 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Concept 107</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Type 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Concept 108</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Type 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Concept 109</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Type 9</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -13915,7 +13740,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -14016,7 +13841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -14091,7 +13916,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -14124,7 +13949,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -14157,7 +13982,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -14223,64 +14048,12 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
           <t>4, Person</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>@graph</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>@graph</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add filterable and searchable to Property
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -676,7 +676,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -744,7 +744,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -760,17 +760,27 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>cms:propertyFilterable</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>group</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>range</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>searchable</t>
         </is>
       </c>
     </row>
@@ -782,17 +792,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>&lt;class 'filter'&gt;</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Cultural context</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Cultural%20context</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -804,17 +824,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>&lt;class 'filter'&gt;</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Extent</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Extent</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -826,17 +856,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>&lt;class 'filter'&gt;</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Language</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Language</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -848,17 +888,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>&lt;class 'filter'&gt;</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Material</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Material</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -870,17 +920,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>&lt;class 'filter'&gt;</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Medium</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -892,17 +952,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>&lt;class 'filter'&gt;</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Publisher</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Publisher</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -914,17 +984,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>&lt;class 'filter'&gt;</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Source</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Source</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -936,17 +1016,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>&lt;class 'filter'&gt;</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Spatial</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Spatial</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -958,17 +1048,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>&lt;class 'filter'&gt;</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Subject</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Subject</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -980,17 +1080,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>&lt;class 'filter'&gt;</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Technique</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Technique</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -1002,17 +1112,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>&lt;class 'filter'&gt;</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Type</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
@@ -13949,7 +14069,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -14048,7 +14168,7 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">

</xml_diff>

<commit_message>
regenerate synthetic data with dcterms:description and dcterms:title properties
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -676,7 +676,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -744,7 +744,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -760,7 +760,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>cms:propertyFilterable</t>
+          <t>filterable</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -792,7 +792,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>&lt;class 'filter'&gt;</t>
+          <t>true</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -819,12 +819,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>dcterms:extent</t>
+          <t>dcterms:description</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>&lt;class 'filter'&gt;</t>
+          <t>false</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -834,12 +834,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Extent</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Extent</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Description</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -851,12 +851,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>dcterms:language</t>
+          <t>dcterms:extent</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>&lt;class 'filter'&gt;</t>
+          <t>true</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -866,12 +866,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Language</t>
+          <t>Extent</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Language</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Extent</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -883,12 +883,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>vra:material</t>
+          <t>dcterms:language</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>&lt;class 'filter'&gt;</t>
+          <t>true</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -898,12 +898,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Material</t>
+          <t>Language</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Material</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Language</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -915,12 +915,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>dcterms:medium</t>
+          <t>vra:material</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>&lt;class 'filter'&gt;</t>
+          <t>true</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -930,12 +930,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Material</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Medium</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Material</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -947,12 +947,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>dcterms:publisher</t>
+          <t>dcterms:medium</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>&lt;class 'filter'&gt;</t>
+          <t>true</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -962,12 +962,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Publisher</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Publisher</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Medium</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -979,12 +979,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>dcterms:source</t>
+          <t>dcterms:publisher</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>&lt;class 'filter'&gt;</t>
+          <t>true</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -994,12 +994,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Source</t>
+          <t>Publisher</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Source</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Publisher</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1011,12 +1011,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>dcterms:spatial</t>
+          <t>dcterms:source</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>&lt;class 'filter'&gt;</t>
+          <t>true</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1026,12 +1026,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Spatial</t>
+          <t>Source</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Spatial</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Source</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1043,12 +1043,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>dcterms:subject</t>
+          <t>dcterms:spatial</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>&lt;class 'filter'&gt;</t>
+          <t>true</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1058,12 +1058,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Subject</t>
+          <t>Spatial</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Subject</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Spatial</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1075,12 +1075,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>vra:technique</t>
+          <t>dcterms:subject</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>&lt;class 'filter'&gt;</t>
+          <t>true</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1090,12 +1090,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Technique</t>
+          <t>Subject</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Technique</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Subject</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1107,30 +1107,94 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>vra:technique</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Technique</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Technique</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>dcterms:title</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Title</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>dcterms:type</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>&lt;class 'filter'&gt;</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
         <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_group</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:property_range:Type</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>true</t>
         </is>
@@ -14069,7 +14133,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -14102,7 +14166,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -14135,7 +14199,7 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -14168,7 +14232,7 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">

</xml_diff>

<commit_message>
regenerate synthetic data with correct WorkOpening
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -18,8 +18,9 @@
     <sheet name="Work" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="WorkClosing" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="WorkCreation" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="License" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="RightsStatement" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="WorkOpening" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="License" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="RightsStatement" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -495,6 +496,32 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>@graph</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -600,7 +627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -676,7 +703,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -14100,7 +14127,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -14199,7 +14226,7 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -14232,7 +14259,7 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">

</xml_diff>

<commit_message>
only inline anonymous models in a model's named graph
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -15,12 +15,13 @@
     <sheet name="Organization" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Person" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Collection" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Work" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="WorkClosing" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="WorkCreation" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="WorkOpening" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="License" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="RightsStatement" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="NamedLocation" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Work" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="WorkClosing" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="WorkCreation" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="WorkOpening" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="License" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="RightsStatement" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -522,6 +523,32 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>@graph</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -627,7 +654,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -703,7 +730,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -14127,7 +14154,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -14193,7 +14220,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -14305,7 +14332,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14316,8 +14343,174 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>@graph</t>
-        </is>
+          <t>@id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>wgs:lat</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>wgs:long</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work0Location</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>42.728104</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-73.68757600000001</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work1Location</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>42.728104</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-73.68757600000001</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work2Location</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>42.728104</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-73.68757600000001</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work3Location</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>42.728104</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-73.68757600000001</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work4Location</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>42.728104</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-73.68757600000001</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work5Location</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>42.728104</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-73.68757600000001</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work6Location</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>42.728104</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-73.68757600000001</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work7Location</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>42.728104</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-73.68757600000001</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork8Location</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>42.728104</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-73.68757600000001</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork9Location</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>42.728104</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-73.68757600000001</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork10Location</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>42.728104</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-73.68757600000001</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork11Location</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>42.728104</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-73.68757600000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
regenerate synthetic data with new thumbnail size
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -3171,7 +3171,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I257"/>
+  <dimension ref="A1:I267"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13569,12 +13569,12 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image</t>
+          <t>http://example.com/organization0:Image0</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Organization 0 image</t>
+          <t>Organization 0 image 0</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -13584,7 +13584,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="E222" t="inlineStr">
@@ -13599,7 +13599,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Organization 0 image rights holder</t>
+          <t>Organization 0 image 0 rights holder</t>
         </is>
       </c>
       <c r="H222" t="inlineStr">
@@ -13609,29 +13609,29 @@
       </c>
       <c r="I222" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image</t>
+          <t>http://example.com/organization0:Image1</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Organization 1 image</t>
+          <t>Organization 0 image 1</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>http://example.com/organization1</t>
+          <t>http://example.com/organization0</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="E223" t="inlineStr">
@@ -13646,7 +13646,7 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Organization 1 image rights holder</t>
+          <t>Organization 0 image 1 rights holder</t>
         </is>
       </c>
       <c r="H223" t="inlineStr">
@@ -13656,29 +13656,29 @@
       </c>
       <c r="I223" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image</t>
+          <t>http://example.com/organization1:Image0</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Organization 2 image</t>
+          <t>Organization 1 image 0</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>http://example.com/organization2</t>
+          <t>http://example.com/organization1</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="E224" t="inlineStr">
@@ -13693,7 +13693,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Organization 2 image rights holder</t>
+          <t>Organization 1 image 0 rights holder</t>
         </is>
       </c>
       <c r="H224" t="inlineStr">
@@ -13703,29 +13703,29 @@
       </c>
       <c r="I224" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image</t>
+          <t>http://example.com/organization1:Image1</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Organization 3 image</t>
+          <t>Organization 1 image 1</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>http://example.com/organization3</t>
+          <t>http://example.com/organization1</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="E225" t="inlineStr">
@@ -13740,7 +13740,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Organization 3 image rights holder</t>
+          <t>Organization 1 image 1 rights holder</t>
         </is>
       </c>
       <c r="H225" t="inlineStr">
@@ -13750,29 +13750,29 @@
       </c>
       <c r="I225" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image</t>
+          <t>http://example.com/organization2:Image0</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Organization 4 image</t>
+          <t>Organization 2 image 0</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>http://example.com/organization4</t>
+          <t>http://example.com/organization2</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="E226" t="inlineStr">
@@ -13787,7 +13787,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Organization 4 image rights holder</t>
+          <t>Organization 2 image 0 rights holder</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
@@ -13797,29 +13797,29 @@
       </c>
       <c r="I226" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image</t>
+          <t>http://example.com/organization2:Image1</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Person 0 image</t>
+          <t>Organization 2 image 1</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>http://example.com/person0</t>
+          <t>http://example.com/organization2</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="E227" t="inlineStr">
@@ -13834,7 +13834,7 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Person 0 image rights holder</t>
+          <t>Organization 2 image 1 rights holder</t>
         </is>
       </c>
       <c r="H227" t="inlineStr">
@@ -13844,29 +13844,29 @@
       </c>
       <c r="I227" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image</t>
+          <t>http://example.com/organization3:Image0</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Person 1 image</t>
+          <t>Organization 3 image 0</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>http://example.com/person1</t>
+          <t>http://example.com/organization3</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="E228" t="inlineStr">
@@ -13881,7 +13881,7 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Person 1 image rights holder</t>
+          <t>Organization 3 image 0 rights holder</t>
         </is>
       </c>
       <c r="H228" t="inlineStr">
@@ -13891,29 +13891,29 @@
       </c>
       <c r="I228" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image</t>
+          <t>http://example.com/organization3:Image1</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Person 2 image</t>
+          <t>Organization 3 image 1</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>http://example.com/person2</t>
+          <t>http://example.com/organization3</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="E229" t="inlineStr">
@@ -13928,7 +13928,7 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Person 2 image rights holder</t>
+          <t>Organization 3 image 1 rights holder</t>
         </is>
       </c>
       <c r="H229" t="inlineStr">
@@ -13938,29 +13938,29 @@
       </c>
       <c r="I229" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image</t>
+          <t>http://example.com/organization4:Image0</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Person 3 image</t>
+          <t>Organization 4 image 0</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>http://example.com/person3</t>
+          <t>http://example.com/organization4</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="E230" t="inlineStr">
@@ -13975,7 +13975,7 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Person 3 image rights holder</t>
+          <t>Organization 4 image 0 rights holder</t>
         </is>
       </c>
       <c r="H230" t="inlineStr">
@@ -13985,29 +13985,29 @@
       </c>
       <c r="I230" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image</t>
+          <t>http://example.com/organization4:Image1</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Person 4 image</t>
+          <t>Organization 4 image 1</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>http://example.com/person4</t>
+          <t>http://example.com/organization4</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="E231" t="inlineStr">
@@ -14022,7 +14022,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Person 4 image rights holder</t>
+          <t>Organization 4 image 1 rights holder</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
@@ -14032,24 +14032,24 @@
       </c>
       <c r="I231" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0:Image0</t>
+          <t>http://example.com/person0:Image0</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Collection0Work0 image 0</t>
+          <t>Person 0 image 0</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0</t>
+          <t>http://example.com/person0</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
@@ -14069,7 +14069,7 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Collection0Work0 image 0 rights holder</t>
+          <t>Person 0 image 0 rights holder</t>
         </is>
       </c>
       <c r="H232" t="inlineStr">
@@ -14086,17 +14086,17 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0:Image1</t>
+          <t>http://example.com/person0:Image1</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Collection0Work0 image 1</t>
+          <t>Person 0 image 1</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0</t>
+          <t>http://example.com/person0</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
@@ -14116,7 +14116,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Collection0Work0 image 1 rights holder</t>
+          <t>Person 0 image 1 rights holder</t>
         </is>
       </c>
       <c r="H233" t="inlineStr">
@@ -14133,17 +14133,17 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image0</t>
+          <t>http://example.com/person1:Image0</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Collection0Work1 image 0</t>
+          <t>Person 1 image 0</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1</t>
+          <t>http://example.com/person1</t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
@@ -14163,7 +14163,7 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Collection0Work1 image 0 rights holder</t>
+          <t>Person 1 image 0 rights holder</t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
@@ -14180,17 +14180,17 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image1</t>
+          <t>http://example.com/person1:Image1</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Collection0Work1 image 1</t>
+          <t>Person 1 image 1</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1</t>
+          <t>http://example.com/person1</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
@@ -14210,7 +14210,7 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Collection0Work1 image 1 rights holder</t>
+          <t>Person 1 image 1 rights holder</t>
         </is>
       </c>
       <c r="H235" t="inlineStr">
@@ -14227,17 +14227,17 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2:Image0</t>
+          <t>http://example.com/person2:Image0</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Collection0Work2 image 0</t>
+          <t>Person 2 image 0</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2</t>
+          <t>http://example.com/person2</t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
@@ -14257,7 +14257,7 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Collection0Work2 image 0 rights holder</t>
+          <t>Person 2 image 0 rights holder</t>
         </is>
       </c>
       <c r="H236" t="inlineStr">
@@ -14274,17 +14274,17 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2:Image1</t>
+          <t>http://example.com/person2:Image1</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Collection0Work2 image 1</t>
+          <t>Person 2 image 1</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2</t>
+          <t>http://example.com/person2</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
@@ -14304,7 +14304,7 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Collection0Work2 image 1 rights holder</t>
+          <t>Person 2 image 1 rights holder</t>
         </is>
       </c>
       <c r="H237" t="inlineStr">
@@ -14321,17 +14321,17 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image0</t>
+          <t>http://example.com/person3:Image0</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Collection0Work3 image 0</t>
+          <t>Person 3 image 0</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3</t>
+          <t>http://example.com/person3</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
@@ -14351,7 +14351,7 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Collection0Work3 image 0 rights holder</t>
+          <t>Person 3 image 0 rights holder</t>
         </is>
       </c>
       <c r="H238" t="inlineStr">
@@ -14368,17 +14368,17 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image1</t>
+          <t>http://example.com/person3:Image1</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Collection0Work3 image 1</t>
+          <t>Person 3 image 1</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3</t>
+          <t>http://example.com/person3</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
@@ -14398,7 +14398,7 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Collection0Work3 image 1 rights holder</t>
+          <t>Person 3 image 1 rights holder</t>
         </is>
       </c>
       <c r="H239" t="inlineStr">
@@ -14415,17 +14415,17 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image0</t>
+          <t>http://example.com/person4:Image0</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Collection1 image 0</t>
+          <t>Person 4 image 0</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>http://example.com/collection1</t>
+          <t>http://example.com/person4</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
@@ -14445,7 +14445,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Collection1 image 0 rights holder</t>
+          <t>Person 4 image 0 rights holder</t>
         </is>
       </c>
       <c r="H240" t="inlineStr">
@@ -14462,17 +14462,17 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image1</t>
+          <t>http://example.com/person4:Image1</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Collection1 image 1</t>
+          <t>Person 4 image 1</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>http://example.com/collection1</t>
+          <t>http://example.com/person4</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
@@ -14492,7 +14492,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Collection1 image 1 rights holder</t>
+          <t>Person 4 image 1 rights holder</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
@@ -14509,17 +14509,17 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4:Image0</t>
+          <t>http://example.com/collection0/work0:Image0</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Collection1Work4 image 0</t>
+          <t>Collection0Work0 image 0</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4</t>
+          <t>http://example.com/collection0/work0</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
@@ -14539,7 +14539,7 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Collection1Work4 image 0 rights holder</t>
+          <t>Collection0Work0 image 0 rights holder</t>
         </is>
       </c>
       <c r="H242" t="inlineStr">
@@ -14556,17 +14556,17 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4:Image1</t>
+          <t>http://example.com/collection0/work0:Image1</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Collection1Work4 image 1</t>
+          <t>Collection0Work0 image 1</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4</t>
+          <t>http://example.com/collection0/work0</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
@@ -14586,7 +14586,7 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Collection1Work4 image 1 rights holder</t>
+          <t>Collection0Work0 image 1 rights holder</t>
         </is>
       </c>
       <c r="H243" t="inlineStr">
@@ -14603,17 +14603,17 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:Image0</t>
+          <t>http://example.com/collection0/work1:Image0</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Collection1Work5 image 0</t>
+          <t>Collection0Work1 image 0</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5</t>
+          <t>http://example.com/collection0/work1</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
@@ -14633,7 +14633,7 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Collection1Work5 image 0 rights holder</t>
+          <t>Collection0Work1 image 0 rights holder</t>
         </is>
       </c>
       <c r="H244" t="inlineStr">
@@ -14650,17 +14650,17 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:Image1</t>
+          <t>http://example.com/collection0/work1:Image1</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Collection1Work5 image 1</t>
+          <t>Collection0Work1 image 1</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5</t>
+          <t>http://example.com/collection0/work1</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
@@ -14680,7 +14680,7 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Collection1Work5 image 1 rights holder</t>
+          <t>Collection0Work1 image 1 rights holder</t>
         </is>
       </c>
       <c r="H245" t="inlineStr">
@@ -14697,17 +14697,17 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6:Image0</t>
+          <t>http://example.com/collection0/work2:Image0</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Collection1Work6 image 0</t>
+          <t>Collection0Work2 image 0</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6</t>
+          <t>http://example.com/collection0/work2</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
@@ -14727,7 +14727,7 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Collection1Work6 image 0 rights holder</t>
+          <t>Collection0Work2 image 0 rights holder</t>
         </is>
       </c>
       <c r="H246" t="inlineStr">
@@ -14744,17 +14744,17 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6:Image1</t>
+          <t>http://example.com/collection0/work2:Image1</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Collection1Work6 image 1</t>
+          <t>Collection0Work2 image 1</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6</t>
+          <t>http://example.com/collection0/work2</t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
@@ -14774,7 +14774,7 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Collection1Work6 image 1 rights holder</t>
+          <t>Collection0Work2 image 1 rights holder</t>
         </is>
       </c>
       <c r="H247" t="inlineStr">
@@ -14791,17 +14791,17 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image0</t>
+          <t>http://example.com/collection0/work3:Image0</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Collection1Work7 image 0</t>
+          <t>Collection0Work3 image 0</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7</t>
+          <t>http://example.com/collection0/work3</t>
         </is>
       </c>
       <c r="D248" t="inlineStr">
@@ -14821,7 +14821,7 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Collection1Work7 image 0 rights holder</t>
+          <t>Collection0Work3 image 0 rights holder</t>
         </is>
       </c>
       <c r="H248" t="inlineStr">
@@ -14838,17 +14838,17 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image1</t>
+          <t>http://example.com/collection0/work3:Image1</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Collection1Work7 image 1</t>
+          <t>Collection0Work3 image 1</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7</t>
+          <t>http://example.com/collection0/work3</t>
         </is>
       </c>
       <c r="D249" t="inlineStr">
@@ -14868,7 +14868,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Collection1Work7 image 1 rights holder</t>
+          <t>Collection0Work3 image 1 rights holder</t>
         </is>
       </c>
       <c r="H249" t="inlineStr">
@@ -14885,17 +14885,17 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8:Image0</t>
+          <t>http://example.com/collection1:Image0</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>FreestandingWork8 image 0</t>
+          <t>Collection1 image 0</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8</t>
+          <t>http://example.com/collection1</t>
         </is>
       </c>
       <c r="D250" t="inlineStr">
@@ -14915,7 +14915,7 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>FreestandingWork8 image 0 rights holder</t>
+          <t>Collection1 image 0 rights holder</t>
         </is>
       </c>
       <c r="H250" t="inlineStr">
@@ -14932,17 +14932,17 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8:Image1</t>
+          <t>http://example.com/collection1:Image1</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>FreestandingWork8 image 1</t>
+          <t>Collection1 image 1</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8</t>
+          <t>http://example.com/collection1</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
@@ -14962,7 +14962,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>FreestandingWork8 image 1 rights holder</t>
+          <t>Collection1 image 1 rights holder</t>
         </is>
       </c>
       <c r="H251" t="inlineStr">
@@ -14979,17 +14979,17 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:Image0</t>
+          <t>http://example.com/collection1/work4:Image0</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>FreestandingWork9 image 0</t>
+          <t>Collection1Work4 image 0</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9</t>
+          <t>http://example.com/collection1/work4</t>
         </is>
       </c>
       <c r="D252" t="inlineStr">
@@ -15009,7 +15009,7 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>FreestandingWork9 image 0 rights holder</t>
+          <t>Collection1Work4 image 0 rights holder</t>
         </is>
       </c>
       <c r="H252" t="inlineStr">
@@ -15026,17 +15026,17 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:Image1</t>
+          <t>http://example.com/collection1/work4:Image1</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>FreestandingWork9 image 1</t>
+          <t>Collection1Work4 image 1</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9</t>
+          <t>http://example.com/collection1/work4</t>
         </is>
       </c>
       <c r="D253" t="inlineStr">
@@ -15056,7 +15056,7 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>FreestandingWork9 image 1 rights holder</t>
+          <t>Collection1Work4 image 1 rights holder</t>
         </is>
       </c>
       <c r="H253" t="inlineStr">
@@ -15073,17 +15073,17 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10:Image0</t>
+          <t>http://example.com/collection1/work5:Image0</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>FreestandingWork10 image 0</t>
+          <t>Collection1Work5 image 0</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10</t>
+          <t>http://example.com/collection1/work5</t>
         </is>
       </c>
       <c r="D254" t="inlineStr">
@@ -15103,7 +15103,7 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>FreestandingWork10 image 0 rights holder</t>
+          <t>Collection1Work5 image 0 rights holder</t>
         </is>
       </c>
       <c r="H254" t="inlineStr">
@@ -15120,17 +15120,17 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10:Image1</t>
+          <t>http://example.com/collection1/work5:Image1</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>FreestandingWork10 image 1</t>
+          <t>Collection1Work5 image 1</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10</t>
+          <t>http://example.com/collection1/work5</t>
         </is>
       </c>
       <c r="D255" t="inlineStr">
@@ -15150,7 +15150,7 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>FreestandingWork10 image 1 rights holder</t>
+          <t>Collection1Work5 image 1 rights holder</t>
         </is>
       </c>
       <c r="H255" t="inlineStr">
@@ -15167,17 +15167,17 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:Image0</t>
+          <t>http://example.com/collection1/work6:Image0</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>FreestandingWork11 image 0</t>
+          <t>Collection1Work6 image 0</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11</t>
+          <t>http://example.com/collection1/work6</t>
         </is>
       </c>
       <c r="D256" t="inlineStr">
@@ -15197,7 +15197,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>FreestandingWork11 image 0 rights holder</t>
+          <t>Collection1Work6 image 0 rights holder</t>
         </is>
       </c>
       <c r="H256" t="inlineStr">
@@ -15214,45 +15214,515 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
+          <t>http://example.com/collection1/work6:Image1</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>Collection1Work6 image 1</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work6</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="G257" t="inlineStr">
+        <is>
+          <t>Collection1Work6 image 1 rights holder</t>
+        </is>
+      </c>
+      <c r="H257" t="inlineStr">
+        <is>
+          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
+        </is>
+      </c>
+      <c r="I257" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work7:Image0</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>Collection1Work7 image 0</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work7</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="G258" t="inlineStr">
+        <is>
+          <t>Collection1Work7 image 0 rights holder</t>
+        </is>
+      </c>
+      <c r="H258" t="inlineStr">
+        <is>
+          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
+        </is>
+      </c>
+      <c r="I258" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work7:Image1</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>Collection1Work7 image 1</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work7</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="G259" t="inlineStr">
+        <is>
+          <t>Collection1Work7 image 1 rights holder</t>
+        </is>
+      </c>
+      <c r="H259" t="inlineStr">
+        <is>
+          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
+        </is>
+      </c>
+      <c r="I259" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork8:Image0</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>FreestandingWork8 image 0</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork8</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="G260" t="inlineStr">
+        <is>
+          <t>FreestandingWork8 image 0 rights holder</t>
+        </is>
+      </c>
+      <c r="H260" t="inlineStr">
+        <is>
+          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
+        </is>
+      </c>
+      <c r="I260" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork8:Image1</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>FreestandingWork8 image 1</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork8</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="G261" t="inlineStr">
+        <is>
+          <t>FreestandingWork8 image 1 rights holder</t>
+        </is>
+      </c>
+      <c r="H261" t="inlineStr">
+        <is>
+          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
+        </is>
+      </c>
+      <c r="I261" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork9:Image0</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>FreestandingWork9 image 0</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork9</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="G262" t="inlineStr">
+        <is>
+          <t>FreestandingWork9 image 0 rights holder</t>
+        </is>
+      </c>
+      <c r="H262" t="inlineStr">
+        <is>
+          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
+        </is>
+      </c>
+      <c r="I262" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork9:Image1</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>FreestandingWork9 image 1</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork9</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="G263" t="inlineStr">
+        <is>
+          <t>FreestandingWork9 image 1 rights holder</t>
+        </is>
+      </c>
+      <c r="H263" t="inlineStr">
+        <is>
+          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
+        </is>
+      </c>
+      <c r="I263" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork10:Image0</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>FreestandingWork10 image 0</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork10</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="G264" t="inlineStr">
+        <is>
+          <t>FreestandingWork10 image 0 rights holder</t>
+        </is>
+      </c>
+      <c r="H264" t="inlineStr">
+        <is>
+          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
+        </is>
+      </c>
+      <c r="I264" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork10:Image1</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>FreestandingWork10 image 1</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork10</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="G265" t="inlineStr">
+        <is>
+          <t>FreestandingWork10 image 1 rights holder</t>
+        </is>
+      </c>
+      <c r="H265" t="inlineStr">
+        <is>
+          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
+        </is>
+      </c>
+      <c r="I265" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork11:Image0</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>FreestandingWork11 image 0</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork11</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="G266" t="inlineStr">
+        <is>
+          <t>FreestandingWork11 image 0 rights holder</t>
+        </is>
+      </c>
+      <c r="H266" t="inlineStr">
+        <is>
+          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
+        </is>
+      </c>
+      <c r="I266" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
           <t>http://example.com/freestandingwork11:Image1</t>
         </is>
       </c>
-      <c r="B257" t="inlineStr">
+      <c r="B267" t="inlineStr">
         <is>
           <t>FreestandingWork11 image 1</t>
         </is>
       </c>
-      <c r="C257" t="inlineStr">
+      <c r="C267" t="inlineStr">
         <is>
           <t>http://example.com/freestandingwork11</t>
         </is>
       </c>
-      <c r="D257" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="E257" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="F257" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="G257" t="inlineStr">
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="G267" t="inlineStr">
         <is>
           <t>FreestandingWork11 image 1 rights holder</t>
         </is>
       </c>
-      <c r="H257" t="inlineStr">
-        <is>
-          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
-        </is>
-      </c>
-      <c r="I257" t="inlineStr">
+      <c r="H267" t="inlineStr">
+        <is>
+          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
+        </is>
+      </c>
+      <c r="I267" t="inlineStr">
         <is>
           <t>1000</t>
         </is>
@@ -15472,7 +15942,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -15505,7 +15975,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -15538,7 +16008,7 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -15571,7 +16041,7 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">

</xml_diff>

<commit_message>
synthetic data pipeline working again
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -8,20 +8,20 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="PropertyGroup" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Property" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Concept" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Image" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Organization" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Person" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Collection" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="NamedLocation" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Work" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="WorkClosing" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="WorkCreation" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="WorkOpening" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="License" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="RightsStatement" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="CmsPropertyGroup" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="CmsProperty" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="CmsConcept" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="CmsImage" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="CmsOrganization" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="CmsPerson" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="CmsCollection" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="CmsNamedLocation" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="CmsWork" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="CmsWorkClosing" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="CmsWorkCreation" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="CmsWorkOpening" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="CmsLicense" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="CmsRightsStatement" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1298,7 +1298,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Concept 0</t>
+          <t>CmsConcept 0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1315,7 +1315,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Concept 1</t>
+          <t>CmsConcept 1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1332,7 +1332,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Concept 2</t>
+          <t>CmsConcept 2</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Concept 3</t>
+          <t>CmsConcept 3</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1366,7 +1366,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Concept 4</t>
+          <t>CmsConcept 4</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1383,7 +1383,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Concept 5</t>
+          <t>CmsConcept 5</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1400,7 +1400,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Concept 6</t>
+          <t>CmsConcept 6</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Concept 7</t>
+          <t>CmsConcept 7</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1434,7 +1434,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Concept 8</t>
+          <t>CmsConcept 8</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Concept 9</t>
+          <t>CmsConcept 9</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1468,7 +1468,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Concept 10</t>
+          <t>CmsConcept 10</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Concept 11</t>
+          <t>CmsConcept 11</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Concept 12</t>
+          <t>CmsConcept 12</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1519,7 +1519,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Concept 13</t>
+          <t>CmsConcept 13</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1536,7 +1536,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Concept 14</t>
+          <t>CmsConcept 14</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Concept 15</t>
+          <t>CmsConcept 15</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1570,7 +1570,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Concept 16</t>
+          <t>CmsConcept 16</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1587,7 +1587,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Concept 17</t>
+          <t>CmsConcept 17</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1604,7 +1604,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Concept 18</t>
+          <t>CmsConcept 18</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Concept 19</t>
+          <t>CmsConcept 19</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Concept 20</t>
+          <t>CmsConcept 20</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1655,7 +1655,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Concept 21</t>
+          <t>CmsConcept 21</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1672,7 +1672,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Concept 22</t>
+          <t>CmsConcept 22</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Concept 23</t>
+          <t>CmsConcept 23</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1706,7 +1706,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Concept 24</t>
+          <t>CmsConcept 24</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Concept 25</t>
+          <t>CmsConcept 25</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1740,7 +1740,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Concept 26</t>
+          <t>CmsConcept 26</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1757,7 +1757,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Concept 27</t>
+          <t>CmsConcept 27</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1774,7 +1774,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Concept 28</t>
+          <t>CmsConcept 28</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1791,7 +1791,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Concept 29</t>
+          <t>CmsConcept 29</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1808,7 +1808,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Concept 30</t>
+          <t>CmsConcept 30</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Concept 31</t>
+          <t>CmsConcept 31</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1842,7 +1842,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Concept 32</t>
+          <t>CmsConcept 32</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1859,7 +1859,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Concept 33</t>
+          <t>CmsConcept 33</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Concept 34</t>
+          <t>CmsConcept 34</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1893,7 +1893,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Concept 35</t>
+          <t>CmsConcept 35</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Concept 36</t>
+          <t>CmsConcept 36</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1927,7 +1927,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Concept 37</t>
+          <t>CmsConcept 37</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1944,7 +1944,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Concept 38</t>
+          <t>CmsConcept 38</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Concept 39</t>
+          <t>CmsConcept 39</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1978,7 +1978,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Concept 40</t>
+          <t>CmsConcept 40</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1995,7 +1995,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Concept 41</t>
+          <t>CmsConcept 41</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2012,7 +2012,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Concept 42</t>
+          <t>CmsConcept 42</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Concept 43</t>
+          <t>CmsConcept 43</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2046,7 +2046,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Concept 44</t>
+          <t>CmsConcept 44</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2063,7 +2063,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Concept 45</t>
+          <t>CmsConcept 45</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2080,7 +2080,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Concept 46</t>
+          <t>CmsConcept 46</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2097,7 +2097,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Concept 47</t>
+          <t>CmsConcept 47</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2114,7 +2114,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Concept 48</t>
+          <t>CmsConcept 48</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Concept 49</t>
+          <t>CmsConcept 49</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2148,7 +2148,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Concept 50</t>
+          <t>CmsConcept 50</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2165,7 +2165,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Concept 51</t>
+          <t>CmsConcept 51</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2182,7 +2182,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Concept 52</t>
+          <t>CmsConcept 52</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2199,7 +2199,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Concept 53</t>
+          <t>CmsConcept 53</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2216,7 +2216,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Concept 54</t>
+          <t>CmsConcept 54</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Concept 55</t>
+          <t>CmsConcept 55</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2250,7 +2250,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Concept 56</t>
+          <t>CmsConcept 56</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2267,7 +2267,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Concept 57</t>
+          <t>CmsConcept 57</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2284,7 +2284,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Concept 58</t>
+          <t>CmsConcept 58</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Concept 59</t>
+          <t>CmsConcept 59</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2318,7 +2318,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Concept 60</t>
+          <t>CmsConcept 60</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2335,7 +2335,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Concept 61</t>
+          <t>CmsConcept 61</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2352,7 +2352,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Concept 62</t>
+          <t>CmsConcept 62</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Concept 63</t>
+          <t>CmsConcept 63</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2386,7 +2386,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Concept 64</t>
+          <t>CmsConcept 64</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2403,7 +2403,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Concept 65</t>
+          <t>CmsConcept 65</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2420,7 +2420,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Concept 66</t>
+          <t>CmsConcept 66</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Concept 67</t>
+          <t>CmsConcept 67</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2454,7 +2454,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Concept 68</t>
+          <t>CmsConcept 68</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2471,7 +2471,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Concept 69</t>
+          <t>CmsConcept 69</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Concept 70</t>
+          <t>CmsConcept 70</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Concept 71</t>
+          <t>CmsConcept 71</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2522,7 +2522,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Concept 72</t>
+          <t>CmsConcept 72</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2539,7 +2539,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Concept 73</t>
+          <t>CmsConcept 73</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2556,7 +2556,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Concept 74</t>
+          <t>CmsConcept 74</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2573,7 +2573,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Concept 75</t>
+          <t>CmsConcept 75</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2590,7 +2590,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Concept 76</t>
+          <t>CmsConcept 76</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2607,7 +2607,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Concept 77</t>
+          <t>CmsConcept 77</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2624,7 +2624,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Concept 78</t>
+          <t>CmsConcept 78</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2641,7 +2641,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Concept 79</t>
+          <t>CmsConcept 79</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Concept 80</t>
+          <t>CmsConcept 80</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2675,7 +2675,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Concept 81</t>
+          <t>CmsConcept 81</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2692,7 +2692,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Concept 82</t>
+          <t>CmsConcept 82</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2709,7 +2709,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Concept 83</t>
+          <t>CmsConcept 83</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Concept 84</t>
+          <t>CmsConcept 84</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2743,7 +2743,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Concept 85</t>
+          <t>CmsConcept 85</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2760,7 +2760,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Concept 86</t>
+          <t>CmsConcept 86</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2777,7 +2777,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Concept 87</t>
+          <t>CmsConcept 87</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2794,7 +2794,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Concept 88</t>
+          <t>CmsConcept 88</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2811,7 +2811,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Concept 89</t>
+          <t>CmsConcept 89</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2828,7 +2828,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Concept 90</t>
+          <t>CmsConcept 90</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2845,7 +2845,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Concept 91</t>
+          <t>CmsConcept 91</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2862,7 +2862,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Concept 92</t>
+          <t>CmsConcept 92</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2879,7 +2879,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Concept 93</t>
+          <t>CmsConcept 93</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2896,7 +2896,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Concept 94</t>
+          <t>CmsConcept 94</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Concept 95</t>
+          <t>CmsConcept 95</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2930,7 +2930,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Concept 96</t>
+          <t>CmsConcept 96</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2947,7 +2947,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Concept 97</t>
+          <t>CmsConcept 97</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2964,7 +2964,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Concept 98</t>
+          <t>CmsConcept 98</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2981,7 +2981,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Concept 99</t>
+          <t>CmsConcept 99</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2998,7 +2998,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Concept 100</t>
+          <t>CmsConcept 100</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3015,7 +3015,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Concept 101</t>
+          <t>CmsConcept 101</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3032,7 +3032,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Concept 102</t>
+          <t>CmsConcept 102</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Concept 103</t>
+          <t>CmsConcept 103</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Concept 104</t>
+          <t>CmsConcept 104</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3083,7 +3083,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Concept 105</t>
+          <t>CmsConcept 105</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3100,7 +3100,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Concept 106</t>
+          <t>CmsConcept 106</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3117,7 +3117,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Concept 107</t>
+          <t>CmsConcept 107</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3134,7 +3134,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Concept 108</t>
+          <t>CmsConcept 108</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Concept 109</t>
+          <t>CmsConcept 109</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3229,7 +3229,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:CmsImage0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -3276,7 +3276,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:CmsImage1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3323,7 +3323,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:CmsImage0</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3370,7 +3370,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:CmsImage1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3417,7 +3417,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:CmsImage0</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3464,7 +3464,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:CmsImage1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3511,7 +3511,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:CmsImage0</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3558,7 +3558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:CmsImage1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -3605,7 +3605,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:CmsImage0</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -3652,7 +3652,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:CmsImage1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -3699,7 +3699,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:CmsImage0</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -3746,7 +3746,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:CmsImage1</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -3793,7 +3793,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:CmsImage0</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -3840,7 +3840,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:CmsImage1</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -3887,7 +3887,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:CmsImage0</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -3934,7 +3934,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:CmsImage1</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -3981,7 +3981,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:CmsImage0</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:CmsImage1</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -4075,7 +4075,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:CmsImage0</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -4122,7 +4122,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:CmsImage1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -4169,7 +4169,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:CmsImage0</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -4216,7 +4216,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:CmsImage1</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -4263,7 +4263,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:CmsImage0</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -4310,7 +4310,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:CmsImage1</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -4357,7 +4357,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:CmsImage0</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -4404,7 +4404,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:CmsImage1</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -4451,7 +4451,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:CmsImage0</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -4498,7 +4498,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:CmsImage1</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -4545,7 +4545,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:CmsImage0</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -4592,7 +4592,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:CmsImage1</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -4639,7 +4639,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:CmsImage0</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -4686,7 +4686,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:CmsImage1</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -4733,7 +4733,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:CmsImage0</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -4780,7 +4780,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:CmsImage1</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4827,7 +4827,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:CmsImage0</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -4874,7 +4874,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:CmsImage1</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -4921,7 +4921,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:CmsImage0</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -4968,7 +4968,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:CmsImage1</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -5015,7 +5015,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:CmsImage0</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -5062,7 +5062,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:CmsImage1</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -5109,7 +5109,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:CmsImage0</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -5156,7 +5156,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:CmsImage1</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -5203,7 +5203,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:CmsImage0</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -5250,7 +5250,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:CmsImage1</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -5297,7 +5297,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:CmsImage0</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -5344,7 +5344,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:CmsImage1</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -5391,7 +5391,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:CmsImage0</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -5438,7 +5438,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:CmsImage1</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -5485,7 +5485,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:CmsImage0</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -5532,7 +5532,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:CmsImage1</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -5579,7 +5579,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:CmsImage0</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -5626,7 +5626,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:CmsImage1</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -5673,7 +5673,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:CmsImage0</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -5720,7 +5720,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:CmsImage1</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -5767,7 +5767,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:CmsImage0</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -5814,7 +5814,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:CmsImage1</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -5861,7 +5861,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:CmsImage0</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -5908,7 +5908,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:CmsImage1</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -5955,7 +5955,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:CmsImage0</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -6002,7 +6002,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:CmsImage1</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -6049,7 +6049,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:CmsImage0</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -6096,7 +6096,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:CmsImage1</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -6143,7 +6143,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:CmsImage0</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -6190,7 +6190,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:CmsImage1</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -6237,7 +6237,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:CmsImage0</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -6284,7 +6284,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:CmsImage1</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -6331,7 +6331,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:CmsImage0</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -6378,7 +6378,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:CmsImage1</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -6425,7 +6425,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:CmsImage0</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -6472,7 +6472,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:CmsImage1</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -6519,7 +6519,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:CmsImage0</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -6566,7 +6566,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:CmsImage1</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -6613,7 +6613,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:CmsImage0</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -6660,7 +6660,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:CmsImage1</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6707,7 +6707,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:CmsImage0</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6754,7 +6754,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:CmsImage1</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6801,7 +6801,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:CmsImage0</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -6848,7 +6848,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:CmsImage1</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6895,7 +6895,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:CmsImage0</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6942,7 +6942,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:CmsImage1</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6989,7 +6989,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:CmsImage0</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -7036,7 +7036,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:CmsImage1</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -7083,7 +7083,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:CmsImage0</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -7130,7 +7130,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:CmsImage1</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -7177,7 +7177,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:CmsImage0</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -7224,7 +7224,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:CmsImage1</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -7271,7 +7271,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:CmsImage0</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -7318,7 +7318,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:CmsImage1</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -7365,7 +7365,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:CmsImage0</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -7412,7 +7412,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:CmsImage1</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -7459,7 +7459,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:CmsImage0</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -7506,7 +7506,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:CmsImage1</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -7553,7 +7553,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:CmsImage0</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -7600,7 +7600,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:CmsImage1</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -7647,7 +7647,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:CmsImage0</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -7694,7 +7694,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:CmsImage1</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -7741,7 +7741,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:CmsImage0</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -7788,7 +7788,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:CmsImage1</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -7835,7 +7835,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:CmsImage0</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -7882,7 +7882,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:CmsImage1</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -7929,7 +7929,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:CmsImage0</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -7976,7 +7976,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:CmsImage1</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -8023,7 +8023,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:CmsImage0</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -8070,7 +8070,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:CmsImage1</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -8117,7 +8117,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:CmsImage0</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -8164,7 +8164,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:CmsImage1</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -8211,7 +8211,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:CmsImage0</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -8258,7 +8258,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:CmsImage1</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -8305,7 +8305,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:CmsImage0</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -8352,7 +8352,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:CmsImage1</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -8399,7 +8399,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:CmsImage0</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -8446,7 +8446,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:CmsImage1</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -8493,7 +8493,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:CmsImage0</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -8540,7 +8540,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:CmsImage1</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -8587,7 +8587,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:CmsImage0</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -8634,7 +8634,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:CmsImage1</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -8681,7 +8681,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:CmsImage0</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -8728,7 +8728,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:CmsImage1</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -8775,7 +8775,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:CmsImage0</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -8822,7 +8822,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:CmsImage1</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -8869,7 +8869,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:CmsImage0</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -8916,7 +8916,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:CmsImage1</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -8963,7 +8963,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:CmsImage0</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -9010,7 +9010,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:CmsImage1</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -9057,7 +9057,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:CmsImage0</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -9104,7 +9104,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:CmsImage1</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -9151,7 +9151,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:CmsImage0</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -9198,7 +9198,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:CmsImage1</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -9245,7 +9245,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:CmsImage0</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -9292,7 +9292,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:CmsImage1</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -9339,7 +9339,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:CmsImage0</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -9386,7 +9386,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:CmsImage1</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -9433,7 +9433,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:CmsImage0</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -9480,7 +9480,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:CmsImage1</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -9527,7 +9527,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:CmsImage0</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -9574,7 +9574,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:CmsImage1</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -9621,7 +9621,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:CmsImage0</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -9668,7 +9668,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:CmsImage1</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -9715,7 +9715,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:CmsImage0</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -9762,7 +9762,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:CmsImage1</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -9809,7 +9809,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:CmsImage0</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -9856,7 +9856,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:CmsImage1</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -9903,7 +9903,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:CmsImage0</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -9950,7 +9950,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:CmsImage1</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -9997,7 +9997,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:CmsImage0</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -10044,7 +10044,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:CmsImage1</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -10091,7 +10091,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:CmsImage0</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -10138,7 +10138,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:CmsImage1</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -10185,7 +10185,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:CmsImage0</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -10232,7 +10232,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:CmsImage1</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -10279,7 +10279,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:CmsImage0</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -10326,7 +10326,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:CmsImage1</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -10373,7 +10373,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:CmsImage0</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -10420,7 +10420,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:CmsImage1</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -10467,7 +10467,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:CmsImage0</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -10514,7 +10514,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:CmsImage1</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -10561,7 +10561,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:CmsImage0</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -10608,7 +10608,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:CmsImage1</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -10655,7 +10655,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:CmsImage0</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -10702,7 +10702,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:CmsImage1</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -10749,7 +10749,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:CmsImage0</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -10796,7 +10796,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:CmsImage1</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -10843,7 +10843,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:CmsImage0</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -10890,7 +10890,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:CmsImage1</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -10937,7 +10937,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:CmsImage0</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -10984,7 +10984,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:CmsImage1</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -11031,7 +11031,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:CmsImage0</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -11078,7 +11078,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:CmsImage1</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -11125,7 +11125,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:CmsImage0</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -11172,7 +11172,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:CmsImage1</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -11219,7 +11219,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:CmsImage0</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -11266,7 +11266,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:CmsImage1</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -11313,7 +11313,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:CmsImage0</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -11360,7 +11360,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:CmsImage1</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -11407,7 +11407,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:CmsImage0</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -11454,7 +11454,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:CmsImage1</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -11501,7 +11501,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:CmsImage0</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -11548,7 +11548,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:CmsImage1</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -11595,7 +11595,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:CmsImage0</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -11642,7 +11642,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:CmsImage1</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -11689,7 +11689,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:CmsImage0</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -11736,7 +11736,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:CmsImage1</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -11783,7 +11783,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:CmsImage0</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -11830,7 +11830,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:CmsImage1</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -11877,7 +11877,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:CmsImage0</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -11924,7 +11924,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:CmsImage1</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -11971,7 +11971,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:CmsImage0</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -12018,7 +12018,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:CmsImage1</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -12065,7 +12065,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:CmsImage0</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -12112,7 +12112,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:CmsImage1</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -12159,7 +12159,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:CmsImage0</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -12206,7 +12206,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:CmsImage1</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -12253,7 +12253,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:CmsImage0</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -12300,7 +12300,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:CmsImage1</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -12347,7 +12347,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:CmsImage0</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -12394,7 +12394,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:CmsImage1</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -12441,7 +12441,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:CmsImage0</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -12488,7 +12488,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:CmsImage1</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -12535,7 +12535,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:CmsImage0</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -12582,7 +12582,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:CmsImage1</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -12629,7 +12629,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:CmsImage0</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -12676,7 +12676,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:CmsImage1</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -12723,7 +12723,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:CmsImage0</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -12770,7 +12770,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:CmsImage1</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -12817,7 +12817,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:CmsImage0</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -12864,7 +12864,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:CmsImage1</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -12911,7 +12911,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:CmsImage0</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -12958,7 +12958,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:CmsImage1</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -13005,7 +13005,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:CmsImage0</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -13052,7 +13052,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:CmsImage1</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -13099,7 +13099,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:CmsImage0</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -13146,7 +13146,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:CmsImage1</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -13193,7 +13193,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:CmsImage0</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -13240,7 +13240,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:CmsImage1</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
@@ -13287,7 +13287,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:CmsImage0</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -13334,7 +13334,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:CmsImage1</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -13381,7 +13381,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:CmsImage0</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -13428,7 +13428,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:CmsImage1</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
@@ -13475,7 +13475,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:CmsImage0</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -13522,7 +13522,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:CmsImage1</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -13569,12 +13569,12 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0</t>
+          <t>http://example.com/organization0:CmsImage0</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Organization 0 image 0</t>
+          <t>CmsOrganization 0 image 0</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -13599,7 +13599,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Organization 0 image 0 rights holder</t>
+          <t>CmsOrganization 0 image 0 rights holder</t>
         </is>
       </c>
       <c r="H222" t="inlineStr">
@@ -13616,12 +13616,12 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image1</t>
+          <t>http://example.com/organization0:CmsImage1</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Organization 0 image 1</t>
+          <t>CmsOrganization 0 image 1</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -13646,7 +13646,7 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Organization 0 image 1 rights holder</t>
+          <t>CmsOrganization 0 image 1 rights holder</t>
         </is>
       </c>
       <c r="H223" t="inlineStr">
@@ -13663,12 +13663,12 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image0</t>
+          <t>http://example.com/organization1:CmsImage0</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Organization 1 image 0</t>
+          <t>CmsOrganization 1 image 0</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -13693,7 +13693,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Organization 1 image 0 rights holder</t>
+          <t>CmsOrganization 1 image 0 rights holder</t>
         </is>
       </c>
       <c r="H224" t="inlineStr">
@@ -13710,12 +13710,12 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image1</t>
+          <t>http://example.com/organization1:CmsImage1</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Organization 1 image 1</t>
+          <t>CmsOrganization 1 image 1</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -13740,7 +13740,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Organization 1 image 1 rights holder</t>
+          <t>CmsOrganization 1 image 1 rights holder</t>
         </is>
       </c>
       <c r="H225" t="inlineStr">
@@ -13757,12 +13757,12 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0</t>
+          <t>http://example.com/organization2:CmsImage0</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Organization 2 image 0</t>
+          <t>CmsOrganization 2 image 0</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -13787,7 +13787,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Organization 2 image 0 rights holder</t>
+          <t>CmsOrganization 2 image 0 rights holder</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
@@ -13804,12 +13804,12 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image1</t>
+          <t>http://example.com/organization2:CmsImage1</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Organization 2 image 1</t>
+          <t>CmsOrganization 2 image 1</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -13834,7 +13834,7 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Organization 2 image 1 rights holder</t>
+          <t>CmsOrganization 2 image 1 rights holder</t>
         </is>
       </c>
       <c r="H227" t="inlineStr">
@@ -13851,12 +13851,12 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image0</t>
+          <t>http://example.com/organization3:CmsImage0</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Organization 3 image 0</t>
+          <t>CmsOrganization 3 image 0</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -13881,7 +13881,7 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Organization 3 image 0 rights holder</t>
+          <t>CmsOrganization 3 image 0 rights holder</t>
         </is>
       </c>
       <c r="H228" t="inlineStr">
@@ -13898,12 +13898,12 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image1</t>
+          <t>http://example.com/organization3:CmsImage1</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Organization 3 image 1</t>
+          <t>CmsOrganization 3 image 1</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -13928,7 +13928,7 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Organization 3 image 1 rights holder</t>
+          <t>CmsOrganization 3 image 1 rights holder</t>
         </is>
       </c>
       <c r="H229" t="inlineStr">
@@ -13945,12 +13945,12 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0</t>
+          <t>http://example.com/organization4:CmsImage0</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Organization 4 image 0</t>
+          <t>CmsOrganization 4 image 0</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -13975,7 +13975,7 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Organization 4 image 0 rights holder</t>
+          <t>CmsOrganization 4 image 0 rights holder</t>
         </is>
       </c>
       <c r="H230" t="inlineStr">
@@ -13992,12 +13992,12 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image1</t>
+          <t>http://example.com/organization4:CmsImage1</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Organization 4 image 1</t>
+          <t>CmsOrganization 4 image 1</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -14022,7 +14022,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Organization 4 image 1 rights holder</t>
+          <t>CmsOrganization 4 image 1 rights holder</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
@@ -14039,12 +14039,12 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image0</t>
+          <t>http://example.com/person0:CmsImage0</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Person 0 image 0</t>
+          <t>CmsPerson 0 image 0</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -14069,7 +14069,7 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Person 0 image 0 rights holder</t>
+          <t>CmsPerson 0 image 0 rights holder</t>
         </is>
       </c>
       <c r="H232" t="inlineStr">
@@ -14086,12 +14086,12 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image1</t>
+          <t>http://example.com/person0:CmsImage1</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Person 0 image 1</t>
+          <t>CmsPerson 0 image 1</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -14116,7 +14116,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Person 0 image 1 rights holder</t>
+          <t>CmsPerson 0 image 1 rights holder</t>
         </is>
       </c>
       <c r="H233" t="inlineStr">
@@ -14133,12 +14133,12 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image0</t>
+          <t>http://example.com/person1:CmsImage0</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Person 1 image 0</t>
+          <t>CmsPerson 1 image 0</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
@@ -14163,7 +14163,7 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Person 1 image 0 rights holder</t>
+          <t>CmsPerson 1 image 0 rights holder</t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
@@ -14180,12 +14180,12 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image1</t>
+          <t>http://example.com/person1:CmsImage1</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Person 1 image 1</t>
+          <t>CmsPerson 1 image 1</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -14210,7 +14210,7 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Person 1 image 1 rights holder</t>
+          <t>CmsPerson 1 image 1 rights holder</t>
         </is>
       </c>
       <c r="H235" t="inlineStr">
@@ -14227,12 +14227,12 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image0</t>
+          <t>http://example.com/person2:CmsImage0</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Person 2 image 0</t>
+          <t>CmsPerson 2 image 0</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -14257,7 +14257,7 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Person 2 image 0 rights holder</t>
+          <t>CmsPerson 2 image 0 rights holder</t>
         </is>
       </c>
       <c r="H236" t="inlineStr">
@@ -14274,12 +14274,12 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image1</t>
+          <t>http://example.com/person2:CmsImage1</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Person 2 image 1</t>
+          <t>CmsPerson 2 image 1</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -14304,7 +14304,7 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Person 2 image 1 rights holder</t>
+          <t>CmsPerson 2 image 1 rights holder</t>
         </is>
       </c>
       <c r="H237" t="inlineStr">
@@ -14321,12 +14321,12 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0</t>
+          <t>http://example.com/person3:CmsImage0</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Person 3 image 0</t>
+          <t>CmsPerson 3 image 0</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
@@ -14351,7 +14351,7 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Person 3 image 0 rights holder</t>
+          <t>CmsPerson 3 image 0 rights holder</t>
         </is>
       </c>
       <c r="H238" t="inlineStr">
@@ -14368,12 +14368,12 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image1</t>
+          <t>http://example.com/person3:CmsImage1</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Person 3 image 1</t>
+          <t>CmsPerson 3 image 1</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -14398,7 +14398,7 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Person 3 image 1 rights holder</t>
+          <t>CmsPerson 3 image 1 rights holder</t>
         </is>
       </c>
       <c r="H239" t="inlineStr">
@@ -14415,12 +14415,12 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image0</t>
+          <t>http://example.com/person4:CmsImage0</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Person 4 image 0</t>
+          <t>CmsPerson 4 image 0</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -14445,7 +14445,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Person 4 image 0 rights holder</t>
+          <t>CmsPerson 4 image 0 rights holder</t>
         </is>
       </c>
       <c r="H240" t="inlineStr">
@@ -14462,12 +14462,12 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image1</t>
+          <t>http://example.com/person4:CmsImage1</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Person 4 image 1</t>
+          <t>CmsPerson 4 image 1</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -14492,7 +14492,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Person 4 image 1 rights holder</t>
+          <t>CmsPerson 4 image 1 rights holder</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
@@ -14509,12 +14509,12 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0:Image0</t>
+          <t>http://example.com/collection0/work0:CmsImage0</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Collection0Work0 image 0</t>
+          <t>CmsCollection0CmsWork0 image 0</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -14539,7 +14539,7 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Collection0Work0 image 0 rights holder</t>
+          <t>CmsCollection0CmsWork0 image 0 rights holder</t>
         </is>
       </c>
       <c r="H242" t="inlineStr">
@@ -14556,12 +14556,12 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0:Image1</t>
+          <t>http://example.com/collection0/work0:CmsImage1</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Collection0Work0 image 1</t>
+          <t>CmsCollection0CmsWork0 image 1</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -14586,7 +14586,7 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Collection0Work0 image 1 rights holder</t>
+          <t>CmsCollection0CmsWork0 image 1 rights holder</t>
         </is>
       </c>
       <c r="H243" t="inlineStr">
@@ -14603,12 +14603,12 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image0</t>
+          <t>http://example.com/collection0/work1:CmsImage0</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Collection0Work1 image 0</t>
+          <t>CmsCollection0CmsWork1 image 0</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -14633,7 +14633,7 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Collection0Work1 image 0 rights holder</t>
+          <t>CmsCollection0CmsWork1 image 0 rights holder</t>
         </is>
       </c>
       <c r="H244" t="inlineStr">
@@ -14650,12 +14650,12 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image1</t>
+          <t>http://example.com/collection0/work1:CmsImage1</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Collection0Work1 image 1</t>
+          <t>CmsCollection0CmsWork1 image 1</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
@@ -14680,7 +14680,7 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Collection0Work1 image 1 rights holder</t>
+          <t>CmsCollection0CmsWork1 image 1 rights holder</t>
         </is>
       </c>
       <c r="H245" t="inlineStr">
@@ -14697,12 +14697,12 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2:Image0</t>
+          <t>http://example.com/collection0/work2:CmsImage0</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Collection0Work2 image 0</t>
+          <t>CmsCollection0CmsWork2 image 0</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
@@ -14727,7 +14727,7 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Collection0Work2 image 0 rights holder</t>
+          <t>CmsCollection0CmsWork2 image 0 rights holder</t>
         </is>
       </c>
       <c r="H246" t="inlineStr">
@@ -14744,12 +14744,12 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2:Image1</t>
+          <t>http://example.com/collection0/work2:CmsImage1</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Collection0Work2 image 1</t>
+          <t>CmsCollection0CmsWork2 image 1</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
@@ -14774,7 +14774,7 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Collection0Work2 image 1 rights holder</t>
+          <t>CmsCollection0CmsWork2 image 1 rights holder</t>
         </is>
       </c>
       <c r="H247" t="inlineStr">
@@ -14791,12 +14791,12 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image0</t>
+          <t>http://example.com/collection0/work3:CmsImage0</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Collection0Work3 image 0</t>
+          <t>CmsCollection0CmsWork3 image 0</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -14821,7 +14821,7 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Collection0Work3 image 0 rights holder</t>
+          <t>CmsCollection0CmsWork3 image 0 rights holder</t>
         </is>
       </c>
       <c r="H248" t="inlineStr">
@@ -14838,12 +14838,12 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image1</t>
+          <t>http://example.com/collection0/work3:CmsImage1</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Collection0Work3 image 1</t>
+          <t>CmsCollection0CmsWork3 image 1</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
@@ -14868,7 +14868,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Collection0Work3 image 1 rights holder</t>
+          <t>CmsCollection0CmsWork3 image 1 rights holder</t>
         </is>
       </c>
       <c r="H249" t="inlineStr">
@@ -14885,12 +14885,12 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image0</t>
+          <t>http://example.com/collection1:CmsImage0</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Collection1 image 0</t>
+          <t>CmsCollection1 image 0</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -14915,7 +14915,7 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Collection1 image 0 rights holder</t>
+          <t>CmsCollection1 image 0 rights holder</t>
         </is>
       </c>
       <c r="H250" t="inlineStr">
@@ -14932,12 +14932,12 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image1</t>
+          <t>http://example.com/collection1:CmsImage1</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Collection1 image 1</t>
+          <t>CmsCollection1 image 1</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
@@ -14962,7 +14962,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Collection1 image 1 rights holder</t>
+          <t>CmsCollection1 image 1 rights holder</t>
         </is>
       </c>
       <c r="H251" t="inlineStr">
@@ -14979,12 +14979,12 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4:Image0</t>
+          <t>http://example.com/collection1/work4:CmsImage0</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Collection1Work4 image 0</t>
+          <t>CmsCollection1CmsWork4 image 0</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -15009,7 +15009,7 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Collection1Work4 image 0 rights holder</t>
+          <t>CmsCollection1CmsWork4 image 0 rights holder</t>
         </is>
       </c>
       <c r="H252" t="inlineStr">
@@ -15026,12 +15026,12 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4:Image1</t>
+          <t>http://example.com/collection1/work4:CmsImage1</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Collection1Work4 image 1</t>
+          <t>CmsCollection1CmsWork4 image 1</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -15056,7 +15056,7 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Collection1Work4 image 1 rights holder</t>
+          <t>CmsCollection1CmsWork4 image 1 rights holder</t>
         </is>
       </c>
       <c r="H253" t="inlineStr">
@@ -15073,12 +15073,12 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:Image0</t>
+          <t>http://example.com/collection1/work5:CmsImage0</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Collection1Work5 image 0</t>
+          <t>CmsCollection1CmsWork5 image 0</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -15103,7 +15103,7 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Collection1Work5 image 0 rights holder</t>
+          <t>CmsCollection1CmsWork5 image 0 rights holder</t>
         </is>
       </c>
       <c r="H254" t="inlineStr">
@@ -15120,12 +15120,12 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:Image1</t>
+          <t>http://example.com/collection1/work5:CmsImage1</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Collection1Work5 image 1</t>
+          <t>CmsCollection1CmsWork5 image 1</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -15150,7 +15150,7 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Collection1Work5 image 1 rights holder</t>
+          <t>CmsCollection1CmsWork5 image 1 rights holder</t>
         </is>
       </c>
       <c r="H255" t="inlineStr">
@@ -15167,12 +15167,12 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6:Image0</t>
+          <t>http://example.com/collection1/work6:CmsImage0</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Collection1Work6 image 0</t>
+          <t>CmsCollection1CmsWork6 image 0</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -15197,7 +15197,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Collection1Work6 image 0 rights holder</t>
+          <t>CmsCollection1CmsWork6 image 0 rights holder</t>
         </is>
       </c>
       <c r="H256" t="inlineStr">
@@ -15214,12 +15214,12 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6:Image1</t>
+          <t>http://example.com/collection1/work6:CmsImage1</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Collection1Work6 image 1</t>
+          <t>CmsCollection1CmsWork6 image 1</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -15244,7 +15244,7 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Collection1Work6 image 1 rights holder</t>
+          <t>CmsCollection1CmsWork6 image 1 rights holder</t>
         </is>
       </c>
       <c r="H257" t="inlineStr">
@@ -15261,12 +15261,12 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image0</t>
+          <t>http://example.com/collection1/work7:CmsImage0</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Collection1Work7 image 0</t>
+          <t>CmsCollection1CmsWork7 image 0</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
@@ -15291,7 +15291,7 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Collection1Work7 image 0 rights holder</t>
+          <t>CmsCollection1CmsWork7 image 0 rights holder</t>
         </is>
       </c>
       <c r="H258" t="inlineStr">
@@ -15308,12 +15308,12 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image1</t>
+          <t>http://example.com/collection1/work7:CmsImage1</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Collection1Work7 image 1</t>
+          <t>CmsCollection1CmsWork7 image 1</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
@@ -15338,7 +15338,7 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Collection1Work7 image 1 rights holder</t>
+          <t>CmsCollection1CmsWork7 image 1 rights holder</t>
         </is>
       </c>
       <c r="H259" t="inlineStr">
@@ -15355,7 +15355,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8:Image0</t>
+          <t>http://example.com/freestandingwork8:CmsImage0</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
@@ -15402,7 +15402,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8:Image1</t>
+          <t>http://example.com/freestandingwork8:CmsImage1</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -15449,7 +15449,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:Image0</t>
+          <t>http://example.com/freestandingwork9:CmsImage0</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -15496,7 +15496,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:Image1</t>
+          <t>http://example.com/freestandingwork9:CmsImage1</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -15543,7 +15543,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10:Image0</t>
+          <t>http://example.com/freestandingwork10:CmsImage0</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -15590,7 +15590,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10:Image1</t>
+          <t>http://example.com/freestandingwork10:CmsImage1</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -15637,7 +15637,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:Image0</t>
+          <t>http://example.com/freestandingwork11:CmsImage0</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -15684,7 +15684,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:Image1</t>
+          <t>http://example.com/freestandingwork11:CmsImage1</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
@@ -15772,7 +15772,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Organization 0</t>
+          <t>CmsOrganization 0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -15785,7 +15785,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Organization 1</t>
+          <t>CmsOrganization 1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -15798,7 +15798,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Organization 2</t>
+          <t>CmsOrganization 2</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -15811,7 +15811,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Organization 3</t>
+          <t>CmsOrganization 3</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -15824,7 +15824,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Organization 4</t>
+          <t>CmsOrganization 4</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -15898,23 +15898,23 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>CmsPerson</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Person 0</t>
+          <t>CmsPerson 0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0, Person</t>
+          <t>0, CmsPerson</t>
         </is>
       </c>
     </row>
@@ -15931,12 +15931,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>CmsPerson</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Person 1</t>
+          <t>CmsPerson 1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -15947,7 +15947,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1, Person</t>
+          <t>1, CmsPerson</t>
         </is>
       </c>
     </row>
@@ -15964,23 +15964,23 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>CmsPerson</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Person 2</t>
+          <t>CmsPerson 2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2, Person</t>
+          <t>2, CmsPerson</t>
         </is>
       </c>
     </row>
@@ -15997,23 +15997,23 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>CmsPerson</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Person 3</t>
+          <t>CmsPerson 3</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>3, Person</t>
+          <t>3, CmsPerson</t>
         </is>
       </c>
     </row>
@@ -16030,12 +16030,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>CmsPerson</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Person 4</t>
+          <t>CmsPerson 4</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -16046,7 +16046,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>4, Person</t>
+          <t>4, CmsPerson</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix named model delegation
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -15,7 +15,7 @@
     <sheet name="CmsOrganization" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="CmsPerson" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="CmsCollection" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="CmsNamedLocation" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="CmsLocation" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="CmsWork" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="CmsWorkClosing" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="CmsWorkCreation" sheetId="12" state="visible" r:id="rId12"/>
@@ -730,7 +730,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -16008,7 +16008,7 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">

</xml_diff>

<commit_message>
allow anonymous events and include one (WorkClosing) in the synthetic data set
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -730,7 +730,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -15909,7 +15909,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">

</xml_diff>

<commit_message>
fix bug involving serializing two named models to the same named graph
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -730,7 +730,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -15909,7 +15909,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -15942,7 +15942,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -16041,7 +16041,7 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">

</xml_diff>

<commit_message>
allow blank node agents
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -15909,7 +15909,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -15975,7 +15975,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -16008,7 +16008,7 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">

</xml_diff>

<commit_message>
RdfFileLoader: use the model subject as the graph name instead of a hashed name
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -15942,7 +15942,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -16008,7 +16008,7 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">

</xml_diff>

<commit_message>
next pass at having Loader return Iterable[Model] so there's no need for CollectingLoader
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,482 @@
           <t>@graph</t>
         </is>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>_:N36c7bc4d92d44c88bacd037ff87ba05f</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>http://example.com/organization4</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>CmsCollection0CmsWork1 alternative title 0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>CmsCollection0CmsWork1Id0</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>CmsCollection0CmsWork1 provenance 0</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>CmsCollection0CmsWork1 rights holder</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work1Location</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>CmsCollection0CmsWork1</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>_:N510676b3d8b443a2afb2a9971c3537a6</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>http://example.com/person1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>CmsCollection0CmsWork3 alternative title 1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>CmsCollection0CmsWork3Id1</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>CmsCollection0CmsWork3 provenance 1</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>CmsCollection0CmsWork3 rights holder</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work3Location</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>CmsCollection0CmsWork3</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work5</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>_:N58606298470241209bb2700f9e3fe503</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>http://example.com/person2</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>CmsCollection1CmsWork5 alternative title 0</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>CmsCollection1CmsWork5Id1</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>CmsCollection1CmsWork5 provenance 1</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>http://www.wikidata.org/entity/Q937690</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>CmsCollection1CmsWork5 rights holder</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work5Location</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>CmsCollection1CmsWork5</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work7</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>_:N1e91d7d345d740af942a4ec3675c491f</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>http://example.com/organization0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>CmsCollection1CmsWork7 alternative title 0</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>CmsCollection1CmsWork7Id1</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>CmsCollection1CmsWork7 provenance 1</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>CmsCollection1CmsWork7 rights holder</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work7Location</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>CmsCollection1CmsWork7</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork9</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>_:N1081149d193f40c9bf030f02263d17fb</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>http://example.com/organization2</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>FreestandingWork9 alternative title 1</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>FreestandingWork9Id0</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>FreestandingWork9 provenance 1</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>http://www.wikidata.org/entity/Q937690</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>FreestandingWork9 rights holder</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork9Location</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>FreestandingWork9</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork11</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>_:Ncd0885c7667941da907dd764fb85f66d</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>http://example.com/organization3</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>FreestandingWork11 alternative title 1</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>FreestandingWork11Id1</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>FreestandingWork11 provenance 1</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>FreestandingWork11 rights holder</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork11Location</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>FreestandingWork11</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -471,7 +947,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +959,144 @@
       <c r="A1" t="inlineStr">
         <is>
           <t>@graph</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>_:N354ca23e310247c5944d7fe1282f23a3</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>_:N50223acaeda2456ab66346fcaf396f53</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CmsCollection0CmsWork1 closing</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>_:N61f2e6ea207e469b89e6376baa941367</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>_:N1aec5af3f5b648cc86a7ad4fff4be4b9</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CmsCollection0CmsWork3 closing</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work3</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>_:N88c8da7c75b349b48ec25b099b752e0a</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>_:N121d882f44834070a912a6d4250668c8</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CmsCollection1CmsWork5 closing</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work5</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>_:Nb2543f5b52f54e539fe1b24c5734d6a6</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>_:N88a70d0ae292437296e8b567ae84a8f1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>CmsCollection1CmsWork7 closing</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work7</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>_:Ne663e7fcdc734012a5f31e7b997b00c7</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>_:Nc89113797dd1469e98d721b3df6945ec</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>FreestandingWork9 closing</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork9</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>_:Nfd5aea41fe8b435a9168fc60922cd255</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>_:Ned5bfbeb5fa94974b669000ddf126474</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>FreestandingWork11 closing</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork11</t>
         </is>
       </c>
     </row>
@@ -523,7 +1137,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,6 +1149,144 @@
       <c r="A1" t="inlineStr">
         <is>
           <t>@graph</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work1Opening</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>_:N50223acaeda2456ab66346fcaf396f53</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CmsCollection0CmsWork1 opening</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work3Opening</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>_:N1aec5af3f5b648cc86a7ad4fff4be4b9</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CmsCollection0CmsWork3 opening</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work3</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work5Opening</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>_:N121d882f44834070a912a6d4250668c8</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CmsCollection1CmsWork5 opening</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work5</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work7Opening</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>_:N88a70d0ae292437296e8b567ae84a8f1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>CmsCollection1CmsWork7 opening</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work7</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork9Opening</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>_:Nc89113797dd1469e98d721b3df6945ec</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>FreestandingWork9 opening</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork9</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork11Opening</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>_:Ned5bfbeb5fa94974b669000ddf126474</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>FreestandingWork11 opening</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork11</t>
         </is>
       </c>
     </row>
@@ -15939,13 +16691,12 @@
           <t>CmsPerson 1</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
-        <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
         <is>
           <t>1, CmsPerson</t>
         </is>
@@ -16005,13 +16756,12 @@
           <t>CmsPerson 3</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>http://www.wikidata.org/entity/Q7251</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
-        <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
         <is>
           <t>3, CmsPerson</t>
         </is>
@@ -16041,7 +16791,7 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>http://www.wikidata.org/entity/Q7251</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -16061,7 +16811,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16073,6 +16823,18 @@
       <c r="A1" t="inlineStr">
         <is>
           <t>@graph</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CmsCollection1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add more-itertools and consume() the loaded pipelines everywhere
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N36c7bc4d92d44c88bacd037ff87ba05f</t>
+          <t>_:N1b67ed7ad3d74a6985b6de1610cb99d7</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -483,13 +483,13 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1 alternative title 0</t>
+          <t>CmsCollection0CmsWork1 alternative title 1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1Id0</t>
+          <t>CmsCollection0CmsWork1Id1</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -509,7 +509,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+          <t>http://www.wikidata.org/entity/Q937690</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -534,7 +534,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
         </is>
       </c>
       <c r="U2" t="inlineStr"/>
@@ -554,7 +554,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N510676b3d8b443a2afb2a9971c3537a6</t>
+          <t>_:N9682d3b7fd254a77a2ee9b7e55c9c9e5</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -564,7 +564,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork3 alternative title 1</t>
+          <t>CmsCollection0CmsWork3 alternative title 0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -590,7 +590,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+          <t>http://www.wikidata.org/entity/Q937690</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -615,7 +615,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104</t>
         </is>
       </c>
       <c r="U3" t="inlineStr"/>
@@ -635,7 +635,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N58606298470241209bb2700f9e3fe503</t>
+          <t>_:N1ecc13cc932542b38b02e061e5e98f5a</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 alternative title 0</t>
+          <t>CmsCollection1CmsWork5 alternative title 1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -696,7 +696,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106</t>
         </is>
       </c>
       <c r="U4" t="inlineStr"/>
@@ -716,12 +716,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N1e91d7d345d740af942a4ec3675c491f</t>
+          <t>_:Nfaaa2930c33d46a18eb51d89e16822e3</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>http://example.com/organization0</t>
+          <t>http://example.com/person4</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -739,7 +739,7 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 provenance 1</t>
+          <t>CmsCollection1CmsWork7 provenance 0</t>
         </is>
       </c>
       <c r="K5" t="inlineStr"/>
@@ -752,7 +752,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+          <t>http://www.wikidata.org/entity/Q937690</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -792,30 +792,30 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>_:N1081149d193f40c9bf030f02263d17fb</t>
+          <t>_:N3b8beb311c79491aa36df60bf2393e70</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>http://example.com/organization2</t>
+          <t>http://example.com/organization1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 alternative title 1</t>
+          <t>FreestandingWork9 alternative title 0</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>FreestandingWork9Id0</t>
+          <t>FreestandingWork9Id1</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 provenance 1</t>
+          <t>FreestandingWork9 provenance 0</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -868,7 +868,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>_:Ncd0885c7667941da907dd764fb85f66d</t>
+          <t>_:Nbdf8f714e5f14a4bb9ed15b441088b5b</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -884,14 +884,14 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>FreestandingWork11Id1</t>
+          <t>FreestandingWork11Id0</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>FreestandingWork11 provenance 1</t>
+          <t>FreestandingWork11 provenance 0</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
@@ -904,7 +904,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+          <t>http://www.wikidata.org/entity/Q937690</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -965,13 +965,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>_:N354ca23e310247c5944d7fe1282f23a3</t>
+          <t>_:N78f9fb8b601b4dd8b244387a47fd655e</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N50223acaeda2456ab66346fcaf396f53</t>
+          <t>_:N3f2c1769594a4d76bd141a9d07512e81</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -988,13 +988,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>_:N61f2e6ea207e469b89e6376baa941367</t>
+          <t>_:N9de5b4a7a8774c339267d1314709a5e7</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N1aec5af3f5b648cc86a7ad4fff4be4b9</t>
+          <t>_:Naebc8b6f28cc4f8aa989f31190202631</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1011,13 +1011,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>_:N88c8da7c75b349b48ec25b099b752e0a</t>
+          <t>_:N8ac5352da322401f9aefdb9752cb99e3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N121d882f44834070a912a6d4250668c8</t>
+          <t>_:N102adedbd7334ec1a0a5191426911adf</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1034,13 +1034,13 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>_:Nb2543f5b52f54e539fe1b24c5734d6a6</t>
+          <t>_:Nac31e4d88060489ebb7309897f69c567</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N88a70d0ae292437296e8b567ae84a8f1</t>
+          <t>_:N151e370315f94c979009a2f553ee75de</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1057,13 +1057,13 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>_:Ne663e7fcdc734012a5f31e7b997b00c7</t>
+          <t>_:Na7912610025a4598b65b43b70441490c</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:Nc89113797dd1469e98d721b3df6945ec</t>
+          <t>_:Nb1e1d5606b664221a07f7ca5717c1638</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1080,13 +1080,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>_:Nfd5aea41fe8b435a9168fc60922cd255</t>
+          <t>_:Nacc0614712b0414794b225b9feb472cc</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:Ned5bfbeb5fa94974b669000ddf126474</t>
+          <t>_:N755686b71e2949a2b6b1dc97cef8208a</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1161,7 +1161,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N50223acaeda2456ab66346fcaf396f53</t>
+          <t>_:N3f2c1769594a4d76bd141a9d07512e81</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1184,7 +1184,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N1aec5af3f5b648cc86a7ad4fff4be4b9</t>
+          <t>_:Naebc8b6f28cc4f8aa989f31190202631</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1207,7 +1207,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N121d882f44834070a912a6d4250668c8</t>
+          <t>_:N102adedbd7334ec1a0a5191426911adf</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1230,7 +1230,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N88a70d0ae292437296e8b567ae84a8f1</t>
+          <t>_:N151e370315f94c979009a2f553ee75de</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1253,7 +1253,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:Nc89113797dd1469e98d721b3df6945ec</t>
+          <t>_:Nb1e1d5606b664221a07f7ca5717c1638</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1276,7 +1276,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:Ned5bfbeb5fa94974b669000ddf126474</t>
+          <t>_:N755686b71e2949a2b6b1dc97cef8208a</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1482,7 +1482,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -16661,7 +16661,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -16758,7 +16758,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">

</xml_diff>

<commit_message>
regenerate synthetic data with owl:sameAs
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,12 +473,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:Nb34f2db31dc94dbe8928d336382bd884</t>
+          <t>_:N5291ff32bdef4c16bff266afc9f31987</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/organization4</t>
+          <t>http://example.com/organization3</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -509,37 +509,42 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
+          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>CmsCollection0CmsWork1 rights holder</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
           <t>wd:Q937690</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>CmsCollection0CmsWork1 rights holder</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>http://example.com/collection0/work1Location</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>CmsCollection0CmsWork1</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -554,12 +559,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N51f23b2402494ae7b4d8fd512e6ac741</t>
+          <t>_:N8e0a3c6d200d4591bb764282907d2f85</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person0</t>
+          <t>http://example.com/person1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -570,7 +575,7 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork3Id0</t>
+          <t>CmsCollection0CmsWork3Id1</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -590,37 +595,42 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
+          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>CmsCollection0CmsWork3 rights holder</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
           <t>wd:Q937690</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>CmsCollection0CmsWork3 rights holder</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>http://example.com/collection0/work3Location</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>CmsCollection0CmsWork3</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -635,7 +645,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N63b45561f8a444eeb14d295bd0497b4a</t>
+          <t>_:N1e1541d7dc074e9cae7f42ae5d065327</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -686,22 +696,27 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
+          <t>wd:Q937690</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
           <t>http://example.com/collection1/work5Location</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>CmsCollection1CmsWork5</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr"/>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105</t>
+        </is>
+      </c>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -716,12 +731,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N8e749165974246f9ab44d98b6620732f</t>
+          <t>_:Nfb42d45daa2e4b6085bc4c60dc2c6870</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>http://example.com/organization0</t>
+          <t>http://example.com/person4</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -739,7 +754,7 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 provenance 1</t>
+          <t>CmsCollection1CmsWork7 provenance 0</t>
         </is>
       </c>
       <c r="K5" t="inlineStr"/>
@@ -752,37 +767,42 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
+          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>CmsCollection1CmsWork7 rights holder</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
           <t>wd:Q937690</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>CmsCollection1CmsWork7 rights holder</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>http://example.com/collection1/work7Location</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>CmsCollection1CmsWork7</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -792,7 +812,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>_:N93bf7f40ab864c368de72ddaffa00e6a</t>
+          <t>_:N8b5edc0eb13a473e9fd823fd358bfcaa</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -808,14 +828,14 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>FreestandingWork9Id0</t>
+          <t>FreestandingWork9Id1</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 provenance 1</t>
+          <t>FreestandingWork9 provenance 0</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -828,37 +848,42 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
+          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>FreestandingWork9 rights holder</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
           <t>wd:Q937690</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>FreestandingWork9 rights holder</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
+      <c r="R6" t="inlineStr">
         <is>
           <t>http://example.com/freestandingwork9Location</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr">
+      <c r="S6" t="inlineStr">
         <is>
           <t>FreestandingWork9</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr"/>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100</t>
+        </is>
+      </c>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -868,12 +893,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>_:Nc8d7f4f651844ec6ad57e18f113c54aa</t>
+          <t>_:N10d4fbfe3ca6447b9884458c2fd3ab3d</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>http://example.com/organization4</t>
+          <t>http://example.com/organization3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -919,22 +944,27 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
+          <t>wd:Q937690</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
           <t>http://example.com/freestandingwork11Location</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr">
+      <c r="S7" t="inlineStr">
         <is>
           <t>FreestandingWork11</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr"/>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
+        </is>
+      </c>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -965,13 +995,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>_:N4bda910410e3424091b5213541674b4f</t>
+          <t>_:Nc1fee9b79e3b4b8c8e67cbfa21556a45</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:Nddcb2a0e20f0419db5c787193f716f15</t>
+          <t>_:N666d44be377445239b4c5b0223e603a0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -988,13 +1018,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>_:N712c4fed1a664137a4de71f27ab5fbb1</t>
+          <t>_:Ne85a14f001c340c5a566928f06fcd38a</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Ne79352a07ac747378f2ad003a89aeebd</t>
+          <t>_:Ndc336b4aa3c44a319624566d26a0105c</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1011,13 +1041,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>_:N34cf0c202d92404fa6ae28fc3523eca4</t>
+          <t>_:N88d47c9b3f324beda90884f8b3b30776</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:Ne2ed338ece0746b299aa002a60a93b29</t>
+          <t>_:Nd3407ea41e374e64afcd0efac8ad4a2f</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1034,13 +1064,13 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>_:N34499101c1eb49d9983028ba8db0a96d</t>
+          <t>_:N4b4d291bdf5e49caa74664b1384e1550</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:Naccfccea0dc84e56bbc0c38178ce9221</t>
+          <t>_:N74aad167e2bf447db83867725976c60b</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1057,13 +1087,13 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>_:Nd0c780c62c284cc1a6c6d246192289e1</t>
+          <t>_:Nae59d01485b54ae8b4ad2fbe5a87a466</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:N56feb0d1baac490ca2164e441f697a04</t>
+          <t>_:N03e2561d366649419b01c4a5864bc33f</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1080,13 +1110,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>_:Nc57f3dc0b8d441ef94f914bccdcdcc3c</t>
+          <t>_:Na6174989b0584455bf9566240387b94d</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:Na9a68ea311bf49188991c470f38eddf0</t>
+          <t>_:N7fc12851b24940138cef0a4ab13fd2de</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1161,7 +1191,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:Nddcb2a0e20f0419db5c787193f716f15</t>
+          <t>_:N666d44be377445239b4c5b0223e603a0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1184,7 +1214,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Ne79352a07ac747378f2ad003a89aeebd</t>
+          <t>_:Ndc336b4aa3c44a319624566d26a0105c</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1207,7 +1237,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:Ne2ed338ece0746b299aa002a60a93b29</t>
+          <t>_:Nd3407ea41e374e64afcd0efac8ad4a2f</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1230,7 +1260,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:Naccfccea0dc84e56bbc0c38178ce9221</t>
+          <t>_:N74aad167e2bf447db83867725976c60b</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1253,7 +1283,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:N56feb0d1baac490ca2164e441f697a04</t>
+          <t>_:N03e2561d366649419b01c4a5864bc33f</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1276,7 +1306,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:Na9a68ea311bf49188991c470f38eddf0</t>
+          <t>_:N7fc12851b24940138cef0a4ab13fd2de</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1482,7 +1512,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -17908,7 +17938,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17949,6 +17979,11 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>sortName</t>
         </is>
       </c>
@@ -17982,6 +18017,11 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>wd:Q7251</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>0, CmsPerson</t>
         </is>
       </c>
@@ -18014,6 +18054,11 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>wd:Q7251</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>1, CmsPerson</t>
         </is>
       </c>
@@ -18042,10 +18087,15 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
+          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>wd:Q7251</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>2, CmsPerson</t>
         </is>
@@ -18079,6 +18129,11 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>wd:Q7251</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>3, CmsPerson</t>
         </is>
       </c>
@@ -18111,6 +18166,11 @@
         </is>
       </c>
       <c r="G6" t="inlineStr">
+        <is>
+          <t>wd:Q7251</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>4, CmsPerson</t>
         </is>

</xml_diff>

<commit_message>
ReferenceValidator: use full class name in method name to accommodate non-CMS types
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -666,7 +666,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N70517a85cdef419fbf26d8e92b525085</t>
+          <t>_:Ne8227b46c9974d46a3bcc9f6ae3abd14</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -682,7 +682,7 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1Id0</t>
+          <t>CmsCollection0CmsWork1Id1</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -752,12 +752,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Nc5152b0f430343fbbfa31f96e506a334</t>
+          <t>_:N6c85af05453c4df69069f1f97884180a</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person1</t>
+          <t>http://example.com/person0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -818,7 +818,7 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104</t>
         </is>
       </c>
       <c r="V3" t="inlineStr"/>
@@ -838,7 +838,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:Nf19a6a2606164586b2def5968678f513</t>
+          <t>_:Nbca42478582846a885adda29847afff4</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -861,7 +861,7 @@
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 provenance 1</t>
+          <t>CmsCollection1CmsWork5 provenance 0</t>
         </is>
       </c>
       <c r="K4" t="inlineStr"/>
@@ -924,23 +924,23 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N6d12c39bac724503b1c6aa58ed61a183</t>
+          <t>_:N7a84f1163ffe4709a681ce5e742ec193</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>http://example.com/organization0</t>
+          <t>http://example.com/person4</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 alternative title 0</t>
+          <t>CmsCollection1CmsWork7 alternative title 1</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7Id0</t>
+          <t>CmsCollection1CmsWork7Id1</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>_:N19da515736d54f9c8a9484a036e78fc6</t>
+          <t>_:N5c78c639b9714b638b8b2b662c6e0563</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1015,13 +1015,13 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 alternative title 1</t>
+          <t>FreestandingWork9 alternative title 0</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>FreestandingWork9Id1</t>
+          <t>FreestandingWork9Id0</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -1086,12 +1086,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>_:Nda9d8242e2b24e1d8d64a8db18f12c4a</t>
+          <t>_:Nd29b075073c040fb800a676c6295b76a</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>http://example.com/organization4</t>
+          <t>http://example.com/organization3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1152,7 +1152,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
         </is>
       </c>
       <c r="U7" t="inlineStr"/>
@@ -1188,13 +1188,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>_:Nadaa13421b834001a888378f133689e7</t>
+          <t>_:Ndd1dc3ce897545999378fdb08c840e4a</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N486198a9e9404afd808fa77e0f8f2047</t>
+          <t>_:N0dd9e86983b445b4a68134ec49e4c210</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1211,13 +1211,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>_:N968b5fe9a13d4ff8870893b62ca25e26</t>
+          <t>_:N0f84c8205f394a61819703b8620485c3</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N46c2f62fb763438db810e7b7a4dad719</t>
+          <t>_:Nd2382d3861df4467a336dcc71d49d902</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1234,13 +1234,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>_:N19f6bbd3de8f41afbbf73548afdee9ca</t>
+          <t>_:Neaf5fae07dae4f91a468e2cfa081a066</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N754fe39a87e04ad6b1568e0e8969fb5b</t>
+          <t>_:Nf2689075158740228e20d07fc423c200</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1257,13 +1257,13 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>_:N5fe7c0757fd24579b0861231f846d8a2</t>
+          <t>_:N24af2fc7193a419fa584727384fde638</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N01e4fe6cb228471087fb5d778e59f416</t>
+          <t>_:Nf3dcefad2d19487a8f3b687f4059735b</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1280,13 +1280,13 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>_:N6aab37f2de744e56983360a44c6e5391</t>
+          <t>_:N49c6d7509f6a43beb36ac7ca6904a2f9</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:N5a4a2948c1824ca991c3b63b6bab3989</t>
+          <t>_:Nb9eb50f11645437e99fc0a3081786a39</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1303,13 +1303,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>_:N12bd454f188544428ec6c284a64d4c8c</t>
+          <t>_:Ndd7a0563da6841de827d3ae55d053a32</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:N848cd6834732481f95b52151b3d150f5</t>
+          <t>_:Nab77dd39560c403491720856b0469177</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1384,7 +1384,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N486198a9e9404afd808fa77e0f8f2047</t>
+          <t>_:N0dd9e86983b445b4a68134ec49e4c210</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1407,7 +1407,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N46c2f62fb763438db810e7b7a4dad719</t>
+          <t>_:Nd2382d3861df4467a336dcc71d49d902</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1430,7 +1430,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N754fe39a87e04ad6b1568e0e8969fb5b</t>
+          <t>_:Nf2689075158740228e20d07fc423c200</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1453,7 +1453,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N01e4fe6cb228471087fb5d778e59f416</t>
+          <t>_:Nf3dcefad2d19487a8f3b687f4059735b</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1476,7 +1476,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:N5a4a2948c1824ca991c3b63b6bab3989</t>
+          <t>_:Nb9eb50f11645437e99fc0a3081786a39</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1499,7 +1499,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:N848cd6834732481f95b52151b3d150f5</t>
+          <t>_:Nab77dd39560c403491720856b0469177</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">

</xml_diff>

<commit_message>
read synthetic data from a file instead of embedding
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -13,7 +13,7 @@
     <sheet name="CmsProperty" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="CmsConcept" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="CmsOrganization" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="WikidataItem" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="WikibaseItem" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="CmsPerson" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="CmsCollection" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="CmsLocation" sheetId="10" state="visible" r:id="rId10"/>
@@ -666,7 +666,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:Ne8227b46c9974d46a3bcc9f6ae3abd14</t>
+          <t>_:N5810638ef50247fabd0b9f1c77bd3431</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -752,12 +752,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N6c85af05453c4df69069f1f97884180a</t>
+          <t>_:N102db01445524a069fd1633f9f32ece0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person0</t>
+          <t>http://example.com/person1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -775,7 +775,7 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork3 provenance 0</t>
+          <t>CmsCollection0CmsWork3 provenance 1</t>
         </is>
       </c>
       <c r="K3" t="inlineStr"/>
@@ -838,7 +838,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:Nbca42478582846a885adda29847afff4</t>
+          <t>_:Nb6a631ce63094b25bf07f55b03019102</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -848,20 +848,20 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 alternative title 1</t>
+          <t>CmsCollection1CmsWork5 alternative title 0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5Id1</t>
+          <t>CmsCollection1CmsWork5Id0</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 provenance 0</t>
+          <t>CmsCollection1CmsWork5 provenance 1</t>
         </is>
       </c>
       <c r="K4" t="inlineStr"/>
@@ -904,7 +904,7 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106</t>
         </is>
       </c>
       <c r="V4" t="inlineStr"/>
@@ -924,7 +924,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N7a84f1163ffe4709a681ce5e742ec193</t>
+          <t>_:N8493a2705b5c46fd84ed651092b5fcc5</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 alternative title 1</t>
+          <t>CmsCollection1CmsWork7 alternative title 0</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -947,7 +947,7 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 provenance 0</t>
+          <t>CmsCollection1CmsWork7 provenance 1</t>
         </is>
       </c>
       <c r="K5" t="inlineStr"/>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>_:N5c78c639b9714b638b8b2b662c6e0563</t>
+          <t>_:Nb826e435842f410481ae209a59d338aa</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1015,7 +1015,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 alternative title 0</t>
+          <t>FreestandingWork9 alternative title 1</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1028,7 +1028,7 @@
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 provenance 1</t>
+          <t>FreestandingWork9 provenance 0</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100</t>
         </is>
       </c>
       <c r="U6" t="inlineStr"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>_:Nd29b075073c040fb800a676c6295b76a</t>
+          <t>_:N2157f8c5f78644768bbc0715a726912f</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1152,7 +1152,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
         </is>
       </c>
       <c r="U7" t="inlineStr"/>
@@ -1188,13 +1188,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>_:Ndd1dc3ce897545999378fdb08c840e4a</t>
+          <t>_:N09c97928df2d47f1a1715d1bfa770682</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N0dd9e86983b445b4a68134ec49e4c210</t>
+          <t>_:N60a129640cf644d0b654dfe33d7c99b6</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1211,13 +1211,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>_:N0f84c8205f394a61819703b8620485c3</t>
+          <t>_:Ndd8bc9ae8e0044e9bd290a9c1eef8b1b</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Nd2382d3861df4467a336dcc71d49d902</t>
+          <t>_:N94b7ddd8989547a895f85e006ead6c97</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1234,13 +1234,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>_:Neaf5fae07dae4f91a468e2cfa081a066</t>
+          <t>_:Nbfbbb2940bc34a25abd790e6d59afbd5</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:Nf2689075158740228e20d07fc423c200</t>
+          <t>_:N727b090a7ab24c8782fdce7801594d54</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1257,13 +1257,13 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>_:N24af2fc7193a419fa584727384fde638</t>
+          <t>_:N06ac9b27f5854875904dbff1d02a4e07</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:Nf3dcefad2d19487a8f3b687f4059735b</t>
+          <t>_:Nf1202cd120dd47c4b58f2e73425a582c</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1280,13 +1280,13 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>_:N49c6d7509f6a43beb36ac7ca6904a2f9</t>
+          <t>_:N9fe20b2265f14b4e8a7734b78ac273a8</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:Nb9eb50f11645437e99fc0a3081786a39</t>
+          <t>_:Na7bb78d3844b4b56898dc7381f1ed059</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1303,13 +1303,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>_:Ndd7a0563da6841de827d3ae55d053a32</t>
+          <t>_:N1b84ea80c36a4dff901fcb80e7bddae3</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:Nab77dd39560c403491720856b0469177</t>
+          <t>_:Nf562d1eb5d26445fb432efbcd4acbcc9</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1384,7 +1384,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N0dd9e86983b445b4a68134ec49e4c210</t>
+          <t>_:N60a129640cf644d0b654dfe33d7c99b6</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1407,7 +1407,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Nd2382d3861df4467a336dcc71d49d902</t>
+          <t>_:N94b7ddd8989547a895f85e006ead6c97</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1430,7 +1430,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:Nf2689075158740228e20d07fc423c200</t>
+          <t>_:N727b090a7ab24c8782fdce7801594d54</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1453,7 +1453,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:Nf3dcefad2d19487a8f3b687f4059735b</t>
+          <t>_:Nf1202cd120dd47c4b58f2e73425a582c</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1476,7 +1476,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:Nb9eb50f11645437e99fc0a3081786a39</t>
+          <t>_:Na7bb78d3844b4b56898dc7381f1ed059</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1499,7 +1499,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:Nab77dd39560c403491720856b0469177</t>
+          <t>_:Nf562d1eb5d26445fb432efbcd4acbcc9</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">

</xml_diff>

<commit_message>
WikidataEnricher: resolve related items to get a full type hierarchy
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -666,30 +666,30 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N5810638ef50247fabd0b9f1c77bd3431</t>
+          <t>_:Nc567c036f99a41cc9e0148c633049a60</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/organization3</t>
+          <t>http://example.com/organization4</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1 alternative title 1</t>
+          <t>CmsCollection0CmsWork1 alternative title 0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1Id1</t>
+          <t>CmsCollection0CmsWork1Id0</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1 provenance 0</t>
+          <t>CmsCollection0CmsWork1 provenance 1</t>
         </is>
       </c>
       <c r="K2" t="inlineStr"/>
@@ -732,7 +732,7 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
         </is>
       </c>
       <c r="V2" t="inlineStr"/>
@@ -752,12 +752,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N102db01445524a069fd1633f9f32ece0</t>
+          <t>_:Nedcadcc2e793425588240c8a1bcceb55</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person1</t>
+          <t>http://example.com/person0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -768,7 +768,7 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork3Id0</t>
+          <t>CmsCollection0CmsWork3Id1</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -838,7 +838,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:Nb6a631ce63094b25bf07f55b03019102</t>
+          <t>_:N73d1f755c85c4a928483f10e2b054ca6</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 alternative title 0</t>
+          <t>CmsCollection1CmsWork5 alternative title 1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -904,7 +904,7 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105</t>
         </is>
       </c>
       <c r="V4" t="inlineStr"/>
@@ -924,7 +924,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N8493a2705b5c46fd84ed651092b5fcc5</t>
+          <t>_:N032db3ea94f74aa2b4ee57d73173304b</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -940,14 +940,14 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7Id1</t>
+          <t>CmsCollection1CmsWork7Id0</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 provenance 1</t>
+          <t>CmsCollection1CmsWork7 provenance 0</t>
         </is>
       </c>
       <c r="K5" t="inlineStr"/>
@@ -1005,30 +1005,30 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>_:Nb826e435842f410481ae209a59d338aa</t>
+          <t>_:Nfbe4e899e61c4e579f3f7e9a7b1ebb83</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>http://example.com/organization1</t>
+          <t>http://example.com/organization2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 alternative title 1</t>
+          <t>FreestandingWork9 alternative title 0</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>FreestandingWork9Id0</t>
+          <t>FreestandingWork9Id1</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 provenance 0</t>
+          <t>FreestandingWork9 provenance 1</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109</t>
         </is>
       </c>
       <c r="U6" t="inlineStr"/>
@@ -1086,12 +1086,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>_:N2157f8c5f78644768bbc0715a726912f</t>
+          <t>_:N0a8e5eb4dc364da599fbcb23894ec198</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>http://example.com/organization3</t>
+          <t>http://example.com/organization4</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1102,7 +1102,7 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>FreestandingWork11Id0</t>
+          <t>FreestandingWork11Id1</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -1188,13 +1188,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>_:N09c97928df2d47f1a1715d1bfa770682</t>
+          <t>_:N4254e29086664f0dae1d3e48ec24d1b6</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N60a129640cf644d0b654dfe33d7c99b6</t>
+          <t>_:Nddd06bc9340e4778a457a042dec15d34</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1211,13 +1211,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>_:Ndd8bc9ae8e0044e9bd290a9c1eef8b1b</t>
+          <t>_:N33287ab2def7420a87360d4312c5bdf8</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N94b7ddd8989547a895f85e006ead6c97</t>
+          <t>_:Nc64014a4cde949deaa53d01f419cdf55</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1234,13 +1234,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>_:Nbfbbb2940bc34a25abd790e6d59afbd5</t>
+          <t>_:Na04e302138b04f3dade7d80b90f615ce</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N727b090a7ab24c8782fdce7801594d54</t>
+          <t>_:N25d5449e22ac488da37cc39f04594b76</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1257,13 +1257,13 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>_:N06ac9b27f5854875904dbff1d02a4e07</t>
+          <t>_:Ncf2e862331b14c5d8b93e913f91c616e</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:Nf1202cd120dd47c4b58f2e73425a582c</t>
+          <t>_:N74d0b54ca09441879e888edc45406982</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1280,13 +1280,13 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>_:N9fe20b2265f14b4e8a7734b78ac273a8</t>
+          <t>_:N9afd0e9d078d404d88d58fceae853d47</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:Na7bb78d3844b4b56898dc7381f1ed059</t>
+          <t>_:N12440732f0654826957808bebd87879b</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1303,13 +1303,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>_:N1b84ea80c36a4dff901fcb80e7bddae3</t>
+          <t>_:N1cce929b109646fb8d8e95680e8b6f1d</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:Nf562d1eb5d26445fb432efbcd4acbcc9</t>
+          <t>_:N4ff4b16f678e4bb19d75d236016c2782</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1384,7 +1384,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N60a129640cf644d0b654dfe33d7c99b6</t>
+          <t>_:Nddd06bc9340e4778a457a042dec15d34</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1407,7 +1407,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N94b7ddd8989547a895f85e006ead6c97</t>
+          <t>_:Nc64014a4cde949deaa53d01f419cdf55</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1430,7 +1430,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N727b090a7ab24c8782fdce7801594d54</t>
+          <t>_:N25d5449e22ac488da37cc39f04594b76</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1453,7 +1453,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:Nf1202cd120dd47c4b58f2e73425a582c</t>
+          <t>_:N74d0b54ca09441879e888edc45406982</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1476,7 +1476,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:Na7bb78d3844b4b56898dc7381f1ed059</t>
+          <t>_:N12440732f0654826957808bebd87879b</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1499,7 +1499,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:Nf562d1eb5d26445fb432efbcd4acbcc9</t>
+          <t>_:N4ff4b16f678e4bb19d75d236016c2782</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">

</xml_diff>

<commit_message>
etl: WikidataItem: cut down loaded RDF
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -666,12 +666,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:Nc567c036f99a41cc9e0148c633049a60</t>
+          <t>_:N3e06727f8e624edfae132632f64eca90</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/organization4</t>
+          <t>http://example.com/organization3</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -752,7 +752,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Nedcadcc2e793425588240c8a1bcceb55</t>
+          <t>_:Neb9ed50049964b01aa889cafbaebca74</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -818,7 +818,7 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103</t>
         </is>
       </c>
       <c r="V3" t="inlineStr"/>
@@ -838,17 +838,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N73d1f755c85c4a928483f10e2b054ca6</t>
+          <t>_:N94d92baeef54447b973a44af77cd60ee</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person3</t>
+          <t>http://example.com/person2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 alternative title 1</t>
+          <t>CmsCollection1CmsWork5 alternative title 0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -924,17 +924,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N032db3ea94f74aa2b4ee57d73173304b</t>
+          <t>_:N789d7df36c734532a8c7b501098c00d4</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>http://example.com/person4</t>
+          <t>http://example.com/organization0</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 alternative title 0</t>
+          <t>CmsCollection1CmsWork7 alternative title 1</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -947,7 +947,7 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 provenance 0</t>
+          <t>CmsCollection1CmsWork7 provenance 1</t>
         </is>
       </c>
       <c r="K5" t="inlineStr"/>
@@ -1005,17 +1005,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>_:Nfbe4e899e61c4e579f3f7e9a7b1ebb83</t>
+          <t>_:N7a67edd2c6a14d6e8a4c1e4d977cd670</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>http://example.com/organization2</t>
+          <t>http://example.com/organization1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 alternative title 0</t>
+          <t>FreestandingWork9 alternative title 1</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1028,7 +1028,7 @@
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 provenance 1</t>
+          <t>FreestandingWork9 provenance 0</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100</t>
         </is>
       </c>
       <c r="U6" t="inlineStr"/>
@@ -1086,17 +1086,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>_:N0a8e5eb4dc364da599fbcb23894ec198</t>
+          <t>_:Na19116e1d54c4b6d91eaa893ebbd0162</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>http://example.com/organization4</t>
+          <t>http://example.com/organization3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>FreestandingWork11 alternative title 0</t>
+          <t>FreestandingWork11 alternative title 1</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -1109,7 +1109,7 @@
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>FreestandingWork11 provenance 0</t>
+          <t>FreestandingWork11 provenance 1</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
@@ -1188,13 +1188,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>_:N4254e29086664f0dae1d3e48ec24d1b6</t>
+          <t>_:N00f42f6db6b242d3aefb0ee047ddc7ae</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:Nddd06bc9340e4778a457a042dec15d34</t>
+          <t>_:N171f1109b61b43fa81f161f6fe15db00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1211,13 +1211,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>_:N33287ab2def7420a87360d4312c5bdf8</t>
+          <t>_:Ncaf0a51df02146f891c2aec439b1ea9b</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Nc64014a4cde949deaa53d01f419cdf55</t>
+          <t>_:N81647bd550c94976bad78b3afbcbb366</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1234,13 +1234,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>_:Na04e302138b04f3dade7d80b90f615ce</t>
+          <t>_:Nfbec17ceba9d4e27b1f5200a39ca4730</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N25d5449e22ac488da37cc39f04594b76</t>
+          <t>_:Na67ce142815f4520be2c18b0ca17b92f</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1257,13 +1257,13 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>_:Ncf2e862331b14c5d8b93e913f91c616e</t>
+          <t>_:Ncf152b4be0df4e70953e5705c667c5aa</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N74d0b54ca09441879e888edc45406982</t>
+          <t>_:N20ba0e867e5f4e2a9168aba47abaa781</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1280,13 +1280,13 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>_:N9afd0e9d078d404d88d58fceae853d47</t>
+          <t>_:Ncf27c1254e804042b374217a72661e62</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:N12440732f0654826957808bebd87879b</t>
+          <t>_:N44b6abbf540e4120afc737eba9d61cae</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1303,13 +1303,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>_:N1cce929b109646fb8d8e95680e8b6f1d</t>
+          <t>_:N7702e8ab0bd04acf83c63c001821b0fb</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:N4ff4b16f678e4bb19d75d236016c2782</t>
+          <t>_:N57daa86fd1b34106825f3af81e3d3c65</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1384,7 +1384,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:Nddd06bc9340e4778a457a042dec15d34</t>
+          <t>_:N171f1109b61b43fa81f161f6fe15db00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1407,7 +1407,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Nc64014a4cde949deaa53d01f419cdf55</t>
+          <t>_:N81647bd550c94976bad78b3afbcbb366</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1430,7 +1430,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N25d5449e22ac488da37cc39f04594b76</t>
+          <t>_:Na67ce142815f4520be2c18b0ca17b92f</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1453,7 +1453,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N74d0b54ca09441879e888edc45406982</t>
+          <t>_:N20ba0e867e5f4e2a9168aba47abaa781</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1476,7 +1476,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:N12440732f0654826957808bebd87879b</t>
+          <t>_:N44b6abbf540e4120afc737eba9d61cae</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1499,7 +1499,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:N4ff4b16f678e4bb19d75d236016c2782</t>
+          <t>_:N57daa86fd1b34106825f3af81e3d3c65</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">

</xml_diff>

<commit_message>
SyntheticDataPipeline: remove explicit Wikipedia references, will get from Wikidata
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -638,7 +638,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X7"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -666,12 +666,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:Nfca21cd83e464a49a903529d1437d9ba</t>
+          <t>_:N90d5762d076a49c9af27a8269dd195f8</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/organization4</t>
+          <t>http://example.com/organization3</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -682,7 +682,7 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1Id0</t>
+          <t>CmsCollection0CmsWork1Id1</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -702,42 +702,37 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+          <t>CmsCollection0CmsWork1 rights holder</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1 rights holder</t>
+          <t>wd:Q937690</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>wd:Q937690</t>
+          <t>http://example.com/collection0/work1Location</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1Location</t>
+          <t>CmsCollection0CmsWork1</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
         </is>
       </c>
+      <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -752,7 +747,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Na065c6fd78c6435794179638b1d97225</t>
+          <t>_:N89aabe6abf44417f918c61e714012cf8</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -788,42 +783,37 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+          <t>CmsCollection0CmsWork3 rights holder</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork3 rights holder</t>
+          <t>wd:Q937690</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>wd:Q937690</t>
+          <t>http://example.com/collection0/work3Location</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3Location</t>
+          <t>CmsCollection0CmsWork3</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork3</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104</t>
         </is>
       </c>
+      <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -838,7 +828,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N9f7478b27b5f4207859e3ebfa3b5edae</t>
+          <t>_:N5298469317144359a9bcef900c615546</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -848,20 +838,20 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 alternative title 1</t>
+          <t>CmsCollection1CmsWork5 alternative title 0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5Id0</t>
+          <t>CmsCollection1CmsWork5Id1</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 provenance 1</t>
+          <t>CmsCollection1CmsWork5 provenance 0</t>
         </is>
       </c>
       <c r="K4" t="inlineStr"/>
@@ -874,42 +864,37 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+          <t>CmsCollection1CmsWork5 rights holder</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 rights holder</t>
+          <t>wd:Q937690</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>wd:Q937690</t>
+          <t>http://example.com/collection1/work5Location</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5Location</t>
+          <t>CmsCollection1CmsWork5</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105</t>
         </is>
       </c>
+      <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -924,12 +909,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:Nca0cdc5910cb41f499c3ca7912db4a22</t>
+          <t>_:N004d25f733d447db887ea4ab57afb96a</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>http://example.com/person4</t>
+          <t>http://example.com/organization0</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -960,42 +945,37 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+          <t>CmsCollection1CmsWork7 rights holder</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 rights holder</t>
+          <t>wd:Q937690</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>wd:Q937690</t>
+          <t>http://example.com/collection1/work7Location</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7Location</t>
+          <t>CmsCollection1CmsWork7</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107</t>
         </is>
       </c>
+      <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
-      <c r="X5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1005,7 +985,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>_:N9530af3d2fa0408d9a8809344ee19e0d</t>
+          <t>_:N89b9c73435b1469fb687ef734cf91a4d</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1021,14 +1001,14 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>FreestandingWork9Id1</t>
+          <t>FreestandingWork9Id0</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 provenance 0</t>
+          <t>FreestandingWork9 provenance 1</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -1041,42 +1021,37 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+          <t>FreestandingWork9 rights holder</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 rights holder</t>
+          <t>wd:Q937690</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>wd:Q937690</t>
+          <t>http://example.com/freestandingwork9Location</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9Location</t>
+          <t>FreestandingWork9</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>FreestandingWork9</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100</t>
         </is>
       </c>
+      <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1086,30 +1061,30 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>_:N7faa25cc95094d7ebefceb4942de812f</t>
+          <t>_:N8171d18bb01c4c4e9f7ff2e28e01a382</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>http://example.com/organization4</t>
+          <t>http://example.com/organization3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>FreestandingWork11 alternative title 1</t>
+          <t>FreestandingWork11 alternative title 0</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>FreestandingWork11Id1</t>
+          <t>FreestandingWork11Id0</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>FreestandingWork11 provenance 1</t>
+          <t>FreestandingWork11 provenance 0</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
@@ -1122,42 +1097,37 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Pilot-ACE</t>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+          <t>FreestandingWork11 rights holder</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>FreestandingWork11 rights holder</t>
+          <t>wd:Q937690</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>wd:Q937690</t>
+          <t>http://example.com/freestandingwork11Location</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11Location</t>
+          <t>FreestandingWork11</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>FreestandingWork11</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
           <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
         </is>
       </c>
+      <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1188,13 +1158,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>_:Nf4445e19b5d64aea8c205c3c82b580bf</t>
+          <t>_:Nc43ed6543fa94597899e13cfea6324f8</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N8abd39b5908d4ea09acc2b45d6b815c2</t>
+          <t>_:N894cc2438c72473f9386aaa3b4bee0d3</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1211,13 +1181,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>_:Nb7a3f07c142e4e26b1f30e67542ea003</t>
+          <t>_:Nf824c9b841cc4a1a8f342ab649cdd1b8</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N9dc5841ebc5c4a53b70b89f0bb28de98</t>
+          <t>_:N5efb0948b86d46d293bcaeb42a2a739a</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1234,13 +1204,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>_:N4c4091bbfbcc4549831976b7781bcab0</t>
+          <t>_:Nbbfb7935f6a14132956a26885e5bd4a7</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N325d98829862447c9b70fe26c8aa3ca1</t>
+          <t>_:N8d829491d7dc4c70935c20707d55f38e</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1257,13 +1227,13 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>_:N302931230fc8418c8595218376792779</t>
+          <t>_:N72a5f37692d84b96a9569702b44810cf</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N1157156d6fcf44ec8fae457c2ac90821</t>
+          <t>_:Nbe41bcda5b8940e1b49f52784d3b0c48</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1280,13 +1250,13 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>_:Nb506613c68be454db1bed455b57ffd1e</t>
+          <t>_:N7e805ec167e3446eb6bb2b81233240e1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:Ne0cd77215a1c427a8df03683201395bb</t>
+          <t>_:Nb473a3eef21a4066a5a6a17ab801f6a8</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1303,13 +1273,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>_:Nb66459a5784e45ca82ab8582bdd74604</t>
+          <t>_:Nfbcbc8db3fe74dc0b5d5a3f30c8c826f</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:Nc838cfd98baf44fe9bc307dbc4307df1</t>
+          <t>_:N03885bd6d8874174bd36295e81ec5193</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1384,7 +1354,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N8abd39b5908d4ea09acc2b45d6b815c2</t>
+          <t>_:N894cc2438c72473f9386aaa3b4bee0d3</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1407,7 +1377,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N9dc5841ebc5c4a53b70b89f0bb28de98</t>
+          <t>_:N5efb0948b86d46d293bcaeb42a2a739a</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1430,7 +1400,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N325d98829862447c9b70fe26c8aa3ca1</t>
+          <t>_:N8d829491d7dc4c70935c20707d55f38e</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1453,7 +1423,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N1157156d6fcf44ec8fae457c2ac90821</t>
+          <t>_:Nbe41bcda5b8940e1b49f52784d3b0c48</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1476,7 +1446,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:Ne0cd77215a1c427a8df03683201395bb</t>
+          <t>_:Nb473a3eef21a4066a5a6a17ab801f6a8</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1499,7 +1469,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:Nc838cfd98baf44fe9bc307dbc4307df1</t>
+          <t>_:N03885bd6d8874174bd36295e81ec5193</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1705,7 +1675,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -18157,7 +18127,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18193,15 +18163,10 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>relation</t>
+          <t>sameAs</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
-        <is>
-          <t>sameAs</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
         <is>
           <t>sortName</t>
         </is>
@@ -18231,15 +18196,10 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>wd:Q7251</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
-        <is>
-          <t>wd:Q7251</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
         <is>
           <t>0, CmsPerson</t>
         </is>
@@ -18268,15 +18228,10 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>wd:Q7251</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
-        <is>
-          <t>wd:Q7251</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
         <is>
           <t>1, CmsPerson</t>
         </is>
@@ -18306,15 +18261,10 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>wd:Q7251</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
-        <is>
-          <t>wd:Q7251</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
         <is>
           <t>2, CmsPerson</t>
         </is>
@@ -18343,15 +18293,10 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>wd:Q7251</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
-        <is>
-          <t>wd:Q7251</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
         <is>
           <t>3, CmsPerson</t>
         </is>
@@ -18381,15 +18326,10 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>http://en.wikipedia.org/wiki/Alan_Turing</t>
+          <t>wd:Q7251</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
-        <is>
-          <t>wd:Q7251</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
         <is>
           <t>4, CmsPerson</t>
         </is>

</xml_diff>

<commit_message>
SyntheticDataPipeline: only have one Work sameAs and one Person sameAs so all the models don't fall into the same group
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -638,7 +638,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -666,23 +666,23 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N90d5762d076a49c9af27a8269dd195f8</t>
+          <t>_:N00fa1d48fadf47d384985bd4c094e573</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/organization3</t>
+          <t>http://example.com/organization4</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1 alternative title 1</t>
+          <t>CmsCollection0CmsWork1 alternative title 0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1Id1</t>
+          <t>CmsCollection0CmsWork1Id0</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -712,27 +712,22 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>wd:Q937690</t>
+          <t>http://example.com/collection0/work1Location</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1Location</t>
+          <t>CmsCollection0CmsWork1</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
-        </is>
-      </c>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -747,7 +742,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N89aabe6abf44417f918c61e714012cf8</t>
+          <t>_:N722458c0fbe944558e6aa6583a1698a2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -770,7 +765,7 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork3 provenance 1</t>
+          <t>CmsCollection0CmsWork3 provenance 0</t>
         </is>
       </c>
       <c r="K3" t="inlineStr"/>
@@ -793,27 +788,22 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>wd:Q937690</t>
+          <t>http://example.com/collection0/work3Location</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3Location</t>
+          <t>CmsCollection0CmsWork3</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork3</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104</t>
-        </is>
-      </c>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -828,17 +818,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N5298469317144359a9bcef900c615546</t>
+          <t>_:N135efa3017db45f18a70366d925697e0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person2</t>
+          <t>http://example.com/person3</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 alternative title 0</t>
+          <t>CmsCollection1CmsWork5 alternative title 1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -851,7 +841,7 @@
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 provenance 0</t>
+          <t>CmsCollection1CmsWork5 provenance 1</t>
         </is>
       </c>
       <c r="K4" t="inlineStr"/>
@@ -874,27 +864,22 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>wd:Q937690</t>
+          <t>http://example.com/collection1/work5Location</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5Location</t>
+          <t>CmsCollection1CmsWork5</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105</t>
-        </is>
-      </c>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -909,7 +894,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N004d25f733d447db887ea4ab57afb96a</t>
+          <t>_:N10724d85d5f143d18cda26923e59ba32</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -919,20 +904,20 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 alternative title 0</t>
+          <t>CmsCollection1CmsWork7 alternative title 1</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7Id1</t>
+          <t>CmsCollection1CmsWork7Id0</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 provenance 0</t>
+          <t>CmsCollection1CmsWork7 provenance 1</t>
         </is>
       </c>
       <c r="K5" t="inlineStr"/>
@@ -955,27 +940,22 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>wd:Q937690</t>
+          <t>http://example.com/collection1/work7Location</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7Location</t>
+          <t>CmsCollection1CmsWork7</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107</t>
-        </is>
-      </c>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -985,12 +965,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>_:N89b9c73435b1469fb687ef734cf91a4d</t>
+          <t>_:Na2058460227a45dcb8072e79710e80d2</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>http://example.com/organization2</t>
+          <t>http://example.com/organization1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1008,7 +988,7 @@
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 provenance 1</t>
+          <t>FreestandingWork9 provenance 0</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -1031,27 +1011,22 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>wd:Q937690</t>
+          <t>http://example.com/freestandingwork9Location</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9Location</t>
+          <t>FreestandingWork9</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>FreestandingWork9</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100</t>
-        </is>
-      </c>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1061,23 +1036,23 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>_:N8171d18bb01c4c4e9f7ff2e28e01a382</t>
+          <t>_:N0ca084e5a9ad4a1090c8d977a58f28db</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>http://example.com/organization3</t>
+          <t>http://example.com/organization4</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>FreestandingWork11 alternative title 0</t>
+          <t>FreestandingWork11 alternative title 1</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>FreestandingWork11Id0</t>
+          <t>FreestandingWork11Id1</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -1107,27 +1082,22 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>wd:Q937690</t>
+          <t>http://example.com/freestandingwork11Location</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11Location</t>
+          <t>FreestandingWork11</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>FreestandingWork11</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
-        </is>
-      </c>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1158,13 +1128,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>_:Nc43ed6543fa94597899e13cfea6324f8</t>
+          <t>_:N2061341608bd426f8b6ae3181e9f21e9</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N894cc2438c72473f9386aaa3b4bee0d3</t>
+          <t>_:Nf85a5bbf34694182876717869155ee40</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1181,13 +1151,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>_:Nf824c9b841cc4a1a8f342ab649cdd1b8</t>
+          <t>_:Nccfd3f3040d14a1cac2b86658bd611e5</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N5efb0948b86d46d293bcaeb42a2a739a</t>
+          <t>_:Na1e7971f85534bbf9720c059728850c2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1204,13 +1174,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>_:Nbbfb7935f6a14132956a26885e5bd4a7</t>
+          <t>_:N90c3265aa22c4710b0505144dfba3aba</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N8d829491d7dc4c70935c20707d55f38e</t>
+          <t>_:Nb2d297c21bb84abf83653d98f4eac18a</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1227,13 +1197,13 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>_:N72a5f37692d84b96a9569702b44810cf</t>
+          <t>_:N36abd647d0474e64816c5c5849efc83a</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:Nbe41bcda5b8940e1b49f52784d3b0c48</t>
+          <t>_:N87d2d0c2f94e4a8991fe449606589c66</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1250,13 +1220,13 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>_:N7e805ec167e3446eb6bb2b81233240e1</t>
+          <t>_:N3219ced4aec54cfcb05605431cbdd8bb</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:Nb473a3eef21a4066a5a6a17ab801f6a8</t>
+          <t>_:N65a6c296b6ef47fbbc47d97d2a750917</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1273,13 +1243,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>_:Nfbcbc8db3fe74dc0b5d5a3f30c8c826f</t>
+          <t>_:N1d4c799acde34f7aac0a66af1b7ff43d</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:N03885bd6d8874174bd36295e81ec5193</t>
+          <t>_:N8d7f9f3db60a498b965aedd962ad9396</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1354,7 +1324,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N894cc2438c72473f9386aaa3b4bee0d3</t>
+          <t>_:Nf85a5bbf34694182876717869155ee40</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1377,7 +1347,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N5efb0948b86d46d293bcaeb42a2a739a</t>
+          <t>_:Na1e7971f85534bbf9720c059728850c2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1400,7 +1370,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N8d829491d7dc4c70935c20707d55f38e</t>
+          <t>_:Nb2d297c21bb84abf83653d98f4eac18a</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1423,7 +1393,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:Nbe41bcda5b8940e1b49f52784d3b0c48</t>
+          <t>_:N87d2d0c2f94e4a8991fe449606589c66</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1446,7 +1416,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:Nb473a3eef21a4066a5a6a17ab801f6a8</t>
+          <t>_:N65a6c296b6ef47fbbc47d97d2a750917</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1469,7 +1439,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:N03885bd6d8874174bd36295e81ec5193</t>
+          <t>_:N8d7f9f3db60a498b965aedd962ad9396</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -18228,11 +18198,6 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>wd:Q7251</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
           <t>1, CmsPerson</t>
         </is>
       </c>
@@ -18261,11 +18226,6 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>wd:Q7251</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
           <t>2, CmsPerson</t>
         </is>
       </c>
@@ -18293,11 +18253,6 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>wd:Q7251</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
           <t>3, CmsPerson</t>
         </is>
       </c>
@@ -18325,11 +18280,6 @@
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
-        <is>
-          <t>wd:Q7251</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
         <is>
           <t>4, CmsPerson</t>
         </is>

</xml_diff>

<commit_message>
WikidataEnricher: yield Wikidata's CC license if any Wikidata models are yielded
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -14,14 +14,14 @@
     <sheet name="CmsConcept" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="CmsOrganization" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="WikibaseItem" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="CmsPerson" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="CmsCollection" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="CmsLocation" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="CmsWork" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="CmsWorkClosing" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="CmsWorkCreation" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="CmsWorkOpening" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="CmsLicense" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="CmsLicense" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="CmsPerson" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="CmsCollection" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="CmsLocation" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="CmsWork" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="CmsWorkClosing" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="CmsWorkCreation" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="CmsWorkOpening" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="CmsRightsStatement" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
@@ -446,6 +446,44 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>@graph</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CmsCollection1</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -632,7 +670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -666,7 +704,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N00fa1d48fadf47d384985bd4c094e573</t>
+          <t>_:Nd7306759dd8947ff80d8396c45aa03e3</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -689,7 +727,7 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1 provenance 1</t>
+          <t>CmsCollection0CmsWork1 provenance 0</t>
         </is>
       </c>
       <c r="K2" t="inlineStr"/>
@@ -722,7 +760,7 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
         </is>
       </c>
       <c r="T2" t="inlineStr"/>
@@ -742,7 +780,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N722458c0fbe944558e6aa6583a1698a2</t>
+          <t>_:Nbc01e82424164b53b2312cb2f76ada79</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -752,7 +790,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork3 alternative title 1</t>
+          <t>CmsCollection0CmsWork3 alternative title 0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -765,7 +803,7 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork3 provenance 0</t>
+          <t>CmsCollection0CmsWork3 provenance 1</t>
         </is>
       </c>
       <c r="K3" t="inlineStr"/>
@@ -818,7 +856,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N135efa3017db45f18a70366d925697e0</t>
+          <t>_:N1eb1e4c86c9b4b7e8b933f167cbc0fdb</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -841,7 +879,7 @@
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 provenance 1</t>
+          <t>CmsCollection1CmsWork5 provenance 0</t>
         </is>
       </c>
       <c r="K4" t="inlineStr"/>
@@ -894,23 +932,23 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N10724d85d5f143d18cda26923e59ba32</t>
+          <t>_:N935c12d7d6ea49c2adc62f4b0ae2d331</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>http://example.com/organization0</t>
+          <t>http://example.com/person4</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 alternative title 1</t>
+          <t>CmsCollection1CmsWork7 alternative title 0</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7Id0</t>
+          <t>CmsCollection1CmsWork7Id1</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -965,7 +1003,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>_:Na2058460227a45dcb8072e79710e80d2</t>
+          <t>_:Nc215499302154b2b82844fd70f81745b</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -981,7 +1019,7 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>FreestandingWork9Id0</t>
+          <t>FreestandingWork9Id1</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -1036,7 +1074,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>_:N0ca084e5a9ad4a1090c8d977a58f28db</t>
+          <t>_:N46244880dcc24b3683fe5abffb21c61c</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1046,20 +1084,20 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>FreestandingWork11 alternative title 1</t>
+          <t>FreestandingWork11 alternative title 0</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>FreestandingWork11Id1</t>
+          <t>FreestandingWork11Id0</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>FreestandingWork11 provenance 0</t>
+          <t>FreestandingWork11 provenance 1</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
@@ -1092,7 +1130,7 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
         </is>
       </c>
       <c r="S7" t="inlineStr"/>
@@ -1104,7 +1142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1128,13 +1166,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>_:N2061341608bd426f8b6ae3181e9f21e9</t>
+          <t>_:Na6dcbef6a65f48d2a572d651d0b4f00d</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:Nf85a5bbf34694182876717869155ee40</t>
+          <t>_:Ne42fb63fe0be4dc487a15dcf31a078da</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1151,13 +1189,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>_:Nccfd3f3040d14a1cac2b86658bd611e5</t>
+          <t>_:N515bb30fe0f04967960ad5c3154aa13f</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Na1e7971f85534bbf9720c059728850c2</t>
+          <t>_:Nbba877dfbeff4c329cb4fc1a59cc683e</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1174,13 +1212,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>_:N90c3265aa22c4710b0505144dfba3aba</t>
+          <t>_:Nb6b28b031023474792c192c64c639a59</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:Nb2d297c21bb84abf83653d98f4eac18a</t>
+          <t>_:N8368f34bfbd748ae9cfa408ffcff75a0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1197,13 +1235,13 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>_:N36abd647d0474e64816c5c5849efc83a</t>
+          <t>_:N84164218f2b441bebdec0d34ed2c657f</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N87d2d0c2f94e4a8991fe449606589c66</t>
+          <t>_:N200d3cffb1474ac6b143c5d338bcf644</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1220,13 +1258,13 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>_:N3219ced4aec54cfcb05605431cbdd8bb</t>
+          <t>_:N6f4c4d089e5b46c09a6a6ffd3b254e41</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:N65a6c296b6ef47fbbc47d97d2a750917</t>
+          <t>_:Nf6ade8393fca4fba88a45a07a81fe6dd</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1243,13 +1281,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>_:N1d4c799acde34f7aac0a66af1b7ff43d</t>
+          <t>_:N206ca6b572504188be661e2f7845d7f3</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:N8d7f9f3db60a498b965aedd962ad9396</t>
+          <t>_:Ncdcfdce879d446deb664b20e2d57c83e</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1268,7 +1306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1294,7 +1332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1324,7 +1362,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:Nf85a5bbf34694182876717869155ee40</t>
+          <t>_:Ne42fb63fe0be4dc487a15dcf31a078da</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1347,7 +1385,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Na1e7971f85534bbf9720c059728850c2</t>
+          <t>_:Nbba877dfbeff4c329cb4fc1a59cc683e</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1370,7 +1408,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:Nb2d297c21bb84abf83653d98f4eac18a</t>
+          <t>_:N8368f34bfbd748ae9cfa408ffcff75a0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1393,7 +1431,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N87d2d0c2f94e4a8991fe449606589c66</t>
+          <t>_:N200d3cffb1474ac6b143c5d338bcf644</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1416,7 +1454,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:N65a6c296b6ef47fbbc47d97d2a750917</t>
+          <t>_:Nf6ade8393fca4fba88a45a07a81fe6dd</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1439,7 +1477,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:N8d7f9f3db60a498b965aedd962ad9396</t>
+          <t>_:Ncdcfdce879d446deb664b20e2d57c83e</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1450,117 +1488,6 @@
       <c r="E7" t="inlineStr">
         <is>
           <t>http://example.com/freestandingwork11</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>@id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>cc:deprecatedOn</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>cc:legalcode</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>cc:licenseClass</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>cc:permits</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>cc:prohibits</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>cc:requires</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>dc:creator</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>foaf:logo</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>identifier</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nc</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>NonCommercial 1.0 Generic</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>1.0</t>
         </is>
       </c>
     </row>
@@ -18097,7 +18024,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18113,175 +18040,105 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>familyName</t>
+          <t>cc:legalcode</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>givenName</t>
+          <t>cc:licenseClass</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>cc:permits</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>page</t>
+          <t>cc:requires</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>sameAs</t>
+          <t>dc:creator</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>sortName</t>
+          <t>foaf:logo</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>version</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>http://example.com/person0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CmsPerson</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CmsPerson 0</t>
-        </is>
-      </c>
+          <t>http://creativecommons.org/licenses/by-sa/3.0/</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>wd:Q7251</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>0, CmsPerson</t>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>by-sa</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Attribution-ShareAlike 3.0 Unported</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>3.0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://example.com/person1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CmsPerson</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CmsPerson 1</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>1, CmsPerson</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>http://example.com/person2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CmsPerson</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>CmsPerson 2</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2, CmsPerson</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>http://example.com/person3</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>CmsPerson</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>CmsPerson 3</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>3, CmsPerson</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>http://example.com/person4</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>CmsPerson</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>CmsPerson 4</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>4, CmsPerson</t>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nc</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>NonCommercial 1.0 Generic</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>1.0</t>
         </is>
       </c>
     </row>
@@ -18296,7 +18153,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18307,19 +18164,180 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>@graph</t>
+          <t>@id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>familyName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>givenName</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>page</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sortName</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>http://example.com/collection1</t>
+          <t>http://example.com/person0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CmsCollection1</t>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CmsPerson</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CmsPerson 0</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>wd:Q7251</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0, CmsPerson</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>http://example.com/person1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CmsPerson</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CmsPerson 1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1, CmsPerson</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>http://example.com/person2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CmsPerson</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CmsPerson 2</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2, CmsPerson</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>http://example.com/person3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CmsPerson</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>CmsPerson 3</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>3, CmsPerson</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>http://example.com/person4</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CmsPerson</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>CmsPerson 4</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>4, CmsPerson</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
WikidataEnricher: add Wikidata rights statement, too
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -15,14 +15,14 @@
     <sheet name="CmsOrganization" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="WikibaseItem" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="CmsLicense" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="CmsPerson" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="CmsCollection" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="CmsLocation" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="CmsWork" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="CmsWorkClosing" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="CmsWorkCreation" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="CmsWorkOpening" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="CmsRightsStatement" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="CmsRightsStatement" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="CmsPerson" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="CmsCollection" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="CmsLocation" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="CmsWork" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="CmsWorkClosing" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="CmsWorkCreation" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="CmsWorkOpening" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -446,6 +446,205 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>@id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>familyName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>givenName</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>page</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sortName</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>http://example.com/person0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CmsPerson</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CmsPerson 0</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>wd:Q7251</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0, CmsPerson</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>http://example.com/person1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CmsPerson</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CmsPerson 1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1, CmsPerson</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>http://example.com/person2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CmsPerson</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CmsPerson 2</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2, CmsPerson</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>http://example.com/person3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CmsPerson</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>CmsPerson 3</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>3, CmsPerson</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>http://example.com/person4</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CmsPerson</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>CmsPerson 4</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>4, CmsPerson</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -478,7 +677,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -670,7 +869,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -704,7 +903,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:Nd7306759dd8947ff80d8396c45aa03e3</t>
+          <t>_:N5590e6700b504be586ffd05d60f0cca0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -714,13 +913,13 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1 alternative title 0</t>
+          <t>CmsCollection0CmsWork1 alternative title 1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1Id0</t>
+          <t>CmsCollection0CmsWork1Id1</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -780,7 +979,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Nbc01e82424164b53b2312cb2f76ada79</t>
+          <t>_:Ne4af7062079541eb84000863aa26fecf</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -790,7 +989,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork3 alternative title 0</t>
+          <t>CmsCollection0CmsWork3 alternative title 1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -836,7 +1035,7 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104</t>
         </is>
       </c>
       <c r="T3" t="inlineStr"/>
@@ -856,30 +1055,30 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N1eb1e4c86c9b4b7e8b933f167cbc0fdb</t>
+          <t>_:N3ee33dfc96f6452db26ab81af9fc777d</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person3</t>
+          <t>http://example.com/person2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 alternative title 1</t>
+          <t>CmsCollection1CmsWork5 alternative title 0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5Id1</t>
+          <t>CmsCollection1CmsWork5Id0</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 provenance 0</t>
+          <t>CmsCollection1CmsWork5 provenance 1</t>
         </is>
       </c>
       <c r="K4" t="inlineStr"/>
@@ -912,7 +1111,7 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105</t>
         </is>
       </c>
       <c r="T4" t="inlineStr"/>
@@ -932,7 +1131,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N935c12d7d6ea49c2adc62f4b0ae2d331</t>
+          <t>_:N5db74a2b9e95490f8f7686b3671df02e</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1003,7 +1202,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>_:Nc215499302154b2b82844fd70f81745b</t>
+          <t>_:Nbc25b2c144764be3bf0d60b491860d91</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1013,7 +1212,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 alternative title 0</t>
+          <t>FreestandingWork9 alternative title 1</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1026,7 +1225,7 @@
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 provenance 0</t>
+          <t>FreestandingWork9 provenance 1</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -1074,7 +1273,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>_:N46244880dcc24b3683fe5abffb21c61c</t>
+          <t>_:N801b2c50f922446fa6f1b7770541b720</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1084,20 +1283,20 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>FreestandingWork11 alternative title 0</t>
+          <t>FreestandingWork11 alternative title 1</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>FreestandingWork11Id0</t>
+          <t>FreestandingWork11Id1</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>FreestandingWork11 provenance 1</t>
+          <t>FreestandingWork11 provenance 0</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
@@ -1130,7 +1329,7 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
         </is>
       </c>
       <c r="S7" t="inlineStr"/>
@@ -1142,7 +1341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1166,13 +1365,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>_:Na6dcbef6a65f48d2a572d651d0b4f00d</t>
+          <t>_:N7c0e2658427c4b82b5471c9d40c284e1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:Ne42fb63fe0be4dc487a15dcf31a078da</t>
+          <t>_:Nca69d65df1794081b163f51e5dc87110</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1189,13 +1388,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>_:N515bb30fe0f04967960ad5c3154aa13f</t>
+          <t>_:Nb1195ba6f3d747b9976eef92f05685f6</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Nbba877dfbeff4c329cb4fc1a59cc683e</t>
+          <t>_:Ne5e5b11f01394324b8ca921773c11cac</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1212,13 +1411,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>_:Nb6b28b031023474792c192c64c639a59</t>
+          <t>_:N38b606b93e7a4bd5bf34dc15ebd56b81</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N8368f34bfbd748ae9cfa408ffcff75a0</t>
+          <t>_:Nb8e005f8fac447ed82b8994f6d548e4c</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1235,13 +1434,13 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>_:N84164218f2b441bebdec0d34ed2c657f</t>
+          <t>_:Nc3adf01041b5403f939d46e667d9ff00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N200d3cffb1474ac6b143c5d338bcf644</t>
+          <t>_:N0526ee091b9246c0a1ac2e40aadb5300</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1258,13 +1457,13 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>_:N6f4c4d089e5b46c09a6a6ffd3b254e41</t>
+          <t>_:N72352baa48444934a59eac00f36e2a2e</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:Nf6ade8393fca4fba88a45a07a81fe6dd</t>
+          <t>_:N39c5f7ac412f409d9e2cd4a92e9a14a5</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1281,13 +1480,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>_:N206ca6b572504188be661e2f7845d7f3</t>
+          <t>_:Nd50353992c01417d8b2037a3e29ecaa3</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:Ncdcfdce879d446deb664b20e2d57c83e</t>
+          <t>_:N1de91241a60c4f47bbbd7cd5474748cf</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1306,7 +1505,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1332,7 +1531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1362,7 +1561,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:Ne42fb63fe0be4dc487a15dcf31a078da</t>
+          <t>_:Nca69d65df1794081b163f51e5dc87110</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1385,7 +1584,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Nbba877dfbeff4c329cb4fc1a59cc683e</t>
+          <t>_:Ne5e5b11f01394324b8ca921773c11cac</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1408,7 +1607,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N8368f34bfbd748ae9cfa408ffcff75a0</t>
+          <t>_:Nb8e005f8fac447ed82b8994f6d548e4c</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1431,7 +1630,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N200d3cffb1474ac6b143c5d338bcf644</t>
+          <t>_:N0526ee091b9246c0a1ac2e40aadb5300</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1454,7 +1653,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:Nf6ade8393fca4fba88a45a07a81fe6dd</t>
+          <t>_:N39c5f7ac412f409d9e2cd4a92e9a14a5</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1477,7 +1676,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:Ncdcfdce879d446deb664b20e2d57c83e</t>
+          <t>_:N1de91241a60c4f47bbbd7cd5474748cf</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1488,101 +1687,6 @@
       <c r="E7" t="inlineStr">
         <is>
           <t>http://example.com/freestandingwork11</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>@id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>definition</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>identifier</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>note</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>prefLabel</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>scopeNote</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>This Item is protected by copyright and/or related rights.
-  You are free to use this Item in any way that is permitted by the copyright and related rights legislation that applies to your use. In addition, no permission is required from the rights-holder(s) for educational uses.
-  For other uses, you need to obtain permission from the rights-holder(s).</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>This Rights Statement indicates that the Item labeled with this Rights Statement is in copyright but that educational use is allowed without the need to obtain additional permission.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>InC-EDU</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>In Copyright - Educational Use Permitted</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>This Rights Statement can be used only for copyrighted Items for which the organization making the Item available is the rights-holder or has been explicitly authorized by the rights-holder(s) to allow third parties to use their Work(s) for educational purposes without first obtaining permission.</t>
         </is>
       </c>
     </row>
@@ -18153,7 +18257,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18169,175 +18273,110 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>familyName</t>
+          <t>definition</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>givenName</t>
+          <t>description</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>identifier</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>page</t>
+          <t>note</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>sameAs</t>
+          <t>prefLabel</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>sortName</t>
+          <t>scopeNote</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>http://example.com/person0</t>
+          <t>http://rightsstatements.org/vocab/InC/1.0/</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>This Item is protected by copyright and/or related rights.
+  You are free to use this Item in any way that is permitted by the copyright and related rights legislation that applies to your use.
+  For other uses you need to obtain permission from the rights-holder(s).</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CmsPerson</t>
+          <t>This Rights Statement indicates that the Item labeled with this Rights Statement is in copyright.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CmsPerson 0</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>InC</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>wd:Q7251</t>
+          <t>In Copyright</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0, CmsPerson</t>
+          <t>This Rights Statement can be used for an Item that is in copyright. Using this statement implies that the organization making this Item available has determined that the Item is in copyright and either is the rights-holder, has obtained permission from the rights-holder(s) to make their Work(s) available, or makes the Item available under an exception or limitation to copyright (including Fair Use) that entitles it to make the Item available.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://example.com/person1</t>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>This Item is protected by copyright and/or related rights.
+  You are free to use this Item in any way that is permitted by the copyright and related rights legislation that applies to your use. In addition, no permission is required from the rights-holder(s) for educational uses.
+  For other uses, you need to obtain permission from the rights-holder(s).</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CmsPerson</t>
+          <t>This Rights Statement indicates that the Item labeled with this Rights Statement is in copyright but that educational use is allowed without the need to obtain additional permission.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CmsPerson 1</t>
+          <t>InC-EDU</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1, CmsPerson</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>http://example.com/person2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CmsPerson</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>CmsPerson 2</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2, CmsPerson</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>http://example.com/person3</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>CmsPerson</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>CmsPerson 3</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>3, CmsPerson</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>http://example.com/person4</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>CmsPerson</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>CmsPerson 4</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>4, CmsPerson</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>In Copyright - Educational Use Permitted</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>This Rights Statement can be used only for copyrighted Items for which the organization making the Item available is the rights-holder or has been explicitly authorized by the rights-holder(s) to allow third parties to use their Work(s) for educational purposes without first obtaining permission.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
WikidataEnricher: add wdt:P18 image support and enrich appropriately
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -903,12 +903,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N5590e6700b504be586ffd05d60f0cca0</t>
+          <t>_:N1f7f11d5335541778f5eb233c6b66191</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/organization4</t>
+          <t>http://example.com/organization3</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -926,7 +926,7 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1 provenance 0</t>
+          <t>CmsCollection0CmsWork1 provenance 1</t>
         </is>
       </c>
       <c r="K2" t="inlineStr"/>
@@ -959,7 +959,7 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
         </is>
       </c>
       <c r="T2" t="inlineStr"/>
@@ -979,7 +979,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Ne4af7062079541eb84000863aa26fecf</t>
+          <t>_:Nafaabef3ace64cce880dbf9cdac7ef37</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1035,7 +1035,7 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103</t>
         </is>
       </c>
       <c r="T3" t="inlineStr"/>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N3ee33dfc96f6452db26ab81af9fc777d</t>
+          <t>_:N7e04a2dca5904446a09d2b2fc594a1d3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1065,13 +1065,13 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 alternative title 0</t>
+          <t>CmsCollection1CmsWork5 alternative title 1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5Id0</t>
+          <t>CmsCollection1CmsWork5Id1</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106</t>
         </is>
       </c>
       <c r="T4" t="inlineStr"/>
@@ -1131,23 +1131,23 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N5db74a2b9e95490f8f7686b3671df02e</t>
+          <t>_:N03e636dde17e4a7a8cb0ff783d6e858f</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>http://example.com/person4</t>
+          <t>http://example.com/organization0</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 alternative title 0</t>
+          <t>CmsCollection1CmsWork7 alternative title 1</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7Id1</t>
+          <t>CmsCollection1CmsWork7Id0</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107</t>
         </is>
       </c>
       <c r="T5" t="inlineStr"/>
@@ -1202,7 +1202,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>_:Nbc25b2c144764be3bf0d60b491860d91</t>
+          <t>_:N430dd966c5f6469f8ca27d4a67384be1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1212,7 +1212,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 alternative title 1</t>
+          <t>FreestandingWork9 alternative title 0</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1273,12 +1273,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>_:N801b2c50f922446fa6f1b7770541b720</t>
+          <t>_:N30c940f0b45c405483c789fc9335e323</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>http://example.com/organization4</t>
+          <t>http://example.com/organization3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1365,13 +1365,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>_:N7c0e2658427c4b82b5471c9d40c284e1</t>
+          <t>_:Nbb35479ad1d646dd80842e8c9795df6c</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:Nca69d65df1794081b163f51e5dc87110</t>
+          <t>_:Nc158d3c01669490298d576827ac9de64</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1388,13 +1388,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>_:Nb1195ba6f3d747b9976eef92f05685f6</t>
+          <t>_:Ne016fa7f5d92418e9e4170c9e824ce1f</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Ne5e5b11f01394324b8ca921773c11cac</t>
+          <t>_:N556ebbcf163041cd94e469d5a21e8344</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1411,13 +1411,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>_:N38b606b93e7a4bd5bf34dc15ebd56b81</t>
+          <t>_:N06d359c44f4144199cf063df46320bcf</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:Nb8e005f8fac447ed82b8994f6d548e4c</t>
+          <t>_:N8de3432738b042eaab948ba55d14ce0b</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1434,13 +1434,13 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>_:Nc3adf01041b5403f939d46e667d9ff00</t>
+          <t>_:Nc6c740ab856941f2a0436ce79bfc182d</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N0526ee091b9246c0a1ac2e40aadb5300</t>
+          <t>_:N2ded0283362f423e9ac769f075367800</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1457,13 +1457,13 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>_:N72352baa48444934a59eac00f36e2a2e</t>
+          <t>_:N4c9a654a5ac24bd0a153ecd4c1205dde</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:N39c5f7ac412f409d9e2cd4a92e9a14a5</t>
+          <t>_:Nbfa144b776ea4d738c78de97ed117045</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1480,13 +1480,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>_:Nd50353992c01417d8b2037a3e29ecaa3</t>
+          <t>_:N7e75ba26fcac4b49a879f9eb0b34a59a</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:N1de91241a60c4f47bbbd7cd5474748cf</t>
+          <t>_:Nb1ab92d7755644adbd735a6bdfa8a80f</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1561,7 +1561,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:Nca69d65df1794081b163f51e5dc87110</t>
+          <t>_:Nc158d3c01669490298d576827ac9de64</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1584,7 +1584,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Ne5e5b11f01394324b8ca921773c11cac</t>
+          <t>_:N556ebbcf163041cd94e469d5a21e8344</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1607,7 +1607,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:Nb8e005f8fac447ed82b8994f6d548e4c</t>
+          <t>_:N8de3432738b042eaab948ba55d14ce0b</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1630,7 +1630,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N0526ee091b9246c0a1ac2e40aadb5300</t>
+          <t>_:N2ded0283362f423e9ac769f075367800</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1653,7 +1653,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:N39c5f7ac412f409d9e2cd4a92e9a14a5</t>
+          <t>_:Nbfa144b776ea4d738c78de97ed117045</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1676,7 +1676,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:N1de91241a60c4f47bbbd7cd5474748cf</t>
+          <t>_:Nb1ab92d7755644adbd735a6bdfa8a80f</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1744,7 +1744,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I295"/>
+  <dimension ref="A1:I297"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13928,59 +13928,49 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>http://example.com/person0:CmsImage0</t>
+          <t>http://commons.wikimedia.org/wiki/Special:FilePath/Alan%20Turing%20Aged%2016.jpg</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>CmsPerson 0 image 0</t>
+          <t>Possibly Arthur Reginald Chaffin (1893-1954)</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>http://example.com/person0</t>
+          <t>Passport photo of Alan Turing at age 16</t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>wd:Q7251</t>
         </is>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
         <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+          <t>http://commons.wikimedia.org/wiki/File:Alan%20Turing%20Aged%2016.jpg</t>
         </is>
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>CmsPerson 0 image 0 rights holder</t>
-        </is>
-      </c>
-      <c r="H260" t="inlineStr">
-        <is>
-          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
-        </is>
-      </c>
-      <c r="I260" t="inlineStr">
-        <is>
-          <t>1000</t>
+          <t>https://upload.wikimedia.org/wikipedia/commons/a/a1/Alan_Turing_Aged_16.jpg</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>http://example.com/person0:CmsImage1</t>
+          <t>http://example.com/person0:CmsImage0</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>CmsPerson 0 image 1</t>
+          <t>CmsPerson 0 image 0</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
@@ -14005,7 +13995,7 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>CmsPerson 0 image 1 rights holder</t>
+          <t>CmsPerson 0 image 0 rights holder</t>
         </is>
       </c>
       <c r="H261" t="inlineStr">
@@ -14022,17 +14012,17 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>http://example.com/person1:CmsImage0</t>
+          <t>http://example.com/person0:CmsImage1</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>CmsPerson 1 image 0</t>
+          <t>CmsPerson 0 image 1</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>http://example.com/person1</t>
+          <t>http://example.com/person0</t>
         </is>
       </c>
       <c r="D262" t="inlineStr">
@@ -14052,7 +14042,7 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>CmsPerson 1 image 0 rights holder</t>
+          <t>CmsPerson 0 image 1 rights holder</t>
         </is>
       </c>
       <c r="H262" t="inlineStr">
@@ -14069,12 +14059,12 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>http://example.com/person1:CmsImage1</t>
+          <t>http://example.com/person1:CmsImage0</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>CmsPerson 1 image 1</t>
+          <t>CmsPerson 1 image 0</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
@@ -14099,7 +14089,7 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>CmsPerson 1 image 1 rights holder</t>
+          <t>CmsPerson 1 image 0 rights holder</t>
         </is>
       </c>
       <c r="H263" t="inlineStr">
@@ -14116,17 +14106,17 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>http://example.com/person2:CmsImage0</t>
+          <t>http://example.com/person1:CmsImage1</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>CmsPerson 2 image 0</t>
+          <t>CmsPerson 1 image 1</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>http://example.com/person2</t>
+          <t>http://example.com/person1</t>
         </is>
       </c>
       <c r="D264" t="inlineStr">
@@ -14146,7 +14136,7 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>CmsPerson 2 image 0 rights holder</t>
+          <t>CmsPerson 1 image 1 rights holder</t>
         </is>
       </c>
       <c r="H264" t="inlineStr">
@@ -14163,12 +14153,12 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>http://example.com/person2:CmsImage1</t>
+          <t>http://example.com/person2:CmsImage0</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>CmsPerson 2 image 1</t>
+          <t>CmsPerson 2 image 0</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
@@ -14193,7 +14183,7 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>CmsPerson 2 image 1 rights holder</t>
+          <t>CmsPerson 2 image 0 rights holder</t>
         </is>
       </c>
       <c r="H265" t="inlineStr">
@@ -14210,17 +14200,17 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>http://example.com/person3:CmsImage0</t>
+          <t>http://example.com/person2:CmsImage1</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>CmsPerson 3 image 0</t>
+          <t>CmsPerson 2 image 1</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>http://example.com/person3</t>
+          <t>http://example.com/person2</t>
         </is>
       </c>
       <c r="D266" t="inlineStr">
@@ -14240,7 +14230,7 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>CmsPerson 3 image 0 rights holder</t>
+          <t>CmsPerson 2 image 1 rights holder</t>
         </is>
       </c>
       <c r="H266" t="inlineStr">
@@ -14257,12 +14247,12 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>http://example.com/person3:CmsImage1</t>
+          <t>http://example.com/person3:CmsImage0</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>CmsPerson 3 image 1</t>
+          <t>CmsPerson 3 image 0</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -14287,7 +14277,7 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>CmsPerson 3 image 1 rights holder</t>
+          <t>CmsPerson 3 image 0 rights holder</t>
         </is>
       </c>
       <c r="H267" t="inlineStr">
@@ -14304,17 +14294,17 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>http://example.com/person4:CmsImage0</t>
+          <t>http://example.com/person3:CmsImage1</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>CmsPerson 4 image 0</t>
+          <t>CmsPerson 3 image 1</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>http://example.com/person4</t>
+          <t>http://example.com/person3</t>
         </is>
       </c>
       <c r="D268" t="inlineStr">
@@ -14334,7 +14324,7 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>CmsPerson 4 image 0 rights holder</t>
+          <t>CmsPerson 3 image 1 rights holder</t>
         </is>
       </c>
       <c r="H268" t="inlineStr">
@@ -14351,12 +14341,12 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>http://example.com/person4:CmsImage1</t>
+          <t>http://example.com/person4:CmsImage0</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>CmsPerson 4 image 1</t>
+          <t>CmsPerson 4 image 0</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
@@ -14381,7 +14371,7 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>CmsPerson 4 image 1 rights holder</t>
+          <t>CmsPerson 4 image 0 rights holder</t>
         </is>
       </c>
       <c r="H269" t="inlineStr">
@@ -14398,17 +14388,17 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0:CmsImage0</t>
+          <t>http://example.com/person4:CmsImage1</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork0 image 0</t>
+          <t>CmsPerson 4 image 1</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0</t>
+          <t>http://example.com/person4</t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
@@ -14428,7 +14418,7 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork0 image 0 rights holder</t>
+          <t>CmsPerson 4 image 1 rights holder</t>
         </is>
       </c>
       <c r="H270" t="inlineStr">
@@ -14445,64 +14435,59 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0:CmsImage1</t>
+          <t>http://commons.wikimedia.org/wiki/Special:FilePath/Pilot%20ACE%20computer-2.jpg</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork0 image 1</t>
+          <t>Steve Elliott</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0</t>
+          <t>Pilot ACE computer on display at Science Museum in London</t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>wd:Q937690</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+          <t>http://rightsstatements.org/vocab/InC/1.0/</t>
         </is>
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork0 image 1 rights holder</t>
+          <t>http://commons.wikimedia.org/wiki/File:Pilot%20ACE%20computer-2.jpg</t>
         </is>
       </c>
       <c r="H271" t="inlineStr">
         <is>
-          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
-        </is>
-      </c>
-      <c r="I271" t="inlineStr">
-        <is>
-          <t>1000</t>
+          <t>https://upload.wikimedia.org/wikipedia/commons/c/c6/Pilot_ACE_computer-2.jpg</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:CmsImage0</t>
+          <t>http://example.com/collection0/work0:CmsImage0</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1 image 0</t>
+          <t>CmsCollection0CmsWork0 image 0</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1</t>
+          <t>http://example.com/collection0/work0</t>
         </is>
       </c>
       <c r="D272" t="inlineStr">
@@ -14522,7 +14507,7 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1 image 0 rights holder</t>
+          <t>CmsCollection0CmsWork0 image 0 rights holder</t>
         </is>
       </c>
       <c r="H272" t="inlineStr">
@@ -14539,17 +14524,17 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:CmsImage1</t>
+          <t>http://example.com/collection0/work0:CmsImage1</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1 image 1</t>
+          <t>CmsCollection0CmsWork0 image 1</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1</t>
+          <t>http://example.com/collection0/work0</t>
         </is>
       </c>
       <c r="D273" t="inlineStr">
@@ -14569,7 +14554,7 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork1 image 1 rights holder</t>
+          <t>CmsCollection0CmsWork0 image 1 rights holder</t>
         </is>
       </c>
       <c r="H273" t="inlineStr">
@@ -14586,17 +14571,17 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2:CmsImage0</t>
+          <t>http://example.com/collection0/work1:CmsImage0</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork2 image 0</t>
+          <t>CmsCollection0CmsWork1 image 0</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2</t>
+          <t>http://example.com/collection0/work1</t>
         </is>
       </c>
       <c r="D274" t="inlineStr">
@@ -14616,7 +14601,7 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork2 image 0 rights holder</t>
+          <t>CmsCollection0CmsWork1 image 0 rights holder</t>
         </is>
       </c>
       <c r="H274" t="inlineStr">
@@ -14633,17 +14618,17 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2:CmsImage1</t>
+          <t>http://example.com/collection0/work1:CmsImage1</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork2 image 1</t>
+          <t>CmsCollection0CmsWork1 image 1</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2</t>
+          <t>http://example.com/collection0/work1</t>
         </is>
       </c>
       <c r="D275" t="inlineStr">
@@ -14663,7 +14648,7 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork2 image 1 rights holder</t>
+          <t>CmsCollection0CmsWork1 image 1 rights holder</t>
         </is>
       </c>
       <c r="H275" t="inlineStr">
@@ -14680,17 +14665,17 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:CmsImage0</t>
+          <t>http://example.com/collection0/work2:CmsImage0</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork3 image 0</t>
+          <t>CmsCollection0CmsWork2 image 0</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3</t>
+          <t>http://example.com/collection0/work2</t>
         </is>
       </c>
       <c r="D276" t="inlineStr">
@@ -14710,7 +14695,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork3 image 0 rights holder</t>
+          <t>CmsCollection0CmsWork2 image 0 rights holder</t>
         </is>
       </c>
       <c r="H276" t="inlineStr">
@@ -14727,17 +14712,17 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:CmsImage1</t>
+          <t>http://example.com/collection0/work2:CmsImage1</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork3 image 1</t>
+          <t>CmsCollection0CmsWork2 image 1</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3</t>
+          <t>http://example.com/collection0/work2</t>
         </is>
       </c>
       <c r="D277" t="inlineStr">
@@ -14757,7 +14742,7 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>CmsCollection0CmsWork3 image 1 rights holder</t>
+          <t>CmsCollection0CmsWork2 image 1 rights holder</t>
         </is>
       </c>
       <c r="H277" t="inlineStr">
@@ -14774,17 +14759,17 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:CmsImage0</t>
+          <t>http://example.com/collection0/work3:CmsImage0</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>CmsCollection1 image 0</t>
+          <t>CmsCollection0CmsWork3 image 0</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>http://example.com/collection1</t>
+          <t>http://example.com/collection0/work3</t>
         </is>
       </c>
       <c r="D278" t="inlineStr">
@@ -14804,7 +14789,7 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>CmsCollection1 image 0 rights holder</t>
+          <t>CmsCollection0CmsWork3 image 0 rights holder</t>
         </is>
       </c>
       <c r="H278" t="inlineStr">
@@ -14821,17 +14806,17 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:CmsImage1</t>
+          <t>http://example.com/collection0/work3:CmsImage1</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>CmsCollection1 image 1</t>
+          <t>CmsCollection0CmsWork3 image 1</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>http://example.com/collection1</t>
+          <t>http://example.com/collection0/work3</t>
         </is>
       </c>
       <c r="D279" t="inlineStr">
@@ -14851,7 +14836,7 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>CmsCollection1 image 1 rights holder</t>
+          <t>CmsCollection0CmsWork3 image 1 rights holder</t>
         </is>
       </c>
       <c r="H279" t="inlineStr">
@@ -14868,17 +14853,17 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4:CmsImage0</t>
+          <t>http://example.com/collection1:CmsImage0</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork4 image 0</t>
+          <t>CmsCollection1 image 0</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4</t>
+          <t>http://example.com/collection1</t>
         </is>
       </c>
       <c r="D280" t="inlineStr">
@@ -14898,7 +14883,7 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork4 image 0 rights holder</t>
+          <t>CmsCollection1 image 0 rights holder</t>
         </is>
       </c>
       <c r="H280" t="inlineStr">
@@ -14915,17 +14900,17 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4:CmsImage1</t>
+          <t>http://example.com/collection1:CmsImage1</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork4 image 1</t>
+          <t>CmsCollection1 image 1</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4</t>
+          <t>http://example.com/collection1</t>
         </is>
       </c>
       <c r="D281" t="inlineStr">
@@ -14945,7 +14930,7 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork4 image 1 rights holder</t>
+          <t>CmsCollection1 image 1 rights holder</t>
         </is>
       </c>
       <c r="H281" t="inlineStr">
@@ -14962,17 +14947,17 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:CmsImage0</t>
+          <t>http://example.com/collection1/work4:CmsImage0</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 image 0</t>
+          <t>CmsCollection1CmsWork4 image 0</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5</t>
+          <t>http://example.com/collection1/work4</t>
         </is>
       </c>
       <c r="D282" t="inlineStr">
@@ -14992,7 +14977,7 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 image 0 rights holder</t>
+          <t>CmsCollection1CmsWork4 image 0 rights holder</t>
         </is>
       </c>
       <c r="H282" t="inlineStr">
@@ -15009,17 +14994,17 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:CmsImage1</t>
+          <t>http://example.com/collection1/work4:CmsImage1</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 image 1</t>
+          <t>CmsCollection1CmsWork4 image 1</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5</t>
+          <t>http://example.com/collection1/work4</t>
         </is>
       </c>
       <c r="D283" t="inlineStr">
@@ -15039,7 +15024,7 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork5 image 1 rights holder</t>
+          <t>CmsCollection1CmsWork4 image 1 rights holder</t>
         </is>
       </c>
       <c r="H283" t="inlineStr">
@@ -15056,17 +15041,17 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6:CmsImage0</t>
+          <t>http://example.com/collection1/work5:CmsImage0</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork6 image 0</t>
+          <t>CmsCollection1CmsWork5 image 0</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6</t>
+          <t>http://example.com/collection1/work5</t>
         </is>
       </c>
       <c r="D284" t="inlineStr">
@@ -15086,7 +15071,7 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork6 image 0 rights holder</t>
+          <t>CmsCollection1CmsWork5 image 0 rights holder</t>
         </is>
       </c>
       <c r="H284" t="inlineStr">
@@ -15103,17 +15088,17 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6:CmsImage1</t>
+          <t>http://example.com/collection1/work5:CmsImage1</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork6 image 1</t>
+          <t>CmsCollection1CmsWork5 image 1</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6</t>
+          <t>http://example.com/collection1/work5</t>
         </is>
       </c>
       <c r="D285" t="inlineStr">
@@ -15133,7 +15118,7 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork6 image 1 rights holder</t>
+          <t>CmsCollection1CmsWork5 image 1 rights holder</t>
         </is>
       </c>
       <c r="H285" t="inlineStr">
@@ -15150,17 +15135,17 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:CmsImage0</t>
+          <t>http://example.com/collection1/work6:CmsImage0</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 image 0</t>
+          <t>CmsCollection1CmsWork6 image 0</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7</t>
+          <t>http://example.com/collection1/work6</t>
         </is>
       </c>
       <c r="D286" t="inlineStr">
@@ -15180,7 +15165,7 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 image 0 rights holder</t>
+          <t>CmsCollection1CmsWork6 image 0 rights holder</t>
         </is>
       </c>
       <c r="H286" t="inlineStr">
@@ -15197,17 +15182,17 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:CmsImage1</t>
+          <t>http://example.com/collection1/work6:CmsImage1</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 image 1</t>
+          <t>CmsCollection1CmsWork6 image 1</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7</t>
+          <t>http://example.com/collection1/work6</t>
         </is>
       </c>
       <c r="D287" t="inlineStr">
@@ -15227,7 +15212,7 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>CmsCollection1CmsWork7 image 1 rights holder</t>
+          <t>CmsCollection1CmsWork6 image 1 rights holder</t>
         </is>
       </c>
       <c r="H287" t="inlineStr">
@@ -15244,17 +15229,17 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8:CmsImage0</t>
+          <t>http://example.com/collection1/work7:CmsImage0</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>FreestandingWork8 image 0</t>
+          <t>CmsCollection1CmsWork7 image 0</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8</t>
+          <t>http://example.com/collection1/work7</t>
         </is>
       </c>
       <c r="D288" t="inlineStr">
@@ -15274,7 +15259,7 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>FreestandingWork8 image 0 rights holder</t>
+          <t>CmsCollection1CmsWork7 image 0 rights holder</t>
         </is>
       </c>
       <c r="H288" t="inlineStr">
@@ -15291,17 +15276,17 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8:CmsImage1</t>
+          <t>http://example.com/collection1/work7:CmsImage1</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>FreestandingWork8 image 1</t>
+          <t>CmsCollection1CmsWork7 image 1</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8</t>
+          <t>http://example.com/collection1/work7</t>
         </is>
       </c>
       <c r="D289" t="inlineStr">
@@ -15321,7 +15306,7 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>FreestandingWork8 image 1 rights holder</t>
+          <t>CmsCollection1CmsWork7 image 1 rights holder</t>
         </is>
       </c>
       <c r="H289" t="inlineStr">
@@ -15338,17 +15323,17 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:CmsImage0</t>
+          <t>http://example.com/freestandingwork8:CmsImage0</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>FreestandingWork9 image 0</t>
+          <t>FreestandingWork8 image 0</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9</t>
+          <t>http://example.com/freestandingwork8</t>
         </is>
       </c>
       <c r="D290" t="inlineStr">
@@ -15368,7 +15353,7 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>FreestandingWork9 image 0 rights holder</t>
+          <t>FreestandingWork8 image 0 rights holder</t>
         </is>
       </c>
       <c r="H290" t="inlineStr">
@@ -15385,17 +15370,17 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:CmsImage1</t>
+          <t>http://example.com/freestandingwork8:CmsImage1</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>FreestandingWork9 image 1</t>
+          <t>FreestandingWork8 image 1</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9</t>
+          <t>http://example.com/freestandingwork8</t>
         </is>
       </c>
       <c r="D291" t="inlineStr">
@@ -15415,7 +15400,7 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>FreestandingWork9 image 1 rights holder</t>
+          <t>FreestandingWork8 image 1 rights holder</t>
         </is>
       </c>
       <c r="H291" t="inlineStr">
@@ -15432,17 +15417,17 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10:CmsImage0</t>
+          <t>http://example.com/freestandingwork9:CmsImage0</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>FreestandingWork10 image 0</t>
+          <t>FreestandingWork9 image 0</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10</t>
+          <t>http://example.com/freestandingwork9</t>
         </is>
       </c>
       <c r="D292" t="inlineStr">
@@ -15462,7 +15447,7 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>FreestandingWork10 image 0 rights holder</t>
+          <t>FreestandingWork9 image 0 rights holder</t>
         </is>
       </c>
       <c r="H292" t="inlineStr">
@@ -15479,17 +15464,17 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10:CmsImage1</t>
+          <t>http://example.com/freestandingwork9:CmsImage1</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>FreestandingWork10 image 1</t>
+          <t>FreestandingWork9 image 1</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10</t>
+          <t>http://example.com/freestandingwork9</t>
         </is>
       </c>
       <c r="D293" t="inlineStr">
@@ -15509,7 +15494,7 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>FreestandingWork10 image 1 rights holder</t>
+          <t>FreestandingWork9 image 1 rights holder</t>
         </is>
       </c>
       <c r="H293" t="inlineStr">
@@ -15526,17 +15511,17 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:CmsImage0</t>
+          <t>http://example.com/freestandingwork10:CmsImage0</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>FreestandingWork11 image 0</t>
+          <t>FreestandingWork10 image 0</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11</t>
+          <t>http://example.com/freestandingwork10</t>
         </is>
       </c>
       <c r="D294" t="inlineStr">
@@ -15556,7 +15541,7 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>FreestandingWork11 image 0 rights holder</t>
+          <t>FreestandingWork10 image 0 rights holder</t>
         </is>
       </c>
       <c r="H294" t="inlineStr">
@@ -15573,45 +15558,139 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
+          <t>http://example.com/freestandingwork10:CmsImage1</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>FreestandingWork10 image 1</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork10</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="F295" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="G295" t="inlineStr">
+        <is>
+          <t>FreestandingWork10 image 1 rights holder</t>
+        </is>
+      </c>
+      <c r="H295" t="inlineStr">
+        <is>
+          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
+        </is>
+      </c>
+      <c r="I295" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork11:CmsImage0</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>FreestandingWork11 image 0</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork11</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="G296" t="inlineStr">
+        <is>
+          <t>FreestandingWork11 image 0 rights holder</t>
+        </is>
+      </c>
+      <c r="H296" t="inlineStr">
+        <is>
+          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
+        </is>
+      </c>
+      <c r="I296" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
           <t>http://example.com/freestandingwork11:CmsImage1</t>
         </is>
       </c>
-      <c r="B295" t="inlineStr">
+      <c r="B297" t="inlineStr">
         <is>
           <t>FreestandingWork11 image 1</t>
         </is>
       </c>
-      <c r="C295" t="inlineStr">
+      <c r="C297" t="inlineStr">
         <is>
           <t>http://example.com/freestandingwork11</t>
         </is>
       </c>
-      <c r="D295" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="E295" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="F295" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="G295" t="inlineStr">
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
+        </is>
+      </c>
+      <c r="G297" t="inlineStr">
         <is>
           <t>FreestandingWork11 image 1 rights holder</t>
         </is>
       </c>
-      <c r="H295" t="inlineStr">
-        <is>
-          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
-        </is>
-      </c>
-      <c r="I295" t="inlineStr">
+      <c r="H297" t="inlineStr">
+        <is>
+          <t>https://paradicms.org/img/placeholder/1000x1000.png</t>
+        </is>
+      </c>
+      <c r="I297" t="inlineStr">
         <is>
           <t>1000</t>
         </is>
@@ -18128,7 +18207,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18243,6 +18322,61 @@
       <c r="L3" t="inlineStr">
         <is>
           <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>mark</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Public Domain Mark 1.0</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>by-sa</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Attribution-ShareAlike 2.0 Generic</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2.0</t>
         </is>
       </c>
     </row>
@@ -18327,7 +18461,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -18366,7 +18500,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">

</xml_diff>

<commit_message>
add ncsu sameAs to synthetic data freestanding work 1
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -508,7 +508,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image1:Thumbnail200x200</t>
+          <t>http://example.com/person0:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image1:Thumbnail400x400</t>
+          <t>http://example.com/person1:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -568,7 +568,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image1</t>
+          <t>http://example.com/person2:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -596,7 +596,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image1:Thumbnail200x200</t>
+          <t>http://example.com/person3:Image0</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -623,7 +623,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image1:Thumbnail800x800</t>
+          <t>http://example.com/person4:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -886,7 +886,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N81d8f1a34e7941b585ec13277d3239bd</t>
+          <t>_:N7b1e5e5f61c249ce947f836bae94d708</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -904,7 +904,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N4062160156e2432296669ee3a075971d</t>
+          <t>_:N6251f3ba129743acbdfb02b7f3748d12</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -922,7 +922,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N8a1b72e6e7124b26870c90b5739b37e2</t>
+          <t>_:Nc18fdcbaa2f544cb829b4f21997b0c49</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -940,7 +940,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N24d1015f8b2a423f8c503a73dead4943</t>
+          <t>_:N2c2badeb39424532a523eda50f82a976</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -958,7 +958,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:Nf7147a94fa494036bfc07c0101e2010a</t>
+          <t>_:N1651b1019c374db9afc43e8a520272a9</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -976,7 +976,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:N9170a80b23ce4fa085ada31800d0096b</t>
+          <t>_:N40f268c129794ec2bb38ced8832064fe</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -996,7 +996,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>_:N7ef39d8b815b4d8ca6dcadec034e0ff9</t>
+          <t>_:N424edfef4d2c4114a238452c5c16953d</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1029,13 +1029,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Collection0Work1 alternative title 0</t>
+          <t>Collection0Work1 alternative title 1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Collection0Work1Id1</t>
+          <t>Collection0Work1Id0</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -1050,12 +1050,12 @@
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>_:N78dcacdf8d0444eb8677c2155e164189</t>
+          <t>_:Ne7510d048a224db0985773cfb8bc0af4</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image1:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work1:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -1075,22 +1075,27 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
+          <t>https://d.lib.ncsu.edu/collections/catalog/0002030</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
           <t>http://example.com/collection0/work1Location</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>Collection0Work1</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr"/>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
+        </is>
+      </c>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1100,12 +1105,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>_:Naf6a274502ce457d8e5e553bd649ed8c</t>
+          <t>_:Ne5b76b56abe1409facce98cb9a53f12b</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://example.com/person1</t>
+          <t>http://example.com/person0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1116,7 +1121,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Collection0Work3Id1</t>
+          <t>Collection0Work3Id0</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -1131,12 +1136,12 @@
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3Opening</t>
+          <t>http://example.com/collection0/work3Creation</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image1:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work3:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -1181,7 +1186,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>_:N7b09d6adffe847088a8a2c6407397274</t>
+          <t>_:N9f30581ec49b4ce2bf752745c10aa807</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1191,20 +1196,20 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Collection1Work5 alternative title 1</t>
+          <t>Collection1Work5 alternative title 0</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Collection1Work5Id0</t>
+          <t>Collection1Work5Id1</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Collection1Work5 provenance 0</t>
+          <t>Collection1Work5 provenance 1</t>
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
@@ -1212,7 +1217,7 @@
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
-          <t>_:N4e8d66aa354a4f6fba10b0de3b87d93d</t>
+          <t>_:N487dbcb83bac44819b1f846bff5b4748</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -1247,7 +1252,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105</t>
         </is>
       </c>
       <c r="U4" t="inlineStr"/>
@@ -1262,7 +1267,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>_:Nb13a9cc4aa3e4888bb146098dc3404a3</t>
+          <t>_:N940c399b3bd64f35947784159521dc30</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1272,20 +1277,20 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Collection1Work7 alternative title 1</t>
+          <t>Collection1Work7 alternative title 0</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Collection1Work7Id0</t>
+          <t>Collection1Work7Id1</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Collection1Work7 provenance 0</t>
+          <t>Collection1Work7 provenance 1</t>
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
@@ -1293,12 +1298,12 @@
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7Opening</t>
+          <t>http://example.com/collection1/work7Creation</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image1</t>
+          <t>http://example.com/collection1/work7:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1343,7 +1348,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>_:N9f4a85e680b04465a2ee6c4e84a2461b</t>
+          <t>_:N674da56f87bc4c1ea69388fa3e5c345c</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1353,20 +1358,20 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 alternative title 0</t>
+          <t>FreestandingWork9 alternative title 1</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>FreestandingWork9Id0</t>
+          <t>FreestandingWork9Id1</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 provenance 1</t>
+          <t>FreestandingWork9 provenance 0</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -1374,12 +1379,12 @@
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9Creation</t>
+          <t>_:Nbffae5cdc8804553ad78526757cfa494</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:Image0:Thumbnail600x600</t>
+          <t>http://example.com/freestandingwork9:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -1424,7 +1429,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>_:N0614f818e7c3489da703efd33b078e0f</t>
+          <t>_:N2487adb27377414d9df62d6ffac62ef5</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1434,13 +1439,13 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>FreestandingWork11 alternative title 0</t>
+          <t>FreestandingWork11 alternative title 1</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>FreestandingWork11Id0</t>
+          <t>FreestandingWork11Id1</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -1455,12 +1460,12 @@
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11Opening</t>
+          <t>http://example.com/freestandingwork11Creation</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:Image0</t>
+          <t>http://example.com/freestandingwork11:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -1531,12 +1536,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5</t>
+          <t>http://example.com/collection1/work6</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image0:Thumbnail400x400</t>
+          <t>http://example.com/collection1:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1807,7 +1812,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -2022,7 +2027,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -2237,7 +2242,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>vra:culturalContext:Image0:Thumbnail600x600</t>
+          <t>vra:culturalContext:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -2667,7 +2672,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>dcterms:description:Image0:Thumbnail400x400</t>
+          <t>dcterms:description:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2882,7 +2887,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>dcterms:description:Image1:Thumbnail600x600</t>
+          <t>dcterms:description:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -3097,7 +3102,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0:Thumbnail400x400</t>
+          <t>dcterms:extent:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -3312,7 +3317,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image1:Thumbnail200x200</t>
+          <t>dcterms:extent:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -3527,7 +3532,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>dcterms:language:Image0:Thumbnail800x800</t>
+          <t>dcterms:language:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -3957,7 +3962,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>vra:material:Image0:Thumbnail400x400</t>
+          <t>vra:material:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -4387,7 +4392,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image0:Thumbnail800x800</t>
+          <t>dcterms:medium:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -5677,7 +5682,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image0:Thumbnail600x600</t>
+          <t>dcterms:spatial:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -5892,7 +5897,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image1:Thumbnail400x400</t>
+          <t>dcterms:spatial:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -6107,7 +6112,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image0:Thumbnail400x400</t>
+          <t>dcterms:subject:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
@@ -6322,7 +6327,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image1:Thumbnail600x600</t>
+          <t>dcterms:subject:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
@@ -6537,7 +6542,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>vra:technique:Image0:Thumbnail600x600</t>
+          <t>vra:technique:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
@@ -6752,7 +6757,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>vra:technique:Image1:Thumbnail800x800</t>
+          <t>vra:technique:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
@@ -6967,7 +6972,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>dcterms:title:Image0:Thumbnail600x600</t>
+          <t>dcterms:title:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
@@ -7397,7 +7402,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>dcterms:type:Image0:Thumbnail200x200</t>
+          <t>dcterms:type:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
@@ -7827,7 +7832,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
@@ -8042,7 +8047,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
@@ -8257,7 +8262,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
@@ -8472,7 +8477,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H161" t="inlineStr">
@@ -8687,7 +8692,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H166" t="inlineStr">
@@ -8902,7 +8907,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
@@ -9117,7 +9122,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">
@@ -9332,7 +9337,7 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H181" t="inlineStr">
@@ -9762,7 +9767,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H191" t="inlineStr">
@@ -10192,7 +10197,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H201" t="inlineStr">
@@ -10407,7 +10412,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
@@ -10622,7 +10627,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H211" t="inlineStr">
@@ -11052,7 +11057,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H221" t="inlineStr">
@@ -11267,7 +11272,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
@@ -11482,7 +11487,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
@@ -11697,7 +11702,7 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H236" t="inlineStr">
@@ -11912,7 +11917,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
@@ -12127,7 +12132,7 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H246" t="inlineStr">
@@ -12342,7 +12347,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H251" t="inlineStr">
@@ -12557,7 +12562,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H256" t="inlineStr">
@@ -12987,7 +12992,7 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H266" t="inlineStr">
@@ -13202,7 +13207,7 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H271" t="inlineStr">
@@ -13417,7 +13422,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H276" t="inlineStr">
@@ -13632,7 +13637,7 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H281" t="inlineStr">
@@ -13847,7 +13852,7 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H286" t="inlineStr">
@@ -14062,7 +14067,7 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H291" t="inlineStr">
@@ -14492,7 +14497,7 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H301" t="inlineStr">
@@ -14707,7 +14712,7 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H306" t="inlineStr">
@@ -14922,7 +14927,7 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H311" t="inlineStr">
@@ -15137,7 +15142,7 @@
       </c>
       <c r="G316" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H316" t="inlineStr">
@@ -15567,7 +15572,7 @@
       </c>
       <c r="G326" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H326" t="inlineStr">
@@ -15997,7 +16002,7 @@
       </c>
       <c r="G336" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H336" t="inlineStr">
@@ -16642,7 +16647,7 @@
       </c>
       <c r="G351" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H351" t="inlineStr">
@@ -16857,7 +16862,7 @@
       </c>
       <c r="G356" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H356" t="inlineStr">
@@ -17287,7 +17292,7 @@
       </c>
       <c r="G366" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H366" t="inlineStr">
@@ -17502,7 +17507,7 @@
       </c>
       <c r="G371" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H371" t="inlineStr">
@@ -17717,7 +17722,7 @@
       </c>
       <c r="G376" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H376" t="inlineStr">
@@ -17932,7 +17937,7 @@
       </c>
       <c r="G381" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H381" t="inlineStr">
@@ -18362,7 +18367,7 @@
       </c>
       <c r="G391" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H391" t="inlineStr">
@@ -18577,7 +18582,7 @@
       </c>
       <c r="G396" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H396" t="inlineStr">
@@ -19007,7 +19012,7 @@
       </c>
       <c r="G406" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H406" t="inlineStr">
@@ -19222,7 +19227,7 @@
       </c>
       <c r="G411" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H411" t="inlineStr">
@@ -19652,7 +19657,7 @@
       </c>
       <c r="G421" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H421" t="inlineStr">
@@ -19867,7 +19872,7 @@
       </c>
       <c r="G426" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H426" t="inlineStr">
@@ -20082,7 +20087,7 @@
       </c>
       <c r="G431" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H431" t="inlineStr">
@@ -20512,7 +20517,7 @@
       </c>
       <c r="G441" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H441" t="inlineStr">
@@ -20942,7 +20947,7 @@
       </c>
       <c r="G451" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H451" t="inlineStr">
@@ -21372,7 +21377,7 @@
       </c>
       <c r="G461" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H461" t="inlineStr">
@@ -21587,7 +21592,7 @@
       </c>
       <c r="G466" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H466" t="inlineStr">
@@ -21802,7 +21807,7 @@
       </c>
       <c r="G471" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H471" t="inlineStr">
@@ -22017,7 +22022,7 @@
       </c>
       <c r="G476" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H476" t="inlineStr">
@@ -22232,7 +22237,7 @@
       </c>
       <c r="G481" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H481" t="inlineStr">
@@ -22662,7 +22667,7 @@
       </c>
       <c r="G491" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H491" t="inlineStr">
@@ -22877,7 +22882,7 @@
       </c>
       <c r="G496" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H496" t="inlineStr">
@@ -23092,7 +23097,7 @@
       </c>
       <c r="G501" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H501" t="inlineStr">
@@ -23307,7 +23312,7 @@
       </c>
       <c r="G506" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H506" t="inlineStr">
@@ -23952,7 +23957,7 @@
       </c>
       <c r="G521" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H521" t="inlineStr">
@@ -24167,7 +24172,7 @@
       </c>
       <c r="G526" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H526" t="inlineStr">
@@ -24382,7 +24387,7 @@
       </c>
       <c r="G531" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H531" t="inlineStr">
@@ -24597,7 +24602,7 @@
       </c>
       <c r="G536" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H536" t="inlineStr">
@@ -24812,7 +24817,7 @@
       </c>
       <c r="G541" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H541" t="inlineStr">
@@ -25027,7 +25032,7 @@
       </c>
       <c r="G546" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H546" t="inlineStr">
@@ -25242,7 +25247,7 @@
       </c>
       <c r="G551" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H551" t="inlineStr">
@@ -25457,7 +25462,7 @@
       </c>
       <c r="G556" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H556" t="inlineStr">
@@ -25672,7 +25677,7 @@
       </c>
       <c r="G561" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H561" t="inlineStr">
@@ -25887,7 +25892,7 @@
       </c>
       <c r="G566" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H566" t="inlineStr">
@@ -26102,7 +26107,7 @@
       </c>
       <c r="G571" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H571" t="inlineStr">
@@ -26317,7 +26322,7 @@
       </c>
       <c r="G576" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H576" t="inlineStr">
@@ -26532,7 +26537,7 @@
       </c>
       <c r="G581" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H581" t="inlineStr">
@@ -26747,7 +26752,7 @@
       </c>
       <c r="G586" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H586" t="inlineStr">
@@ -26962,7 +26967,7 @@
       </c>
       <c r="G591" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H591" t="inlineStr">
@@ -27177,7 +27182,7 @@
       </c>
       <c r="G596" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H596" t="inlineStr">
@@ -27392,7 +27397,7 @@
       </c>
       <c r="G601" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H601" t="inlineStr">
@@ -27607,7 +27612,7 @@
       </c>
       <c r="G606" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H606" t="inlineStr">
@@ -28037,7 +28042,7 @@
       </c>
       <c r="G616" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H616" t="inlineStr">
@@ -28252,7 +28257,7 @@
       </c>
       <c r="G621" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H621" t="inlineStr">
@@ -28467,7 +28472,7 @@
       </c>
       <c r="G626" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H626" t="inlineStr">
@@ -28682,7 +28687,7 @@
       </c>
       <c r="G631" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H631" t="inlineStr">
@@ -28897,7 +28902,7 @@
       </c>
       <c r="G636" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H636" t="inlineStr">
@@ -29112,7 +29117,7 @@
       </c>
       <c r="G641" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H641" t="inlineStr">
@@ -29327,7 +29332,7 @@
       </c>
       <c r="G646" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H646" t="inlineStr">
@@ -29542,7 +29547,7 @@
       </c>
       <c r="G651" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H651" t="inlineStr">
@@ -29972,7 +29977,7 @@
       </c>
       <c r="G661" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H661" t="inlineStr">
@@ -30832,7 +30837,7 @@
       </c>
       <c r="G681" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H681" t="inlineStr">
@@ -31047,7 +31052,7 @@
       </c>
       <c r="G686" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H686" t="inlineStr">
@@ -31262,7 +31267,7 @@
       </c>
       <c r="G691" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H691" t="inlineStr">
@@ -31477,7 +31482,7 @@
       </c>
       <c r="G696" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H696" t="inlineStr">
@@ -31692,7 +31697,7 @@
       </c>
       <c r="G701" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H701" t="inlineStr">
@@ -31907,7 +31912,7 @@
       </c>
       <c r="G706" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H706" t="inlineStr">
@@ -32122,7 +32127,7 @@
       </c>
       <c r="G711" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H711" t="inlineStr">
@@ -32767,7 +32772,7 @@
       </c>
       <c r="G726" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H726" t="inlineStr">
@@ -32982,7 +32987,7 @@
       </c>
       <c r="G731" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H731" t="inlineStr">
@@ -33197,7 +33202,7 @@
       </c>
       <c r="G736" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H736" t="inlineStr">
@@ -33412,7 +33417,7 @@
       </c>
       <c r="G741" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H741" t="inlineStr">
@@ -33627,7 +33632,7 @@
       </c>
       <c r="G746" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H746" t="inlineStr">
@@ -33842,7 +33847,7 @@
       </c>
       <c r="G751" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H751" t="inlineStr">
@@ -34057,7 +34062,7 @@
       </c>
       <c r="G756" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H756" t="inlineStr">
@@ -34272,7 +34277,7 @@
       </c>
       <c r="G761" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H761" t="inlineStr">
@@ -34487,7 +34492,7 @@
       </c>
       <c r="G766" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H766" t="inlineStr">
@@ -34702,7 +34707,7 @@
       </c>
       <c r="G771" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H771" t="inlineStr">
@@ -34917,7 +34922,7 @@
       </c>
       <c r="G776" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H776" t="inlineStr">
@@ -35347,7 +35352,7 @@
       </c>
       <c r="G786" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H786" t="inlineStr">
@@ -35777,7 +35782,7 @@
       </c>
       <c r="G796" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H796" t="inlineStr">
@@ -35992,7 +35997,7 @@
       </c>
       <c r="G801" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H801" t="inlineStr">
@@ -36637,7 +36642,7 @@
       </c>
       <c r="G816" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H816" t="inlineStr">
@@ -36852,7 +36857,7 @@
       </c>
       <c r="G821" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H821" t="inlineStr">
@@ -37282,7 +37287,7 @@
       </c>
       <c r="G831" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H831" t="inlineStr">
@@ -37497,7 +37502,7 @@
       </c>
       <c r="G836" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H836" t="inlineStr">
@@ -37712,7 +37717,7 @@
       </c>
       <c r="G841" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H841" t="inlineStr">
@@ -37927,7 +37932,7 @@
       </c>
       <c r="G846" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H846" t="inlineStr">
@@ -38142,7 +38147,7 @@
       </c>
       <c r="G851" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H851" t="inlineStr">
@@ -38357,7 +38362,7 @@
       </c>
       <c r="G856" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H856" t="inlineStr">
@@ -38572,7 +38577,7 @@
       </c>
       <c r="G861" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H861" t="inlineStr">
@@ -39002,7 +39007,7 @@
       </c>
       <c r="G871" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H871" t="inlineStr">
@@ -39217,7 +39222,7 @@
       </c>
       <c r="G876" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H876" t="inlineStr">
@@ -39432,7 +39437,7 @@
       </c>
       <c r="G881" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H881" t="inlineStr">
@@ -39647,7 +39652,7 @@
       </c>
       <c r="G886" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H886" t="inlineStr">
@@ -39862,7 +39867,7 @@
       </c>
       <c r="G891" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H891" t="inlineStr">
@@ -40077,7 +40082,7 @@
       </c>
       <c r="G896" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H896" t="inlineStr">
@@ -40507,7 +40512,7 @@
       </c>
       <c r="G906" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H906" t="inlineStr">
@@ -40722,7 +40727,7 @@
       </c>
       <c r="G911" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H911" t="inlineStr">
@@ -40937,7 +40942,7 @@
       </c>
       <c r="G916" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H916" t="inlineStr">
@@ -41152,7 +41157,7 @@
       </c>
       <c r="G921" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H921" t="inlineStr">
@@ -41582,7 +41587,7 @@
       </c>
       <c r="G931" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H931" t="inlineStr">
@@ -41797,7 +41802,7 @@
       </c>
       <c r="G936" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H936" t="inlineStr">
@@ -42012,7 +42017,7 @@
       </c>
       <c r="G941" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H941" t="inlineStr">
@@ -42442,7 +42447,7 @@
       </c>
       <c r="G951" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H951" t="inlineStr">
@@ -42657,7 +42662,7 @@
       </c>
       <c r="G956" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H956" t="inlineStr">
@@ -42872,7 +42877,7 @@
       </c>
       <c r="G961" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H961" t="inlineStr">
@@ -43087,7 +43092,7 @@
       </c>
       <c r="G966" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H966" t="inlineStr">
@@ -43302,7 +43307,7 @@
       </c>
       <c r="G971" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H971" t="inlineStr">
@@ -43517,7 +43522,7 @@
       </c>
       <c r="G976" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H976" t="inlineStr">
@@ -43732,7 +43737,7 @@
       </c>
       <c r="G981" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H981" t="inlineStr">
@@ -43947,7 +43952,7 @@
       </c>
       <c r="G986" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H986" t="inlineStr">
@@ -44162,7 +44167,7 @@
       </c>
       <c r="G991" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H991" t="inlineStr">
@@ -44592,7 +44597,7 @@
       </c>
       <c r="G1001" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1001" t="inlineStr">
@@ -44807,7 +44812,7 @@
       </c>
       <c r="G1006" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1006" t="inlineStr">
@@ -45022,7 +45027,7 @@
       </c>
       <c r="G1011" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1011" t="inlineStr">
@@ -45237,7 +45242,7 @@
       </c>
       <c r="G1016" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1016" t="inlineStr">
@@ -45452,7 +45457,7 @@
       </c>
       <c r="G1021" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1021" t="inlineStr">
@@ -45667,7 +45672,7 @@
       </c>
       <c r="G1026" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1026" t="inlineStr">
@@ -45882,7 +45887,7 @@
       </c>
       <c r="G1031" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1031" t="inlineStr">
@@ -46097,7 +46102,7 @@
       </c>
       <c r="G1036" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1036" t="inlineStr">
@@ -46312,7 +46317,7 @@
       </c>
       <c r="G1041" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1041" t="inlineStr">
@@ -46527,7 +46532,7 @@
       </c>
       <c r="G1046" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1046" t="inlineStr">
@@ -46742,7 +46747,7 @@
       </c>
       <c r="G1051" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1051" t="inlineStr">
@@ -46957,7 +46962,7 @@
       </c>
       <c r="G1056" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1056" t="inlineStr">
@@ -47172,7 +47177,7 @@
       </c>
       <c r="G1061" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1061" t="inlineStr">
@@ -47387,7 +47392,7 @@
       </c>
       <c r="G1066" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1066" t="inlineStr">
@@ -47602,7 +47607,7 @@
       </c>
       <c r="G1071" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1071" t="inlineStr">
@@ -47817,7 +47822,7 @@
       </c>
       <c r="G1076" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1076" t="inlineStr">
@@ -48032,7 +48037,7 @@
       </c>
       <c r="G1081" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1081" t="inlineStr">
@@ -48247,7 +48252,7 @@
       </c>
       <c r="G1086" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1086" t="inlineStr">
@@ -48462,7 +48467,7 @@
       </c>
       <c r="G1091" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1091" t="inlineStr">
@@ -48892,7 +48897,7 @@
       </c>
       <c r="G1101" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1101" t="inlineStr">
@@ -49537,7 +49542,7 @@
       </c>
       <c r="G1116" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1116" t="inlineStr">
@@ -50397,7 +50402,7 @@
       </c>
       <c r="G1136" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1136" t="inlineStr">
@@ -50612,7 +50617,7 @@
       </c>
       <c r="G1141" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1141" t="inlineStr">
@@ -50827,7 +50832,7 @@
       </c>
       <c r="G1146" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1146" t="inlineStr">
@@ -51042,7 +51047,7 @@
       </c>
       <c r="G1151" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1151" t="inlineStr">
@@ -51257,7 +51262,7 @@
       </c>
       <c r="G1156" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1156" t="inlineStr">
@@ -51472,7 +51477,7 @@
       </c>
       <c r="G1161" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1161" t="inlineStr">
@@ -51687,7 +51692,7 @@
       </c>
       <c r="G1166" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1166" t="inlineStr">
@@ -52332,7 +52337,7 @@
       </c>
       <c r="G1181" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1181" t="inlineStr">
@@ -52547,7 +52552,7 @@
       </c>
       <c r="G1186" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1186" t="inlineStr">
@@ -52762,7 +52767,7 @@
       </c>
       <c r="G1191" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1191" t="inlineStr">
@@ -52977,7 +52982,7 @@
       </c>
       <c r="G1196" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1196" t="inlineStr">
@@ -53192,7 +53197,7 @@
       </c>
       <c r="G1201" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1201" t="inlineStr">
@@ -53407,7 +53412,7 @@
       </c>
       <c r="G1206" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1206" t="inlineStr">
@@ -53622,7 +53627,7 @@
       </c>
       <c r="G1211" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1211" t="inlineStr">
@@ -54052,7 +54057,7 @@
       </c>
       <c r="G1221" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1221" t="inlineStr">
@@ -54267,7 +54272,7 @@
       </c>
       <c r="G1226" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1226" t="inlineStr">
@@ -54482,7 +54487,7 @@
       </c>
       <c r="G1231" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1231" t="inlineStr">
@@ -55127,7 +55132,7 @@
       </c>
       <c r="G1246" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization0:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1246" t="inlineStr">
@@ -55342,7 +55347,7 @@
       </c>
       <c r="G1251" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image1:Thumbnail600x600</t>
+          <t>http://example.com/organization0:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1251" t="inlineStr">
@@ -55557,7 +55562,7 @@
       </c>
       <c r="G1256" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization1:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1256" t="inlineStr">
@@ -55772,7 +55777,7 @@
       </c>
       <c r="G1261" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image1:Thumbnail600x600</t>
+          <t>http://example.com/organization1:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1261" t="inlineStr">
@@ -55987,7 +55992,7 @@
       </c>
       <c r="G1266" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0:Thumbnail600x600</t>
+          <t>http://example.com/organization2:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1266" t="inlineStr">
@@ -56202,7 +56207,7 @@
       </c>
       <c r="G1271" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image1:Thumbnail200x200</t>
+          <t>http://example.com/organization2:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1271" t="inlineStr">
@@ -56417,7 +56422,7 @@
       </c>
       <c r="G1276" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image0:Thumbnail800x800</t>
+          <t>http://example.com/organization3:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1276" t="inlineStr">
@@ -57062,7 +57067,7 @@
       </c>
       <c r="G1291" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image1:Thumbnail600x600</t>
+          <t>http://example.com/organization4:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1291" t="inlineStr">
@@ -57277,7 +57282,7 @@
       </c>
       <c r="G1296" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image0:Thumbnail400x400</t>
+          <t>http://example.com/person0:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1296" t="inlineStr">
@@ -57954,7 +57959,7 @@
       </c>
       <c r="G1312" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image1:Thumbnail400x400</t>
+          <t>http://example.com/person1:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1312" t="inlineStr">
@@ -58169,7 +58174,7 @@
       </c>
       <c r="G1317" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image0:Thumbnail800x800</t>
+          <t>http://example.com/person2:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1317" t="inlineStr">
@@ -58384,7 +58389,7 @@
       </c>
       <c r="G1322" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image1:Thumbnail600x600</t>
+          <t>http://example.com/person2:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1322" t="inlineStr">
@@ -58599,7 +58604,7 @@
       </c>
       <c r="G1327" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0:Thumbnail800x800</t>
+          <t>http://example.com/person3:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1327" t="inlineStr">
@@ -58814,7 +58819,7 @@
       </c>
       <c r="G1332" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image1:Thumbnail400x400</t>
+          <t>http://example.com/person3:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1332" t="inlineStr">
@@ -59244,7 +59249,7 @@
       </c>
       <c r="G1342" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image1:Thumbnail200x200</t>
+          <t>http://example.com/person4:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1342" t="inlineStr">
@@ -59674,7 +59679,7 @@
       </c>
       <c r="G1352" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0:Image1:Thumbnail400x400</t>
+          <t>http://example.com/collection0/work0:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1352" t="inlineStr">
@@ -59926,7 +59931,7 @@
       </c>
       <c r="G1358" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work1:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1358" t="inlineStr">
@@ -60356,7 +60361,7 @@
       </c>
       <c r="G1368" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work2:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1368" t="inlineStr">
@@ -60786,7 +60791,7 @@
       </c>
       <c r="G1378" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image0:Thumbnail600x600</t>
+          <t>http://example.com/collection0/work3:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1378" t="inlineStr">
@@ -61001,7 +61006,7 @@
       </c>
       <c r="G1383" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image1:Thumbnail400x400</t>
+          <t>http://example.com/collection0/work3:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1383" t="inlineStr">
@@ -61216,7 +61221,7 @@
       </c>
       <c r="G1388" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection1:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1388" t="inlineStr">
@@ -61431,7 +61436,7 @@
       </c>
       <c r="G1393" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image1:Thumbnail600x600</t>
+          <t>http://example.com/collection1:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1393" t="inlineStr">
@@ -61646,7 +61651,7 @@
       </c>
       <c r="G1398" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4:Image0:Thumbnail400x400</t>
+          <t>http://example.com/collection1/work4:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1398" t="inlineStr">
@@ -61861,7 +61866,7 @@
       </c>
       <c r="G1403" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4:Image1:Thumbnail600x600</t>
+          <t>http://example.com/collection1/work4:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1403" t="inlineStr">
@@ -62291,7 +62296,7 @@
       </c>
       <c r="G1413" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:Image1:Thumbnail200x200</t>
+          <t>http://example.com/collection1/work5:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1413" t="inlineStr">
@@ -62506,7 +62511,7 @@
       </c>
       <c r="G1418" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6:Image0:Thumbnail800x800</t>
+          <t>http://example.com/collection1/work6:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1418" t="inlineStr">
@@ -62721,7 +62726,7 @@
       </c>
       <c r="G1423" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6:Image1:Thumbnail600x600</t>
+          <t>http://example.com/collection1/work6:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1423" t="inlineStr">
@@ -62936,7 +62941,7 @@
       </c>
       <c r="G1428" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image0:Thumbnail800x800</t>
+          <t>http://example.com/collection1/work7:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1428" t="inlineStr">
@@ -63366,7 +63371,7 @@
       </c>
       <c r="G1438" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8:Image0:Thumbnail800x800</t>
+          <t>http://example.com/freestandingwork8:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1438" t="inlineStr">
@@ -63581,7 +63586,7 @@
       </c>
       <c r="G1443" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8:Image1:Thumbnail400x400</t>
+          <t>http://example.com/freestandingwork8:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1443" t="inlineStr">
@@ -64011,7 +64016,7 @@
       </c>
       <c r="G1453" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:Image1:Thumbnail400x400</t>
+          <t>http://example.com/freestandingwork9:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1453" t="inlineStr">
@@ -64226,7 +64231,7 @@
       </c>
       <c r="G1458" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10:Image0:Thumbnail800x800</t>
+          <t>http://example.com/freestandingwork10:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1458" t="inlineStr">
@@ -64656,7 +64661,7 @@
       </c>
       <c r="G1468" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:Image0:Thumbnail400x400</t>
+          <t>http://example.com/freestandingwork11:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1468" t="inlineStr">
@@ -64949,7 +64954,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>vra:culturalContext:Image1:Thumbnail800x800</t>
+          <t>vra:culturalContext:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -64981,7 +64986,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dcterms:description:Image0:Thumbnail400x400</t>
+          <t>dcterms:description:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -65013,7 +65018,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0:Thumbnail800x800</t>
+          <t>dcterms:extent:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -65045,7 +65050,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dcterms:language:Image1:Thumbnail400x400</t>
+          <t>dcterms:language:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -65077,7 +65082,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>vra:material:Image0:Thumbnail400x400</t>
+          <t>vra:material:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -65109,7 +65114,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image0</t>
+          <t>dcterms:medium:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -65173,7 +65178,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>dcterms:source:Image0</t>
+          <t>dcterms:source:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -65205,7 +65210,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image0</t>
+          <t>dcterms:spatial:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -65237,7 +65242,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image1:Thumbnail200x200</t>
+          <t>dcterms:subject:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -65269,7 +65274,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>vra:technique:Image0:Thumbnail600x600</t>
+          <t>vra:technique:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -65301,7 +65306,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>dcterms:title:Image0</t>
+          <t>dcterms:title:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -65333,7 +65338,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>dcterms:type:Image0:Thumbnail600x600</t>
+          <t>dcterms:type:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -65402,7 +65407,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -65460,7 +65465,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -65482,7 +65487,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -65504,7 +65509,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -65526,7 +65531,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -65548,7 +65553,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -65570,7 +65575,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -65592,7 +65597,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -65614,7 +65619,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -65702,7 +65707,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -65724,7 +65729,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -65746,7 +65751,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -65768,7 +65773,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -65834,7 +65839,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -65856,7 +65861,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -65878,7 +65883,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -65900,7 +65905,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -65922,7 +65927,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -65944,7 +65949,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -65966,7 +65971,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -65988,7 +65993,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -66010,7 +66015,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -66032,7 +66037,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -66054,7 +66059,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -66098,7 +66103,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -66120,7 +66125,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -66142,7 +66147,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -66164,7 +66169,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -66186,7 +66191,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -66208,7 +66213,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -66230,7 +66235,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -66252,7 +66257,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -66274,7 +66279,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -66296,7 +66301,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -66318,7 +66323,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -66340,7 +66345,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -66362,7 +66367,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -66384,7 +66389,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -66406,7 +66411,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -66428,7 +66433,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -66450,7 +66455,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -66472,7 +66477,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -66494,7 +66499,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -66516,7 +66521,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -66538,7 +66543,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -66560,7 +66565,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -66582,7 +66587,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -66604,7 +66609,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -66626,7 +66631,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -66648,7 +66653,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -66692,7 +66697,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -66714,7 +66719,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -66758,7 +66763,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -66802,7 +66807,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -66824,7 +66829,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -66846,7 +66851,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -66868,7 +66873,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -66890,7 +66895,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -66956,7 +66961,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -66978,7 +66983,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -67000,7 +67005,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image1</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -67022,7 +67027,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -67044,7 +67049,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -67066,7 +67071,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -67088,7 +67093,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -67132,7 +67137,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -67154,7 +67159,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -67176,7 +67181,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -67198,7 +67203,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -67220,7 +67225,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -67242,7 +67247,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -67264,7 +67269,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -67286,7 +67291,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -67330,7 +67335,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -67352,7 +67357,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -67396,7 +67401,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -67418,7 +67423,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -67440,7 +67445,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -67462,7 +67467,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -67484,7 +67489,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image1</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -67506,7 +67511,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -67528,7 +67533,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image1</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -67550,7 +67555,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -67594,7 +67599,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -67616,7 +67621,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -67638,7 +67643,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -67660,7 +67665,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -67704,7 +67709,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -67726,7 +67731,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -67748,7 +67753,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -67770,7 +67775,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -67792,7 +67797,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image0</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -67814,7 +67819,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -67836,7 +67841,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -67858,7 +67863,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image0</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -67921,7 +67926,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0:Thumbnail200x200</t>
+          <t>http://example.com/organization0:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -67939,7 +67944,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image1:Thumbnail400x400</t>
+          <t>http://example.com/organization1:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -67957,7 +67962,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0:Thumbnail600x600</t>
+          <t>http://example.com/organization2:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -67993,7 +67998,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0:Thumbnail800x800</t>
+          <t>http://example.com/organization4:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -68065,14 +68070,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
+          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
+          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
regenerate synthetic data with NCSU resolved
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -21,7 +21,8 @@
     <sheet name="CmsWorkCreation" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="CmsWorkOpening" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="CmsWork" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="SchemaCollection" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="SchemaCreativeWork" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="SchemaCollection" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -508,7 +509,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image1:Thumbnail400x400</t>
+          <t>http://example.com/person0:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -541,7 +542,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image0:Thumbnail400x400</t>
+          <t>http://example.com/person1:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -596,7 +597,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0</t>
+          <t>http://example.com/person3:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -623,7 +624,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image0:Thumbnail600x600</t>
+          <t>http://example.com/person4:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -886,7 +887,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N7b1e5e5f61c249ce947f836bae94d708</t>
+          <t>_:Nebf60f75571849d1890e1f05207ceaf7</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -904,7 +905,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N6251f3ba129743acbdfb02b7f3748d12</t>
+          <t>_:N8c1783b4dfe446a78a5d9c92a809f04d</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -922,7 +923,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:Nc18fdcbaa2f544cb829b4f21997b0c49</t>
+          <t>_:N29d5f9d6a7414504bae40eb5819a8323</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -940,7 +941,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N2c2badeb39424532a523eda50f82a976</t>
+          <t>_:Nbe9dbfaa2a3c4b6bb9fa9d5fd1506381</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -958,7 +959,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:N1651b1019c374db9afc43e8a520272a9</t>
+          <t>_:N6cd9cc734d004ca7a03d8caf2cfe0e6a</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -976,7 +977,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:N40f268c129794ec2bb38ced8832064fe</t>
+          <t>_:N0d5a75bb491043cf9d2d7422478332c7</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1019,17 +1020,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>_:N424edfef4d2c4114a238452c5c16953d</t>
+          <t>_:Nef730a3bb21d4b03a2795c92b999e9ec</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://example.com/organization4</t>
+          <t>http://example.com/organization3</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Collection0Work1 alternative title 1</t>
+          <t>Collection0Work1 alternative title 0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -1042,7 +1043,7 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Collection0Work1 provenance 1</t>
+          <t>Collection0Work1 provenance 0</t>
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
@@ -1050,12 +1051,12 @@
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>_:Ne7510d048a224db0985773cfb8bc0af4</t>
+          <t>http://example.com/collection0/work1Opening</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image1:Thumbnail600x600</t>
+          <t>http://example.com/collection0/work1:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -1090,7 +1091,7 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
         </is>
       </c>
       <c r="V2" t="inlineStr"/>
@@ -1105,12 +1106,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>_:Ne5b76b56abe1409facce98cb9a53f12b</t>
+          <t>_:Nd772a7b207ca423f9db36eedfea5d314</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://example.com/person0</t>
+          <t>http://example.com/person1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1136,7 +1137,7 @@
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3Creation</t>
+          <t>_:N1e8d5d55bc794c4fbd9ca01c4b11b021</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -1171,7 +1172,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103</t>
         </is>
       </c>
       <c r="U3" t="inlineStr"/>
@@ -1186,12 +1187,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>_:N9f30581ec49b4ce2bf752745c10aa807</t>
+          <t>_:N816a291b75784a84a6d94a4a19b4c5d5</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>http://example.com/person2</t>
+          <t>http://example.com/person3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1202,7 +1203,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Collection1Work5Id1</t>
+          <t>Collection1Work5Id0</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -1217,12 +1218,12 @@
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
-          <t>_:N487dbcb83bac44819b1f846bff5b4748</t>
+          <t>http://example.com/collection1/work5Opening</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:Image0:Thumbnail600x600</t>
+          <t>http://example.com/collection1/work5:Image0</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -1252,7 +1253,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106</t>
         </is>
       </c>
       <c r="U4" t="inlineStr"/>
@@ -1267,7 +1268,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>_:N940c399b3bd64f35947784159521dc30</t>
+          <t>_:N3f70a425cff84f7a9c6af1112acb4b62</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1298,12 +1299,12 @@
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7Creation</t>
+          <t>http://example.com/collection1/work7Opening</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image1:Thumbnail400x400</t>
+          <t>http://example.com/collection1/work7:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1333,7 +1334,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107</t>
         </is>
       </c>
       <c r="U5" t="inlineStr"/>
@@ -1348,17 +1349,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>_:N674da56f87bc4c1ea69388fa3e5c345c</t>
+          <t>_:N176bcf49c25945579348d710c7fcbabc</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>http://example.com/organization1</t>
+          <t>http://example.com/organization2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 alternative title 1</t>
+          <t>FreestandingWork9 alternative title 0</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1379,12 +1380,12 @@
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr">
         <is>
-          <t>_:Nbffae5cdc8804553ad78526757cfa494</t>
+          <t>http://example.com/freestandingwork9Creation</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:Image0:Thumbnail200x200</t>
+          <t>http://example.com/freestandingwork9:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -1414,7 +1415,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100</t>
         </is>
       </c>
       <c r="U6" t="inlineStr"/>
@@ -1429,7 +1430,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>_:N2487adb27377414d9df62d6ffac62ef5</t>
+          <t>_:N56c6602e30cf46c5adc693b75ce1d1fb</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1439,20 +1440,20 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>FreestandingWork11 alternative title 1</t>
+          <t>FreestandingWork11 alternative title 0</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>FreestandingWork11Id1</t>
+          <t>FreestandingWork11Id0</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>FreestandingWork11 provenance 1</t>
+          <t>FreestandingWork11 provenance 0</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
@@ -1460,12 +1461,12 @@
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11Creation</t>
+          <t>http://example.com/freestandingwork11Opening</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:Image0:Thumbnail400x400</t>
+          <t>http://example.com/freestandingwork11:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -1495,7 +1496,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
         </is>
       </c>
       <c r="U7" t="inlineStr"/>
@@ -1508,6 +1509,32 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>@graph</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1536,12 +1563,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6</t>
+          <t>http://example.com/collection1/work5</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image0:Thumbnail800x800</t>
+          <t>http://example.com/collection1:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1812,7 +1839,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -2027,7 +2054,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -2242,7 +2269,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>vra:culturalContext:Image0:Thumbnail400x400</t>
+          <t>vra:culturalContext:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -2457,7 +2484,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>vra:culturalContext:Image1:Thumbnail400x400</t>
+          <t>vra:culturalContext:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -2887,7 +2914,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>dcterms:description:Image1:Thumbnail800x800</t>
+          <t>dcterms:description:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -3102,7 +3129,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0:Thumbnail200x200</t>
+          <t>dcterms:extent:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -3317,7 +3344,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image1:Thumbnail600x600</t>
+          <t>dcterms:extent:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -3747,7 +3774,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>dcterms:language:Image1:Thumbnail800x800</t>
+          <t>dcterms:language:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -3962,7 +3989,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>vra:material:Image0:Thumbnail200x200</t>
+          <t>vra:material:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -4177,7 +4204,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>vra:material:Image1:Thumbnail200x200</t>
+          <t>vra:material:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -4392,7 +4419,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image0:Thumbnail600x600</t>
+          <t>dcterms:medium:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -5252,7 +5279,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>dcterms:source:Image0:Thumbnail200x200</t>
+          <t>dcterms:source:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -5467,7 +5494,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>dcterms:source:Image1:Thumbnail400x400</t>
+          <t>dcterms:source:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
@@ -5682,7 +5709,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image0:Thumbnail400x400</t>
+          <t>dcterms:spatial:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -5897,7 +5924,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image1:Thumbnail600x600</t>
+          <t>dcterms:spatial:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -6112,7 +6139,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image0:Thumbnail600x600</t>
+          <t>dcterms:subject:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
@@ -6327,7 +6354,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image1:Thumbnail200x200</t>
+          <t>dcterms:subject:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
@@ -6542,7 +6569,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>vra:technique:Image0:Thumbnail800x800</t>
+          <t>vra:technique:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
@@ -6757,7 +6784,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>vra:technique:Image1:Thumbnail400x400</t>
+          <t>vra:technique:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
@@ -6972,7 +6999,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>dcterms:title:Image0:Thumbnail800x800</t>
+          <t>dcterms:title:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
@@ -7187,7 +7214,7 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>dcterms:title:Image1:Thumbnail600x600</t>
+          <t>dcterms:title:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
@@ -7402,7 +7429,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>dcterms:type:Image0:Thumbnail400x400</t>
+          <t>dcterms:type:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
@@ -7832,7 +7859,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
@@ -8047,7 +8074,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
@@ -8262,7 +8289,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
@@ -8477,7 +8504,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H161" t="inlineStr">
@@ -8907,7 +8934,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
@@ -9122,7 +9149,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">
@@ -9767,7 +9794,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H191" t="inlineStr">
@@ -10197,7 +10224,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H201" t="inlineStr">
@@ -10412,7 +10439,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
@@ -10627,7 +10654,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H211" t="inlineStr">
@@ -11487,7 +11514,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
@@ -11917,7 +11944,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
@@ -12132,7 +12159,7 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H246" t="inlineStr">
@@ -12347,7 +12374,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H251" t="inlineStr">
@@ -12562,7 +12589,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H256" t="inlineStr">
@@ -12777,7 +12804,7 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H261" t="inlineStr">
@@ -12992,7 +13019,7 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H266" t="inlineStr">
@@ -13207,7 +13234,7 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H271" t="inlineStr">
@@ -13422,7 +13449,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H276" t="inlineStr">
@@ -13637,7 +13664,7 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H281" t="inlineStr">
@@ -13852,7 +13879,7 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H286" t="inlineStr">
@@ -14067,7 +14094,7 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H291" t="inlineStr">
@@ -14282,7 +14309,7 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H296" t="inlineStr">
@@ -14497,7 +14524,7 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H301" t="inlineStr">
@@ -14712,7 +14739,7 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H306" t="inlineStr">
@@ -15142,7 +15169,7 @@
       </c>
       <c r="G316" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H316" t="inlineStr">
@@ -15357,7 +15384,7 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H321" t="inlineStr">
@@ -15572,7 +15599,7 @@
       </c>
       <c r="G326" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H326" t="inlineStr">
@@ -15787,7 +15814,7 @@
       </c>
       <c r="G331" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H331" t="inlineStr">
@@ -16002,7 +16029,7 @@
       </c>
       <c r="G336" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H336" t="inlineStr">
@@ -16217,7 +16244,7 @@
       </c>
       <c r="G341" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H341" t="inlineStr">
@@ -16432,7 +16459,7 @@
       </c>
       <c r="G346" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H346" t="inlineStr">
@@ -16647,7 +16674,7 @@
       </c>
       <c r="G351" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H351" t="inlineStr">
@@ -16862,7 +16889,7 @@
       </c>
       <c r="G356" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H356" t="inlineStr">
@@ -17077,7 +17104,7 @@
       </c>
       <c r="G361" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H361" t="inlineStr">
@@ -17507,7 +17534,7 @@
       </c>
       <c r="G371" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H371" t="inlineStr">
@@ -17722,7 +17749,7 @@
       </c>
       <c r="G376" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H376" t="inlineStr">
@@ -17937,7 +17964,7 @@
       </c>
       <c r="G381" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H381" t="inlineStr">
@@ -18367,7 +18394,7 @@
       </c>
       <c r="G391" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H391" t="inlineStr">
@@ -18797,7 +18824,7 @@
       </c>
       <c r="G401" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H401" t="inlineStr">
@@ -19012,7 +19039,7 @@
       </c>
       <c r="G406" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H406" t="inlineStr">
@@ -19227,7 +19254,7 @@
       </c>
       <c r="G411" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H411" t="inlineStr">
@@ -19442,7 +19469,7 @@
       </c>
       <c r="G416" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H416" t="inlineStr">
@@ -19657,7 +19684,7 @@
       </c>
       <c r="G421" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H421" t="inlineStr">
@@ -19872,7 +19899,7 @@
       </c>
       <c r="G426" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H426" t="inlineStr">
@@ -20087,7 +20114,7 @@
       </c>
       <c r="G431" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H431" t="inlineStr">
@@ -20302,7 +20329,7 @@
       </c>
       <c r="G436" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H436" t="inlineStr">
@@ -20517,7 +20544,7 @@
       </c>
       <c r="G441" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H441" t="inlineStr">
@@ -20732,7 +20759,7 @@
       </c>
       <c r="G446" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H446" t="inlineStr">
@@ -20947,7 +20974,7 @@
       </c>
       <c r="G451" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H451" t="inlineStr">
@@ -21162,7 +21189,7 @@
       </c>
       <c r="G456" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H456" t="inlineStr">
@@ -21377,7 +21404,7 @@
       </c>
       <c r="G461" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H461" t="inlineStr">
@@ -21592,7 +21619,7 @@
       </c>
       <c r="G466" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H466" t="inlineStr">
@@ -22022,7 +22049,7 @@
       </c>
       <c r="G476" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H476" t="inlineStr">
@@ -22237,7 +22264,7 @@
       </c>
       <c r="G481" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H481" t="inlineStr">
@@ -22452,7 +22479,7 @@
       </c>
       <c r="G486" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H486" t="inlineStr">
@@ -22667,7 +22694,7 @@
       </c>
       <c r="G491" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H491" t="inlineStr">
@@ -22882,7 +22909,7 @@
       </c>
       <c r="G496" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H496" t="inlineStr">
@@ -23097,7 +23124,7 @@
       </c>
       <c r="G501" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H501" t="inlineStr">
@@ -23312,7 +23339,7 @@
       </c>
       <c r="G506" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H506" t="inlineStr">
@@ -23527,7 +23554,7 @@
       </c>
       <c r="G511" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H511" t="inlineStr">
@@ -23957,7 +23984,7 @@
       </c>
       <c r="G521" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H521" t="inlineStr">
@@ -24602,7 +24629,7 @@
       </c>
       <c r="G536" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H536" t="inlineStr">
@@ -24817,7 +24844,7 @@
       </c>
       <c r="G541" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H541" t="inlineStr">
@@ -25032,7 +25059,7 @@
       </c>
       <c r="G546" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H546" t="inlineStr">
@@ -25247,7 +25274,7 @@
       </c>
       <c r="G551" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H551" t="inlineStr">
@@ -25462,7 +25489,7 @@
       </c>
       <c r="G556" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H556" t="inlineStr">
@@ -25677,7 +25704,7 @@
       </c>
       <c r="G561" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H561" t="inlineStr">
@@ -25892,7 +25919,7 @@
       </c>
       <c r="G566" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H566" t="inlineStr">
@@ -26107,7 +26134,7 @@
       </c>
       <c r="G571" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H571" t="inlineStr">
@@ -26322,7 +26349,7 @@
       </c>
       <c r="G576" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H576" t="inlineStr">
@@ -26537,7 +26564,7 @@
       </c>
       <c r="G581" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H581" t="inlineStr">
@@ -26752,7 +26779,7 @@
       </c>
       <c r="G586" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H586" t="inlineStr">
@@ -26967,7 +26994,7 @@
       </c>
       <c r="G591" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H591" t="inlineStr">
@@ -27182,7 +27209,7 @@
       </c>
       <c r="G596" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H596" t="inlineStr">
@@ -27397,7 +27424,7 @@
       </c>
       <c r="G601" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H601" t="inlineStr">
@@ -27612,7 +27639,7 @@
       </c>
       <c r="G606" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H606" t="inlineStr">
@@ -27827,7 +27854,7 @@
       </c>
       <c r="G611" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H611" t="inlineStr">
@@ -28042,7 +28069,7 @@
       </c>
       <c r="G616" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H616" t="inlineStr">
@@ -28257,7 +28284,7 @@
       </c>
       <c r="G621" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H621" t="inlineStr">
@@ -28902,7 +28929,7 @@
       </c>
       <c r="G636" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H636" t="inlineStr">
@@ -29117,7 +29144,7 @@
       </c>
       <c r="G641" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H641" t="inlineStr">
@@ -29332,7 +29359,7 @@
       </c>
       <c r="G646" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H646" t="inlineStr">
@@ -29547,7 +29574,7 @@
       </c>
       <c r="G651" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H651" t="inlineStr">
@@ -29977,7 +30004,7 @@
       </c>
       <c r="G661" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H661" t="inlineStr">
@@ -30192,7 +30219,7 @@
       </c>
       <c r="G666" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H666" t="inlineStr">
@@ -30407,7 +30434,7 @@
       </c>
       <c r="G671" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H671" t="inlineStr">
@@ -30622,7 +30649,7 @@
       </c>
       <c r="G676" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H676" t="inlineStr">
@@ -30837,7 +30864,7 @@
       </c>
       <c r="G681" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H681" t="inlineStr">
@@ -31267,7 +31294,7 @@
       </c>
       <c r="G691" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H691" t="inlineStr">
@@ -31482,7 +31509,7 @@
       </c>
       <c r="G696" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H696" t="inlineStr">
@@ -31912,7 +31939,7 @@
       </c>
       <c r="G706" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H706" t="inlineStr">
@@ -32127,7 +32154,7 @@
       </c>
       <c r="G711" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H711" t="inlineStr">
@@ -32557,7 +32584,7 @@
       </c>
       <c r="G721" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H721" t="inlineStr">
@@ -32772,7 +32799,7 @@
       </c>
       <c r="G726" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H726" t="inlineStr">
@@ -32987,7 +33014,7 @@
       </c>
       <c r="G731" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H731" t="inlineStr">
@@ -33202,7 +33229,7 @@
       </c>
       <c r="G736" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H736" t="inlineStr">
@@ -33417,7 +33444,7 @@
       </c>
       <c r="G741" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H741" t="inlineStr">
@@ -33632,7 +33659,7 @@
       </c>
       <c r="G746" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H746" t="inlineStr">
@@ -33847,7 +33874,7 @@
       </c>
       <c r="G751" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H751" t="inlineStr">
@@ -34062,7 +34089,7 @@
       </c>
       <c r="G756" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H756" t="inlineStr">
@@ -34277,7 +34304,7 @@
       </c>
       <c r="G761" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H761" t="inlineStr">
@@ -34492,7 +34519,7 @@
       </c>
       <c r="G766" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H766" t="inlineStr">
@@ -34707,7 +34734,7 @@
       </c>
       <c r="G771" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H771" t="inlineStr">
@@ -35137,7 +35164,7 @@
       </c>
       <c r="G781" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H781" t="inlineStr">
@@ -35352,7 +35379,7 @@
       </c>
       <c r="G786" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H786" t="inlineStr">
@@ -35567,7 +35594,7 @@
       </c>
       <c r="G791" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H791" t="inlineStr">
@@ -35782,7 +35809,7 @@
       </c>
       <c r="G796" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H796" t="inlineStr">
@@ -36427,7 +36454,7 @@
       </c>
       <c r="G811" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H811" t="inlineStr">
@@ -36642,7 +36669,7 @@
       </c>
       <c r="G816" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H816" t="inlineStr">
@@ -36857,7 +36884,7 @@
       </c>
       <c r="G821" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H821" t="inlineStr">
@@ -37717,7 +37744,7 @@
       </c>
       <c r="G841" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H841" t="inlineStr">
@@ -38362,7 +38389,7 @@
       </c>
       <c r="G856" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H856" t="inlineStr">
@@ -38577,7 +38604,7 @@
       </c>
       <c r="G861" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H861" t="inlineStr">
@@ -38792,7 +38819,7 @@
       </c>
       <c r="G866" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H866" t="inlineStr">
@@ -39652,7 +39679,7 @@
       </c>
       <c r="G886" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H886" t="inlineStr">
@@ -39867,7 +39894,7 @@
       </c>
       <c r="G891" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H891" t="inlineStr">
@@ -40082,7 +40109,7 @@
       </c>
       <c r="G896" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H896" t="inlineStr">
@@ -40297,7 +40324,7 @@
       </c>
       <c r="G901" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H901" t="inlineStr">
@@ -40727,7 +40754,7 @@
       </c>
       <c r="G911" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H911" t="inlineStr">
@@ -41157,7 +41184,7 @@
       </c>
       <c r="G921" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H921" t="inlineStr">
@@ -41372,7 +41399,7 @@
       </c>
       <c r="G926" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H926" t="inlineStr">
@@ -41802,7 +41829,7 @@
       </c>
       <c r="G936" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H936" t="inlineStr">
@@ -42017,7 +42044,7 @@
       </c>
       <c r="G941" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H941" t="inlineStr">
@@ -42232,7 +42259,7 @@
       </c>
       <c r="G946" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H946" t="inlineStr">
@@ -42447,7 +42474,7 @@
       </c>
       <c r="G951" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H951" t="inlineStr">
@@ -42877,7 +42904,7 @@
       </c>
       <c r="G961" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H961" t="inlineStr">
@@ -43522,7 +43549,7 @@
       </c>
       <c r="G976" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H976" t="inlineStr">
@@ -43737,7 +43764,7 @@
       </c>
       <c r="G981" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H981" t="inlineStr">
@@ -43952,7 +43979,7 @@
       </c>
       <c r="G986" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H986" t="inlineStr">
@@ -44382,7 +44409,7 @@
       </c>
       <c r="G996" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H996" t="inlineStr">
@@ -44597,7 +44624,7 @@
       </c>
       <c r="G1001" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1001" t="inlineStr">
@@ -44812,7 +44839,7 @@
       </c>
       <c r="G1006" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1006" t="inlineStr">
@@ -45027,7 +45054,7 @@
       </c>
       <c r="G1011" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1011" t="inlineStr">
@@ -45242,7 +45269,7 @@
       </c>
       <c r="G1016" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1016" t="inlineStr">
@@ -45457,7 +45484,7 @@
       </c>
       <c r="G1021" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1021" t="inlineStr">
@@ -45672,7 +45699,7 @@
       </c>
       <c r="G1026" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1026" t="inlineStr">
@@ -46317,7 +46344,7 @@
       </c>
       <c r="G1041" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1041" t="inlineStr">
@@ -46532,7 +46559,7 @@
       </c>
       <c r="G1046" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1046" t="inlineStr">
@@ -46747,7 +46774,7 @@
       </c>
       <c r="G1051" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1051" t="inlineStr">
@@ -47177,7 +47204,7 @@
       </c>
       <c r="G1061" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1061" t="inlineStr">
@@ -47392,7 +47419,7 @@
       </c>
       <c r="G1066" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1066" t="inlineStr">
@@ -47607,7 +47634,7 @@
       </c>
       <c r="G1071" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1071" t="inlineStr">
@@ -47822,7 +47849,7 @@
       </c>
       <c r="G1076" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1076" t="inlineStr">
@@ -48682,7 +48709,7 @@
       </c>
       <c r="G1096" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1096" t="inlineStr">
@@ -48897,7 +48924,7 @@
       </c>
       <c r="G1101" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1101" t="inlineStr">
@@ -49112,7 +49139,7 @@
       </c>
       <c r="G1106" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1106" t="inlineStr">
@@ -49327,7 +49354,7 @@
       </c>
       <c r="G1111" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1111" t="inlineStr">
@@ -49542,7 +49569,7 @@
       </c>
       <c r="G1116" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1116" t="inlineStr">
@@ -49757,7 +49784,7 @@
       </c>
       <c r="G1121" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1121" t="inlineStr">
@@ -50402,7 +50429,7 @@
       </c>
       <c r="G1136" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1136" t="inlineStr">
@@ -50832,7 +50859,7 @@
       </c>
       <c r="G1146" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1146" t="inlineStr">
@@ -51047,7 +51074,7 @@
       </c>
       <c r="G1151" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1151" t="inlineStr">
@@ -51477,7 +51504,7 @@
       </c>
       <c r="G1161" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1161" t="inlineStr">
@@ -51692,7 +51719,7 @@
       </c>
       <c r="G1166" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1166" t="inlineStr">
@@ -51907,7 +51934,7 @@
       </c>
       <c r="G1171" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1171" t="inlineStr">
@@ -52122,7 +52149,7 @@
       </c>
       <c r="G1176" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1176" t="inlineStr">
@@ -52337,7 +52364,7 @@
       </c>
       <c r="G1181" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1181" t="inlineStr">
@@ -52552,7 +52579,7 @@
       </c>
       <c r="G1186" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1186" t="inlineStr">
@@ -52767,7 +52794,7 @@
       </c>
       <c r="G1191" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1191" t="inlineStr">
@@ -52982,7 +53009,7 @@
       </c>
       <c r="G1196" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1196" t="inlineStr">
@@ -53412,7 +53439,7 @@
       </c>
       <c r="G1206" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1206" t="inlineStr">
@@ -53842,7 +53869,7 @@
       </c>
       <c r="G1216" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1216" t="inlineStr">
@@ -54272,7 +54299,7 @@
       </c>
       <c r="G1226" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1226" t="inlineStr">
@@ -54487,7 +54514,7 @@
       </c>
       <c r="G1231" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1231" t="inlineStr">
@@ -54702,7 +54729,7 @@
       </c>
       <c r="G1236" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1236" t="inlineStr">
@@ -55347,7 +55374,7 @@
       </c>
       <c r="G1251" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image1:Thumbnail200x200</t>
+          <t>http://example.com/organization0:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1251" t="inlineStr">
@@ -55562,7 +55589,7 @@
       </c>
       <c r="G1256" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image0:Thumbnail600x600</t>
+          <t>http://example.com/organization1:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1256" t="inlineStr">
@@ -55777,7 +55804,7 @@
       </c>
       <c r="G1261" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image1:Thumbnail800x800</t>
+          <t>http://example.com/organization1:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1261" t="inlineStr">
@@ -55992,7 +56019,7 @@
       </c>
       <c r="G1266" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0:Thumbnail200x200</t>
+          <t>http://example.com/organization2:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1266" t="inlineStr">
@@ -56207,7 +56234,7 @@
       </c>
       <c r="G1271" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image1:Thumbnail800x800</t>
+          <t>http://example.com/organization2:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1271" t="inlineStr">
@@ -56422,7 +56449,7 @@
       </c>
       <c r="G1276" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image0:Thumbnail600x600</t>
+          <t>http://example.com/organization3:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1276" t="inlineStr">
@@ -56637,7 +56664,7 @@
       </c>
       <c r="G1281" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image1:Thumbnail600x600</t>
+          <t>http://example.com/organization3:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1281" t="inlineStr">
@@ -56852,7 +56879,7 @@
       </c>
       <c r="G1286" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0:Thumbnail800x800</t>
+          <t>http://example.com/organization4:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1286" t="inlineStr">
@@ -57067,7 +57094,7 @@
       </c>
       <c r="G1291" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image1:Thumbnail800x800</t>
+          <t>http://example.com/organization4:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1291" t="inlineStr">
@@ -57282,7 +57309,7 @@
       </c>
       <c r="G1296" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image0:Thumbnail800x800</t>
+          <t>http://example.com/person0:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1296" t="inlineStr">
@@ -57497,7 +57524,7 @@
       </c>
       <c r="G1301" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image1:Thumbnail800x800</t>
+          <t>http://example.com/person0:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1301" t="inlineStr">
@@ -57959,7 +57986,7 @@
       </c>
       <c r="G1312" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image1:Thumbnail800x800</t>
+          <t>http://example.com/person1:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1312" t="inlineStr">
@@ -58174,7 +58201,7 @@
       </c>
       <c r="G1317" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image0:Thumbnail600x600</t>
+          <t>http://example.com/person2:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1317" t="inlineStr">
@@ -58389,7 +58416,7 @@
       </c>
       <c r="G1322" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image1:Thumbnail200x200</t>
+          <t>http://example.com/person2:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1322" t="inlineStr">
@@ -58604,7 +58631,7 @@
       </c>
       <c r="G1327" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0:Thumbnail600x600</t>
+          <t>http://example.com/person3:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1327" t="inlineStr">
@@ -58819,7 +58846,7 @@
       </c>
       <c r="G1332" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image1:Thumbnail600x600</t>
+          <t>http://example.com/person3:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1332" t="inlineStr">
@@ -59034,7 +59061,7 @@
       </c>
       <c r="G1337" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image0:Thumbnail400x400</t>
+          <t>http://example.com/person4:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1337" t="inlineStr">
@@ -59249,7 +59276,7 @@
       </c>
       <c r="G1342" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image1:Thumbnail800x800</t>
+          <t>http://example.com/person4:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1342" t="inlineStr">
@@ -59464,7 +59491,7 @@
       </c>
       <c r="G1347" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0:Image0:Thumbnail400x400</t>
+          <t>http://example.com/collection0/work0:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1347" t="inlineStr">
@@ -59679,7 +59706,7 @@
       </c>
       <c r="G1352" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0:Image1:Thumbnail800x800</t>
+          <t>http://example.com/collection0/work0:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1352" t="inlineStr">
@@ -59931,7 +59958,7 @@
       </c>
       <c r="G1358" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image0:Thumbnail800x800</t>
+          <t>http://example.com/collection0/work1:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1358" t="inlineStr">
@@ -60146,7 +60173,7 @@
       </c>
       <c r="G1363" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image1:Thumbnail800x800</t>
+          <t>http://example.com/collection0/work1:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1363" t="inlineStr">
@@ -60361,7 +60388,7 @@
       </c>
       <c r="G1368" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2:Image0:Thumbnail800x800</t>
+          <t>http://example.com/collection0/work2:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1368" t="inlineStr">
@@ -60576,7 +60603,7 @@
       </c>
       <c r="G1373" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2:Image1:Thumbnail600x600</t>
+          <t>http://example.com/collection0/work2:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1373" t="inlineStr">
@@ -60791,7 +60818,7 @@
       </c>
       <c r="G1378" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image0:Thumbnail800x800</t>
+          <t>http://example.com/collection0/work3:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1378" t="inlineStr">
@@ -61221,7 +61248,7 @@
       </c>
       <c r="G1388" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image0:Thumbnail400x400</t>
+          <t>http://example.com/collection1:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1388" t="inlineStr">
@@ -61866,7 +61893,7 @@
       </c>
       <c r="G1403" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4:Image1:Thumbnail200x200</t>
+          <t>http://example.com/collection1/work4:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1403" t="inlineStr">
@@ -62081,7 +62108,7 @@
       </c>
       <c r="G1408" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection1/work5:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1408" t="inlineStr">
@@ -62296,7 +62323,7 @@
       </c>
       <c r="G1413" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:Image1:Thumbnail800x800</t>
+          <t>http://example.com/collection1/work5:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1413" t="inlineStr">
@@ -62511,7 +62538,7 @@
       </c>
       <c r="G1418" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection1/work6:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1418" t="inlineStr">
@@ -62726,7 +62753,7 @@
       </c>
       <c r="G1423" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6:Image1:Thumbnail400x400</t>
+          <t>http://example.com/collection1/work6:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1423" t="inlineStr">
@@ -63156,7 +63183,7 @@
       </c>
       <c r="G1433" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image1:Thumbnail600x600</t>
+          <t>http://example.com/collection1/work7:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1433" t="inlineStr">
@@ -63371,7 +63398,7 @@
       </c>
       <c r="G1438" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8:Image0:Thumbnail600x600</t>
+          <t>http://example.com/freestandingwork8:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1438" t="inlineStr">
@@ -63586,7 +63613,7 @@
       </c>
       <c r="G1443" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8:Image1:Thumbnail600x600</t>
+          <t>http://example.com/freestandingwork8:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1443" t="inlineStr">
@@ -63801,7 +63828,7 @@
       </c>
       <c r="G1448" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:Image0:Thumbnail600x600</t>
+          <t>http://example.com/freestandingwork9:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1448" t="inlineStr">
@@ -64231,7 +64258,7 @@
       </c>
       <c r="G1458" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10:Image0:Thumbnail400x400</t>
+          <t>http://example.com/freestandingwork10:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1458" t="inlineStr">
@@ -64446,7 +64473,7 @@
       </c>
       <c r="G1463" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10:Image1:Thumbnail800x800</t>
+          <t>http://example.com/freestandingwork10:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1463" t="inlineStr">
@@ -64661,7 +64688,7 @@
       </c>
       <c r="G1468" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:Image0:Thumbnail200x200</t>
+          <t>http://example.com/freestandingwork11:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1468" t="inlineStr">
@@ -64954,7 +64981,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>vra:culturalContext:Image0:Thumbnail400x400</t>
+          <t>vra:culturalContext:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -64986,7 +65013,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dcterms:description:Image0:Thumbnail600x600</t>
+          <t>dcterms:description:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -65018,7 +65045,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image1:Thumbnail800x800</t>
+          <t>dcterms:extent:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -65050,7 +65077,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dcterms:language:Image0:Thumbnail800x800</t>
+          <t>dcterms:language:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -65082,7 +65109,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>vra:material:Image0:Thumbnail600x600</t>
+          <t>vra:material:Image0</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -65114,7 +65141,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image1:Thumbnail800x800</t>
+          <t>dcterms:medium:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -65146,7 +65173,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image1:Thumbnail400x400</t>
+          <t>dcterms:publisher:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -65178,7 +65205,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>dcterms:source:Image1:Thumbnail400x400</t>
+          <t>dcterms:source:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -65210,7 +65237,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image1:Thumbnail600x600</t>
+          <t>dcterms:spatial:Image0</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -65242,7 +65269,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image1:Thumbnail400x400</t>
+          <t>dcterms:subject:Image0</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -65306,7 +65333,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>dcterms:title:Image1:Thumbnail800x800</t>
+          <t>dcterms:title:Image0</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -65338,7 +65365,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>dcterms:type:Image1:Thumbnail400x400</t>
+          <t>dcterms:type:Image0</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -65407,7 +65434,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -65465,7 +65492,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -65509,7 +65536,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -65531,7 +65558,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -65553,7 +65580,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -65575,7 +65602,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -65597,7 +65624,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -65619,7 +65646,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -65641,7 +65668,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -65663,7 +65690,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -65685,7 +65712,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -65707,7 +65734,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -65729,7 +65756,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -65751,7 +65778,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -65773,7 +65800,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -65795,7 +65822,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -65817,7 +65844,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -65861,7 +65888,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -65883,7 +65910,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -65905,7 +65932,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -65927,7 +65954,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -65949,7 +65976,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -65971,7 +65998,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -65993,7 +66020,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -66015,7 +66042,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -66037,7 +66064,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -66059,7 +66086,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -66103,7 +66130,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -66125,7 +66152,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -66147,7 +66174,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -66169,7 +66196,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -66191,7 +66218,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -66213,7 +66240,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -66235,7 +66262,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -66279,7 +66306,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -66323,7 +66350,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -66367,7 +66394,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -66389,7 +66416,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -66411,7 +66438,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -66433,7 +66460,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -66455,7 +66482,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -66477,7 +66504,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -66499,7 +66526,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -66521,7 +66548,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -66543,7 +66570,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -66565,7 +66592,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -66609,7 +66636,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -66631,7 +66658,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -66653,7 +66680,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -66675,7 +66702,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -66697,7 +66724,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -66719,7 +66746,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -66741,7 +66768,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -66763,7 +66790,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -66785,7 +66812,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -66807,7 +66834,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -66829,7 +66856,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -66851,7 +66878,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -66873,7 +66900,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -66917,7 +66944,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -66939,7 +66966,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -66961,7 +66988,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -66983,7 +67010,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -67027,7 +67054,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -67049,7 +67076,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -67071,7 +67098,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -67093,7 +67120,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -67137,7 +67164,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -67159,7 +67186,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -67181,7 +67208,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -67225,7 +67252,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -67247,7 +67274,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -67269,7 +67296,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -67291,7 +67318,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -67313,7 +67340,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -67335,7 +67362,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -67357,7 +67384,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -67379,7 +67406,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -67401,7 +67428,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -67423,7 +67450,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -67445,7 +67472,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -67467,7 +67494,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image0</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -67489,7 +67516,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -67511,7 +67538,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -67533,7 +67560,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -67555,7 +67582,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:Image1</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -67577,7 +67604,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -67599,7 +67626,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image1</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -67621,7 +67648,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -67643,7 +67670,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image0</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -67665,7 +67692,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -67687,7 +67714,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -67709,7 +67736,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -67731,7 +67758,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -67753,7 +67780,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -67775,7 +67802,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image0</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -67797,7 +67824,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -67819,7 +67846,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -67841,7 +67868,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -67863,7 +67890,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -67926,7 +67953,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0:Thumbnail800x800</t>
+          <t>http://example.com/organization0:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -67944,7 +67971,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization1:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -67962,7 +67989,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0:Thumbnail200x200</t>
+          <t>http://example.com/organization2:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -67980,7 +68007,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image1</t>
+          <t>http://example.com/organization3:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -67998,7 +68025,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization4:Image0</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -68070,21 +68097,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
+          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
SyntheticDataPipeline: use both CmsCollection and SchemaCollection
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -23,6 +23,7 @@
     <sheet name="CmsWork" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="SchemaCreativeWork" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="SchemaCollection" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="CmsCollection" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -509,7 +510,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image0:Thumbnail800x800</t>
+          <t>http://example.com/person0:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -597,7 +598,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0:Thumbnail200x200</t>
+          <t>http://example.com/person3:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -624,7 +625,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image0:Thumbnail400x400</t>
+          <t>http://example.com/person4:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -887,7 +888,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:Nebf60f75571849d1890e1f05207ceaf7</t>
+          <t>_:N450e3b06214b4a57be21b446f711b4a1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -905,7 +906,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:N8c1783b4dfe446a78a5d9c92a809f04d</t>
+          <t>_:Nd7e41159625f48a59d184fc48abda03c</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -923,7 +924,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:N29d5f9d6a7414504bae40eb5819a8323</t>
+          <t>_:Nfb2dd42f39524fef9a81bac062cef028</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -941,7 +942,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:Nbe9dbfaa2a3c4b6bb9fa9d5fd1506381</t>
+          <t>_:N7f7bc72dd99b44bbb74bf984616811b2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -959,7 +960,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:N6cd9cc734d004ca7a03d8caf2cfe0e6a</t>
+          <t>_:Nbe0b73d79d5a488fbbffd1ec3bff5608</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -977,7 +978,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:N0d5a75bb491043cf9d2d7422478332c7</t>
+          <t>_:Nd36be1596f314b7f93308d0d128c94f7</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1020,17 +1021,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>_:Nef730a3bb21d4b03a2795c92b999e9ec</t>
+          <t>_:Nc074ca4443864f47b096be7c2e2a3590</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://example.com/organization3</t>
+          <t>http://example.com/organization4</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Collection0Work1 alternative title 0</t>
+          <t>Collection0Work1 alternative title 1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -1056,7 +1057,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image1:Thumbnail400x400</t>
+          <t>http://example.com/collection0/work1:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -1091,7 +1092,7 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
         </is>
       </c>
       <c r="V2" t="inlineStr"/>
@@ -1106,7 +1107,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>_:Nd772a7b207ca423f9db36eedfea5d314</t>
+          <t>_:N7453f9f634ba4e0b8b17d788a4da18d6</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1122,7 +1123,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Collection0Work3Id0</t>
+          <t>Collection0Work3Id1</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -1137,12 +1138,12 @@
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>_:N1e8d5d55bc794c4fbd9ca01c4b11b021</t>
+          <t>http://example.com/collection0/work3Opening</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image1:Thumbnail600x600</t>
+          <t>http://example.com/collection0/work3:Image1</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -1187,12 +1188,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>_:N816a291b75784a84a6d94a4a19b4c5d5</t>
+          <t>_:N85da660d17784f2b9ada9c5f147eadab</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>http://example.com/person3</t>
+          <t>http://example.com/person2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1218,7 +1219,7 @@
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5Opening</t>
+          <t>_:Nb1e39e06f0e5433dba7075ad6f8aae6c</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -1268,17 +1269,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>_:N3f70a425cff84f7a9c6af1112acb4b62</t>
+          <t>_:N14a61067ffb24775bbf209a950d8a898</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>http://example.com/organization0</t>
+          <t>http://example.com/person4</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Collection1Work7 alternative title 0</t>
+          <t>Collection1Work7 alternative title 1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -1291,7 +1292,7 @@
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Collection1Work7 provenance 1</t>
+          <t>Collection1Work7 provenance 0</t>
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
@@ -1299,12 +1300,12 @@
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7Opening</t>
+          <t>_:N5cfcd730df994793bf74f4149625943e</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image0:Thumbnail400x400</t>
+          <t>http://example.com/collection1/work7:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1334,7 +1335,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108</t>
         </is>
       </c>
       <c r="U5" t="inlineStr"/>
@@ -1349,17 +1350,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>_:N176bcf49c25945579348d710c7fcbabc</t>
+          <t>_:N873ea496508340eaa73efa9fcfd9bfcb</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>http://example.com/organization2</t>
+          <t>http://example.com/organization1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>FreestandingWork9 alternative title 0</t>
+          <t>FreestandingWork9 alternative title 1</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1415,7 +1416,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109</t>
         </is>
       </c>
       <c r="U6" t="inlineStr"/>
@@ -1430,7 +1431,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>_:N56c6602e30cf46c5adc693b75ce1d1fb</t>
+          <t>_:Nf5398d05920543d9880fc6af3dbe3316</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1446,7 +1447,7 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>FreestandingWork11Id0</t>
+          <t>FreestandingWork11Id1</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -1466,7 +1467,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:Image0:Thumbnail200x200</t>
+          <t>http://example.com/freestandingwork11:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -1540,6 +1541,32 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>@graph</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1551,7 +1578,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>@graph</t>
+          <t>@id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>hasPart</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>title</t>
         </is>
       </c>
     </row>
@@ -1561,14 +1603,10 @@
           <t>http://example.com/collection1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>http://example.com/collection1/work5</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image0:Thumbnail600x600</t>
+          <t>http://example.com/collection1:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2054,7 +2092,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -2269,7 +2307,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>vra:culturalContext:Image0:Thumbnail200x200</t>
+          <t>vra:culturalContext:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -2484,7 +2522,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>vra:culturalContext:Image1:Thumbnail800x800</t>
+          <t>vra:culturalContext:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -2699,7 +2737,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>dcterms:description:Image0:Thumbnail200x200</t>
+          <t>dcterms:description:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -3129,7 +3167,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0:Thumbnail600x600</t>
+          <t>dcterms:extent:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -3344,7 +3382,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image1:Thumbnail800x800</t>
+          <t>dcterms:extent:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -3559,7 +3597,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>dcterms:language:Image0:Thumbnail600x600</t>
+          <t>dcterms:language:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -3774,7 +3812,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>dcterms:language:Image1:Thumbnail600x600</t>
+          <t>dcterms:language:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -3989,7 +4027,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>vra:material:Image0:Thumbnail400x400</t>
+          <t>vra:material:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -4204,7 +4242,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>vra:material:Image1:Thumbnail800x800</t>
+          <t>vra:material:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -4419,7 +4457,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image0:Thumbnail200x200</t>
+          <t>dcterms:medium:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -4634,7 +4672,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image1:Thumbnail600x600</t>
+          <t>dcterms:medium:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -4849,7 +4887,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image0:Thumbnail400x400</t>
+          <t>dcterms:publisher:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -5064,7 +5102,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image1:Thumbnail600x600</t>
+          <t>dcterms:publisher:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
@@ -5494,7 +5532,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>dcterms:source:Image1:Thumbnail200x200</t>
+          <t>dcterms:source:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
@@ -5709,7 +5747,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image0:Thumbnail200x200</t>
+          <t>dcterms:spatial:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -5924,7 +5962,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image1:Thumbnail800x800</t>
+          <t>dcterms:spatial:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -6139,7 +6177,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image0:Thumbnail200x200</t>
+          <t>dcterms:subject:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
@@ -6784,7 +6822,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>vra:technique:Image1:Thumbnail800x800</t>
+          <t>vra:technique:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
@@ -6999,7 +7037,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>dcterms:title:Image0:Thumbnail200x200</t>
+          <t>dcterms:title:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
@@ -7214,7 +7252,7 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>dcterms:title:Image1:Thumbnail800x800</t>
+          <t>dcterms:title:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
@@ -7429,7 +7467,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>dcterms:type:Image0:Thumbnail800x800</t>
+          <t>dcterms:type:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
@@ -7644,7 +7682,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>dcterms:type:Image1:Thumbnail200x200</t>
+          <t>dcterms:type:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
@@ -7859,7 +7897,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
@@ -8289,7 +8327,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
@@ -8504,7 +8542,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H161" t="inlineStr">
@@ -8934,7 +8972,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
@@ -9149,7 +9187,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">
@@ -9364,7 +9402,7 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H181" t="inlineStr">
@@ -9579,7 +9617,7 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H186" t="inlineStr">
@@ -9794,7 +9832,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H191" t="inlineStr">
@@ -10009,7 +10047,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
@@ -10439,7 +10477,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
@@ -10654,7 +10692,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H211" t="inlineStr">
@@ -11084,7 +11122,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H221" t="inlineStr">
@@ -11299,7 +11337,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
@@ -11514,7 +11552,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
@@ -11729,7 +11767,7 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H236" t="inlineStr">
@@ -11944,7 +11982,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
@@ -12159,7 +12197,7 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H246" t="inlineStr">
@@ -12374,7 +12412,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H251" t="inlineStr">
@@ -12589,7 +12627,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H256" t="inlineStr">
@@ -13019,7 +13057,7 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H266" t="inlineStr">
@@ -13234,7 +13272,7 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H271" t="inlineStr">
@@ -13449,7 +13487,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H276" t="inlineStr">
@@ -13664,7 +13702,7 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H281" t="inlineStr">
@@ -13879,7 +13917,7 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H286" t="inlineStr">
@@ -14094,7 +14132,7 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H291" t="inlineStr">
@@ -14309,7 +14347,7 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H296" t="inlineStr">
@@ -14524,7 +14562,7 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H301" t="inlineStr">
@@ -14739,7 +14777,7 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H306" t="inlineStr">
@@ -14954,7 +14992,7 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H311" t="inlineStr">
@@ -15169,7 +15207,7 @@
       </c>
       <c r="G316" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H316" t="inlineStr">
@@ -15384,7 +15422,7 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H321" t="inlineStr">
@@ -15599,7 +15637,7 @@
       </c>
       <c r="G326" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H326" t="inlineStr">
@@ -16029,7 +16067,7 @@
       </c>
       <c r="G336" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H336" t="inlineStr">
@@ -16459,7 +16497,7 @@
       </c>
       <c r="G346" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H346" t="inlineStr">
@@ -16889,7 +16927,7 @@
       </c>
       <c r="G356" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H356" t="inlineStr">
@@ -17319,7 +17357,7 @@
       </c>
       <c r="G366" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H366" t="inlineStr">
@@ -17964,7 +18002,7 @@
       </c>
       <c r="G381" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H381" t="inlineStr">
@@ -18609,7 +18647,7 @@
       </c>
       <c r="G396" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H396" t="inlineStr">
@@ -18824,7 +18862,7 @@
       </c>
       <c r="G401" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H401" t="inlineStr">
@@ -19254,7 +19292,7 @@
       </c>
       <c r="G411" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H411" t="inlineStr">
@@ -19469,7 +19507,7 @@
       </c>
       <c r="G416" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H416" t="inlineStr">
@@ -19684,7 +19722,7 @@
       </c>
       <c r="G421" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H421" t="inlineStr">
@@ -19899,7 +19937,7 @@
       </c>
       <c r="G426" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H426" t="inlineStr">
@@ -20329,7 +20367,7 @@
       </c>
       <c r="G436" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H436" t="inlineStr">
@@ -20544,7 +20582,7 @@
       </c>
       <c r="G441" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H441" t="inlineStr">
@@ -20759,7 +20797,7 @@
       </c>
       <c r="G446" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H446" t="inlineStr">
@@ -21189,7 +21227,7 @@
       </c>
       <c r="G456" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H456" t="inlineStr">
@@ -21404,7 +21442,7 @@
       </c>
       <c r="G461" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H461" t="inlineStr">
@@ -21619,7 +21657,7 @@
       </c>
       <c r="G466" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H466" t="inlineStr">
@@ -21834,7 +21872,7 @@
       </c>
       <c r="G471" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H471" t="inlineStr">
@@ -22049,7 +22087,7 @@
       </c>
       <c r="G476" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H476" t="inlineStr">
@@ -22264,7 +22302,7 @@
       </c>
       <c r="G481" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H481" t="inlineStr">
@@ -22479,7 +22517,7 @@
       </c>
       <c r="G486" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H486" t="inlineStr">
@@ -22694,7 +22732,7 @@
       </c>
       <c r="G491" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H491" t="inlineStr">
@@ -22909,7 +22947,7 @@
       </c>
       <c r="G496" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H496" t="inlineStr">
@@ -23124,7 +23162,7 @@
       </c>
       <c r="G501" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H501" t="inlineStr">
@@ -23339,7 +23377,7 @@
       </c>
       <c r="G506" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H506" t="inlineStr">
@@ -23984,7 +24022,7 @@
       </c>
       <c r="G521" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H521" t="inlineStr">
@@ -24199,7 +24237,7 @@
       </c>
       <c r="G526" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H526" t="inlineStr">
@@ -24414,7 +24452,7 @@
       </c>
       <c r="G531" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H531" t="inlineStr">
@@ -24629,7 +24667,7 @@
       </c>
       <c r="G536" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H536" t="inlineStr">
@@ -24844,7 +24882,7 @@
       </c>
       <c r="G541" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H541" t="inlineStr">
@@ -25059,7 +25097,7 @@
       </c>
       <c r="G546" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H546" t="inlineStr">
@@ -25274,7 +25312,7 @@
       </c>
       <c r="G551" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H551" t="inlineStr">
@@ -25489,7 +25527,7 @@
       </c>
       <c r="G556" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H556" t="inlineStr">
@@ -25919,7 +25957,7 @@
       </c>
       <c r="G566" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H566" t="inlineStr">
@@ -26349,7 +26387,7 @@
       </c>
       <c r="G576" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H576" t="inlineStr">
@@ -26564,7 +26602,7 @@
       </c>
       <c r="G581" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H581" t="inlineStr">
@@ -26779,7 +26817,7 @@
       </c>
       <c r="G586" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H586" t="inlineStr">
@@ -26994,7 +27032,7 @@
       </c>
       <c r="G591" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H591" t="inlineStr">
@@ -27209,7 +27247,7 @@
       </c>
       <c r="G596" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H596" t="inlineStr">
@@ -27424,7 +27462,7 @@
       </c>
       <c r="G601" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H601" t="inlineStr">
@@ -27639,7 +27677,7 @@
       </c>
       <c r="G606" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H606" t="inlineStr">
@@ -27854,7 +27892,7 @@
       </c>
       <c r="G611" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H611" t="inlineStr">
@@ -28069,7 +28107,7 @@
       </c>
       <c r="G616" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H616" t="inlineStr">
@@ -28284,7 +28322,7 @@
       </c>
       <c r="G621" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H621" t="inlineStr">
@@ -28499,7 +28537,7 @@
       </c>
       <c r="G626" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H626" t="inlineStr">
@@ -28929,7 +28967,7 @@
       </c>
       <c r="G636" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H636" t="inlineStr">
@@ -29144,7 +29182,7 @@
       </c>
       <c r="G641" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H641" t="inlineStr">
@@ -29359,7 +29397,7 @@
       </c>
       <c r="G646" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H646" t="inlineStr">
@@ -29574,7 +29612,7 @@
       </c>
       <c r="G651" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H651" t="inlineStr">
@@ -30434,7 +30472,7 @@
       </c>
       <c r="G671" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H671" t="inlineStr">
@@ -30649,7 +30687,7 @@
       </c>
       <c r="G676" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H676" t="inlineStr">
@@ -30864,7 +30902,7 @@
       </c>
       <c r="G681" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H681" t="inlineStr">
@@ -31079,7 +31117,7 @@
       </c>
       <c r="G686" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H686" t="inlineStr">
@@ -31294,7 +31332,7 @@
       </c>
       <c r="G691" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H691" t="inlineStr">
@@ -31509,7 +31547,7 @@
       </c>
       <c r="G696" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H696" t="inlineStr">
@@ -31724,7 +31762,7 @@
       </c>
       <c r="G701" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H701" t="inlineStr">
@@ -31939,7 +31977,7 @@
       </c>
       <c r="G706" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H706" t="inlineStr">
@@ -32369,7 +32407,7 @@
       </c>
       <c r="G716" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H716" t="inlineStr">
@@ -32584,7 +32622,7 @@
       </c>
       <c r="G721" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H721" t="inlineStr">
@@ -32799,7 +32837,7 @@
       </c>
       <c r="G726" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H726" t="inlineStr">
@@ -33014,7 +33052,7 @@
       </c>
       <c r="G731" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H731" t="inlineStr">
@@ -33229,7 +33267,7 @@
       </c>
       <c r="G736" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H736" t="inlineStr">
@@ -33444,7 +33482,7 @@
       </c>
       <c r="G741" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H741" t="inlineStr">
@@ -33659,7 +33697,7 @@
       </c>
       <c r="G746" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H746" t="inlineStr">
@@ -34734,7 +34772,7 @@
       </c>
       <c r="G771" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H771" t="inlineStr">
@@ -34949,7 +34987,7 @@
       </c>
       <c r="G776" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H776" t="inlineStr">
@@ -35164,7 +35202,7 @@
       </c>
       <c r="G781" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H781" t="inlineStr">
@@ -35379,7 +35417,7 @@
       </c>
       <c r="G786" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H786" t="inlineStr">
@@ -35594,7 +35632,7 @@
       </c>
       <c r="G791" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H791" t="inlineStr">
@@ -35809,7 +35847,7 @@
       </c>
       <c r="G796" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H796" t="inlineStr">
@@ -36024,7 +36062,7 @@
       </c>
       <c r="G801" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H801" t="inlineStr">
@@ -36239,7 +36277,7 @@
       </c>
       <c r="G806" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H806" t="inlineStr">
@@ -36454,7 +36492,7 @@
       </c>
       <c r="G811" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H811" t="inlineStr">
@@ -36669,7 +36707,7 @@
       </c>
       <c r="G816" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H816" t="inlineStr">
@@ -36884,7 +36922,7 @@
       </c>
       <c r="G821" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H821" t="inlineStr">
@@ -37099,7 +37137,7 @@
       </c>
       <c r="G826" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H826" t="inlineStr">
@@ -37314,7 +37352,7 @@
       </c>
       <c r="G831" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H831" t="inlineStr">
@@ -37529,7 +37567,7 @@
       </c>
       <c r="G836" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H836" t="inlineStr">
@@ -37744,7 +37782,7 @@
       </c>
       <c r="G841" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H841" t="inlineStr">
@@ -37959,7 +37997,7 @@
       </c>
       <c r="G846" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H846" t="inlineStr">
@@ -38389,7 +38427,7 @@
       </c>
       <c r="G856" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H856" t="inlineStr">
@@ -38819,7 +38857,7 @@
       </c>
       <c r="G866" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H866" t="inlineStr">
@@ -39034,7 +39072,7 @@
       </c>
       <c r="G871" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H871" t="inlineStr">
@@ -39249,7 +39287,7 @@
       </c>
       <c r="G876" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H876" t="inlineStr">
@@ -39679,7 +39717,7 @@
       </c>
       <c r="G886" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H886" t="inlineStr">
@@ -39894,7 +39932,7 @@
       </c>
       <c r="G891" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H891" t="inlineStr">
@@ -40324,7 +40362,7 @@
       </c>
       <c r="G901" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H901" t="inlineStr">
@@ -40539,7 +40577,7 @@
       </c>
       <c r="G906" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H906" t="inlineStr">
@@ -40754,7 +40792,7 @@
       </c>
       <c r="G911" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H911" t="inlineStr">
@@ -40969,7 +41007,7 @@
       </c>
       <c r="G916" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H916" t="inlineStr">
@@ -41184,7 +41222,7 @@
       </c>
       <c r="G921" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H921" t="inlineStr">
@@ -41399,7 +41437,7 @@
       </c>
       <c r="G926" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H926" t="inlineStr">
@@ -41829,7 +41867,7 @@
       </c>
       <c r="G936" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H936" t="inlineStr">
@@ -42259,7 +42297,7 @@
       </c>
       <c r="G946" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H946" t="inlineStr">
@@ -42474,7 +42512,7 @@
       </c>
       <c r="G951" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H951" t="inlineStr">
@@ -42689,7 +42727,7 @@
       </c>
       <c r="G956" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H956" t="inlineStr">
@@ -42904,7 +42942,7 @@
       </c>
       <c r="G961" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H961" t="inlineStr">
@@ -43119,7 +43157,7 @@
       </c>
       <c r="G966" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H966" t="inlineStr">
@@ -43334,7 +43372,7 @@
       </c>
       <c r="G971" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H971" t="inlineStr">
@@ -43549,7 +43587,7 @@
       </c>
       <c r="G976" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H976" t="inlineStr">
@@ -43979,7 +44017,7 @@
       </c>
       <c r="G986" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H986" t="inlineStr">
@@ -44194,7 +44232,7 @@
       </c>
       <c r="G991" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H991" t="inlineStr">
@@ -44409,7 +44447,7 @@
       </c>
       <c r="G996" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H996" t="inlineStr">
@@ -44624,7 +44662,7 @@
       </c>
       <c r="G1001" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1001" t="inlineStr">
@@ -44839,7 +44877,7 @@
       </c>
       <c r="G1006" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1006" t="inlineStr">
@@ -45484,7 +45522,7 @@
       </c>
       <c r="G1021" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1021" t="inlineStr">
@@ -45699,7 +45737,7 @@
       </c>
       <c r="G1026" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1026" t="inlineStr">
@@ -45914,7 +45952,7 @@
       </c>
       <c r="G1031" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1031" t="inlineStr">
@@ -46344,7 +46382,7 @@
       </c>
       <c r="G1041" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1041" t="inlineStr">
@@ -46774,7 +46812,7 @@
       </c>
       <c r="G1051" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1051" t="inlineStr">
@@ -46989,7 +47027,7 @@
       </c>
       <c r="G1056" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1056" t="inlineStr">
@@ -47204,7 +47242,7 @@
       </c>
       <c r="G1061" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1061" t="inlineStr">
@@ -47419,7 +47457,7 @@
       </c>
       <c r="G1066" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1066" t="inlineStr">
@@ -47849,7 +47887,7 @@
       </c>
       <c r="G1076" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1076" t="inlineStr">
@@ -48064,7 +48102,7 @@
       </c>
       <c r="G1081" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1081" t="inlineStr">
@@ -48279,7 +48317,7 @@
       </c>
       <c r="G1086" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1086" t="inlineStr">
@@ -48494,7 +48532,7 @@
       </c>
       <c r="G1091" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1091" t="inlineStr">
@@ -49139,7 +49177,7 @@
       </c>
       <c r="G1106" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1106" t="inlineStr">
@@ -49354,7 +49392,7 @@
       </c>
       <c r="G1111" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1111" t="inlineStr">
@@ -49999,7 +50037,7 @@
       </c>
       <c r="G1126" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1126" t="inlineStr">
@@ -50214,7 +50252,7 @@
       </c>
       <c r="G1131" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1131" t="inlineStr">
@@ -50429,7 +50467,7 @@
       </c>
       <c r="G1136" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1136" t="inlineStr">
@@ -51074,7 +51112,7 @@
       </c>
       <c r="G1151" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1151" t="inlineStr">
@@ -51289,7 +51327,7 @@
       </c>
       <c r="G1156" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1156" t="inlineStr">
@@ -51504,7 +51542,7 @@
       </c>
       <c r="G1161" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1161" t="inlineStr">
@@ -51934,7 +51972,7 @@
       </c>
       <c r="G1171" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1171" t="inlineStr">
@@ -52149,7 +52187,7 @@
       </c>
       <c r="G1176" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1176" t="inlineStr">
@@ -52364,7 +52402,7 @@
       </c>
       <c r="G1181" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1181" t="inlineStr">
@@ -52579,7 +52617,7 @@
       </c>
       <c r="G1186" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1186" t="inlineStr">
@@ -52794,7 +52832,7 @@
       </c>
       <c r="G1191" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1191" t="inlineStr">
@@ -53009,7 +53047,7 @@
       </c>
       <c r="G1196" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1196" t="inlineStr">
@@ -53439,7 +53477,7 @@
       </c>
       <c r="G1206" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1206" t="inlineStr">
@@ -53654,7 +53692,7 @@
       </c>
       <c r="G1211" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1211" t="inlineStr">
@@ -53869,7 +53907,7 @@
       </c>
       <c r="G1216" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1216" t="inlineStr">
@@ -54084,7 +54122,7 @@
       </c>
       <c r="G1221" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1221" t="inlineStr">
@@ -54299,7 +54337,7 @@
       </c>
       <c r="G1226" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1226" t="inlineStr">
@@ -54514,7 +54552,7 @@
       </c>
       <c r="G1231" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1231" t="inlineStr">
@@ -54729,7 +54767,7 @@
       </c>
       <c r="G1236" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1236" t="inlineStr">
@@ -54944,7 +54982,7 @@
       </c>
       <c r="G1241" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1241" t="inlineStr">
@@ -55159,7 +55197,7 @@
       </c>
       <c r="G1246" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0:Thumbnail800x800</t>
+          <t>http://example.com/organization0:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1246" t="inlineStr">
@@ -55589,7 +55627,7 @@
       </c>
       <c r="G1256" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization1:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1256" t="inlineStr">
@@ -55804,7 +55842,7 @@
       </c>
       <c r="G1261" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image1:Thumbnail400x400</t>
+          <t>http://example.com/organization1:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1261" t="inlineStr">
@@ -56019,7 +56057,7 @@
       </c>
       <c r="G1266" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0:Thumbnail600x600</t>
+          <t>http://example.com/organization2:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1266" t="inlineStr">
@@ -56879,7 +56917,7 @@
       </c>
       <c r="G1286" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0:Thumbnail200x200</t>
+          <t>http://example.com/organization4:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1286" t="inlineStr">
@@ -57094,7 +57132,7 @@
       </c>
       <c r="G1291" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image1:Thumbnail200x200</t>
+          <t>http://example.com/organization4:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1291" t="inlineStr">
@@ -57309,7 +57347,7 @@
       </c>
       <c r="G1296" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image0:Thumbnail400x400</t>
+          <t>http://example.com/person0:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1296" t="inlineStr">
@@ -57524,7 +57562,7 @@
       </c>
       <c r="G1301" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image1:Thumbnail400x400</t>
+          <t>http://example.com/person0:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1301" t="inlineStr">
@@ -57771,7 +57809,7 @@
       </c>
       <c r="G1307" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image0:Thumbnail800x800</t>
+          <t>http://example.com/person1:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1307" t="inlineStr">
@@ -57986,7 +58024,7 @@
       </c>
       <c r="G1312" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image1:Thumbnail600x600</t>
+          <t>http://example.com/person1:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1312" t="inlineStr">
@@ -58201,7 +58239,7 @@
       </c>
       <c r="G1317" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image0:Thumbnail800x800</t>
+          <t>http://example.com/person2:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1317" t="inlineStr">
@@ -58416,7 +58454,7 @@
       </c>
       <c r="G1322" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image1:Thumbnail800x800</t>
+          <t>http://example.com/person2:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1322" t="inlineStr">
@@ -58631,7 +58669,7 @@
       </c>
       <c r="G1327" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0:Thumbnail200x200</t>
+          <t>http://example.com/person3:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1327" t="inlineStr">
@@ -58846,7 +58884,7 @@
       </c>
       <c r="G1332" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image1:Thumbnail800x800</t>
+          <t>http://example.com/person3:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1332" t="inlineStr">
@@ -59061,7 +59099,7 @@
       </c>
       <c r="G1337" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image0:Thumbnail200x200</t>
+          <t>http://example.com/person4:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1337" t="inlineStr">
@@ -59276,7 +59314,7 @@
       </c>
       <c r="G1342" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image1:Thumbnail600x600</t>
+          <t>http://example.com/person4:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1342" t="inlineStr">
@@ -59706,7 +59744,7 @@
       </c>
       <c r="G1352" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0:Image1:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work0:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1352" t="inlineStr">
@@ -60173,7 +60211,7 @@
       </c>
       <c r="G1363" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image1:Thumbnail600x600</t>
+          <t>http://example.com/collection0/work1:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1363" t="inlineStr">
@@ -60603,7 +60641,7 @@
       </c>
       <c r="G1373" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2:Image1:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work2:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1373" t="inlineStr">
@@ -60818,7 +60856,7 @@
       </c>
       <c r="G1378" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image0:Thumbnail400x400</t>
+          <t>http://example.com/collection0/work3:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1378" t="inlineStr">
@@ -61033,7 +61071,7 @@
       </c>
       <c r="G1383" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image1:Thumbnail600x600</t>
+          <t>http://example.com/collection0/work3:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1383" t="inlineStr">
@@ -61248,7 +61286,7 @@
       </c>
       <c r="G1388" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image0:Thumbnail600x600</t>
+          <t>http://example.com/collection1:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1388" t="inlineStr">
@@ -61678,7 +61716,7 @@
       </c>
       <c r="G1398" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4:Image0:Thumbnail800x800</t>
+          <t>http://example.com/collection1/work4:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1398" t="inlineStr">
@@ -62108,7 +62146,7 @@
       </c>
       <c r="G1408" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:Image0:Thumbnail600x600</t>
+          <t>http://example.com/collection1/work5:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1408" t="inlineStr">
@@ -62323,7 +62361,7 @@
       </c>
       <c r="G1413" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:Image1:Thumbnail200x200</t>
+          <t>http://example.com/collection1/work5:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1413" t="inlineStr">
@@ -62753,7 +62791,7 @@
       </c>
       <c r="G1423" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6:Image1:Thumbnail600x600</t>
+          <t>http://example.com/collection1/work6:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1423" t="inlineStr">
@@ -62968,7 +63006,7 @@
       </c>
       <c r="G1428" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image0:Thumbnail400x400</t>
+          <t>http://example.com/collection1/work7:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1428" t="inlineStr">
@@ -63183,7 +63221,7 @@
       </c>
       <c r="G1433" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image1:Thumbnail200x200</t>
+          <t>http://example.com/collection1/work7:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1433" t="inlineStr">
@@ -63398,7 +63436,7 @@
       </c>
       <c r="G1438" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8:Image0:Thumbnail400x400</t>
+          <t>http://example.com/freestandingwork8:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1438" t="inlineStr">
@@ -63828,7 +63866,7 @@
       </c>
       <c r="G1448" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:Image0:Thumbnail200x200</t>
+          <t>http://example.com/freestandingwork9:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1448" t="inlineStr">
@@ -64473,7 +64511,7 @@
       </c>
       <c r="G1463" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10:Image1:Thumbnail600x600</t>
+          <t>http://example.com/freestandingwork10:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1463" t="inlineStr">
@@ -64688,7 +64726,7 @@
       </c>
       <c r="G1468" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:Image0:Thumbnail600x600</t>
+          <t>http://example.com/freestandingwork11:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1468" t="inlineStr">
@@ -64903,7 +64941,7 @@
       </c>
       <c r="G1473" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:Image1:Thumbnail200x200</t>
+          <t>http://example.com/freestandingwork11:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1473" t="inlineStr">
@@ -64981,7 +65019,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>vra:culturalContext:Image1:Thumbnail400x400</t>
+          <t>vra:culturalContext:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -65013,7 +65051,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dcterms:description:Image1:Thumbnail400x400</t>
+          <t>dcterms:description:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -65045,7 +65083,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0:Thumbnail600x600</t>
+          <t>dcterms:extent:Image1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -65077,7 +65115,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dcterms:language:Image0:Thumbnail200x200</t>
+          <t>dcterms:language:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -65109,7 +65147,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>vra:material:Image0</t>
+          <t>vra:material:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -65141,7 +65179,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image1:Thumbnail200x200</t>
+          <t>dcterms:medium:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -65173,7 +65211,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image1:Thumbnail200x200</t>
+          <t>dcterms:publisher:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -65205,7 +65243,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>dcterms:source:Image0:Thumbnail600x600</t>
+          <t>dcterms:source:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -65237,7 +65275,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image0</t>
+          <t>dcterms:spatial:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -65301,7 +65339,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>vra:technique:Image1:Thumbnail800x800</t>
+          <t>vra:technique:Image1</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -65333,7 +65371,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>dcterms:title:Image0</t>
+          <t>dcterms:title:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -65365,7 +65403,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>dcterms:type:Image0</t>
+          <t>dcterms:type:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -65434,7 +65472,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -65492,7 +65530,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -65514,7 +65552,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -65536,7 +65574,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -65558,7 +65596,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -65580,7 +65618,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -65624,7 +65662,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -65646,7 +65684,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -65668,7 +65706,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -65690,7 +65728,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -65712,7 +65750,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -65734,7 +65772,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -65756,7 +65794,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -65800,7 +65838,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -65822,7 +65860,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -65844,7 +65882,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -65866,7 +65904,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -65910,7 +65948,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -65932,7 +65970,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -65976,7 +66014,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -65998,7 +66036,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -66020,7 +66058,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -66042,7 +66080,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -66064,7 +66102,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -66108,7 +66146,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -66130,7 +66168,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -66152,7 +66190,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -66174,7 +66212,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -66196,7 +66234,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -66218,7 +66256,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -66240,7 +66278,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -66262,7 +66300,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -66284,7 +66322,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -66328,7 +66366,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -66350,7 +66388,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -66372,7 +66410,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -66394,7 +66432,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -66416,7 +66454,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -66460,7 +66498,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -66482,7 +66520,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -66504,7 +66542,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -66526,7 +66564,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -66570,7 +66608,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -66592,7 +66630,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -66614,7 +66652,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -66658,7 +66696,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -66680,7 +66718,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -66702,7 +66740,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -66724,7 +66762,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -66746,7 +66784,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -66768,7 +66806,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -66790,7 +66828,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -66812,7 +66850,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -66834,7 +66872,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -66856,7 +66894,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -66878,7 +66916,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -66900,7 +66938,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -66922,7 +66960,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -66944,7 +66982,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -66966,7 +67004,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -66988,7 +67026,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -67010,7 +67048,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -67032,7 +67070,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -67054,7 +67092,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -67076,7 +67114,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -67098,7 +67136,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -67120,7 +67158,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -67142,7 +67180,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -67164,7 +67202,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -67186,7 +67224,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -67208,7 +67246,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -67252,7 +67290,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -67274,7 +67312,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -67296,7 +67334,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -67318,7 +67356,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -67340,7 +67378,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -67362,7 +67400,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -67384,7 +67422,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -67406,7 +67444,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -67428,7 +67466,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -67450,7 +67488,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -67472,7 +67510,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -67494,7 +67532,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -67516,7 +67554,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -67538,7 +67576,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -67560,7 +67598,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -67604,7 +67642,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -67626,7 +67664,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -67648,7 +67686,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -67670,7 +67708,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -67692,7 +67730,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -67714,7 +67752,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -67736,7 +67774,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -67758,7 +67796,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image0</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -67780,7 +67818,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -67802,7 +67840,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -67824,7 +67862,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -67846,7 +67884,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -67868,7 +67906,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -67890,7 +67928,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -67953,7 +67991,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0:Thumbnail600x600</t>
+          <t>http://example.com/organization0:Image1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -67971,7 +68009,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image1:Thumbnail600x600</t>
+          <t>http://example.com/organization1:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -67989,7 +68027,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image1:Thumbnail800x800</t>
+          <t>http://example.com/organization2:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -68007,7 +68045,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image1:Thumbnail400x400</t>
+          <t>http://example.com/organization3:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -68025,7 +68063,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0</t>
+          <t>http://example.com/organization4:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -68097,21 +68135,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
+          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
SyntheticDataPipeline: add descriptions to all Collections
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -510,7 +510,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image1:Thumbnail800x800</t>
+          <t>http://example.com/person0:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -543,7 +543,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image1:Thumbnail200x200</t>
+          <t>http://example.com/person1:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -570,7 +570,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image0:Thumbnail800x800</t>
+          <t>http://example.com/person2:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -598,7 +598,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0:Thumbnail400x400</t>
+          <t>http://example.com/person3:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -625,7 +625,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image1:Thumbnail800x800</t>
+          <t>http://example.com/person4:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -888,7 +888,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>_:N450e3b06214b4a57be21b446f711b4a1</t>
+          <t>_:Nfe0787cf63334a9e95f41ca9e7f11f54</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -906,7 +906,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>_:Nd7e41159625f48a59d184fc48abda03c</t>
+          <t>_:Nc898bd378f5d4fbca0dce6b854a858b4</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -924,7 +924,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>_:Nfb2dd42f39524fef9a81bac062cef028</t>
+          <t>_:N78dda267ce604f9bb01b01031d52c6b3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -942,7 +942,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>_:N7f7bc72dd99b44bbb74bf984616811b2</t>
+          <t>_:N85a231832c9740628cb1e6e4dc6950ac</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -960,7 +960,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>_:Nbe0b73d79d5a488fbbffd1ec3bff5608</t>
+          <t>_:Nd2b4af6611d542b69ebf15991530472a</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -978,7 +978,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>_:Nd36be1596f314b7f93308d0d128c94f7</t>
+          <t>_:N68be585faee64177b2a19cdc0af0f2f9</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1021,17 +1021,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>_:Nc074ca4443864f47b096be7c2e2a3590</t>
+          <t>_:N411d4e29e2ca4e8eba18a409197f2ab1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://example.com/organization4</t>
+          <t>http://example.com/organization3</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Collection0Work1 alternative title 1</t>
+          <t>Collection0Work1 alternative title 0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -1044,7 +1044,7 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Collection0Work1 provenance 0</t>
+          <t>Collection0Work1 provenance 1</t>
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
@@ -1052,12 +1052,12 @@
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1Opening</t>
+          <t>_:Neb6aef23d1754407ba7c0d69dcf9e7e1</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image1:Thumbnail800x800</t>
+          <t>http://example.com/collection0/work1:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -1092,7 +1092,7 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
         </is>
       </c>
       <c r="V2" t="inlineStr"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>_:N7453f9f634ba4e0b8b17d788a4da18d6</t>
+          <t>_:Nf3a6de6ec7a541c8b6619fe622193ceb</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1130,7 +1130,7 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Collection0Work3 provenance 0</t>
+          <t>Collection0Work3 provenance 1</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
@@ -1138,12 +1138,12 @@
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3Opening</t>
+          <t>http://example.com/collection0/work3Creation</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image1</t>
+          <t>http://example.com/collection0/work3:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -1173,7 +1173,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104</t>
         </is>
       </c>
       <c r="U3" t="inlineStr"/>
@@ -1188,7 +1188,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>_:N85da660d17784f2b9ada9c5f147eadab</t>
+          <t>_:N7096d0ccbaf64100a31b4ceefbb21ecb</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Collection1Work5 alternative title 0</t>
+          <t>Collection1Work5 alternative title 1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -1211,7 +1211,7 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Collection1Work5 provenance 1</t>
+          <t>Collection1Work5 provenance 0</t>
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
@@ -1219,12 +1219,12 @@
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
-          <t>_:Nb1e39e06f0e5433dba7075ad6f8aae6c</t>
+          <t>_:N740c1e570412459998550ace4e852256</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:Image0</t>
+          <t>http://example.com/collection1/work5:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>_:N14a61067ffb24775bbf209a950d8a898</t>
+          <t>_:N99a680575dca4e1b88bd58f8096085cb</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1279,7 +1279,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Collection1Work7 alternative title 1</t>
+          <t>Collection1Work7 alternative title 0</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -1292,7 +1292,7 @@
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Collection1Work7 provenance 0</t>
+          <t>Collection1Work7 provenance 1</t>
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
@@ -1300,12 +1300,12 @@
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr">
         <is>
-          <t>_:N5cfcd730df994793bf74f4149625943e</t>
+          <t>http://example.com/collection1/work7Creation</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image0:Thumbnail600x600</t>
+          <t>http://example.com/collection1/work7:Image0</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -1350,12 +1350,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>_:N873ea496508340eaa73efa9fcfd9bfcb</t>
+          <t>_:N1c900ed89fd14048a8eec74bf9e340b2</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>http://example.com/organization1</t>
+          <t>http://example.com/organization2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1366,7 +1366,7 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>FreestandingWork9Id1</t>
+          <t>FreestandingWork9Id0</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:Image0:Thumbnail800x800</t>
+          <t>http://example.com/freestandingwork9:Image0</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -1431,7 +1431,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>_:Nf5398d05920543d9880fc6af3dbe3316</t>
+          <t>_:N1d146766b8e34b629276a1d0ea1970a0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1454,7 +1454,7 @@
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>FreestandingWork11 provenance 0</t>
+          <t>FreestandingWork11 provenance 1</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
@@ -1462,12 +1462,12 @@
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11Opening</t>
+          <t>http://example.com/freestandingwork11Creation</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:Image1:Thumbnail600x600</t>
+          <t>http://example.com/freestandingwork11:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102</t>
         </is>
       </c>
       <c r="U7" t="inlineStr"/>
@@ -1567,7 +1567,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1578,40 +1578,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>@id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>hasPart</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>image</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>http://example.com/collection1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>http://example.com/collection1:Image1:Thumbnail400x400</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Collection1</t>
+          <t>@graph</t>
         </is>
       </c>
     </row>
@@ -2307,7 +2274,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>vra:culturalContext:Image0:Thumbnail600x600</t>
+          <t>vra:culturalContext:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -2522,7 +2489,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>vra:culturalContext:Image1:Thumbnail600x600</t>
+          <t>vra:culturalContext:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -2737,7 +2704,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>dcterms:description:Image0:Thumbnail800x800</t>
+          <t>dcterms:description:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -3167,7 +3134,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0:Thumbnail400x400</t>
+          <t>dcterms:extent:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -3382,7 +3349,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image1:Thumbnail200x200</t>
+          <t>dcterms:extent:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -3597,7 +3564,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>dcterms:language:Image0:Thumbnail400x400</t>
+          <t>dcterms:language:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -3812,7 +3779,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>dcterms:language:Image1:Thumbnail400x400</t>
+          <t>dcterms:language:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -4027,7 +3994,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>vra:material:Image0:Thumbnail200x200</t>
+          <t>vra:material:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -4672,7 +4639,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image1:Thumbnail800x800</t>
+          <t>dcterms:medium:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -4887,7 +4854,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image0:Thumbnail200x200</t>
+          <t>dcterms:publisher:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -5102,7 +5069,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image1:Thumbnail400x400</t>
+          <t>dcterms:publisher:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
@@ -5317,7 +5284,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>dcterms:source:Image0:Thumbnail800x800</t>
+          <t>dcterms:source:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -5532,7 +5499,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>dcterms:source:Image1:Thumbnail600x600</t>
+          <t>dcterms:source:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
@@ -5747,7 +5714,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image0:Thumbnail400x400</t>
+          <t>dcterms:spatial:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -5962,7 +5929,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image1:Thumbnail400x400</t>
+          <t>dcterms:spatial:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -6177,7 +6144,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image0:Thumbnail400x400</t>
+          <t>dcterms:subject:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
@@ -6607,7 +6574,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>vra:technique:Image0:Thumbnail400x400</t>
+          <t>vra:technique:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
@@ -7037,7 +7004,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>dcterms:title:Image0:Thumbnail400x400</t>
+          <t>dcterms:title:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
@@ -7252,7 +7219,7 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>dcterms:title:Image1:Thumbnail200x200</t>
+          <t>dcterms:title:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
@@ -7467,7 +7434,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>dcterms:type:Image0:Thumbnail200x200</t>
+          <t>dcterms:type:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
@@ -7897,7 +7864,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
@@ -8112,7 +8079,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
@@ -8542,7 +8509,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H161" t="inlineStr">
@@ -8757,7 +8724,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H166" t="inlineStr">
@@ -8972,7 +8939,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
@@ -9187,7 +9154,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">
@@ -9402,7 +9369,7 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H181" t="inlineStr">
@@ -9832,7 +9799,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H191" t="inlineStr">
@@ -10262,7 +10229,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H201" t="inlineStr">
@@ -10477,7 +10444,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
@@ -10907,7 +10874,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H216" t="inlineStr">
@@ -11552,7 +11519,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
@@ -11767,7 +11734,7 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H236" t="inlineStr">
@@ -11982,7 +11949,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
@@ -12197,7 +12164,7 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H246" t="inlineStr">
@@ -12412,7 +12379,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H251" t="inlineStr">
@@ -12627,7 +12594,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H256" t="inlineStr">
@@ -13057,7 +13024,7 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H266" t="inlineStr">
@@ -13272,7 +13239,7 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H271" t="inlineStr">
@@ -13487,7 +13454,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H276" t="inlineStr">
@@ -13702,7 +13669,7 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H281" t="inlineStr">
@@ -13917,7 +13884,7 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H286" t="inlineStr">
@@ -14132,7 +14099,7 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H291" t="inlineStr">
@@ -14562,7 +14529,7 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H301" t="inlineStr">
@@ -14777,7 +14744,7 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H306" t="inlineStr">
@@ -14992,7 +14959,7 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H311" t="inlineStr">
@@ -15207,7 +15174,7 @@
       </c>
       <c r="G316" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H316" t="inlineStr">
@@ -15422,7 +15389,7 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H321" t="inlineStr">
@@ -15637,7 +15604,7 @@
       </c>
       <c r="G326" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H326" t="inlineStr">
@@ -15852,7 +15819,7 @@
       </c>
       <c r="G331" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H331" t="inlineStr">
@@ -16067,7 +16034,7 @@
       </c>
       <c r="G336" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H336" t="inlineStr">
@@ -16282,7 +16249,7 @@
       </c>
       <c r="G341" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H341" t="inlineStr">
@@ -16712,7 +16679,7 @@
       </c>
       <c r="G351" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H351" t="inlineStr">
@@ -16927,7 +16894,7 @@
       </c>
       <c r="G356" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H356" t="inlineStr">
@@ -17142,7 +17109,7 @@
       </c>
       <c r="G361" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H361" t="inlineStr">
@@ -17357,7 +17324,7 @@
       </c>
       <c r="G366" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H366" t="inlineStr">
@@ -17572,7 +17539,7 @@
       </c>
       <c r="G371" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H371" t="inlineStr">
@@ -17787,7 +17754,7 @@
       </c>
       <c r="G376" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H376" t="inlineStr">
@@ -18002,7 +17969,7 @@
       </c>
       <c r="G381" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H381" t="inlineStr">
@@ -18217,7 +18184,7 @@
       </c>
       <c r="G386" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H386" t="inlineStr">
@@ -18432,7 +18399,7 @@
       </c>
       <c r="G391" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H391" t="inlineStr">
@@ -18647,7 +18614,7 @@
       </c>
       <c r="G396" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H396" t="inlineStr">
@@ -18862,7 +18829,7 @@
       </c>
       <c r="G401" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H401" t="inlineStr">
@@ -19077,7 +19044,7 @@
       </c>
       <c r="G406" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H406" t="inlineStr">
@@ -19292,7 +19259,7 @@
       </c>
       <c r="G411" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H411" t="inlineStr">
@@ -19722,7 +19689,7 @@
       </c>
       <c r="G421" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H421" t="inlineStr">
@@ -19937,7 +19904,7 @@
       </c>
       <c r="G426" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H426" t="inlineStr">
@@ -20367,7 +20334,7 @@
       </c>
       <c r="G436" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H436" t="inlineStr">
@@ -20582,7 +20549,7 @@
       </c>
       <c r="G441" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H441" t="inlineStr">
@@ -20797,7 +20764,7 @@
       </c>
       <c r="G446" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H446" t="inlineStr">
@@ -21012,7 +20979,7 @@
       </c>
       <c r="G451" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H451" t="inlineStr">
@@ -21227,7 +21194,7 @@
       </c>
       <c r="G456" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H456" t="inlineStr">
@@ -21442,7 +21409,7 @@
       </c>
       <c r="G461" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H461" t="inlineStr">
@@ -21657,7 +21624,7 @@
       </c>
       <c r="G466" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H466" t="inlineStr">
@@ -21872,7 +21839,7 @@
       </c>
       <c r="G471" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H471" t="inlineStr">
@@ -22087,7 +22054,7 @@
       </c>
       <c r="G476" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H476" t="inlineStr">
@@ -22302,7 +22269,7 @@
       </c>
       <c r="G481" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H481" t="inlineStr">
@@ -22517,7 +22484,7 @@
       </c>
       <c r="G486" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H486" t="inlineStr">
@@ -22732,7 +22699,7 @@
       </c>
       <c r="G491" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H491" t="inlineStr">
@@ -22947,7 +22914,7 @@
       </c>
       <c r="G496" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H496" t="inlineStr">
@@ -23162,7 +23129,7 @@
       </c>
       <c r="G501" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H501" t="inlineStr">
@@ -23377,7 +23344,7 @@
       </c>
       <c r="G506" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H506" t="inlineStr">
@@ -23592,7 +23559,7 @@
       </c>
       <c r="G511" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H511" t="inlineStr">
@@ -24237,7 +24204,7 @@
       </c>
       <c r="G526" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H526" t="inlineStr">
@@ -24452,7 +24419,7 @@
       </c>
       <c r="G531" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H531" t="inlineStr">
@@ -24667,7 +24634,7 @@
       </c>
       <c r="G536" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H536" t="inlineStr">
@@ -24882,7 +24849,7 @@
       </c>
       <c r="G541" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H541" t="inlineStr">
@@ -25097,7 +25064,7 @@
       </c>
       <c r="G546" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H546" t="inlineStr">
@@ -25312,7 +25279,7 @@
       </c>
       <c r="G551" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H551" t="inlineStr">
@@ -25527,7 +25494,7 @@
       </c>
       <c r="G556" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H556" t="inlineStr">
@@ -25742,7 +25709,7 @@
       </c>
       <c r="G561" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H561" t="inlineStr">
@@ -25957,7 +25924,7 @@
       </c>
       <c r="G566" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H566" t="inlineStr">
@@ -26172,7 +26139,7 @@
       </c>
       <c r="G571" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H571" t="inlineStr">
@@ -26387,7 +26354,7 @@
       </c>
       <c r="G576" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H576" t="inlineStr">
@@ -26817,7 +26784,7 @@
       </c>
       <c r="G586" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H586" t="inlineStr">
@@ -27032,7 +26999,7 @@
       </c>
       <c r="G591" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H591" t="inlineStr">
@@ -27247,7 +27214,7 @@
       </c>
       <c r="G596" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H596" t="inlineStr">
@@ -28107,7 +28074,7 @@
       </c>
       <c r="G616" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H616" t="inlineStr">
@@ -28752,7 +28719,7 @@
       </c>
       <c r="G631" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H631" t="inlineStr">
@@ -28967,7 +28934,7 @@
       </c>
       <c r="G636" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H636" t="inlineStr">
@@ -29182,7 +29149,7 @@
       </c>
       <c r="G641" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H641" t="inlineStr">
@@ -29397,7 +29364,7 @@
       </c>
       <c r="G646" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H646" t="inlineStr">
@@ -29827,7 +29794,7 @@
       </c>
       <c r="G656" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H656" t="inlineStr">
@@ -30042,7 +30009,7 @@
       </c>
       <c r="G661" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H661" t="inlineStr">
@@ -30472,7 +30439,7 @@
       </c>
       <c r="G671" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H671" t="inlineStr">
@@ -30687,7 +30654,7 @@
       </c>
       <c r="G676" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H676" t="inlineStr">
@@ -30902,7 +30869,7 @@
       </c>
       <c r="G681" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H681" t="inlineStr">
@@ -31117,7 +31084,7 @@
       </c>
       <c r="G686" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H686" t="inlineStr">
@@ -31332,7 +31299,7 @@
       </c>
       <c r="G691" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H691" t="inlineStr">
@@ -31762,7 +31729,7 @@
       </c>
       <c r="G701" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H701" t="inlineStr">
@@ -31977,7 +31944,7 @@
       </c>
       <c r="G706" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H706" t="inlineStr">
@@ -32192,7 +32159,7 @@
       </c>
       <c r="G711" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H711" t="inlineStr">
@@ -32407,7 +32374,7 @@
       </c>
       <c r="G716" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H716" t="inlineStr">
@@ -32622,7 +32589,7 @@
       </c>
       <c r="G721" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H721" t="inlineStr">
@@ -32837,7 +32804,7 @@
       </c>
       <c r="G726" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H726" t="inlineStr">
@@ -33052,7 +33019,7 @@
       </c>
       <c r="G731" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H731" t="inlineStr">
@@ -33482,7 +33449,7 @@
       </c>
       <c r="G741" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H741" t="inlineStr">
@@ -33697,7 +33664,7 @@
       </c>
       <c r="G746" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H746" t="inlineStr">
@@ -33912,7 +33879,7 @@
       </c>
       <c r="G751" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H751" t="inlineStr">
@@ -34127,7 +34094,7 @@
       </c>
       <c r="G756" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H756" t="inlineStr">
@@ -34342,7 +34309,7 @@
       </c>
       <c r="G761" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H761" t="inlineStr">
@@ -34772,7 +34739,7 @@
       </c>
       <c r="G771" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H771" t="inlineStr">
@@ -34987,7 +34954,7 @@
       </c>
       <c r="G776" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H776" t="inlineStr">
@@ -35417,7 +35384,7 @@
       </c>
       <c r="G786" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H786" t="inlineStr">
@@ -35632,7 +35599,7 @@
       </c>
       <c r="G791" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H791" t="inlineStr">
@@ -35847,7 +35814,7 @@
       </c>
       <c r="G796" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H796" t="inlineStr">
@@ -36062,7 +36029,7 @@
       </c>
       <c r="G801" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H801" t="inlineStr">
@@ -36277,7 +36244,7 @@
       </c>
       <c r="G806" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H806" t="inlineStr">
@@ -36492,7 +36459,7 @@
       </c>
       <c r="G811" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H811" t="inlineStr">
@@ -36707,7 +36674,7 @@
       </c>
       <c r="G816" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H816" t="inlineStr">
@@ -37137,7 +37104,7 @@
       </c>
       <c r="G826" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H826" t="inlineStr">
@@ -37567,7 +37534,7 @@
       </c>
       <c r="G836" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H836" t="inlineStr">
@@ -37782,7 +37749,7 @@
       </c>
       <c r="G841" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H841" t="inlineStr">
@@ -37997,7 +37964,7 @@
       </c>
       <c r="G846" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H846" t="inlineStr">
@@ -38212,7 +38179,7 @@
       </c>
       <c r="G851" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H851" t="inlineStr">
@@ -38427,7 +38394,7 @@
       </c>
       <c r="G856" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H856" t="inlineStr">
@@ -38642,7 +38609,7 @@
       </c>
       <c r="G861" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H861" t="inlineStr">
@@ -38857,7 +38824,7 @@
       </c>
       <c r="G866" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H866" t="inlineStr">
@@ -39502,7 +39469,7 @@
       </c>
       <c r="G881" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H881" t="inlineStr">
@@ -39717,7 +39684,7 @@
       </c>
       <c r="G886" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H886" t="inlineStr">
@@ -39932,7 +39899,7 @@
       </c>
       <c r="G891" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H891" t="inlineStr">
@@ -40147,7 +40114,7 @@
       </c>
       <c r="G896" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H896" t="inlineStr">
@@ -40362,7 +40329,7 @@
       </c>
       <c r="G901" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H901" t="inlineStr">
@@ -40792,7 +40759,7 @@
       </c>
       <c r="G911" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H911" t="inlineStr">
@@ -41437,7 +41404,7 @@
       </c>
       <c r="G926" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H926" t="inlineStr">
@@ -41652,7 +41619,7 @@
       </c>
       <c r="G931" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H931" t="inlineStr">
@@ -41867,7 +41834,7 @@
       </c>
       <c r="G936" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H936" t="inlineStr">
@@ -42082,7 +42049,7 @@
       </c>
       <c r="G941" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H941" t="inlineStr">
@@ -42297,7 +42264,7 @@
       </c>
       <c r="G946" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H946" t="inlineStr">
@@ -42512,7 +42479,7 @@
       </c>
       <c r="G951" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H951" t="inlineStr">
@@ -42727,7 +42694,7 @@
       </c>
       <c r="G956" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H956" t="inlineStr">
@@ -42942,7 +42909,7 @@
       </c>
       <c r="G961" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H961" t="inlineStr">
@@ -43587,7 +43554,7 @@
       </c>
       <c r="G976" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H976" t="inlineStr">
@@ -43802,7 +43769,7 @@
       </c>
       <c r="G981" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H981" t="inlineStr">
@@ -44017,7 +43984,7 @@
       </c>
       <c r="G986" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H986" t="inlineStr">
@@ -44232,7 +44199,7 @@
       </c>
       <c r="G991" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H991" t="inlineStr">
@@ -44447,7 +44414,7 @@
       </c>
       <c r="G996" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H996" t="inlineStr">
@@ -45092,7 +45059,7 @@
       </c>
       <c r="G1011" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1011" t="inlineStr">
@@ -45307,7 +45274,7 @@
       </c>
       <c r="G1016" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1016" t="inlineStr">
@@ -45522,7 +45489,7 @@
       </c>
       <c r="G1021" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1021" t="inlineStr">
@@ -45737,7 +45704,7 @@
       </c>
       <c r="G1026" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1026" t="inlineStr">
@@ -45952,7 +45919,7 @@
       </c>
       <c r="G1031" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1031" t="inlineStr">
@@ -46167,7 +46134,7 @@
       </c>
       <c r="G1036" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1036" t="inlineStr">
@@ -46382,7 +46349,7 @@
       </c>
       <c r="G1041" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1041" t="inlineStr">
@@ -46597,7 +46564,7 @@
       </c>
       <c r="G1046" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1046" t="inlineStr">
@@ -46812,7 +46779,7 @@
       </c>
       <c r="G1051" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1051" t="inlineStr">
@@ -47027,7 +46994,7 @@
       </c>
       <c r="G1056" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1056" t="inlineStr">
@@ -47457,7 +47424,7 @@
       </c>
       <c r="G1066" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1066" t="inlineStr">
@@ -47672,7 +47639,7 @@
       </c>
       <c r="G1071" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1071" t="inlineStr">
@@ -48532,7 +48499,7 @@
       </c>
       <c r="G1091" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1091" t="inlineStr">
@@ -48962,7 +48929,7 @@
       </c>
       <c r="G1101" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1101" t="inlineStr">
@@ -49177,7 +49144,7 @@
       </c>
       <c r="G1106" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1106" t="inlineStr">
@@ -49607,7 +49574,7 @@
       </c>
       <c r="G1116" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1116" t="inlineStr">
@@ -50037,7 +50004,7 @@
       </c>
       <c r="G1126" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1126" t="inlineStr">
@@ -50252,7 +50219,7 @@
       </c>
       <c r="G1131" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1131" t="inlineStr">
@@ -50467,7 +50434,7 @@
       </c>
       <c r="G1136" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1136" t="inlineStr">
@@ -50682,7 +50649,7 @@
       </c>
       <c r="G1141" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1141" t="inlineStr">
@@ -50897,7 +50864,7 @@
       </c>
       <c r="G1146" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1146" t="inlineStr">
@@ -51112,7 +51079,7 @@
       </c>
       <c r="G1151" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1151" t="inlineStr">
@@ -51327,7 +51294,7 @@
       </c>
       <c r="G1156" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1156" t="inlineStr">
@@ -51542,7 +51509,7 @@
       </c>
       <c r="G1161" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1161" t="inlineStr">
@@ -51757,7 +51724,7 @@
       </c>
       <c r="G1166" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:102:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1166" t="inlineStr">
@@ -52187,7 +52154,7 @@
       </c>
       <c r="G1176" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1176" t="inlineStr">
@@ -52402,7 +52369,7 @@
       </c>
       <c r="G1181" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1181" t="inlineStr">
@@ -52617,7 +52584,7 @@
       </c>
       <c r="G1186" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1186" t="inlineStr">
@@ -53262,7 +53229,7 @@
       </c>
       <c r="G1201" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1201" t="inlineStr">
@@ -53692,7 +53659,7 @@
       </c>
       <c r="G1211" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1211" t="inlineStr">
@@ -53907,7 +53874,7 @@
       </c>
       <c r="G1216" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:107:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1216" t="inlineStr">
@@ -54552,7 +54519,7 @@
       </c>
       <c r="G1231" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1231" t="inlineStr">
@@ -54767,7 +54734,7 @@
       </c>
       <c r="G1236" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1236" t="inlineStr">
@@ -55197,7 +55164,7 @@
       </c>
       <c r="G1246" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization0:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1246" t="inlineStr">
@@ -55412,7 +55379,7 @@
       </c>
       <c r="G1251" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image1:Thumbnail800x800</t>
+          <t>http://example.com/organization0:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1251" t="inlineStr">
@@ -55627,7 +55594,7 @@
       </c>
       <c r="G1256" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image0:Thumbnail200x200</t>
+          <t>http://example.com/organization1:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1256" t="inlineStr">
@@ -55842,7 +55809,7 @@
       </c>
       <c r="G1261" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image1:Thumbnail200x200</t>
+          <t>http://example.com/organization1:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1261" t="inlineStr">
@@ -56057,7 +56024,7 @@
       </c>
       <c r="G1266" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0:Thumbnail200x200</t>
+          <t>http://example.com/organization2:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1266" t="inlineStr">
@@ -56272,7 +56239,7 @@
       </c>
       <c r="G1271" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image1:Thumbnail200x200</t>
+          <t>http://example.com/organization2:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1271" t="inlineStr">
@@ -56487,7 +56454,7 @@
       </c>
       <c r="G1276" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization3:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1276" t="inlineStr">
@@ -56702,7 +56669,7 @@
       </c>
       <c r="G1281" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image1:Thumbnail800x800</t>
+          <t>http://example.com/organization3:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1281" t="inlineStr">
@@ -56917,7 +56884,7 @@
       </c>
       <c r="G1286" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0:Thumbnail800x800</t>
+          <t>http://example.com/organization4:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1286" t="inlineStr">
@@ -57347,7 +57314,7 @@
       </c>
       <c r="G1296" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image0:Thumbnail600x600</t>
+          <t>http://example.com/person0:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1296" t="inlineStr">
@@ -57562,7 +57529,7 @@
       </c>
       <c r="G1301" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image1:Thumbnail800x800</t>
+          <t>http://example.com/person0:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1301" t="inlineStr">
@@ -57809,7 +57776,7 @@
       </c>
       <c r="G1307" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image0:Thumbnail200x200</t>
+          <t>http://example.com/person1:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1307" t="inlineStr">
@@ -58024,7 +57991,7 @@
       </c>
       <c r="G1312" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image1:Thumbnail800x800</t>
+          <t>http://example.com/person1:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1312" t="inlineStr">
@@ -58239,7 +58206,7 @@
       </c>
       <c r="G1317" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image0:Thumbnail400x400</t>
+          <t>http://example.com/person2:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1317" t="inlineStr">
@@ -58454,7 +58421,7 @@
       </c>
       <c r="G1322" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image1:Thumbnail400x400</t>
+          <t>http://example.com/person2:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1322" t="inlineStr">
@@ -58669,7 +58636,7 @@
       </c>
       <c r="G1327" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0:Thumbnail800x800</t>
+          <t>http://example.com/person3:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1327" t="inlineStr">
@@ -58884,7 +58851,7 @@
       </c>
       <c r="G1332" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image1:Thumbnail200x200</t>
+          <t>http://example.com/person3:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1332" t="inlineStr">
@@ -59099,7 +59066,7 @@
       </c>
       <c r="G1337" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image0:Thumbnail600x600</t>
+          <t>http://example.com/person4:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1337" t="inlineStr">
@@ -59529,7 +59496,7 @@
       </c>
       <c r="G1347" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work0:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1347" t="inlineStr">
@@ -59744,7 +59711,7 @@
       </c>
       <c r="G1352" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0:Image1:Thumbnail800x800</t>
+          <t>http://example.com/collection0/work0:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1352" t="inlineStr">
@@ -59996,7 +59963,7 @@
       </c>
       <c r="G1358" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image0:Thumbnail600x600</t>
+          <t>http://example.com/collection0/work1:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1358" t="inlineStr">
@@ -60211,7 +60178,7 @@
       </c>
       <c r="G1363" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image1:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work1:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1363" t="inlineStr">
@@ -60426,7 +60393,7 @@
       </c>
       <c r="G1368" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work2:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1368" t="inlineStr">
@@ -60641,7 +60608,7 @@
       </c>
       <c r="G1373" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2:Image1:Thumbnail800x800</t>
+          <t>http://example.com/collection0/work2:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1373" t="inlineStr">
@@ -60856,7 +60823,7 @@
       </c>
       <c r="G1378" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work3:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1378" t="inlineStr">
@@ -61071,7 +61038,7 @@
       </c>
       <c r="G1383" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image1:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work3:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1383" t="inlineStr">
@@ -61286,7 +61253,7 @@
       </c>
       <c r="G1388" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image0:Thumbnail400x400</t>
+          <t>http://example.com/collection1:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1388" t="inlineStr">
@@ -61501,7 +61468,7 @@
       </c>
       <c r="G1393" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image1:Thumbnail400x400</t>
+          <t>http://example.com/collection1:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1393" t="inlineStr">
@@ -61716,7 +61683,7 @@
       </c>
       <c r="G1398" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection1/work4:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1398" t="inlineStr">
@@ -61931,7 +61898,7 @@
       </c>
       <c r="G1403" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4:Image1:Thumbnail400x400</t>
+          <t>http://example.com/collection1/work4:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1403" t="inlineStr">
@@ -62146,7 +62113,7 @@
       </c>
       <c r="G1408" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:Image0:Thumbnail400x400</t>
+          <t>http://example.com/collection1/work5:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1408" t="inlineStr">
@@ -62361,7 +62328,7 @@
       </c>
       <c r="G1413" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:Image1:Thumbnail400x400</t>
+          <t>http://example.com/collection1/work5:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1413" t="inlineStr">
@@ -62791,7 +62758,7 @@
       </c>
       <c r="G1423" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6:Image1:Thumbnail800x800</t>
+          <t>http://example.com/collection1/work6:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1423" t="inlineStr">
@@ -63006,7 +62973,7 @@
       </c>
       <c r="G1428" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image0:Thumbnail800x800</t>
+          <t>http://example.com/collection1/work7:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1428" t="inlineStr">
@@ -63221,7 +63188,7 @@
       </c>
       <c r="G1433" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image1:Thumbnail800x800</t>
+          <t>http://example.com/collection1/work7:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1433" t="inlineStr">
@@ -63436,7 +63403,7 @@
       </c>
       <c r="G1438" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8:Image0:Thumbnail600x600</t>
+          <t>http://example.com/freestandingwork8:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1438" t="inlineStr">
@@ -63651,7 +63618,7 @@
       </c>
       <c r="G1443" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8:Image1:Thumbnail400x400</t>
+          <t>http://example.com/freestandingwork8:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1443" t="inlineStr">
@@ -63866,7 +63833,7 @@
       </c>
       <c r="G1448" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:Image0:Thumbnail800x800</t>
+          <t>http://example.com/freestandingwork9:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1448" t="inlineStr">
@@ -64081,7 +64048,7 @@
       </c>
       <c r="G1453" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:Image1:Thumbnail200x200</t>
+          <t>http://example.com/freestandingwork9:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1453" t="inlineStr">
@@ -64296,7 +64263,7 @@
       </c>
       <c r="G1458" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10:Image0:Thumbnail800x800</t>
+          <t>http://example.com/freestandingwork10:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1458" t="inlineStr">
@@ -64511,7 +64478,7 @@
       </c>
       <c r="G1463" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10:Image1:Thumbnail400x400</t>
+          <t>http://example.com/freestandingwork10:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1463" t="inlineStr">
@@ -64726,7 +64693,7 @@
       </c>
       <c r="G1468" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:Image0:Thumbnail400x400</t>
+          <t>http://example.com/freestandingwork11:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1468" t="inlineStr">
@@ -64941,7 +64908,7 @@
       </c>
       <c r="G1473" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:Image1:Thumbnail800x800</t>
+          <t>http://example.com/freestandingwork11:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1473" t="inlineStr">
@@ -65083,7 +65050,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image1</t>
+          <t>dcterms:extent:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -65115,7 +65082,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dcterms:language:Image1:Thumbnail800x800</t>
+          <t>dcterms:language:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -65147,7 +65114,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>vra:material:Image0:Thumbnail200x200</t>
+          <t>vra:material:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -65179,7 +65146,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image0:Thumbnail200x200</t>
+          <t>dcterms:medium:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -65211,7 +65178,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image0:Thumbnail800x800</t>
+          <t>dcterms:publisher:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -65243,7 +65210,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>dcterms:source:Image0:Thumbnail200x200</t>
+          <t>dcterms:source:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -65307,7 +65274,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image0</t>
+          <t>dcterms:subject:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -65339,7 +65306,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>vra:technique:Image1</t>
+          <t>vra:technique:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -65371,7 +65338,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>dcterms:title:Image0:Thumbnail800x800</t>
+          <t>dcterms:title:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -65472,7 +65439,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -65530,7 +65497,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -65574,7 +65541,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -65618,7 +65585,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -65640,7 +65607,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -65662,7 +65629,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -65684,7 +65651,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -65706,7 +65673,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -65728,7 +65695,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -65772,7 +65739,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -65794,7 +65761,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -65816,7 +65783,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -65860,7 +65827,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -65882,7 +65849,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -65904,7 +65871,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -65926,7 +65893,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -65948,7 +65915,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -65970,7 +65937,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -65992,7 +65959,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -66014,7 +65981,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -66036,7 +66003,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -66058,7 +66025,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -66080,7 +66047,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -66102,7 +66069,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -66124,7 +66091,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -66146,7 +66113,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -66168,7 +66135,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -66190,7 +66157,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -66212,7 +66179,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -66234,7 +66201,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -66256,7 +66223,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -66300,7 +66267,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -66322,7 +66289,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -66344,7 +66311,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -66366,7 +66333,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -66388,7 +66355,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -66410,7 +66377,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -66432,7 +66399,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -66454,7 +66421,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -66476,7 +66443,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -66498,7 +66465,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -66520,7 +66487,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -66542,7 +66509,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -66564,7 +66531,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -66586,7 +66553,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -66608,7 +66575,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -66630,7 +66597,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -66652,7 +66619,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -66696,7 +66663,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -66718,7 +66685,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -66740,7 +66707,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -66762,7 +66729,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -66784,7 +66751,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -66806,7 +66773,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -66828,7 +66795,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -66850,7 +66817,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -66872,7 +66839,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -66894,7 +66861,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -66916,7 +66883,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -66938,7 +66905,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -66960,7 +66927,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -66982,7 +66949,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -67004,7 +66971,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -67026,7 +66993,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -67048,7 +67015,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -67092,7 +67059,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -67114,7 +67081,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -67136,7 +67103,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -67158,7 +67125,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -67180,7 +67147,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -67202,7 +67169,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -67224,7 +67191,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -67268,7 +67235,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -67290,7 +67257,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -67312,7 +67279,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -67356,7 +67323,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -67378,7 +67345,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -67400,7 +67367,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -67422,7 +67389,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -67444,7 +67411,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -67466,7 +67433,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -67488,7 +67455,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -67510,7 +67477,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:90:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -67532,7 +67499,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:91:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -67554,7 +67521,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:92:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -67576,7 +67543,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:93:Image1</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -67598,7 +67565,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:94:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -67620,7 +67587,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:95:Image0</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -67642,7 +67609,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:96:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -67664,7 +67631,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:97:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -67686,7 +67653,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:98:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -67708,7 +67675,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:99:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -67730,7 +67697,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:100:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -67752,7 +67719,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:101:Image1</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -67796,7 +67763,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:103:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -67818,7 +67785,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:104:Image1</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -67840,7 +67807,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:105:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -67862,7 +67829,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:106:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -67906,7 +67873,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:108:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -67928,7 +67895,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:109:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -67991,7 +67958,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image1</t>
+          <t>http://example.com/organization0:Image0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -68027,7 +67994,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization2:Image1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -68045,7 +68012,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image1:Thumbnail200x200</t>
+          <t>http://example.com/organization3:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -68063,7 +68030,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image1:Thumbnail600x600</t>
+          <t>http://example.com/organization4:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">

</xml_diff>

<commit_message>
SyntheticDataPipeline: add descriptions to all works
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -490,7 +490,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image1:Thumbnail400x400</t>
+          <t>http://example.com/organization1:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image0:Thumbnail600x600</t>
+          <t>http://example.com/organization3:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -610,14 +610,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
         </is>
       </c>
     </row>
@@ -742,7 +742,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image1</t>
+          <t>http://example.com/person0:Image0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -775,7 +775,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image0</t>
+          <t>http://example.com/person2:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -803,7 +803,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image0:Thumbnail200x200</t>
+          <t>http://example.com/person4:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -882,7 +882,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image0:Thumbnail200x200</t>
+          <t>http://example.com/person1:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -914,7 +914,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0</t>
+          <t>http://example.com/person3:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person5:Image1</t>
+          <t>http://example.com/person5:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1189,7 +1189,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1201,150 +1201,6 @@
       <c r="A1" t="inlineStr">
         <is>
           <t>@graph</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>http://example.com/collection0/work1Opening</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>_:N35ffe8b5f6094364a8ce098c5bd5425f</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Collection0Work1 opening</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>http://example.com/collection0/work2Opening</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>_:Nc109597e217840ecb3b6b539a7e66938</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Collection0Work2 opening</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>http://example.com/collection1/work4Opening</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>_:N5464327a633b49b1a77615ef6cad5ba8</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Collection1Work4 opening</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>http://example.com/collection1/work5Opening</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>_:Nd180d76ebe64417faa612895144f432c</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Collection1Work5 opening</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>http://example.com/collection1/work7Opening</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>_:Nf870b94661cd4011aad4a8e144f7d494</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Collection1Work7 opening</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork8Opening</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>_:N98d2821caaaf4c3298421752a054f291</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>FreestandingWork8 opening</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork10Opening</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>_:N674b4312ad084ff8b80aea2393258380</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>FreestandingWork10 opening</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork11Opening</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>_:N1e119a360e93453a9c96c5e2e04cdbc2</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>FreestandingWork11 opening</t>
         </is>
       </c>
     </row>
@@ -1359,7 +1215,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1371,322 +1227,6 @@
       <c r="A1" t="inlineStr">
         <is>
           <t>@graph</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>http://example.com/collection0/work2</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>_:N7f522d30d4964ea292b9a7b19cd5e2c8</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>http://example.com/organization5</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Collection0Work2 alternative title 1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Collection0Work2Id1</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Collection0Work2 provenance</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>http://example.com/collection0/work2Opening</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>http://example.com/collection0/work2:Image0</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Collection0Work2 rights holder</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>http://example.com/collection0/work2Location</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>Collection0Work2</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>http://example.com/collection1/work4</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>_:N3ea2e7dba0ff411b9463cbe95fbb774c</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>http://example.com/person1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Collection1Work4 alternative title 0</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Collection1Work4Id1</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Collection1Work4 provenance</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>http://example.com/collection1/work4Creation</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>http://example.com/collection1/work4:Image0:Thumbnail800x800</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>Collection1Work4 rights holder</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>http://example.com/collection1/work4Location</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Collection1Work4</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork8</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>_:Nd64e73d17e4a4673a17f707e3355ee5d</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>http://example.com/person5</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>FreestandingWork8 alternative title 1</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>FreestandingWork8Id0</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>FreestandingWork8 provenance</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork8Opening</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork8:Image0</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>FreestandingWork8 rights holder</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork8Location</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>FreestandingWork8</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork10</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>_:Na97e17d0012640e2862de673834850bf</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>http://example.com/organization1</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>FreestandingWork10 alternative title 1</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>FreestandingWork10Id0</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>FreestandingWork10 provenance</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>_:Nb89fc9d10c884330afe8c1e3793267a9</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork10:Image1:Thumbnail800x800</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC-EDU/1.0/</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>FreestandingWork10 rights holder</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork10Location</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>FreestandingWork10</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71</t>
         </is>
       </c>
     </row>
@@ -1952,7 +1492,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -2718,7 +2258,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0:Thumbnail200x200</t>
+          <t>dcterms:extent:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -3101,7 +2641,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>dcterms:language:Image0:Thumbnail800x800</t>
+          <t>dcterms:language:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -3484,7 +3024,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image0:Thumbnail600x600</t>
+          <t>dcterms:medium:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -4633,7 +4173,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image0:Thumbnail600x600</t>
+          <t>dcterms:spatial:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -5016,7 +4556,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image0:Thumbnail600x600</t>
+          <t>dcterms:subject:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -5399,7 +4939,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>dcterms:title:Image0:Thumbnail600x600</t>
+          <t>dcterms:title:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
@@ -5782,7 +5322,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>dcterms:type:Image0:Thumbnail400x400</t>
+          <t>dcterms:type:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -6165,7 +5705,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>schema:spatial:Image0:Thumbnail200x200</t>
+          <t>schema:spatial:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
@@ -6548,7 +6088,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
@@ -6931,7 +6471,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
@@ -7314,7 +6854,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
@@ -7697,7 +7237,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
@@ -8080,7 +7620,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H150" t="inlineStr">
@@ -8463,7 +8003,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
@@ -8846,7 +8386,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
@@ -9995,7 +9535,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H195" t="inlineStr">
@@ -10378,7 +9918,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H204" t="inlineStr">
@@ -10761,7 +10301,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H213" t="inlineStr">
@@ -11144,7 +10684,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H222" t="inlineStr">
@@ -11910,7 +11450,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H240" t="inlineStr">
@@ -12676,7 +12216,7 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H258" t="inlineStr">
@@ -13059,7 +12599,7 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H267" t="inlineStr">
@@ -13442,7 +12982,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H276" t="inlineStr">
@@ -13825,7 +13365,7 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H285" t="inlineStr">
@@ -14208,7 +13748,7 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H294" t="inlineStr">
@@ -14591,7 +14131,7 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H303" t="inlineStr">
@@ -14974,7 +14514,7 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H312" t="inlineStr">
@@ -15357,7 +14897,7 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H321" t="inlineStr">
@@ -15740,7 +15280,7 @@
       </c>
       <c r="G330" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H330" t="inlineStr">
@@ -16506,7 +16046,7 @@
       </c>
       <c r="G348" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H348" t="inlineStr">
@@ -17272,7 +16812,7 @@
       </c>
       <c r="G366" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H366" t="inlineStr">
@@ -18038,7 +17578,7 @@
       </c>
       <c r="G384" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H384" t="inlineStr">
@@ -18421,7 +17961,7 @@
       </c>
       <c r="G393" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H393" t="inlineStr">
@@ -18804,7 +18344,7 @@
       </c>
       <c r="G402" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H402" t="inlineStr">
@@ -19187,7 +18727,7 @@
       </c>
       <c r="G411" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H411" t="inlineStr">
@@ -19570,7 +19110,7 @@
       </c>
       <c r="G420" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H420" t="inlineStr">
@@ -19953,7 +19493,7 @@
       </c>
       <c r="G429" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H429" t="inlineStr">
@@ -20719,7 +20259,7 @@
       </c>
       <c r="G447" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H447" t="inlineStr">
@@ -21485,7 +21025,7 @@
       </c>
       <c r="G465" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H465" t="inlineStr">
@@ -21868,7 +21408,7 @@
       </c>
       <c r="G474" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H474" t="inlineStr">
@@ -22251,7 +21791,7 @@
       </c>
       <c r="G483" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H483" t="inlineStr">
@@ -23783,7 +23323,7 @@
       </c>
       <c r="G519" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H519" t="inlineStr">
@@ -24166,7 +23706,7 @@
       </c>
       <c r="G528" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H528" t="inlineStr">
@@ -24549,7 +24089,7 @@
       </c>
       <c r="G537" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H537" t="inlineStr">
@@ -25698,7 +25238,7 @@
       </c>
       <c r="G564" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H564" t="inlineStr">
@@ -26847,7 +26387,7 @@
       </c>
       <c r="G591" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H591" t="inlineStr">
@@ -27230,7 +26770,7 @@
       </c>
       <c r="G600" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H600" t="inlineStr">
@@ -27613,7 +27153,7 @@
       </c>
       <c r="G609" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H609" t="inlineStr">
@@ -28379,7 +27919,7 @@
       </c>
       <c r="G627" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H627" t="inlineStr">
@@ -29145,7 +28685,7 @@
       </c>
       <c r="G645" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H645" t="inlineStr">
@@ -29528,7 +29068,7 @@
       </c>
       <c r="G654" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H654" t="inlineStr">
@@ -29911,7 +29451,7 @@
       </c>
       <c r="G663" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H663" t="inlineStr">
@@ -30294,7 +29834,7 @@
       </c>
       <c r="G672" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H672" t="inlineStr">
@@ -30677,7 +30217,7 @@
       </c>
       <c r="G681" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H681" t="inlineStr">
@@ -31060,7 +30600,7 @@
       </c>
       <c r="G690" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H690" t="inlineStr">
@@ -31443,7 +30983,7 @@
       </c>
       <c r="G699" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H699" t="inlineStr">
@@ -31826,7 +31366,7 @@
       </c>
       <c r="G708" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H708" t="inlineStr">
@@ -32975,7 +32515,7 @@
       </c>
       <c r="G735" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H735" t="inlineStr">
@@ -33741,7 +33281,7 @@
       </c>
       <c r="G753" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H753" t="inlineStr">
@@ -34507,7 +34047,7 @@
       </c>
       <c r="G771" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H771" t="inlineStr">
@@ -34890,7 +34430,7 @@
       </c>
       <c r="G780" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H780" t="inlineStr">
@@ -35273,7 +34813,7 @@
       </c>
       <c r="G789" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H789" t="inlineStr">
@@ -35656,7 +35196,7 @@
       </c>
       <c r="G798" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H798" t="inlineStr">
@@ -36039,7 +35579,7 @@
       </c>
       <c r="G807" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H807" t="inlineStr">
@@ -36422,7 +35962,7 @@
       </c>
       <c r="G816" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H816" t="inlineStr">
@@ -36805,7 +36345,7 @@
       </c>
       <c r="G825" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H825" t="inlineStr">
@@ -37188,7 +36728,7 @@
       </c>
       <c r="G834" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H834" t="inlineStr">
@@ -37571,7 +37111,7 @@
       </c>
       <c r="G843" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H843" t="inlineStr">
@@ -37954,7 +37494,7 @@
       </c>
       <c r="G852" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H852" t="inlineStr">
@@ -38337,7 +37877,7 @@
       </c>
       <c r="G861" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H861" t="inlineStr">
@@ -38720,7 +38260,7 @@
       </c>
       <c r="G870" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H870" t="inlineStr">
@@ -39486,7 +39026,7 @@
       </c>
       <c r="G888" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H888" t="inlineStr">
@@ -39869,7 +39409,7 @@
       </c>
       <c r="G897" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H897" t="inlineStr">
@@ -40252,7 +39792,7 @@
       </c>
       <c r="G906" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H906" t="inlineStr">
@@ -40635,7 +40175,7 @@
       </c>
       <c r="G915" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H915" t="inlineStr">
@@ -41018,7 +40558,7 @@
       </c>
       <c r="G924" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0:Thumbnail200x200</t>
+          <t>http://example.com/organization0:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H924" t="inlineStr">
@@ -41784,7 +41324,7 @@
       </c>
       <c r="G942" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization2:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H942" t="inlineStr">
@@ -42167,7 +41707,7 @@
       </c>
       <c r="G951" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image0:Thumbnail800x800</t>
+          <t>http://example.com/organization3:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H951" t="inlineStr">
@@ -42550,7 +42090,7 @@
       </c>
       <c r="G960" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0:Thumbnail800x800</t>
+          <t>http://example.com/organization4:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H960" t="inlineStr">
@@ -42933,7 +42473,7 @@
       </c>
       <c r="G969" t="inlineStr">
         <is>
-          <t>http://example.com/organization5:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization5:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H969" t="inlineStr">
@@ -43316,7 +42856,7 @@
       </c>
       <c r="G978" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image0:Thumbnail600x600</t>
+          <t>http://example.com/person0:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H978" t="inlineStr">
@@ -43731,7 +43271,7 @@
       </c>
       <c r="G988" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image0:Thumbnail400x400</t>
+          <t>http://example.com/person1:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H988" t="inlineStr">
@@ -44114,7 +43654,7 @@
       </c>
       <c r="G997" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image0:Thumbnail400x400</t>
+          <t>http://example.com/person2:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H997" t="inlineStr">
@@ -44497,7 +44037,7 @@
       </c>
       <c r="G1006" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0:Thumbnail600x600</t>
+          <t>http://example.com/person3:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1006" t="inlineStr">
@@ -44880,7 +44420,7 @@
       </c>
       <c r="G1015" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image0:Thumbnail800x800</t>
+          <t>http://example.com/person4:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1015" t="inlineStr">
@@ -45263,7 +44803,7 @@
       </c>
       <c r="G1024" t="inlineStr">
         <is>
-          <t>http://example.com/person5:Image0:Thumbnail800x800</t>
+          <t>http://example.com/person5:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1024" t="inlineStr">
@@ -45646,7 +45186,7 @@
       </c>
       <c r="G1033" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work0:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1033" t="inlineStr">
@@ -46066,7 +45606,7 @@
       </c>
       <c r="G1043" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image0:Thumbnail600x600</t>
+          <t>http://example.com/collection0/work1:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1043" t="inlineStr">
@@ -46449,7 +45989,7 @@
       </c>
       <c r="G1052" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2:Image0:Thumbnail600x600</t>
+          <t>http://example.com/collection0/work2:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1052" t="inlineStr">
@@ -46832,7 +46372,7 @@
       </c>
       <c r="G1061" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image0:Thumbnail800x800</t>
+          <t>http://example.com/collection0/work3:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1061" t="inlineStr">
@@ -47215,7 +46755,7 @@
       </c>
       <c r="G1070" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image0:Thumbnail800x800</t>
+          <t>http://example.com/collection1:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1070" t="inlineStr">
@@ -47598,7 +47138,7 @@
       </c>
       <c r="G1079" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4:Image0:Thumbnail600x600</t>
+          <t>http://example.com/collection1/work4:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1079" t="inlineStr">
@@ -48747,7 +48287,7 @@
       </c>
       <c r="G1106" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection1/work7:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1106" t="inlineStr">
@@ -49513,7 +49053,7 @@
       </c>
       <c r="G1124" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:Image0:Thumbnail200x200</t>
+          <t>http://example.com/freestandingwork9:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1124" t="inlineStr">
@@ -49896,7 +49436,7 @@
       </c>
       <c r="G1133" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10:Image0:Thumbnail800x800</t>
+          <t>http://example.com/freestandingwork10:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1133" t="inlineStr">
@@ -50279,7 +49819,7 @@
       </c>
       <c r="G1142" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:Image0:Thumbnail800x800</t>
+          <t>http://example.com/freestandingwork11:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1142" t="inlineStr">
@@ -50629,7 +50169,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dcterms:description:Image0:Thumbnail200x200</t>
+          <t>dcterms:description:Image0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -50661,7 +50201,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0:Thumbnail200x200</t>
+          <t>dcterms:extent:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -50693,7 +50233,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dcterms:language:Image0:Thumbnail600x600</t>
+          <t>dcterms:language:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -50725,7 +50265,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image0:Thumbnail600x600</t>
+          <t>dcterms:medium:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -50757,7 +50297,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image0:Thumbnail200x200</t>
+          <t>dcterms:publisher:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -50789,7 +50329,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>dcterms:source:Image1:Thumbnail200x200</t>
+          <t>dcterms:source:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -50821,7 +50361,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image1:Thumbnail400x400</t>
+          <t>dcterms:spatial:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -50853,7 +50393,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image0:Thumbnail600x600</t>
+          <t>dcterms:subject:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -50885,7 +50425,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dcterms:title:Image1:Thumbnail600x600</t>
+          <t>dcterms:title:Image1</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -50917,7 +50457,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>dcterms:type:Image1</t>
+          <t>dcterms:type:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -51000,7 +50540,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://schema.org/spatial:Image0:Thumbnail200x200</t>
+          <t>https://schema.org/spatial:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -51069,7 +50609,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -51127,7 +50667,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -51171,7 +50711,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -51193,7 +50733,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -51215,7 +50755,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -51237,7 +50777,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -51259,7 +50799,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -51281,7 +50821,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -51303,7 +50843,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -51347,7 +50887,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -51369,7 +50909,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -51391,7 +50931,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -51435,7 +50975,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -51457,7 +50997,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -51501,7 +51041,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -51523,7 +51063,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -51545,7 +51085,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -51567,7 +51107,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -51589,7 +51129,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -51633,7 +51173,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -51655,7 +51195,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -51677,7 +51217,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -51699,7 +51239,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -51743,7 +51283,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -51765,7 +51305,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -51787,7 +51327,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -51809,7 +51349,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -51831,7 +51371,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -51853,7 +51393,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -51875,7 +51415,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -51897,7 +51437,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -51919,7 +51459,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -51941,7 +51481,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -51985,7 +51525,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -52007,7 +51547,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -52029,7 +51569,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -52051,7 +51591,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -52073,7 +51613,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -52095,7 +51635,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -52117,7 +51657,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -52139,7 +51679,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -52161,7 +51701,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -52183,7 +51723,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -52205,7 +51745,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -52227,7 +51767,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -52249,7 +51789,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -52271,7 +51811,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -52293,7 +51833,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -52315,7 +51855,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -52337,7 +51877,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -52359,7 +51899,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -52381,7 +51921,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -52403,7 +51943,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -52425,7 +51965,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -52447,7 +51987,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -52491,7 +52031,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -52513,7 +52053,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -52535,7 +52075,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -52557,7 +52097,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -52579,7 +52119,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -52601,7 +52141,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -52623,7 +52163,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -52645,7 +52185,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -52689,7 +52229,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -52711,7 +52251,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -52733,7 +52273,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -52755,7 +52295,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -52777,7 +52317,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -52799,7 +52339,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -52821,7 +52361,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -52843,7 +52383,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -52865,7 +52405,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -52940,7 +52480,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -52957,7 +52497,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -52974,7 +52514,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -52991,7 +52531,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -53008,7 +52548,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -53025,7 +52565,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -53042,7 +52582,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -53076,7 +52616,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -53134,7 +52674,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization0:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -53152,7 +52692,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image1:Thumbnail400x400</t>
+          <t>http://example.com/organization2:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -53170,7 +52710,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization4:Image0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">

</xml_diff>

<commit_message>
ResourceBackedModel: add other Resource's directly, to get blank nodes
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -490,7 +490,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization1:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image0</t>
+          <t>http://example.com/organization3:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -534,7 +534,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization5:Image0:Thumbnail200x200</t>
+          <t>http://example.com/organization5:Image0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -610,21 +610,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
+          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
         </is>
       </c>
     </row>
@@ -742,7 +742,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image0:Thumbnail400x400</t>
+          <t>http://example.com/person0:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -775,7 +775,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image0:Thumbnail800x800</t>
+          <t>http://example.com/person2:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -803,7 +803,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image0:Thumbnail400x400</t>
+          <t>http://example.com/person4:Image0</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -882,7 +882,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image1:Thumbnail600x600</t>
+          <t>http://example.com/person1:Image0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -914,7 +914,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0:Thumbnail800x800</t>
+          <t>http://example.com/person3:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person5:Image1</t>
+          <t>http://example.com/person5:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0:Thumbnail400x400</t>
+          <t>dcterms:extent:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2641,7 +2641,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>dcterms:language:Image0:Thumbnail600x600</t>
+          <t>dcterms:language:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>dcterms:source:Image0:Thumbnail200x200</t>
+          <t>dcterms:source:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -4173,7 +4173,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image0:Thumbnail200x200</t>
+          <t>dcterms:spatial:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -4556,7 +4556,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image0:Thumbnail800x800</t>
+          <t>dcterms:subject:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -5322,7 +5322,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>dcterms:type:Image0:Thumbnail600x600</t>
+          <t>dcterms:type:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -6088,7 +6088,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>schema:name:Image0:Thumbnail800x800</t>
+          <t>schema:name:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
@@ -6471,7 +6471,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>schema:spatial:Image0:Thumbnail200x200</t>
+          <t>schema:spatial:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
@@ -6854,7 +6854,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
@@ -7237,7 +7237,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
@@ -7620,7 +7620,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H150" t="inlineStr">
@@ -8003,7 +8003,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
@@ -8386,7 +8386,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
@@ -8769,7 +8769,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H177" t="inlineStr">
@@ -9152,7 +9152,7 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H186" t="inlineStr">
@@ -9535,7 +9535,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H195" t="inlineStr">
@@ -9918,7 +9918,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H204" t="inlineStr">
@@ -10301,7 +10301,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H213" t="inlineStr">
@@ -10684,7 +10684,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H222" t="inlineStr">
@@ -11833,7 +11833,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H249" t="inlineStr">
@@ -12599,7 +12599,7 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H267" t="inlineStr">
@@ -12982,7 +12982,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H276" t="inlineStr">
@@ -13365,7 +13365,7 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H285" t="inlineStr">
@@ -13748,7 +13748,7 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H294" t="inlineStr">
@@ -14131,7 +14131,7 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H303" t="inlineStr">
@@ -14514,7 +14514,7 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H312" t="inlineStr">
@@ -14897,7 +14897,7 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H321" t="inlineStr">
@@ -15280,7 +15280,7 @@
       </c>
       <c r="G330" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H330" t="inlineStr">
@@ -15663,7 +15663,7 @@
       </c>
       <c r="G339" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H339" t="inlineStr">
@@ -16046,7 +16046,7 @@
       </c>
       <c r="G348" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H348" t="inlineStr">
@@ -16429,7 +16429,7 @@
       </c>
       <c r="G357" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H357" t="inlineStr">
@@ -16812,7 +16812,7 @@
       </c>
       <c r="G366" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H366" t="inlineStr">
@@ -17578,7 +17578,7 @@
       </c>
       <c r="G384" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H384" t="inlineStr">
@@ -17961,7 +17961,7 @@
       </c>
       <c r="G393" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H393" t="inlineStr">
@@ -18344,7 +18344,7 @@
       </c>
       <c r="G402" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H402" t="inlineStr">
@@ -18727,7 +18727,7 @@
       </c>
       <c r="G411" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H411" t="inlineStr">
@@ -19110,7 +19110,7 @@
       </c>
       <c r="G420" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H420" t="inlineStr">
@@ -19493,7 +19493,7 @@
       </c>
       <c r="G429" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H429" t="inlineStr">
@@ -20259,7 +20259,7 @@
       </c>
       <c r="G447" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H447" t="inlineStr">
@@ -20642,7 +20642,7 @@
       </c>
       <c r="G456" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H456" t="inlineStr">
@@ -21025,7 +21025,7 @@
       </c>
       <c r="G465" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H465" t="inlineStr">
@@ -21408,7 +21408,7 @@
       </c>
       <c r="G474" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H474" t="inlineStr">
@@ -21791,7 +21791,7 @@
       </c>
       <c r="G483" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H483" t="inlineStr">
@@ -22940,7 +22940,7 @@
       </c>
       <c r="G510" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H510" t="inlineStr">
@@ -23323,7 +23323,7 @@
       </c>
       <c r="G519" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H519" t="inlineStr">
@@ -23706,7 +23706,7 @@
       </c>
       <c r="G528" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H528" t="inlineStr">
@@ -24089,7 +24089,7 @@
       </c>
       <c r="G537" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H537" t="inlineStr">
@@ -24472,7 +24472,7 @@
       </c>
       <c r="G546" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H546" t="inlineStr">
@@ -24855,7 +24855,7 @@
       </c>
       <c r="G555" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H555" t="inlineStr">
@@ -25238,7 +25238,7 @@
       </c>
       <c r="G564" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H564" t="inlineStr">
@@ -25621,7 +25621,7 @@
       </c>
       <c r="G573" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H573" t="inlineStr">
@@ -26004,7 +26004,7 @@
       </c>
       <c r="G582" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H582" t="inlineStr">
@@ -26770,7 +26770,7 @@
       </c>
       <c r="G600" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H600" t="inlineStr">
@@ -27153,7 +27153,7 @@
       </c>
       <c r="G609" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H609" t="inlineStr">
@@ -27536,7 +27536,7 @@
       </c>
       <c r="G618" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H618" t="inlineStr">
@@ -27919,7 +27919,7 @@
       </c>
       <c r="G627" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H627" t="inlineStr">
@@ -28685,7 +28685,7 @@
       </c>
       <c r="G645" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H645" t="inlineStr">
@@ -29068,7 +29068,7 @@
       </c>
       <c r="G654" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H654" t="inlineStr">
@@ -29451,7 +29451,7 @@
       </c>
       <c r="G663" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H663" t="inlineStr">
@@ -29834,7 +29834,7 @@
       </c>
       <c r="G672" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H672" t="inlineStr">
@@ -30217,7 +30217,7 @@
       </c>
       <c r="G681" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H681" t="inlineStr">
@@ -30600,7 +30600,7 @@
       </c>
       <c r="G690" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H690" t="inlineStr">
@@ -30983,7 +30983,7 @@
       </c>
       <c r="G699" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H699" t="inlineStr">
@@ -31366,7 +31366,7 @@
       </c>
       <c r="G708" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H708" t="inlineStr">
@@ -31749,7 +31749,7 @@
       </c>
       <c r="G717" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H717" t="inlineStr">
@@ -32132,7 +32132,7 @@
       </c>
       <c r="G726" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H726" t="inlineStr">
@@ -32515,7 +32515,7 @@
       </c>
       <c r="G735" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H735" t="inlineStr">
@@ -32898,7 +32898,7 @@
       </c>
       <c r="G744" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H744" t="inlineStr">
@@ -33281,7 +33281,7 @@
       </c>
       <c r="G753" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H753" t="inlineStr">
@@ -33664,7 +33664,7 @@
       </c>
       <c r="G762" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H762" t="inlineStr">
@@ -34430,7 +34430,7 @@
       </c>
       <c r="G780" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H780" t="inlineStr">
@@ -34813,7 +34813,7 @@
       </c>
       <c r="G789" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H789" t="inlineStr">
@@ -35196,7 +35196,7 @@
       </c>
       <c r="G798" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H798" t="inlineStr">
@@ -35579,7 +35579,7 @@
       </c>
       <c r="G807" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H807" t="inlineStr">
@@ -35962,7 +35962,7 @@
       </c>
       <c r="G816" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H816" t="inlineStr">
@@ -36345,7 +36345,7 @@
       </c>
       <c r="G825" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H825" t="inlineStr">
@@ -36728,7 +36728,7 @@
       </c>
       <c r="G834" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H834" t="inlineStr">
@@ -37111,7 +37111,7 @@
       </c>
       <c r="G843" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H843" t="inlineStr">
@@ -37877,7 +37877,7 @@
       </c>
       <c r="G861" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H861" t="inlineStr">
@@ -38643,7 +38643,7 @@
       </c>
       <c r="G879" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H879" t="inlineStr">
@@ -39792,7 +39792,7 @@
       </c>
       <c r="G906" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H906" t="inlineStr">
@@ -40175,7 +40175,7 @@
       </c>
       <c r="G915" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H915" t="inlineStr">
@@ -40558,7 +40558,7 @@
       </c>
       <c r="G924" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H924" t="inlineStr">
@@ -41324,7 +41324,7 @@
       </c>
       <c r="G942" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0:Thumbnail800x800</t>
+          <t>http://example.com/organization0:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H942" t="inlineStr">
@@ -42090,7 +42090,7 @@
       </c>
       <c r="G960" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0:Thumbnail800x800</t>
+          <t>http://example.com/organization2:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H960" t="inlineStr">
@@ -42856,7 +42856,7 @@
       </c>
       <c r="G978" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0:Thumbnail600x600</t>
+          <t>http://example.com/organization4:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H978" t="inlineStr">
@@ -43622,7 +43622,7 @@
       </c>
       <c r="G996" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image0:Thumbnail200x200</t>
+          <t>http://example.com/person0:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H996" t="inlineStr">
@@ -44420,7 +44420,7 @@
       </c>
       <c r="G1015" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image0:Thumbnail400x400</t>
+          <t>http://example.com/person2:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1015" t="inlineStr">
@@ -45569,7 +45569,7 @@
       </c>
       <c r="G1042" t="inlineStr">
         <is>
-          <t>http://example.com/person5:Image0:Thumbnail800x800</t>
+          <t>http://example.com/person5:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1042" t="inlineStr">
@@ -45952,7 +45952,7 @@
       </c>
       <c r="G1051" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0:Image0:Thumbnail800x800</t>
+          <t>http://example.com/collection0/work0:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1051" t="inlineStr">
@@ -46755,7 +46755,7 @@
       </c>
       <c r="G1070" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work2:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1070" t="inlineStr">
@@ -47138,7 +47138,7 @@
       </c>
       <c r="G1079" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image0:Thumbnail800x800</t>
+          <t>http://example.com/collection0/work3:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1079" t="inlineStr">
@@ -47521,7 +47521,7 @@
       </c>
       <c r="G1088" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection1:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1088" t="inlineStr">
@@ -48670,7 +48670,7 @@
       </c>
       <c r="G1115" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6:Image0:Thumbnail800x800</t>
+          <t>http://example.com/collection1/work6:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1115" t="inlineStr">
@@ -49053,7 +49053,7 @@
       </c>
       <c r="G1124" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image0:Thumbnail600x600</t>
+          <t>http://example.com/collection1/work7:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1124" t="inlineStr">
@@ -49436,7 +49436,7 @@
       </c>
       <c r="G1133" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8:Image0:Thumbnail600x600</t>
+          <t>http://example.com/freestandingwork8:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1133" t="inlineStr">
@@ -49819,7 +49819,7 @@
       </c>
       <c r="G1142" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:Image0:Thumbnail400x400</t>
+          <t>http://example.com/freestandingwork9:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1142" t="inlineStr">
@@ -50935,7 +50935,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dcterms:description:Image1:Thumbnail400x400</t>
+          <t>dcterms:description:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -50967,7 +50967,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0:Thumbnail400x400</t>
+          <t>dcterms:extent:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -50999,7 +50999,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dcterms:language:Image1:Thumbnail400x400</t>
+          <t>dcterms:language:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -51031,7 +51031,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image1:Thumbnail200x200</t>
+          <t>dcterms:medium:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -51063,7 +51063,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image1:Thumbnail200x200</t>
+          <t>dcterms:publisher:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -51095,7 +51095,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>dcterms:source:Image1:Thumbnail400x400</t>
+          <t>dcterms:source:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -51159,7 +51159,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image0:Thumbnail400x400</t>
+          <t>dcterms:subject:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -51191,7 +51191,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dcterms:title:Image0:Thumbnail200x200</t>
+          <t>dcterms:title:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -51223,7 +51223,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>dcterms:type:Image1:Thumbnail800x800</t>
+          <t>dcterms:type:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -51338,7 +51338,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://schema.org/name:Image0:Thumbnail400x400</t>
+          <t>https://schema.org/name:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -51370,7 +51370,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://schema.org/spatial:Image0:Thumbnail400x400</t>
+          <t>https://schema.org/spatial:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -51439,7 +51439,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -51497,7 +51497,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -51541,7 +51541,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -51563,7 +51563,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -51585,7 +51585,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -51607,7 +51607,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -51629,7 +51629,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -51651,7 +51651,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -51695,7 +51695,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -51717,7 +51717,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -51739,7 +51739,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -51761,7 +51761,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -51783,7 +51783,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -51805,7 +51805,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -51827,7 +51827,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -51849,7 +51849,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -51871,7 +51871,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -51893,7 +51893,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -51915,7 +51915,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -51937,7 +51937,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -51959,7 +51959,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -51981,7 +51981,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -52047,7 +52047,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -52069,7 +52069,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -52091,7 +52091,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -52113,7 +52113,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -52135,7 +52135,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -52157,7 +52157,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -52179,7 +52179,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -52223,7 +52223,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -52245,7 +52245,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -52267,7 +52267,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -52311,7 +52311,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -52377,7 +52377,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -52399,7 +52399,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -52421,7 +52421,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -52509,7 +52509,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -52531,7 +52531,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -52553,7 +52553,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -52575,7 +52575,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -52641,7 +52641,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -52663,7 +52663,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -52707,7 +52707,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -52729,7 +52729,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -52773,7 +52773,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -52795,7 +52795,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -52817,7 +52817,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -52839,7 +52839,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -52883,7 +52883,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -52905,7 +52905,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -52927,7 +52927,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -52949,7 +52949,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -52993,7 +52993,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -53015,7 +53015,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -53037,7 +53037,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -53059,7 +53059,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -53081,7 +53081,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -53103,7 +53103,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -53125,7 +53125,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -53169,7 +53169,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -53213,7 +53213,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -53235,7 +53235,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -53293,7 +53293,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -53310,7 +53310,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -53327,7 +53327,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -53344,7 +53344,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -53361,7 +53361,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -53378,7 +53378,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -53395,7 +53395,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -53412,7 +53412,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -53429,7 +53429,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -53446,7 +53446,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -53504,7 +53504,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0:Thumbnail200x200</t>
+          <t>http://example.com/organization0:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -53522,7 +53522,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image1:Thumbnail600x600</t>
+          <t>http://example.com/organization2:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -53540,7 +53540,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0:Thumbnail600x600</t>
+          <t>http://example.com/organization4:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">

</xml_diff>

<commit_message>
SyntheticDataPipeline: generate named schema:Place's
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -26,9 +26,10 @@
     <sheet name="CmsWorkCreation" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="CmsWorkOpening" sheetId="18" state="visible" r:id="rId18"/>
     <sheet name="CmsWork" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="SchemaCreativeWork" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="CmsCollection" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="SchemaCollection" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="SchemaPlace" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="SchemaCreativeWork" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="CmsCollection" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="SchemaCollection" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -490,7 +491,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image1:Thumbnail600x600</t>
+          <t>http://example.com/organization1:Image1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -512,7 +513,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image1:Thumbnail600x600</t>
+          <t>http://example.com/organization3:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -534,7 +535,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization5:Image0</t>
+          <t>http://example.com/organization5:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -610,14 +611,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
         </is>
       </c>
     </row>
@@ -742,7 +743,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image1:Thumbnail400x400</t>
+          <t>http://example.com/person0:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -775,7 +776,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image1:Thumbnail200x200</t>
+          <t>http://example.com/person2:Image0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -803,7 +804,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image0</t>
+          <t>http://example.com/person4:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -882,7 +883,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image0</t>
+          <t>http://example.com/person1:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -914,7 +915,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0:Thumbnail200x200</t>
+          <t>http://example.com/person3:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -946,7 +947,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person5:Image0:Thumbnail600x600</t>
+          <t>http://example.com/person5:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -971,7 +972,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1012,7 +1013,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1Location</t>
+          <t>http://example.com/collection0/work2Location</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1025,7 +1026,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2Location</t>
+          <t>http://example.com/collection1/work4Location</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1038,7 +1039,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3Location</t>
+          <t>http://example.com/collection1/work6Location</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1051,7 +1052,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4Location</t>
+          <t>http://example.com/freestandingwork8Location</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1064,91 +1065,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5Location</t>
+          <t>http://example.com/freestandingwork10Location</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>42.728104</v>
       </c>
       <c r="C7" t="n">
-        <v>-73.68757600000001</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>http://example.com/collection1/work6Location</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>42.728104</v>
-      </c>
-      <c r="C8" t="n">
-        <v>-73.68757600000001</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>http://example.com/collection1/work7Location</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>42.728104</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-73.68757600000001</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork8Location</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>42.728104</v>
-      </c>
-      <c r="C10" t="n">
-        <v>-73.68757600000001</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork9Location</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>42.728104</v>
-      </c>
-      <c r="C11" t="n">
-        <v>-73.68757600000001</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork10Location</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>42.728104</v>
-      </c>
-      <c r="C12" t="n">
-        <v>-73.68757600000001</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork11Location</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>42.728104</v>
-      </c>
-      <c r="C13" t="n">
         <v>-73.68757600000001</v>
       </c>
     </row>
@@ -1875,7 +1798,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>dcterms:description:Image0:Thumbnail400x400</t>
+          <t>dcterms:description:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -2258,7 +2181,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0:Thumbnail200x200</t>
+          <t>dcterms:extent:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2641,7 +2564,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>dcterms:language:Image0:Thumbnail200x200</t>
+          <t>dcterms:language:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -3407,7 +3330,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image0:Thumbnail400x400</t>
+          <t>dcterms:publisher:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -4173,7 +4096,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image0:Thumbnail400x400</t>
+          <t>dcterms:spatial:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -4556,7 +4479,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image0:Thumbnail600x600</t>
+          <t>dcterms:subject:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -4939,7 +4862,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>dcterms:title:Image0:Thumbnail600x600</t>
+          <t>dcterms:title:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
@@ -5322,7 +5245,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>dcterms:type:Image0:Thumbnail400x400</t>
+          <t>dcterms:type:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -5705,7 +5628,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>schema:description:Image0:Thumbnail400x400</t>
+          <t>schema:description:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
@@ -6088,7 +6011,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>schema:name:Image0:Thumbnail400x400</t>
+          <t>schema:name:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
@@ -7620,7 +7543,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H150" t="inlineStr">
@@ -8003,7 +7926,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
@@ -8769,7 +8692,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H177" t="inlineStr">
@@ -9918,7 +9841,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H204" t="inlineStr">
@@ -10684,7 +10607,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H222" t="inlineStr">
@@ -11067,7 +10990,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
@@ -11450,7 +11373,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H240" t="inlineStr">
@@ -11833,7 +11756,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H249" t="inlineStr">
@@ -12216,7 +12139,7 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H258" t="inlineStr">
@@ -12982,7 +12905,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H276" t="inlineStr">
@@ -13365,7 +13288,7 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H285" t="inlineStr">
@@ -13748,7 +13671,7 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H294" t="inlineStr">
@@ -14514,7 +14437,7 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H312" t="inlineStr">
@@ -14897,7 +14820,7 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H321" t="inlineStr">
@@ -15280,7 +15203,7 @@
       </c>
       <c r="G330" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H330" t="inlineStr">
@@ -15663,7 +15586,7 @@
       </c>
       <c r="G339" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H339" t="inlineStr">
@@ -16046,7 +15969,7 @@
       </c>
       <c r="G348" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H348" t="inlineStr">
@@ -16429,7 +16352,7 @@
       </c>
       <c r="G357" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H357" t="inlineStr">
@@ -16812,7 +16735,7 @@
       </c>
       <c r="G366" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H366" t="inlineStr">
@@ -17195,7 +17118,7 @@
       </c>
       <c r="G375" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H375" t="inlineStr">
@@ -17578,7 +17501,7 @@
       </c>
       <c r="G384" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H384" t="inlineStr">
@@ -18344,7 +18267,7 @@
       </c>
       <c r="G402" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H402" t="inlineStr">
@@ -18727,7 +18650,7 @@
       </c>
       <c r="G411" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H411" t="inlineStr">
@@ -19110,7 +19033,7 @@
       </c>
       <c r="G420" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H420" t="inlineStr">
@@ -19493,7 +19416,7 @@
       </c>
       <c r="G429" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H429" t="inlineStr">
@@ -20259,7 +20182,7 @@
       </c>
       <c r="G447" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H447" t="inlineStr">
@@ -20642,7 +20565,7 @@
       </c>
       <c r="G456" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H456" t="inlineStr">
@@ -21025,7 +20948,7 @@
       </c>
       <c r="G465" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H465" t="inlineStr">
@@ -21791,7 +21714,7 @@
       </c>
       <c r="G483" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H483" t="inlineStr">
@@ -22174,7 +22097,7 @@
       </c>
       <c r="G492" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H492" t="inlineStr">
@@ -23323,7 +23246,7 @@
       </c>
       <c r="G519" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H519" t="inlineStr">
@@ -24089,7 +24012,7 @@
       </c>
       <c r="G537" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H537" t="inlineStr">
@@ -24472,7 +24395,7 @@
       </c>
       <c r="G546" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H546" t="inlineStr">
@@ -24855,7 +24778,7 @@
       </c>
       <c r="G555" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H555" t="inlineStr">
@@ -25238,7 +25161,7 @@
       </c>
       <c r="G564" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H564" t="inlineStr">
@@ -25621,7 +25544,7 @@
       </c>
       <c r="G573" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H573" t="inlineStr">
@@ -26004,7 +25927,7 @@
       </c>
       <c r="G582" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H582" t="inlineStr">
@@ -27153,7 +27076,7 @@
       </c>
       <c r="G609" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H609" t="inlineStr">
@@ -27536,7 +27459,7 @@
       </c>
       <c r="G618" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H618" t="inlineStr">
@@ -27919,7 +27842,7 @@
       </c>
       <c r="G627" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H627" t="inlineStr">
@@ -28302,7 +28225,7 @@
       </c>
       <c r="G636" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H636" t="inlineStr">
@@ -29451,7 +29374,7 @@
       </c>
       <c r="G663" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H663" t="inlineStr">
@@ -30217,7 +30140,7 @@
       </c>
       <c r="G681" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H681" t="inlineStr">
@@ -30600,7 +30523,7 @@
       </c>
       <c r="G690" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H690" t="inlineStr">
@@ -31366,7 +31289,7 @@
       </c>
       <c r="G708" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H708" t="inlineStr">
@@ -31749,7 +31672,7 @@
       </c>
       <c r="G717" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H717" t="inlineStr">
@@ -32132,7 +32055,7 @@
       </c>
       <c r="G726" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H726" t="inlineStr">
@@ -32898,7 +32821,7 @@
       </c>
       <c r="G744" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H744" t="inlineStr">
@@ -33281,7 +33204,7 @@
       </c>
       <c r="G753" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H753" t="inlineStr">
@@ -33664,7 +33587,7 @@
       </c>
       <c r="G762" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H762" t="inlineStr">
@@ -34430,7 +34353,7 @@
       </c>
       <c r="G780" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H780" t="inlineStr">
@@ -34813,7 +34736,7 @@
       </c>
       <c r="G789" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H789" t="inlineStr">
@@ -35196,7 +35119,7 @@
       </c>
       <c r="G798" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H798" t="inlineStr">
@@ -35579,7 +35502,7 @@
       </c>
       <c r="G807" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H807" t="inlineStr">
@@ -35962,7 +35885,7 @@
       </c>
       <c r="G816" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H816" t="inlineStr">
@@ -36728,7 +36651,7 @@
       </c>
       <c r="G834" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H834" t="inlineStr">
@@ -37494,7 +37417,7 @@
       </c>
       <c r="G852" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H852" t="inlineStr">
@@ -37877,7 +37800,7 @@
       </c>
       <c r="G861" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H861" t="inlineStr">
@@ -38260,7 +38183,7 @@
       </c>
       <c r="G870" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H870" t="inlineStr">
@@ -38643,7 +38566,7 @@
       </c>
       <c r="G879" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H879" t="inlineStr">
@@ -39409,7 +39332,7 @@
       </c>
       <c r="G897" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H897" t="inlineStr">
@@ -39792,7 +39715,7 @@
       </c>
       <c r="G906" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H906" t="inlineStr">
@@ -40558,7 +40481,7 @@
       </c>
       <c r="G924" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H924" t="inlineStr">
@@ -40941,7 +40864,7 @@
       </c>
       <c r="G933" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H933" t="inlineStr">
@@ -41324,7 +41247,7 @@
       </c>
       <c r="G942" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0:Thumbnail600x600</t>
+          <t>http://example.com/organization0:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H942" t="inlineStr">
@@ -41707,7 +41630,7 @@
       </c>
       <c r="G951" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization1:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H951" t="inlineStr">
@@ -42090,7 +42013,7 @@
       </c>
       <c r="G960" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization2:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H960" t="inlineStr">
@@ -42856,7 +42779,7 @@
       </c>
       <c r="G978" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0:Thumbnail200x200</t>
+          <t>http://example.com/organization4:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H978" t="inlineStr">
@@ -43239,7 +43162,7 @@
       </c>
       <c r="G987" t="inlineStr">
         <is>
-          <t>http://example.com/organization5:Image0:Thumbnail800x800</t>
+          <t>http://example.com/organization5:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H987" t="inlineStr">
@@ -44037,7 +43960,7 @@
       </c>
       <c r="G1006" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image0:Thumbnail200x200</t>
+          <t>http://example.com/person1:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1006" t="inlineStr">
@@ -44420,7 +44343,7 @@
       </c>
       <c r="G1015" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image0:Thumbnail800x800</t>
+          <t>http://example.com/person2:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1015" t="inlineStr">
@@ -44803,7 +44726,7 @@
       </c>
       <c r="G1024" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0:Thumbnail200x200</t>
+          <t>http://example.com/person3:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1024" t="inlineStr">
@@ -45186,7 +45109,7 @@
       </c>
       <c r="G1033" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image0:Thumbnail200x200</t>
+          <t>http://example.com/person4:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1033" t="inlineStr">
@@ -45569,7 +45492,7 @@
       </c>
       <c r="G1042" t="inlineStr">
         <is>
-          <t>http://example.com/person5:Image0:Thumbnail400x400</t>
+          <t>http://example.com/person5:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1042" t="inlineStr">
@@ -45952,7 +45875,7 @@
       </c>
       <c r="G1051" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0:Image0:Thumbnail600x600</t>
+          <t>http://example.com/collection0/work0:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1051" t="inlineStr">
@@ -46372,7 +46295,7 @@
       </c>
       <c r="G1061" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work1:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1061" t="inlineStr">
@@ -46755,7 +46678,7 @@
       </c>
       <c r="G1070" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2:Image0:Thumbnail800x800</t>
+          <t>http://example.com/collection0/work2:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1070" t="inlineStr">
@@ -47138,7 +47061,7 @@
       </c>
       <c r="G1079" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work3:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1079" t="inlineStr">
@@ -47521,7 +47444,7 @@
       </c>
       <c r="G1088" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image0:Thumbnail600x600</t>
+          <t>http://example.com/collection1:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1088" t="inlineStr">
@@ -47904,7 +47827,7 @@
       </c>
       <c r="G1097" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4:Image0:Thumbnail400x400</t>
+          <t>http://example.com/collection1/work4:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1097" t="inlineStr">
@@ -48287,7 +48210,7 @@
       </c>
       <c r="G1106" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection1/work5:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1106" t="inlineStr">
@@ -48670,7 +48593,7 @@
       </c>
       <c r="G1115" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work6:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection1/work6:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1115" t="inlineStr">
@@ -49436,7 +49359,7 @@
       </c>
       <c r="G1133" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork8:Image0:Thumbnail400x400</t>
+          <t>http://example.com/freestandingwork8:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1133" t="inlineStr">
@@ -50585,7 +50508,7 @@
       </c>
       <c r="G1160" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:Image0:Thumbnail400x400</t>
+          <t>http://example.com/freestandingwork11:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1160" t="inlineStr">
@@ -50778,7 +50701,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -50789,7 +50712,49 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>@graph</t>
+          <t>@id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work1Location</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work3Location</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work5Location</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>http://example.com/collection1/work7Location</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork9Location</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>http://example.com/freestandingwork11Location</t>
         </is>
       </c>
     </row>
@@ -50850,6 +50815,32 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>@graph</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -50967,7 +50958,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0:Thumbnail200x200</t>
+          <t>dcterms:extent:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -50999,7 +50990,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dcterms:language:Image1:Thumbnail200x200</t>
+          <t>dcterms:language:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -51031,7 +51022,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image0:Thumbnail400x400</t>
+          <t>dcterms:medium:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -51063,7 +51054,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image1:Thumbnail400x400</t>
+          <t>dcterms:publisher:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -51095,7 +51086,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>dcterms:source:Image0:Thumbnail600x600</t>
+          <t>dcterms:source:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -51127,7 +51118,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image1:Thumbnail400x400</t>
+          <t>dcterms:spatial:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -51159,7 +51150,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image1:Thumbnail400x400</t>
+          <t>dcterms:subject:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -51191,7 +51182,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dcterms:title:Image1:Thumbnail200x200</t>
+          <t>dcterms:title:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -51223,7 +51214,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>dcterms:type:Image0:Thumbnail800x800</t>
+          <t>dcterms:type:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -51306,7 +51297,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://schema.org/description:Image1:Thumbnail600x600</t>
+          <t>https://schema.org/description:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -51338,7 +51329,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://schema.org/name:Image1:Thumbnail800x800</t>
+          <t>https://schema.org/name:Image1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -51370,7 +51361,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://schema.org/spatial:Image1:Thumbnail600x600</t>
+          <t>https://schema.org/spatial:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -51439,7 +51430,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -51497,7 +51488,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -51519,7 +51510,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -51563,7 +51554,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -51585,7 +51576,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -51607,7 +51598,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -51629,7 +51620,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -51651,7 +51642,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -51695,7 +51686,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -51717,7 +51708,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -51739,7 +51730,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -51761,7 +51752,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -51783,7 +51774,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -51805,7 +51796,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -51827,7 +51818,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -51849,7 +51840,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -51871,7 +51862,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -51915,7 +51906,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -51959,7 +51950,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image1</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -51981,7 +51972,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -52003,7 +51994,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -52025,7 +52016,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -52047,7 +52038,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -52069,7 +52060,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -52091,7 +52082,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -52113,7 +52104,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -52135,7 +52126,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -52157,7 +52148,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -52201,7 +52192,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -52223,7 +52214,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -52245,7 +52236,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -52267,7 +52258,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -52289,7 +52280,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -52311,7 +52302,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -52333,7 +52324,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -52355,7 +52346,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -52377,7 +52368,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -52399,7 +52390,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -52443,7 +52434,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -52465,7 +52456,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -52487,7 +52478,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -52509,7 +52500,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -52531,7 +52522,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -52553,7 +52544,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -52575,7 +52566,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -52597,7 +52588,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -52619,7 +52610,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -52641,7 +52632,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -52663,7 +52654,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -52685,7 +52676,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -52707,7 +52698,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -52729,7 +52720,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -52751,7 +52742,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -52773,7 +52764,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -52795,7 +52786,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -52817,7 +52808,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -52839,7 +52830,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -52861,7 +52852,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -52883,7 +52874,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -52905,7 +52896,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -52927,7 +52918,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -52949,7 +52940,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -52971,7 +52962,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -52993,7 +52984,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -53015,7 +53006,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -53037,7 +53028,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -53059,7 +53050,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -53081,7 +53072,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -53103,7 +53094,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -53125,7 +53116,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -53147,7 +53138,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -53169,7 +53160,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -53191,7 +53182,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -53213,7 +53204,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -53235,7 +53226,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -53293,7 +53284,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -53327,7 +53318,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -53344,7 +53335,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -53361,7 +53352,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -53378,7 +53369,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -53395,7 +53386,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -53412,7 +53403,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -53429,7 +53420,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -53446,7 +53437,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -53504,7 +53495,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization0:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -53522,7 +53513,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0:Thumbnail800x800</t>
+          <t>http://example.com/organization2:Image0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -53540,7 +53531,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image1:Thumbnail200x200</t>
+          <t>http://example.com/organization4:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">

</xml_diff>

<commit_message>
first cut of moving CmsAgent hierarchy to FoafAgent
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -491,7 +491,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image1:Thumbnail400x400</t>
+          <t>http://example.com/organization1:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -501,7 +501,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/organization1page</t>
+          <t>http://example.com/organization1homepage</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image1:Thumbnail600x600</t>
+          <t>http://example.com/organization3:Image0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/organization3page</t>
+          <t>http://example.com/organization3homepage</t>
         </is>
       </c>
     </row>
@@ -535,7 +535,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization5:Image0</t>
+          <t>http://example.com/organization5:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -545,7 +545,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/organization5page</t>
+          <t>http://example.com/organization5homepage</t>
         </is>
       </c>
     </row>
@@ -586,17 +586,17 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>homepage</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>image</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>page</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -621,17 +621,17 @@
           <t>Person</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>http://example.com/person0:Image0:Thumbnail800x800</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
+          <t>http://example.com/person0:Image1:Thumbnail400x400</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>Person 0</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
           <t>http://www.wikidata.org/entity/Q7251</t>
@@ -654,17 +654,17 @@
           <t>Person</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>http://example.com/person2:Image1</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
+          <t>http://example.com/person2:Image0:Thumbnail200x200</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>Person 2</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -682,17 +682,17 @@
           <t>Person</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>http://example.com/person4:Image0</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
+          <t>http://example.com/person4:Image1:Thumbnail400x400</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>Person 4</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -773,7 +773,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://example.com/person1page</t>
+          <t>http://example.com/person1homepage</t>
         </is>
       </c>
     </row>
@@ -795,7 +795,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image1</t>
+          <t>http://example.com/person3:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -805,7 +805,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>http://example.com/person3page</t>
+          <t>http://example.com/person3homepage</t>
         </is>
       </c>
     </row>
@@ -827,7 +827,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person5:Image0</t>
+          <t>http://example.com/person5:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -837,7 +837,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>http://example.com/person5page</t>
+          <t>http://example.com/person5homepage</t>
         </is>
       </c>
     </row>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -1745,7 +1745,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/description:Image0:Thumbnail200x200</t>
+          <t>http://purl.org/dc/terms/description:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/extent:Image0:Thumbnail800x800</t>
+          <t>http://purl.org/dc/terms/extent:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2894,7 +2894,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/medium:Image0:Thumbnail800x800</t>
+          <t>http://purl.org/dc/terms/medium:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -3277,7 +3277,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/publisher:Image0:Thumbnail400x400</t>
+          <t>http://purl.org/dc/terms/publisher:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -3660,7 +3660,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/source:Image0:Thumbnail200x200</t>
+          <t>http://purl.org/dc/terms/source:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -4043,7 +4043,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/spatial:Image0:Thumbnail800x800</t>
+          <t>http://purl.org/dc/terms/spatial:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -4426,7 +4426,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/subject:Image0:Thumbnail600x600</t>
+          <t>http://purl.org/dc/terms/subject:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -4809,7 +4809,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/title:Image0:Thumbnail800x800</t>
+          <t>http://purl.org/dc/terms/title:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
@@ -5192,7 +5192,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/type:Image0:Thumbnail800x800</t>
+          <t>http://purl.org/dc/terms/type:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -5575,7 +5575,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>https://schema.org/description:Image0:Thumbnail800x800</t>
+          <t>https://schema.org/description:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
@@ -6341,7 +6341,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>https://schema.org/spatial:Image0:Thumbnail800x800</t>
+          <t>https://schema.org/spatial:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
@@ -6724,7 +6724,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
@@ -7873,7 +7873,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
@@ -8256,7 +8256,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
@@ -8639,7 +8639,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H177" t="inlineStr">
@@ -9405,7 +9405,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H195" t="inlineStr">
@@ -9788,7 +9788,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H204" t="inlineStr">
@@ -10171,7 +10171,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H213" t="inlineStr">
@@ -10554,7 +10554,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H222" t="inlineStr">
@@ -11320,7 +11320,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H240" t="inlineStr">
@@ -11703,7 +11703,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H249" t="inlineStr">
@@ -12469,7 +12469,7 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H267" t="inlineStr">
@@ -13235,7 +13235,7 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H285" t="inlineStr">
@@ -14001,7 +14001,7 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H303" t="inlineStr">
@@ -14767,7 +14767,7 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H321" t="inlineStr">
@@ -15150,7 +15150,7 @@
       </c>
       <c r="G330" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H330" t="inlineStr">
@@ -15533,7 +15533,7 @@
       </c>
       <c r="G339" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H339" t="inlineStr">
@@ -15916,7 +15916,7 @@
       </c>
       <c r="G348" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H348" t="inlineStr">
@@ -16682,7 +16682,7 @@
       </c>
       <c r="G366" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H366" t="inlineStr">
@@ -17448,7 +17448,7 @@
       </c>
       <c r="G384" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H384" t="inlineStr">
@@ -17831,7 +17831,7 @@
       </c>
       <c r="G393" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H393" t="inlineStr">
@@ -18214,7 +18214,7 @@
       </c>
       <c r="G402" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H402" t="inlineStr">
@@ -18980,7 +18980,7 @@
       </c>
       <c r="G420" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H420" t="inlineStr">
@@ -19746,7 +19746,7 @@
       </c>
       <c r="G438" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H438" t="inlineStr">
@@ -20129,7 +20129,7 @@
       </c>
       <c r="G447" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H447" t="inlineStr">
@@ -20512,7 +20512,7 @@
       </c>
       <c r="G456" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H456" t="inlineStr">
@@ -20895,7 +20895,7 @@
       </c>
       <c r="G465" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H465" t="inlineStr">
@@ -21278,7 +21278,7 @@
       </c>
       <c r="G474" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H474" t="inlineStr">
@@ -21661,7 +21661,7 @@
       </c>
       <c r="G483" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H483" t="inlineStr">
@@ -22044,7 +22044,7 @@
       </c>
       <c r="G492" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H492" t="inlineStr">
@@ -22427,7 +22427,7 @@
       </c>
       <c r="G501" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H501" t="inlineStr">
@@ -22810,7 +22810,7 @@
       </c>
       <c r="G510" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H510" t="inlineStr">
@@ -23193,7 +23193,7 @@
       </c>
       <c r="G519" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H519" t="inlineStr">
@@ -23959,7 +23959,7 @@
       </c>
       <c r="G537" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H537" t="inlineStr">
@@ -24342,7 +24342,7 @@
       </c>
       <c r="G546" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H546" t="inlineStr">
@@ -24725,7 +24725,7 @@
       </c>
       <c r="G555" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H555" t="inlineStr">
@@ -25108,7 +25108,7 @@
       </c>
       <c r="G564" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H564" t="inlineStr">
@@ -26257,7 +26257,7 @@
       </c>
       <c r="G591" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H591" t="inlineStr">
@@ -27023,7 +27023,7 @@
       </c>
       <c r="G609" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H609" t="inlineStr">
@@ -27406,7 +27406,7 @@
       </c>
       <c r="G618" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H618" t="inlineStr">
@@ -28172,7 +28172,7 @@
       </c>
       <c r="G636" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H636" t="inlineStr">
@@ -28938,7 +28938,7 @@
       </c>
       <c r="G654" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H654" t="inlineStr">
@@ -30087,7 +30087,7 @@
       </c>
       <c r="G681" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H681" t="inlineStr">
@@ -30470,7 +30470,7 @@
       </c>
       <c r="G690" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H690" t="inlineStr">
@@ -30853,7 +30853,7 @@
       </c>
       <c r="G699" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H699" t="inlineStr">
@@ -31236,7 +31236,7 @@
       </c>
       <c r="G708" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H708" t="inlineStr">
@@ -32002,7 +32002,7 @@
       </c>
       <c r="G726" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H726" t="inlineStr">
@@ -32385,7 +32385,7 @@
       </c>
       <c r="G735" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H735" t="inlineStr">
@@ -32768,7 +32768,7 @@
       </c>
       <c r="G744" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H744" t="inlineStr">
@@ -33151,7 +33151,7 @@
       </c>
       <c r="G753" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H753" t="inlineStr">
@@ -34683,7 +34683,7 @@
       </c>
       <c r="G789" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H789" t="inlineStr">
@@ -35066,7 +35066,7 @@
       </c>
       <c r="G798" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H798" t="inlineStr">
@@ -35449,7 +35449,7 @@
       </c>
       <c r="G807" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H807" t="inlineStr">
@@ -35832,7 +35832,7 @@
       </c>
       <c r="G816" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H816" t="inlineStr">
@@ -36215,7 +36215,7 @@
       </c>
       <c r="G825" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H825" t="inlineStr">
@@ -36598,7 +36598,7 @@
       </c>
       <c r="G834" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H834" t="inlineStr">
@@ -36981,7 +36981,7 @@
       </c>
       <c r="G843" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H843" t="inlineStr">
@@ -37364,7 +37364,7 @@
       </c>
       <c r="G852" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H852" t="inlineStr">
@@ -37747,7 +37747,7 @@
       </c>
       <c r="G861" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H861" t="inlineStr">
@@ -38896,7 +38896,7 @@
       </c>
       <c r="G888" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H888" t="inlineStr">
@@ -39279,7 +39279,7 @@
       </c>
       <c r="G897" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H897" t="inlineStr">
@@ -39662,7 +39662,7 @@
       </c>
       <c r="G906" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H906" t="inlineStr">
@@ -40045,7 +40045,7 @@
       </c>
       <c r="G915" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H915" t="inlineStr">
@@ -40811,7 +40811,7 @@
       </c>
       <c r="G933" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H933" t="inlineStr">
@@ -41194,7 +41194,7 @@
       </c>
       <c r="G942" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0:Thumbnail600x600</t>
+          <t>http://example.com/organization0:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H942" t="inlineStr">
@@ -41960,7 +41960,7 @@
       </c>
       <c r="G960" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0:Thumbnail600x600</t>
+          <t>http://example.com/organization2:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H960" t="inlineStr">
@@ -42343,7 +42343,7 @@
       </c>
       <c r="G969" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image0:Thumbnail600x600</t>
+          <t>http://example.com/organization3:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H969" t="inlineStr">
@@ -43109,7 +43109,7 @@
       </c>
       <c r="G987" t="inlineStr">
         <is>
-          <t>http://example.com/organization5:Image0:Thumbnail200x200</t>
+          <t>http://example.com/organization5:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H987" t="inlineStr">
@@ -43492,7 +43492,7 @@
       </c>
       <c r="G996" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image0:Thumbnail600x600</t>
+          <t>http://example.com/person0:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H996" t="inlineStr">
@@ -43875,7 +43875,7 @@
       </c>
       <c r="G1005" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image0:Thumbnail200x200</t>
+          <t>http://example.com/person1:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1005" t="inlineStr">
@@ -44258,7 +44258,7 @@
       </c>
       <c r="G1014" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image0:Thumbnail600x600</t>
+          <t>http://example.com/person2:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1014" t="inlineStr">
@@ -44641,7 +44641,7 @@
       </c>
       <c r="G1023" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0:Thumbnail400x400</t>
+          <t>http://example.com/person3:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1023" t="inlineStr">
@@ -45024,7 +45024,7 @@
       </c>
       <c r="G1032" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image0:Thumbnail200x200</t>
+          <t>http://example.com/person4:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1032" t="inlineStr">
@@ -45790,7 +45790,7 @@
       </c>
       <c r="G1050" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work0:Image0:Thumbnail600x600</t>
+          <t>http://example.com/collection0/work0:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1050" t="inlineStr">
@@ -46210,7 +46210,7 @@
       </c>
       <c r="G1060" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work1:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work1:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1060" t="inlineStr">
@@ -46593,7 +46593,7 @@
       </c>
       <c r="G1069" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work2:Image0:Thumbnail600x600</t>
+          <t>http://example.com/collection0/work2:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1069" t="inlineStr">
@@ -46976,7 +46976,7 @@
       </c>
       <c r="G1078" t="inlineStr">
         <is>
-          <t>http://example.com/collection0/work3:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection0/work3:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1078" t="inlineStr">
@@ -47359,7 +47359,7 @@
       </c>
       <c r="G1087" t="inlineStr">
         <is>
-          <t>http://example.com/collection1:Image0:Thumbnail600x600</t>
+          <t>http://example.com/collection1:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1087" t="inlineStr">
@@ -47742,7 +47742,7 @@
       </c>
       <c r="G1096" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work4:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection1/work4:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="H1096" t="inlineStr">
@@ -48125,7 +48125,7 @@
       </c>
       <c r="G1105" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work5:Image0:Thumbnail200x200</t>
+          <t>http://example.com/collection1/work5:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1105" t="inlineStr">
@@ -48891,7 +48891,7 @@
       </c>
       <c r="G1123" t="inlineStr">
         <is>
-          <t>http://example.com/collection1/work7:Image0:Thumbnail800x800</t>
+          <t>http://example.com/collection1/work7:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="H1123" t="inlineStr">
@@ -49657,7 +49657,7 @@
       </c>
       <c r="G1141" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork9:Image0:Thumbnail400x400</t>
+          <t>http://example.com/freestandingwork9:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1141" t="inlineStr">
@@ -50040,7 +50040,7 @@
       </c>
       <c r="G1150" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork10:Image0:Thumbnail200x200</t>
+          <t>http://example.com/freestandingwork10:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="H1150" t="inlineStr">
@@ -50423,7 +50423,7 @@
       </c>
       <c r="G1159" t="inlineStr">
         <is>
-          <t>http://example.com/freestandingwork11:Image0:Thumbnail800x800</t>
+          <t>http://example.com/freestandingwork11:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="H1159" t="inlineStr">
@@ -50841,7 +50841,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/description:Image1</t>
+          <t>http://purl.org/dc/terms/description:Image0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -50873,7 +50873,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/extent:Image0</t>
+          <t>http://purl.org/dc/terms/extent:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -50905,7 +50905,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/language:Image0:Thumbnail200x200</t>
+          <t>http://purl.org/dc/terms/language:Image1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -50937,7 +50937,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/medium:Image1:Thumbnail400x400</t>
+          <t>http://purl.org/dc/terms/medium:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -50969,7 +50969,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/publisher:Image0:Thumbnail600x600</t>
+          <t>http://purl.org/dc/terms/publisher:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -51001,7 +51001,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/source:Image0:Thumbnail800x800</t>
+          <t>http://purl.org/dc/terms/source:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -51033,7 +51033,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/spatial:Image1:Thumbnail600x600</t>
+          <t>http://purl.org/dc/terms/spatial:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -51065,7 +51065,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/subject:Image0:Thumbnail600x600</t>
+          <t>http://purl.org/dc/terms/subject:Image1</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -51097,7 +51097,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/title:Image1:Thumbnail800x800</t>
+          <t>http://purl.org/dc/terms/title:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -51129,7 +51129,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/type:Image0</t>
+          <t>http://purl.org/dc/terms/type:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -51212,7 +51212,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://schema.org/description:Image1</t>
+          <t>https://schema.org/description:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -51244,7 +51244,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://schema.org/name:Image1:Thumbnail400x400</t>
+          <t>https://schema.org/name:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -51276,7 +51276,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://schema.org/spatial:Image1:Thumbnail200x200</t>
+          <t>https://schema.org/spatial:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -51345,7 +51345,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -51403,7 +51403,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -51425,7 +51425,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -51447,7 +51447,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -51469,7 +51469,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -51491,7 +51491,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -51513,7 +51513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -51535,7 +51535,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -51557,7 +51557,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -51579,7 +51579,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -51601,7 +51601,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -51623,7 +51623,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -51645,7 +51645,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -51667,7 +51667,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -51689,7 +51689,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -51711,7 +51711,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -51733,7 +51733,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -51755,7 +51755,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -51777,7 +51777,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -51799,7 +51799,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -51821,7 +51821,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -51843,7 +51843,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -51865,7 +51865,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image1</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -51887,7 +51887,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -51909,7 +51909,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -51931,7 +51931,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -51953,7 +51953,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -51975,7 +51975,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -51997,7 +51997,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -52019,7 +52019,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -52041,7 +52041,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -52063,7 +52063,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -52085,7 +52085,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -52107,7 +52107,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -52129,7 +52129,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -52151,7 +52151,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -52173,7 +52173,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -52217,7 +52217,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -52261,7 +52261,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -52283,7 +52283,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -52327,7 +52327,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -52349,7 +52349,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -52371,7 +52371,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -52393,7 +52393,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -52415,7 +52415,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -52437,7 +52437,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -52459,7 +52459,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -52481,7 +52481,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -52547,7 +52547,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -52569,7 +52569,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -52591,7 +52591,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -52613,7 +52613,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -52635,7 +52635,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -52679,7 +52679,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -52701,7 +52701,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -52723,7 +52723,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -52789,7 +52789,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -52811,7 +52811,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -52833,7 +52833,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -52855,7 +52855,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -52877,7 +52877,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -52899,7 +52899,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -52921,7 +52921,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -52965,7 +52965,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -52987,7 +52987,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -53009,7 +53009,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -53031,7 +53031,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -53053,7 +53053,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -53075,7 +53075,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -53097,7 +53097,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -53119,7 +53119,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -53141,7 +53141,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -53199,7 +53199,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -53216,7 +53216,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -53233,7 +53233,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -53267,7 +53267,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -53284,7 +53284,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -53301,7 +53301,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -53318,7 +53318,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -53335,7 +53335,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -53352,7 +53352,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -53388,17 +53388,17 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>homepage</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>image</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>page</t>
         </is>
       </c>
     </row>
@@ -53408,17 +53408,17 @@
           <t>http://example.com/organization0</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>http://example.com/organization0:Image1:Thumbnail800x800</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
+          <t>http://example.com/organization0:Image0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Organization 0</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -53426,17 +53426,17 @@
           <t>http://example.com/organization2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>http://example.com/organization2:Image0:Thumbnail800x800</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
+          <t>http://example.com/organization2:Image1:Thumbnail200x200</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Organization 2</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -53444,17 +53444,17 @@
           <t>http://example.com/organization4</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>http://example.com/organization4:Image0:Thumbnail400x400</t>
-        </is>
-      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
+          <t>http://example.com/organization4:Image1:Thumbnail800x800</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>Organization 4</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix sundry models test regressions
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image1:Thumbnail800x800</t>
+          <t>http://example.com/organization1:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -532,7 +532,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization5:Image0:Thumbnail800x800</t>
+          <t>http://example.com/organization5:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -608,21 +608,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
+          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
         </is>
       </c>
     </row>
@@ -771,7 +771,7 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image0:Thumbnail600x600</t>
+          <t>http://example.com/person0:Image0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -804,7 +804,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image0:Thumbnail600x600</t>
+          <t>http://example.com/person2:Image1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -832,7 +832,7 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image1:Thumbnail800x800</t>
+          <t>http://example.com/person4:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -910,7 +910,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image0</t>
+          <t>http://example.com/person1:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -942,7 +942,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0</t>
+          <t>http://example.com/person3:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -974,7 +974,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person5:Image0:Thumbnail800x800</t>
+          <t>http://example.com/person5:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/language:Image1:Thumbnail200x200</t>
+          <t>http://purl.org/dc/terms/language:Image1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/medium:Image1:Thumbnail200x200</t>
+          <t>http://purl.org/dc/terms/medium:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1505,7 +1505,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/publisher:Image0</t>
+          <t>http://purl.org/dc/terms/publisher:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/source:Image0:Thumbnail400x400</t>
+          <t>http://purl.org/dc/terms/source:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/subject:Image0:Thumbnail200x200</t>
+          <t>http://purl.org/dc/terms/subject:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/title:Image1:Thumbnail200x200</t>
+          <t>http://purl.org/dc/terms/title:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1665,7 +1665,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/type:Image1</t>
+          <t>http://purl.org/dc/terms/type:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1812,7 +1812,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://schema.org/spatial:Image1:Thumbnail400x400</t>
+          <t>https://schema.org/spatial:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1881,7 +1881,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1939,7 +1939,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1983,7 +1983,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2005,7 +2005,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2049,7 +2049,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2071,7 +2071,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2115,7 +2115,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -2137,7 +2137,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2159,7 +2159,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2181,7 +2181,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2203,7 +2203,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -2225,7 +2225,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -2247,7 +2247,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -2269,7 +2269,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2313,7 +2313,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -2335,7 +2335,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2357,7 +2357,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2379,7 +2379,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2423,7 +2423,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2467,7 +2467,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -2489,7 +2489,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2511,7 +2511,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2555,7 +2555,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2577,7 +2577,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2599,7 +2599,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2621,7 +2621,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2643,7 +2643,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2687,7 +2687,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2709,7 +2709,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2731,7 +2731,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2753,7 +2753,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2775,7 +2775,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2819,7 +2819,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2885,7 +2885,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2907,7 +2907,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2929,7 +2929,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2951,7 +2951,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2973,7 +2973,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2995,7 +2995,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -3017,7 +3017,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -3039,7 +3039,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -3083,7 +3083,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -3105,7 +3105,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -3127,7 +3127,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -3171,7 +3171,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -3193,7 +3193,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -3215,7 +3215,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -3237,7 +3237,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -3259,7 +3259,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -3303,7 +3303,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -3325,7 +3325,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -3347,7 +3347,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -3369,7 +3369,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3391,7 +3391,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3435,7 +3435,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3457,7 +3457,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3479,7 +3479,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3523,7 +3523,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3545,7 +3545,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3567,7 +3567,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3611,7 +3611,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3655,7 +3655,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3677,7 +3677,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3752,7 +3752,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -3769,7 +3769,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -3786,7 +3786,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3803,7 +3803,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -3820,7 +3820,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3837,7 +3837,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1:Thumbnail800x800</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -3871,7 +3871,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1:Thumbnail400x400</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -3888,7 +3888,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail600x600</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -3947,7 +3947,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0:Thumbnail800x800</t>
+          <t>http://example.com/organization0:Image0:Thumbnail400x400</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -3965,7 +3965,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image1:Thumbnail800x800</t>
+          <t>http://example.com/organization2:Image0:Thumbnail200x200</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">

</xml_diff>

<commit_message>
only link work/agent/etc. to the original images, and original images to thumbnails
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image0:Thumbnail600x600</t>
+          <t>http://example.com/organization1:Image1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -510,7 +510,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image1</t>
+          <t>http://example.com/organization3:Image0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -532,7 +532,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization5:Image1:Thumbnail600x600</t>
+          <t>http://example.com/organization5:Image1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -608,21 +608,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
+          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
         </is>
       </c>
     </row>
@@ -832,7 +832,7 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image1:Thumbnail400x400</t>
+          <t>http://example.com/person4:Image1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -910,7 +910,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image0:Thumbnail600x600</t>
+          <t>http://example.com/person1:Image0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -942,7 +942,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image1:Thumbnail400x400</t>
+          <t>http://example.com/person3:Image1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -974,7 +974,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person5:Image0:Thumbnail600x600</t>
+          <t>http://example.com/person5:Image1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1377,7 +1377,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/description:Image1:Thumbnail600x600</t>
+          <t>http://purl.org/dc/terms/description:Image1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1409,7 +1409,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/extent:Image1:Thumbnail200x200</t>
+          <t>http://purl.org/dc/terms/extent:Image1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/language:Image1</t>
+          <t>http://purl.org/dc/terms/language:Image0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/medium:Image0:Thumbnail200x200</t>
+          <t>http://purl.org/dc/terms/medium:Image1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1505,7 +1505,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/publisher:Image1:Thumbnail200x200</t>
+          <t>http://purl.org/dc/terms/publisher:Image0</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/source:Image1:Thumbnail600x600</t>
+          <t>http://purl.org/dc/terms/source:Image0</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1569,7 +1569,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/spatial:Image0:Thumbnail400x400</t>
+          <t>http://purl.org/dc/terms/spatial:Image0</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/subject:Image1:Thumbnail400x400</t>
+          <t>http://purl.org/dc/terms/subject:Image0</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/title:Image0:Thumbnail200x200</t>
+          <t>http://purl.org/dc/terms/title:Image0</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1665,7 +1665,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/type:Image1:Thumbnail200x200</t>
+          <t>http://purl.org/dc/terms/type:Image1</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://schema.org/description:Image1:Thumbnail800x800</t>
+          <t>https://schema.org/description:Image1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1780,7 +1780,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://schema.org/name:Image0:Thumbnail200x200</t>
+          <t>https://schema.org/name:Image1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1812,7 +1812,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://schema.org/spatial:Image0:Thumbnail800x800</t>
+          <t>https://schema.org/spatial:Image0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1881,7 +1881,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1939,7 +1939,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1983,7 +1983,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2049,7 +2049,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2071,7 +2071,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2137,7 +2137,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2159,7 +2159,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2181,7 +2181,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2203,7 +2203,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -2225,7 +2225,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -2247,7 +2247,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2313,7 +2313,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -2335,7 +2335,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2357,7 +2357,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2379,7 +2379,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2423,7 +2423,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2489,7 +2489,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2511,7 +2511,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2555,7 +2555,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2577,7 +2577,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2599,7 +2599,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2621,7 +2621,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2643,7 +2643,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2687,7 +2687,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2709,7 +2709,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2731,7 +2731,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2753,7 +2753,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2775,7 +2775,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2797,7 +2797,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2819,7 +2819,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2863,7 +2863,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2885,7 +2885,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2907,7 +2907,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2929,7 +2929,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2951,7 +2951,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2973,7 +2973,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2995,7 +2995,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -3039,7 +3039,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -3083,7 +3083,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -3105,7 +3105,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -3127,7 +3127,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -3149,7 +3149,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -3171,7 +3171,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -3193,7 +3193,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -3237,7 +3237,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -3259,7 +3259,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -3303,7 +3303,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -3325,7 +3325,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image1</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -3347,7 +3347,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -3369,7 +3369,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3391,7 +3391,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3435,7 +3435,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3457,7 +3457,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3479,7 +3479,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image1</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3523,7 +3523,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3567,7 +3567,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3589,7 +3589,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3611,7 +3611,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3655,7 +3655,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3677,7 +3677,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3735,7 +3735,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3752,7 +3752,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -3769,7 +3769,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -3803,7 +3803,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -3820,7 +3820,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0:Thumbnail200x200</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3837,7 +3837,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1:Thumbnail800x800</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -3854,7 +3854,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -3871,7 +3871,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1:Thumbnail400x400</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -3888,7 +3888,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0:Thumbnail600x600</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -3947,7 +3947,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0:Thumbnail400x400</t>
+          <t>http://example.com/organization0:Image0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -3965,7 +3965,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0:Thumbnail200x200</t>
+          <t>http://example.com/organization2:Image0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -3983,7 +3983,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0:Thumbnail800x800</t>
+          <t>http://example.com/organization4:Image0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">

</xml_diff>

<commit_message>
SyntheticDataPipeline: add location sameAs to Wikidata
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image1</t>
+          <t>http://example.com/organization1:Image0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -510,7 +510,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image0</t>
+          <t>http://example.com/organization3:Image1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -583,7 +583,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -597,6 +597,51 @@
           <t>@id</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>cc:legalcode</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>cc:licenseClass</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>cc:permits</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>cc:requires</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>dc:creator</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>dc:identifier</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>dc:title</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>dcterms:hasVersion</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>foaf:logo</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -604,27 +649,112 @@
           <t>http://creativecommons.org/licenses/by-sa/3.0/</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>by-sa</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Attribution-ShareAlike 3.0 Unported</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
-        </is>
-      </c>
+          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>mark</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Public Domain Mark 1.0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
-        </is>
-      </c>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nc</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>NonCommercial 1.0 Generic</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
+          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>by-sa</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Attribution-ShareAlike 2.0 Generic</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -637,7 +767,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -661,6 +791,26 @@
           <t>identifier</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>skos:definition</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>skos:note</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>skos:prefLabel</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>skos:scopeNote</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -678,6 +828,28 @@
           <t>InC</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>This Item is protected by copyright and/or related rights.
+  You are free to use this Item in any way that is permitted by the copyright and related rights legislation that applies to your use.
+  For other uses you need to obtain permission from the rights-holder(s).</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>In Copyright</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>This Rights Statement can be used for an Item that is in copyright. Using this statement implies that the organization making this Item available has determined that the Item is in copyright and either is the rights-holder, has obtained permission from the rights-holder(s) to make their Work(s) available, or makes the Item available under an exception or limitation to copyright (including Fair Use) that entitles it to make the Item available.</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -693,6 +865,28 @@
       <c r="C3" t="inlineStr">
         <is>
           <t>InC-EDU</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>This Item is protected by copyright and/or related rights.
+  You are free to use this Item in any way that is permitted by the copyright and related rights legislation that applies to your use. In addition, no permission is required from the rights-holder(s) for educational uses.
+  For other uses, you need to obtain permission from the rights-holder(s).</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>In Copyright - Educational Use Permitted</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>This Rights Statement can be used only for copyrighted Items for which the organization making the Item available is the rights-holder or has been explicitly authorized by the rights-holder(s) to allow third parties to use their Work(s) for educational purposes without first obtaining permission.</t>
         </is>
       </c>
     </row>
@@ -771,7 +965,7 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image0</t>
+          <t>http://example.com/person0:Image1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -781,7 +975,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>http://www.wikidata.org/entity/Q7251</t>
+          <t>wd:Q7251</t>
         </is>
       </c>
     </row>
@@ -942,7 +1136,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image1</t>
+          <t>http://example.com/person3:Image0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -974,7 +1168,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person5:Image1</t>
+          <t>http://example.com/person5:Image0</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -999,7 +1193,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1013,11 +1207,21 @@
           <t>@id</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
           <t>http://example.com/collection0/work0Location</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>wd:Q89503830</t>
         </is>
       </c>
     </row>
@@ -1187,7 +1391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1199,65 +1403,6 @@
       <c r="A1" t="inlineStr">
         <is>
           <t>@graph</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>http://commons.wikimedia.org/wiki/Special:FilePath/Alan%20Turing%20Aged%2016.jpg</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Passport photo of Alan Turing at age 16</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://upload.wikimedia.org/wikipedia/commons/a/a1/Alan_Turing_Aged_16.jpg</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Possibly Arthur Reginald Chaffin (1893-1954)</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>http://commons.wikimedia.org/wiki/Special:FilePath/Pilot%20ACE%20computer-2.jpg</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Pilot ACE computer on display at Science Museum in London</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://upload.wikimedia.org/wikipedia/commons/c/c6/Pilot_ACE_computer-2.jpg</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Steve Elliott</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>http://rightsstatements.org/vocab/InC/1.0/</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1512,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/description</t>
+          <t>dcterms:description</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1377,7 +1522,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/description:Image1</t>
+          <t>dcterms:description:Image1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1399,7 +1544,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/extent</t>
+          <t>dcterms:extent</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1409,7 +1554,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/extent:Image1</t>
+          <t>dcterms:extent:Image0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1431,7 +1576,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/language</t>
+          <t>dcterms:language</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1441,7 +1586,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/language:Image0</t>
+          <t>dcterms:language:Image1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1463,7 +1608,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/medium</t>
+          <t>dcterms:medium</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1473,7 +1618,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/medium:Image1</t>
+          <t>dcterms:medium:Image1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1495,7 +1640,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/publisher</t>
+          <t>dcterms:publisher</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1505,7 +1650,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/publisher:Image0</t>
+          <t>dcterms:publisher:Image0</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1527,7 +1672,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/source</t>
+          <t>dcterms:source</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1537,7 +1682,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/source:Image0</t>
+          <t>dcterms:source:Image0</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1559,7 +1704,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/spatial</t>
+          <t>dcterms:spatial</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1569,7 +1714,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/spatial:Image0</t>
+          <t>dcterms:spatial:Image1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1591,7 +1736,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/subject</t>
+          <t>dcterms:subject</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1601,7 +1746,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/subject:Image0</t>
+          <t>dcterms:subject:Image0</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1623,7 +1768,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/title</t>
+          <t>dcterms:title</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1633,7 +1778,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/title:Image0</t>
+          <t>dcterms:title:Image0</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1655,7 +1800,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/type</t>
+          <t>dcterms:type</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1665,7 +1810,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>http://purl.org/dc/terms/type:Image1</t>
+          <t>dcterms:type:Image1</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1738,7 +1883,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://schema.org/description</t>
+          <t>schema:description</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1748,7 +1893,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://schema.org/description:Image1</t>
+          <t>schema:description:Image0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1770,7 +1915,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://schema.org/name</t>
+          <t>schema:name</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1780,7 +1925,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://schema.org/name:Image1</t>
+          <t>schema:name:Image0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1802,7 +1947,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://schema.org/spatial</t>
+          <t>schema:spatial</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1812,7 +1957,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://schema.org/spatial:Image0</t>
+          <t>schema:spatial:Image0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1881,7 +2026,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1939,7 +2084,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1961,7 +2106,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1983,7 +2128,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2115,7 +2260,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -2159,7 +2304,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2467,7 +2612,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -2489,7 +2634,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2511,7 +2656,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2533,7 +2678,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2555,7 +2700,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2599,7 +2744,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2643,7 +2788,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2687,7 +2832,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2709,7 +2854,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2775,7 +2920,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2797,7 +2942,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2863,7 +3008,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2885,7 +3030,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2907,7 +3052,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2929,7 +3074,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2951,7 +3096,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2973,7 +3118,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3017,7 +3162,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -3061,7 +3206,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -3105,7 +3250,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -3149,7 +3294,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -3171,7 +3316,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -3193,7 +3338,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -3215,7 +3360,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -3303,7 +3448,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -3369,7 +3514,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3391,7 +3536,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3435,7 +3580,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3457,7 +3602,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3501,7 +3646,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3523,7 +3668,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3567,7 +3712,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3589,7 +3734,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3633,7 +3778,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3655,7 +3800,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3702,7 +3847,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3726,6 +3871,11 @@
           <t>name</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>rdf:value</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -3743,6 +3893,11 @@
           <t>Concept 80</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Schema Spatial 0</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -3760,6 +3915,11 @@
           <t>Concept 81</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Schema Spatial 1</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -3777,6 +3937,11 @@
           <t>Concept 82</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Schema Spatial 2</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -3786,12 +3951,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>Concept 83</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Schema Spatial 3</t>
         </is>
       </c>
     </row>
@@ -3811,6 +3981,11 @@
           <t>Concept 84</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Schema Spatial 4</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -3828,6 +4003,11 @@
           <t>Concept 85</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Schema Spatial 5</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -3845,6 +4025,11 @@
           <t>Concept 86</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Schema Spatial 6</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -3854,12 +4039,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>Concept 87</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Schema Spatial 7</t>
         </is>
       </c>
     </row>
@@ -3871,12 +4061,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>Concept 88</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Schema Spatial 8</t>
         </is>
       </c>
     </row>
@@ -3888,12 +4083,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>Concept 89</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Schema Spatial 9</t>
         </is>
       </c>
     </row>
@@ -3965,7 +4165,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0</t>
+          <t>http://example.com/organization2:Image1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -3983,7 +4183,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0</t>
+          <t>http://example.com/organization4:Image1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">

</xml_diff>

<commit_message>
remove type P31 predicates, only need subclass relationships
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image0</t>
+          <t>http://example.com/organization1:Image1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -700,7 +700,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -708,29 +708,28 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>by-sa</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Attribution-ShareAlike 2.0 Generic</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>nc</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>NonCommercial 1.0 Generic</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr"/>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -738,23 +737,24 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>by-sa</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Attribution-ShareAlike 2.0 Generic</t>
-        </is>
-      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+          <t>nc</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>NonCommercial 1.0 Generic</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1026,7 +1026,7 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image1</t>
+          <t>http://example.com/person4:Image0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1104,7 +1104,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image0</t>
+          <t>http://example.com/person1:Image1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0</t>
+          <t>http://example.com/person3:Image1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1554,7 +1554,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0</t>
+          <t>dcterms:extent:Image1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1618,7 +1618,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image1</t>
+          <t>dcterms:medium:Image0</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1650,7 +1650,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image0</t>
+          <t>dcterms:publisher:Image1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>dcterms:source:Image0</t>
+          <t>dcterms:source:Image1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dcterms:title:Image0</t>
+          <t>dcterms:title:Image1</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>schema:name:Image0</t>
+          <t>schema:name:Image1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1957,7 +1957,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>schema:spatial:Image0</t>
+          <t>schema:spatial:Image1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2026,7 +2026,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2106,7 +2106,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2172,7 +2172,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2216,7 +2216,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2260,7 +2260,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -2282,7 +2282,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2370,7 +2370,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -2392,7 +2392,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -2414,7 +2414,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -2436,7 +2436,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2480,7 +2480,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2546,7 +2546,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image1</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2568,7 +2568,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2612,7 +2612,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -2634,7 +2634,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2678,7 +2678,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2700,7 +2700,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2766,7 +2766,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2854,7 +2854,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2876,7 +2876,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2920,7 +2920,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2942,7 +2942,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2986,7 +2986,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -3030,7 +3030,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -3096,7 +3096,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -3162,7 +3162,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -3184,7 +3184,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -3206,7 +3206,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -3250,7 +3250,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -3294,7 +3294,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -3404,7 +3404,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -3492,7 +3492,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -3514,7 +3514,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3536,7 +3536,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3558,7 +3558,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3602,7 +3602,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3646,7 +3646,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3668,7 +3668,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3690,7 +3690,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image1</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3712,7 +3712,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3756,7 +3756,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3800,7 +3800,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3885,7 +3885,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3929,7 +3929,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -4017,7 +4017,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -4039,7 +4039,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -4183,7 +4183,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image1</t>
+          <t>http://example.com/organization4:Image0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">

</xml_diff>

<commit_message>
elide everything but P279 and owl:sameAs of type Wikibase items
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -510,7 +510,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image1</t>
+          <t>http://example.com/organization3:Image0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -674,57 +674,57 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
+          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>mark</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Public Domain Mark 1.0</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
+          <t>by-sa</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Attribution-ShareAlike 2.0 Generic</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
+          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>mark</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Public Domain Mark 1.0</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>by-sa</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Attribution-ShareAlike 2.0 Generic</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -837,7 +837,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1026,7 +1026,7 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image0</t>
+          <t>http://example.com/person4:Image1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1104,7 +1104,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image1</t>
+          <t>http://example.com/person1:Image0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image1</t>
+          <t>http://example.com/person3:Image0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person5:Image0</t>
+          <t>http://example.com/person5:Image1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1554,7 +1554,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image1</t>
+          <t>dcterms:extent:Image0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>dcterms:source:Image1</t>
+          <t>dcterms:source:Image0</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dcterms:title:Image1</t>
+          <t>dcterms:title:Image0</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -2150,7 +2150,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2260,7 +2260,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -2282,7 +2282,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2304,7 +2304,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2326,7 +2326,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2348,7 +2348,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -2436,7 +2436,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2458,7 +2458,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -2480,7 +2480,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2524,7 +2524,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2568,7 +2568,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2634,7 +2634,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2678,7 +2678,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2722,7 +2722,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2744,7 +2744,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2766,7 +2766,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2810,7 +2810,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2898,7 +2898,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2986,7 +2986,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -3096,7 +3096,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -3118,7 +3118,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3140,7 +3140,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -3162,7 +3162,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -3184,7 +3184,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -3228,7 +3228,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -3316,7 +3316,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -3338,7 +3338,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -3382,7 +3382,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -3404,7 +3404,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -3448,7 +3448,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -3536,7 +3536,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3580,7 +3580,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3646,7 +3646,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3668,7 +3668,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3712,7 +3712,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3734,7 +3734,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3756,7 +3756,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3885,7 +3885,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3995,7 +3995,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -4147,7 +4147,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0</t>
+          <t>http://example.com/organization0:Image1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">

</xml_diff>

<commit_message>
SyntheticDataPipeline: add anonymous and named locations where there's no sameAs
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -22,9 +22,9 @@
     <sheet name="RightsStatementsDotOrgRightsStatement" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="FoafPerson" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="SchemaPerson" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="SchemaPlace" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="DcPhysicalObject" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="SchemaCreativeWork" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="DcPhysicalObject" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="SchemaCreativeWork" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="SchemaPlace" sheetId="18" state="visible" r:id="rId18"/>
     <sheet name="DcCollection" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="SchemaCollection" sheetId="20" state="visible" r:id="rId20"/>
   </sheets>
@@ -488,7 +488,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image1</t>
+          <t>http://example.com/organization1:Image0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -510,7 +510,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image0</t>
+          <t>http://example.com/organization3:Image1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -674,7 +674,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -682,23 +682,24 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>by-sa</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Attribution-ShareAlike 2.0 Generic</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+          <t>nc</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>NonCommercial 1.0 Generic</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -729,7 +730,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -737,24 +738,23 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>by-sa</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Attribution-ShareAlike 2.0 Generic</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>nc</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>NonCommercial 1.0 Generic</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr"/>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -876,7 +876,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -965,7 +965,7 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image1</t>
+          <t>http://example.com/person0:Image0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -998,7 +998,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image1</t>
+          <t>http://example.com/person2:Image0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person5:Image1</t>
+          <t>http://example.com/person5:Image0</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1193,7 +1193,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1204,101 +1204,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>@id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sameAs</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>http://example.com/collection0/work0Location</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>wd:Q89503830</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>http://example.com/collection0/work1Location</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>http://example.com/collection0/work2Location</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>http://example.com/collection0/work3Location</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>http://example.com/collection1/work4Location</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>http://example.com/collection1/work5Location</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>http://example.com/collection1/work6Location</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>http://example.com/collection1/work7Location</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork8Location</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork9Location</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork10Location</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>http://example.com/freestandingwork11Location</t>
+          <t>@graph</t>
         </is>
       </c>
     </row>
@@ -1339,7 +1245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1350,7 +1256,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>@graph</t>
+          <t>@id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>http://example.com/collection0/work3Location</t>
         </is>
       </c>
     </row>
@@ -1554,7 +1467,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0</t>
+          <t>dcterms:extent:Image1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1650,7 +1563,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image1</t>
+          <t>dcterms:publisher:Image0</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1714,7 +1627,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image1</t>
+          <t>dcterms:spatial:Image0</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1810,7 +1723,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>dcterms:type:Image1</t>
+          <t>dcterms:type:Image0</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1893,7 +1806,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>schema:description:Image0</t>
+          <t>schema:description:Image1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1925,7 +1838,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>schema:name:Image1</t>
+          <t>schema:name:Image0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2084,7 +1997,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2106,7 +2019,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2194,7 +2107,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2260,7 +2173,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -2282,7 +2195,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2304,7 +2217,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2326,7 +2239,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2370,7 +2283,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -2436,7 +2349,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2458,7 +2371,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -2480,7 +2393,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2524,7 +2437,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2590,7 +2503,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2612,7 +2525,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -2700,7 +2613,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2744,7 +2657,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2766,7 +2679,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2788,7 +2701,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2832,7 +2745,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2876,7 +2789,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2898,7 +2811,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2942,7 +2855,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2964,7 +2877,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2986,7 +2899,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -3030,7 +2943,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -3052,7 +2965,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -3074,7 +2987,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -3140,7 +3053,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -3184,7 +3097,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -3206,7 +3119,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -3228,7 +3141,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -3272,7 +3185,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -3316,7 +3229,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -3338,7 +3251,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -3360,7 +3273,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -3382,7 +3295,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -3404,7 +3317,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -3470,7 +3383,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -3514,7 +3427,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3536,7 +3449,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3558,7 +3471,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3580,7 +3493,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3624,7 +3537,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3646,7 +3559,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3668,7 +3581,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3712,7 +3625,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3778,7 +3691,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3822,7 +3735,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3885,7 +3798,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3929,7 +3842,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -3951,7 +3864,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -4017,7 +3930,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">

</xml_diff>

<commit_message>
WikidataEnricher: pull in locations until one has a centroid
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image0</t>
+          <t>http://example.com/organization1:Image1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -583,7 +583,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -726,35 +726,6 @@
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/by-sa/2.0/</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>by-sa</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Attribution-ShareAlike 2.0 Generic</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -876,7 +847,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -998,7 +969,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image0</t>
+          <t>http://example.com/person2:Image1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1104,7 +1075,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image0</t>
+          <t>http://example.com/person1:Image1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1136,7 +1107,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image0</t>
+          <t>http://example.com/person3:Image1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1467,7 +1438,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image1</t>
+          <t>dcterms:extent:Image0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1499,7 +1470,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dcterms:language:Image1</t>
+          <t>dcterms:language:Image0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1531,7 +1502,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image0</t>
+          <t>dcterms:medium:Image1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1563,7 +1534,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image0</t>
+          <t>dcterms:publisher:Image1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1691,7 +1662,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dcterms:title:Image0</t>
+          <t>dcterms:title:Image1</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1838,7 +1809,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>schema:name:Image0</t>
+          <t>schema:name:Image1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1997,7 +1968,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2019,7 +1990,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2041,7 +2012,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2151,7 +2122,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2195,7 +2166,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2239,7 +2210,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2393,7 +2364,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2503,7 +2474,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2547,7 +2518,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2613,7 +2584,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2635,7 +2606,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2657,7 +2628,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2679,7 +2650,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2701,7 +2672,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2723,7 +2694,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2745,7 +2716,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2811,7 +2782,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2855,7 +2826,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2877,7 +2848,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2899,7 +2870,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2921,7 +2892,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2943,7 +2914,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2987,7 +2958,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -3009,7 +2980,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -3031,7 +3002,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3119,7 +3090,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -3207,7 +3178,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -3295,7 +3266,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -3427,7 +3398,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3449,7 +3420,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3471,7 +3442,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3493,7 +3464,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3559,7 +3530,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3647,7 +3618,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3669,7 +3640,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3691,7 +3662,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3713,7 +3684,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3798,7 +3769,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3820,7 +3791,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -3842,7 +3813,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -3864,7 +3835,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3886,7 +3857,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -3908,7 +3879,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3996,7 +3967,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -4060,7 +4031,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image1</t>
+          <t>http://example.com/organization0:Image0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -4078,7 +4049,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image1</t>
+          <t>http://example.com/organization2:Image0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -4096,7 +4067,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0</t>
+          <t>http://example.com/organization4:Image1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">

</xml_diff>

<commit_message>
regenerate synthetic data with Wikidata enrichment
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image1</t>
+          <t>http://example.com/organization1:Image0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -510,7 +510,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image1</t>
+          <t>http://example.com/organization3:Image0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -532,7 +532,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization5:Image1</t>
+          <t>http://example.com/organization5:Image0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -674,58 +674,58 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>mark</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Public Domain Mark 1.0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nc</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>NonCommercial 1.0 Generic</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>mark</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Public Domain Mark 1.0</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nc</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>NonCommercial 1.0 Generic</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -847,7 +847,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -936,7 +936,7 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image0</t>
+          <t>http://example.com/person0:Image1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -969,7 +969,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image1</t>
+          <t>http://example.com/person2:Image0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -997,7 +997,7 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image1</t>
+          <t>http://example.com/person4:Image0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image1</t>
+          <t>http://example.com/person1:Image0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image1</t>
+          <t>http://example.com/person3:Image0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1139,7 +1139,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person5:Image0</t>
+          <t>http://example.com/person5:Image1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0</t>
+          <t>dcterms:extent:Image1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1470,7 +1470,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dcterms:language:Image0</t>
+          <t>dcterms:language:Image1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1534,7 +1534,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image1</t>
+          <t>dcterms:publisher:Image0</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>dcterms:source:Image0</t>
+          <t>dcterms:source:Image1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1662,7 +1662,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dcterms:title:Image1</t>
+          <t>dcterms:title:Image0</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1777,7 +1777,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>schema:description:Image1</t>
+          <t>schema:description:Image0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1968,7 +1968,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:0:Image1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2012,7 +2012,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2232,7 +2232,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -2254,7 +2254,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -2276,7 +2276,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -2298,7 +2298,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -2320,7 +2320,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2364,7 +2364,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2408,7 +2408,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2430,7 +2430,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2452,7 +2452,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2496,7 +2496,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -2518,7 +2518,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2540,7 +2540,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2584,7 +2584,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2606,7 +2606,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2650,7 +2650,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2672,7 +2672,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2694,7 +2694,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2760,7 +2760,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2870,7 +2870,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2892,7 +2892,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2914,7 +2914,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -3002,7 +3002,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3024,7 +3024,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -3090,7 +3090,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -3134,7 +3134,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -3156,7 +3156,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -3178,7 +3178,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -3354,7 +3354,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image1</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -3530,7 +3530,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3574,7 +3574,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3662,7 +3662,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3835,7 +3835,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3857,7 +3857,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -3879,7 +3879,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3923,7 +3923,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -3967,7 +3967,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -4031,7 +4031,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0</t>
+          <t>http://example.com/organization0:Image1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">

</xml_diff>

<commit_message>
SyntheticDataPipeline: use synthetic image URLs
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image0</t>
+          <t>http://example.com/organization1:Image1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -510,7 +510,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image0</t>
+          <t>http://example.com/organization3:Image1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -532,7 +532,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization5:Image0</t>
+          <t>http://example.com/organization5:Image1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -674,58 +674,58 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>mark</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Public Domain Mark 1.0</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nc</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>NonCommercial 1.0 Generic</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>mark</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Public Domain Mark 1.0</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nc</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>NonCommercial 1.0 Generic</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -936,7 +936,7 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image1</t>
+          <t>http://example.com/person0:Image0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -969,7 +969,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image0</t>
+          <t>http://example.com/person2:Image1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1406,7 +1406,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dcterms:description:Image1</t>
+          <t>dcterms:description:Image0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image1</t>
+          <t>dcterms:extent:Image0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1470,7 +1470,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dcterms:language:Image1</t>
+          <t>dcterms:language:Image0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1534,7 +1534,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image0</t>
+          <t>dcterms:publisher:Image1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1598,7 +1598,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image0</t>
+          <t>dcterms:spatial:Image1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1630,7 +1630,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image0</t>
+          <t>dcterms:subject:Image1</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1662,7 +1662,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dcterms:title:Image0</t>
+          <t>dcterms:title:Image1</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1777,7 +1777,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>schema:description:Image0</t>
+          <t>schema:description:Image1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>schema:spatial:Image1</t>
+          <t>schema:spatial:Image0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1990,7 +1990,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2034,7 +2034,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:3:Image1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2056,7 +2056,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2144,7 +2144,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2276,7 +2276,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -2298,7 +2298,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -2342,7 +2342,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -2386,7 +2386,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2408,7 +2408,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2452,7 +2452,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2474,7 +2474,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2628,7 +2628,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2650,7 +2650,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:31:Image1</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2672,7 +2672,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2716,7 +2716,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2782,7 +2782,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2848,7 +2848,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2870,7 +2870,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2892,7 +2892,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2914,7 +2914,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2958,7 +2958,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:45:Image0</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -3068,7 +3068,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -3178,7 +3178,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -3222,7 +3222,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -3244,7 +3244,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -3266,7 +3266,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -3354,7 +3354,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -3398,7 +3398,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3442,7 +3442,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3464,7 +3464,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3530,7 +3530,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3618,7 +3618,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3640,7 +3640,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3684,7 +3684,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3706,7 +3706,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3769,7 +3769,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3835,7 +3835,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3857,7 +3857,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -3879,7 +3879,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3923,7 +3923,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -4049,7 +4049,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0</t>
+          <t>http://example.com/organization2:Image1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -4067,7 +4067,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image1</t>
+          <t>http://example.com/organization4:Image0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">

</xml_diff>

<commit_message>
add schema:ExhibitionEvent's to synthetic data
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -27,6 +27,7 @@
     <sheet name="SchemaPlace" sheetId="18" state="visible" r:id="rId18"/>
     <sheet name="DcCollection" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="SchemaCollection" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="SchemaExhibitionEvent" sheetId="21" state="visible" r:id="rId21"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -510,7 +511,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image0</t>
+          <t>http://example.com/organization3:Image1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -624,22 +625,22 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>dc:identifier</t>
+          <t>dcterms:hasVersion</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>dc:title</t>
+          <t>foaf:logo</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>dcterms:hasVersion</t>
+          <t>identifier</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>foaf:logo</t>
+          <t>title</t>
         </is>
       </c>
     </row>
@@ -656,76 +657,76 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>by-sa</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Attribution-ShareAlike 3.0 Unported</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nc</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>NonCommercial 1.0 Generic</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>mark</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Public Domain Mark 1.0</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>mark</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Public Domain Mark 1.0</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
         <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nc</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>NonCommercial 1.0 Generic</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -754,32 +755,32 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>definition</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>description</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>skos:definition</t>
-        </is>
-      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>skos:note</t>
+          <t>note</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>skos:prefLabel</t>
+          <t>prefLabel</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>skos:scopeNote</t>
+          <t>scopeNote</t>
         </is>
       </c>
     </row>
@@ -790,22 +791,22 @@
         </is>
       </c>
       <c r="B2" t="inlineStr">
-        <is>
-          <t>This Rights Statement indicates that the Item labeled with this Rights Statement is in copyright.</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>InC</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
         <is>
           <t>This Item is protected by copyright and/or related rights.
   You are free to use this Item in any way that is permitted by the copyright and related rights legislation that applies to your use.
   For other uses you need to obtain permission from the rights-holder(s).</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>This Rights Statement indicates that the Item labeled with this Rights Statement is in copyright.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>InC</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
@@ -829,25 +830,25 @@
         </is>
       </c>
       <c r="B3" t="inlineStr">
-        <is>
-          <t>This Rights Statement indicates that the Item labeled with this Rights Statement is in copyright but that educational use is allowed without the need to obtain additional permission.</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>InC-EDU</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
         <is>
           <t>This Item is protected by copyright and/or related rights.
   You are free to use this Item in any way that is permitted by the copyright and related rights legislation that applies to your use. In addition, no permission is required from the rights-holder(s) for educational uses.
   For other uses, you need to obtain permission from the rights-holder(s).</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>This Rights Statement indicates that the Item labeled with this Rights Statement is in copyright but that educational use is allowed without the need to obtain additional permission.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>InC-EDU</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -997,7 +998,7 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image0</t>
+          <t>http://example.com/person4:Image1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1075,7 +1076,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image0</t>
+          <t>http://example.com/person1:Image1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1107,7 +1108,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person3:Image1</t>
+          <t>http://example.com/person3:Image0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1139,7 +1140,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person5:Image1</t>
+          <t>http://example.com/person5:Image0</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1321,6 +1322,110 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>@id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>http://example.com/exhibitionEvent0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>http://example.com/exhibitionEvent0:Image0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Exhibition event 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>_:N1dc60e4dc1d244769d9efac7621b3fd3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>http://example.com/exhibitionEvent1:Image0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Exhibition event 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>http://example.com/exhibitionEvent2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>http://example.com/exhibitionEvent2:Image0</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Exhibition event 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>_:N20f1e14379ef4a6e8306762d2ba5ed40</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>http://example.com/exhibitionEvent3:Image1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Exhibition event 3</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -1406,7 +1511,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dcterms:description:Image1</t>
+          <t>dcterms:description:Image0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1534,7 +1639,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image1</t>
+          <t>dcterms:publisher:Image0</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1566,7 +1671,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>dcterms:source:Image0</t>
+          <t>dcterms:source:Image1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1598,7 +1703,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image0</t>
+          <t>dcterms:spatial:Image1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1662,7 +1767,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dcterms:title:Image0</t>
+          <t>dcterms:title:Image1</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1694,7 +1799,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>dcterms:type:Image1</t>
+          <t>dcterms:type:Image0</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1777,7 +1882,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>schema:description:Image0</t>
+          <t>schema:description:Image1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1841,7 +1946,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>schema:spatial:Image1</t>
+          <t>schema:spatial:Image0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1990,7 +2095,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2078,7 +2183,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:5:Image1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2144,7 +2249,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -2188,7 +2293,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2210,7 +2315,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2232,7 +2337,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -2254,7 +2359,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -2276,7 +2381,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -2320,7 +2425,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2364,7 +2469,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2408,7 +2513,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2430,7 +2535,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:21:Image1</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2474,7 +2579,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2496,7 +2601,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -2540,7 +2645,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2562,7 +2667,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2782,7 +2887,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2804,7 +2909,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:38:Image1</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2826,7 +2931,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2848,7 +2953,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2914,7 +3019,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2936,7 +3041,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -3002,7 +3107,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3024,7 +3129,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -3046,7 +3151,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -3068,7 +3173,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -3090,7 +3195,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -3112,7 +3217,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -3200,7 +3305,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -3222,7 +3327,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -3244,7 +3349,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -3288,7 +3393,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -3332,7 +3437,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -3398,7 +3503,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3420,7 +3525,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3464,7 +3569,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3486,7 +3591,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3508,7 +3613,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3552,7 +3657,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3574,7 +3679,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:73:Image1</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3596,7 +3701,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:74:Image1</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3618,7 +3723,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3684,7 +3789,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:78:Image1</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3791,7 +3896,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -3813,7 +3918,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -3879,7 +3984,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3923,7 +4028,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -3967,7 +4072,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -4067,7 +4172,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image1</t>
+          <t>http://example.com/organization4:Image0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">

</xml_diff>

<commit_message>
regenerate synthetic data with events all having IRIs
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -533,7 +533,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization5:Image0</t>
+          <t>http://example.com/organization5:Image1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -970,7 +970,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image0</t>
+          <t>http://example.com/person2:Image1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1076,7 +1076,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image1</t>
+          <t>http://example.com/person1:Image0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://example.com/person5:Image0</t>
+          <t>http://example.com/person5:Image1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1373,12 +1373,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>_:N1dc60e4dc1d244769d9efac7621b3fd3</t>
+          <t>http://example.com/exhibitionEvent1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/exhibitionEvent1:Image0</t>
+          <t>http://example.com/exhibitionEvent1:Image1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1407,7 +1407,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>_:N20f1e14379ef4a6e8306762d2ba5ed40</t>
+          <t>http://example.com/exhibitionEvent3</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dcterms:language:Image1</t>
+          <t>dcterms:language:Image0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image0</t>
+          <t>dcterms:medium:Image1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1639,7 +1639,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>dcterms:publisher:Image0</t>
+          <t>dcterms:publisher:Image1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1703,7 +1703,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image1</t>
+          <t>dcterms:spatial:Image0</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1735,7 +1735,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image0</t>
+          <t>dcterms:subject:Image1</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1767,7 +1767,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dcterms:title:Image1</t>
+          <t>dcterms:title:Image0</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>dcterms:type:Image0</t>
+          <t>dcterms:type:Image1</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1882,7 +1882,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>schema:description:Image1</t>
+          <t>schema:description:Image0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1914,7 +1914,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>schema:name:Image1</t>
+          <t>schema:name:Image0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2015,7 +2015,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2095,7 +2095,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2205,7 +2205,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2227,7 +2227,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:7:Image1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2249,7 +2249,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -2271,7 +2271,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2315,7 +2315,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2403,7 +2403,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -2425,7 +2425,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -2469,7 +2469,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2557,7 +2557,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2601,7 +2601,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:24:Image0</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -2623,7 +2623,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2645,7 +2645,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2667,7 +2667,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:27:Image0</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2689,7 +2689,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2777,7 +2777,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2865,7 +2865,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2953,7 +2953,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:40:Image0</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2975,7 +2975,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2997,7 +2997,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -3019,7 +3019,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -3041,7 +3041,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:44:Image0</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -3085,7 +3085,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -3107,7 +3107,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -3173,7 +3173,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -3217,7 +3217,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -3261,7 +3261,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:54:Image0</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -3305,7 +3305,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -3371,7 +3371,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:59:Image1</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -3393,7 +3393,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -3459,7 +3459,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:63:Image0</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -3503,7 +3503,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3525,7 +3525,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3547,7 +3547,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:67:Image0</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3591,7 +3591,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:69:Image1</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3635,7 +3635,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3745,7 +3745,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3767,7 +3767,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3811,7 +3811,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3874,7 +3874,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3918,7 +3918,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:82:Image1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -3940,7 +3940,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3962,7 +3962,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -4028,7 +4028,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -4050,7 +4050,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:88:Image0</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -4072,7 +4072,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -4136,7 +4136,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image1</t>
+          <t>http://example.com/organization0:Image0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -4154,7 +4154,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://example.com/organization2:Image0</t>
+          <t>http://example.com/organization2:Image1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">

</xml_diff>

<commit_message>
assert image has a rights statement
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -534,7 +534,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image0</t>
+          <t>http://example.com/organization3:Image1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image0</t>
+          <t>http://example.com/organization3:Image1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -578,7 +578,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://example.com/organization5:Image0</t>
+          <t>http://example.com/organization5:Image1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -600,7 +600,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>http://example.com/organization5:Image0</t>
+          <t>http://example.com/organization5:Image1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -651,7 +651,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -742,7 +742,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/by/4.0/</t>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -750,20 +750,22 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>by</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Attribution 4.0 International</t>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nc</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>NonCommercial 1.0 Generic</t>
         </is>
       </c>
     </row>
@@ -790,36 +792,6 @@
       <c r="H4" t="inlineStr">
         <is>
           <t>Public Domain Mark 1.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nc</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>NonCommercial 1.0 Generic</t>
         </is>
       </c>
     </row>
@@ -904,7 +876,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1070,7 +1042,7 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image1</t>
+          <t>http://example.com/person0:Image0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1103,7 +1075,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image1</t>
+          <t>http://example.com/person0:Image0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1136,7 +1108,7 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image1</t>
+          <t>http://example.com/person2:Image0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1164,7 +1136,7 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>http://example.com/person2:Image1</t>
+          <t>http://example.com/person2:Image0</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1192,7 +1164,7 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image0</t>
+          <t>http://example.com/person4:Image1</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1220,7 +1192,7 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image0</t>
+          <t>http://example.com/person4:Image1</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1298,7 +1270,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image0</t>
+          <t>http://example.com/person1:Image1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1330,7 +1302,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image0</t>
+          <t>http://example.com/person1:Image1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1780,7 +1752,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://example.com/exhibitionEvent2:Image1</t>
+          <t>http://example.com/exhibitionEvent2:Image0</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1797,7 +1769,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>http://example.com/exhibitionEvent2:Image1</t>
+          <t>http://example.com/exhibitionEvent2:Image0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1994,7 +1966,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0</t>
+          <t>dcterms:extent:Image1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2026,7 +1998,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image0</t>
+          <t>dcterms:extent:Image1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2122,7 +2094,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image1</t>
+          <t>dcterms:medium:Image0</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -2154,7 +2126,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image1</t>
+          <t>dcterms:medium:Image0</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2378,7 +2350,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image0</t>
+          <t>dcterms:subject:Image1</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -2410,7 +2382,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image0</t>
+          <t>dcterms:subject:Image1</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -2621,7 +2593,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>schema:description:Image1</t>
+          <t>schema:description:Image0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2653,7 +2625,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>schema:description:Image1</t>
+          <t>schema:description:Image0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2749,7 +2721,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>schema:spatial:Image0</t>
+          <t>schema:spatial:Image1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2781,7 +2753,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>schema:spatial:Image0</t>
+          <t>schema:spatial:Image1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2970,7 +2942,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2992,7 +2964,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3014,7 +2986,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -3036,7 +3008,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3190,7 +3162,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -3212,7 +3184,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -3278,7 +3250,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -3300,7 +3272,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -3366,7 +3338,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -3388,7 +3360,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -3410,7 +3382,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -3432,7 +3404,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -3454,7 +3426,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -3476,7 +3448,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -3498,7 +3470,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -3520,7 +3492,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -3718,7 +3690,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -3740,7 +3712,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -3762,7 +3734,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -3784,7 +3756,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -3806,7 +3778,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -3828,7 +3800,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -3894,7 +3866,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -3916,7 +3888,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -3938,7 +3910,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -3960,7 +3932,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -4202,7 +4174,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -4224,7 +4196,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:29:Image0</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -4246,7 +4218,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -4268,7 +4240,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:30:Image0</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -4334,7 +4306,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -4356,7 +4328,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:32:Image1</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -4422,7 +4394,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -4444,7 +4416,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:34:Image0</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -4466,7 +4438,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -4488,7 +4460,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:35:Image1</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -4510,7 +4482,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -4532,7 +4504,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -4554,7 +4526,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -4576,7 +4548,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -4642,7 +4614,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -4664,7 +4636,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -4730,7 +4702,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -4752,7 +4724,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -4774,7 +4746,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -4796,7 +4768,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -4818,7 +4790,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -4840,7 +4812,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:43:Image1</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -4950,7 +4922,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -4972,7 +4944,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:46:Image1</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -5038,7 +5010,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -5060,7 +5032,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:48:Image1</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -5082,7 +5054,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -5104,7 +5076,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -5126,7 +5098,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -5148,7 +5120,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:50:Image1</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -5170,7 +5142,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -5192,7 +5164,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:51:Image0</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -5258,7 +5230,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -5280,7 +5252,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:53:Image0</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -5346,7 +5318,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -5368,7 +5340,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -5390,7 +5362,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -5412,7 +5384,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -5434,7 +5406,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -5456,7 +5428,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -5478,7 +5450,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -5500,7 +5472,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -5566,7 +5538,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -5588,7 +5560,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -5610,7 +5582,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -5632,7 +5604,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -5654,7 +5626,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -5676,7 +5648,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -5742,7 +5714,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -5764,7 +5736,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:64:Image0</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -5786,7 +5758,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -5808,7 +5780,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -5830,7 +5802,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -5852,7 +5824,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -5918,7 +5890,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -5940,7 +5912,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -6050,7 +6022,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -6072,7 +6044,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -6094,7 +6066,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -6116,7 +6088,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:72:Image1</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -6270,7 +6242,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -6292,7 +6264,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:76:Image1</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -6314,7 +6286,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -6336,7 +6308,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -6487,7 +6459,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -6509,7 +6481,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -6531,7 +6503,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -6553,7 +6525,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -6619,7 +6591,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -6641,7 +6613,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -6707,7 +6679,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -6729,7 +6701,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -6883,7 +6855,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -6905,7 +6877,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:89:Image0</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -6969,7 +6941,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0</t>
+          <t>http://example.com/organization0:Image1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -6987,7 +6959,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://example.com/organization0:Image0</t>
+          <t>http://example.com/organization0:Image1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -7041,7 +7013,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0</t>
+          <t>http://example.com/organization4:Image1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -7059,7 +7031,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>http://example.com/organization4:Image0</t>
+          <t>http://example.com/organization4:Image1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">

</xml_diff>

<commit_message>
cut down Getty images out of IIIF manifest to avoid reproducing the IIIF manifest for every image
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -651,7 +651,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -742,7 +742,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+          <t>http://creativecommons.org/licenses/by/4.0/</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -750,46 +750,74 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nc</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>NonCommercial 1.0 Generic</t>
+          <t>by</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Attribution 4.0 International</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
         <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nc</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>NonCommercial 1.0 Generic</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
         <is>
           <t>mark</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>Public Domain Mark 1.0</t>
         </is>
@@ -914,7 +942,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -953,7 +981,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+          <t>You may need to obtain other permissions for your intended use. For example, other rights such as publicity, privacy or moral rights may limit how you may use the material.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1164,7 +1192,7 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image1</t>
+          <t>http://example.com/person4:Image0</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1192,7 +1220,7 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image1</t>
+          <t>http://example.com/person4:Image0</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1752,7 +1780,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://example.com/exhibitionEvent2:Image0</t>
+          <t>http://example.com/exhibitionEvent2:Image1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1769,7 +1797,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>http://example.com/exhibitionEvent2:Image0</t>
+          <t>http://example.com/exhibitionEvent2:Image1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1786,7 +1814,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>http://example.com/exhibitionEvent3:Image0</t>
+          <t>http://example.com/exhibitionEvent3:Image1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1803,7 +1831,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>http://example.com/exhibitionEvent3:Image0</t>
+          <t>http://example.com/exhibitionEvent3:Image1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1823,7 +1851,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1835,6 +1863,141 @@
       <c r="A1" t="inlineStr">
         <is>
           <t>@graph</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>https://media.getty.edu/iiif/image/fcbc34dd-cd8a-4a5b-8fd6-cd769588b9a8/full/full/0/default.jpg</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>4417</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://rightsstatements.org/vocab/NoC-US/1.0/</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Images provided here are believed to be in the public domain and are available under the terms of the Getty&amp;rsquo;s &lt;a href="http://www.getty.edu/about/opencontent.html"&gt; Open Content Program&lt;/a&gt;.  Texts provided here are © J. Paul Getty Trust, licensed under &lt;a href="https://creativecommons.org/licenses/by/4.0/legalcode"&gt; CC BY 4.0&lt;/a&gt;. Terms of use for the Getty logo can be found &lt;a href="http://www.getty.edu/legal/copyright.html#logo"&gt; here&lt;/a&gt;.&lt;/p&gt;</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2976</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>https://media.getty.edu/iiif/image/dcca6ffd-310c-4b29-bda5-ce238891c958/full/full/0/default.jpg</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>3691</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://rightsstatements.org/vocab/NoC-US/1.0/</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Images provided here are believed to be in the public domain and are available under the terms of the Getty&amp;rsquo;s &lt;a href="http://www.getty.edu/about/opencontent.html"&gt; Open Content Program&lt;/a&gt;.  Texts provided here are © J. Paul Getty Trust, licensed under &lt;a href="https://creativecommons.org/licenses/by/4.0/legalcode"&gt; CC BY 4.0&lt;/a&gt;. Terms of use for the Getty logo can be found &lt;a href="http://www.getty.edu/legal/copyright.html#logo"&gt; here&lt;/a&gt;.&lt;/p&gt;</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1770</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://media.getty.edu/iiif/image/25ebfd39-29d9-45f9-b6a8-bcfd65fcd2bb/full/full/0/default.jpg</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>6493</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://rightsstatements.org/vocab/NoC-US/1.0/</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Images provided here are believed to be in the public domain and are available under the terms of the Getty&amp;rsquo;s &lt;a href="http://www.getty.edu/about/opencontent.html"&gt; Open Content Program&lt;/a&gt;.  Texts provided here are © J. Paul Getty Trust, licensed under &lt;a href="https://creativecommons.org/licenses/by/4.0/legalcode"&gt; CC BY 4.0&lt;/a&gt;. Terms of use for the Getty logo can be found &lt;a href="http://www.getty.edu/legal/copyright.html#logo"&gt; here&lt;/a&gt;.&lt;/p&gt;</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>4307</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>https://media.getty.edu/iiif/image/4e2ed1e3-bc74-4b07-b4dc-a7dfd9fdaac1/full/full/0/default.jpg</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://rightsstatements.org/vocab/NoC-US/1.0/</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Images provided here are believed to be in the public domain and are available under the terms of the Getty&amp;rsquo;s &lt;a href="http://www.getty.edu/about/opencontent.html"&gt; Open Content Program&lt;/a&gt;.  Texts provided here are © J. Paul Getty Trust, licensed under &lt;a href="https://creativecommons.org/licenses/by/4.0/legalcode"&gt; CC BY 4.0&lt;/a&gt;. Terms of use for the Getty logo can be found &lt;a href="http://www.getty.edu/legal/copyright.html#logo"&gt; here&lt;/a&gt;.&lt;/p&gt;</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1188</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>https://media.getty.edu/iiif/image/8a4fe713-1d02-454c-af9d-6f8544dcc716/full/full/0/default.jpg</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://rightsstatements.org/vocab/NoC-US/1.0/</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Images provided here are believed to be in the public domain and are available under the terms of the Getty&amp;rsquo;s &lt;a href="http://www.getty.edu/about/opencontent.html"&gt; Open Content Program&lt;/a&gt;.  Texts provided here are © J. Paul Getty Trust, licensed under &lt;a href="https://creativecommons.org/licenses/by/4.0/legalcode"&gt; CC BY 4.0&lt;/a&gt;. Terms of use for the Getty logo can be found &lt;a href="http://www.getty.edu/legal/copyright.html#logo"&gt; here&lt;/a&gt;.&lt;/p&gt;</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1191</t>
         </is>
       </c>
     </row>
@@ -1902,7 +2065,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dcterms:description:Image1</t>
+          <t>dcterms:description:Image0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1934,7 +2097,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dcterms:description:Image1</t>
+          <t>dcterms:description:Image0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2094,7 +2257,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image0</t>
+          <t>dcterms:medium:Image1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -2126,7 +2289,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image0</t>
+          <t>dcterms:medium:Image1</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2222,7 +2385,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>dcterms:source:Image1</t>
+          <t>dcterms:source:Image0</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -2254,7 +2417,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>dcterms:source:Image1</t>
+          <t>dcterms:source:Image0</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -2286,7 +2449,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image1</t>
+          <t>dcterms:spatial:Image0</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -2318,7 +2481,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>dcterms:spatial:Image1</t>
+          <t>dcterms:spatial:Image0</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -2414,7 +2577,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>dcterms:title:Image0</t>
+          <t>dcterms:title:Image1</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2446,7 +2609,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>dcterms:title:Image0</t>
+          <t>dcterms:title:Image1</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -2478,7 +2641,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>dcterms:type:Image0</t>
+          <t>dcterms:type:Image1</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2510,7 +2673,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>dcterms:type:Image0</t>
+          <t>dcterms:type:Image1</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2657,7 +2820,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>schema:name:Image1</t>
+          <t>schema:name:Image0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2689,7 +2852,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>schema:name:Image1</t>
+          <t>schema:name:Image0</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2721,7 +2884,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>schema:spatial:Image1</t>
+          <t>schema:spatial:Image0</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2753,7 +2916,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>schema:spatial:Image1</t>
+          <t>schema:spatial:Image0</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2822,7 +2985,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2840,7 +3003,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:property_group:Image0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2942,7 +3105,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2964,7 +3127,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3074,7 +3237,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -3096,7 +3259,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:4:Image0</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -3250,7 +3413,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -3272,7 +3435,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:8:Image0</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -3294,7 +3457,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -3316,7 +3479,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:9:Image1</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -3338,7 +3501,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -3360,7 +3523,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:10:Image0</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -3514,7 +3677,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -3536,7 +3699,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:14:Image1</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -3558,7 +3721,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -3580,7 +3743,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -3646,7 +3809,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -3668,7 +3831,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:17:Image1</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -3734,7 +3897,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -3756,7 +3919,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:19:Image0</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -3866,7 +4029,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -3888,7 +4051,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:22:Image1</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -3910,7 +4073,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -3932,7 +4095,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3998,7 +4161,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -4020,7 +4183,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:25:Image1</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -4042,7 +4205,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -4064,7 +4227,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:26:Image0</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -4350,7 +4513,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -4372,7 +4535,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:33:Image0</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -4482,7 +4645,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -4504,7 +4667,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:36:Image0</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -4526,7 +4689,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -4548,7 +4711,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:37:Image0</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -4614,7 +4777,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -4636,7 +4799,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:39:Image1</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -4702,7 +4865,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -4724,7 +4887,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:41:Image0</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -4746,7 +4909,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -4768,7 +4931,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:42:Image0</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -4966,7 +5129,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4988,7 +5151,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:47:Image0</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -5054,7 +5217,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -5076,7 +5239,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:49:Image0</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -5186,7 +5349,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -5208,7 +5371,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:52:Image0</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -5318,7 +5481,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -5340,7 +5503,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:55:Image1</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -5362,7 +5525,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -5384,7 +5547,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:56:Image1</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -5406,7 +5569,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -5428,7 +5591,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:57:Image1</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -5450,7 +5613,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -5472,7 +5635,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:58:Image0</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -5538,7 +5701,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -5560,7 +5723,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:60:Image0</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -5582,7 +5745,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -5604,7 +5767,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:61:Image0</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -5626,7 +5789,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -5648,7 +5811,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:62:Image0</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -5758,7 +5921,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -5780,7 +5943,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:65:Image1</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -5802,7 +5965,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -5824,7 +5987,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:66:Image1</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -5890,7 +6053,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -5912,7 +6075,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:68:Image1</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -5978,7 +6141,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -6000,7 +6163,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:70:Image0</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -6022,7 +6185,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -6044,7 +6207,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:71:Image1</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -6198,7 +6361,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -6220,7 +6383,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:75:Image0</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -6286,7 +6449,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -6308,7 +6471,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:77:Image0</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -6374,7 +6537,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -6396,7 +6559,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:79:Image1</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -6459,7 +6622,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -6481,7 +6644,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:80:Image0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -6503,7 +6666,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -6525,7 +6688,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:81:Image0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -6591,7 +6754,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -6613,7 +6776,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:83:Image1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -6635,7 +6798,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -6657,7 +6820,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:84:Image1</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -6679,7 +6842,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -6701,7 +6864,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:85:Image0</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -6723,7 +6886,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -6745,7 +6908,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:86:Image1</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -6767,7 +6930,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -6789,7 +6952,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:87:Image0</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">

</xml_diff>

<commit_message>
fix handling of work description rights enrichment
</commit_message>
<xml_diff>
--- a/data/synthetic/synthetic_data.xlsx
+++ b/data/synthetic/synthetic_data.xlsx
@@ -490,7 +490,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image1</t>
+          <t>http://example.com/organization1:Image0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/organization1:Image1</t>
+          <t>http://example.com/organization1:Image0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -534,7 +534,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image0</t>
+          <t>http://example.com/organization3:Image1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://example.com/organization3:Image0</t>
+          <t>http://example.com/organization3:Image1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -770,56 +770,56 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/licenses/nc/1.0/</t>
+          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nc</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>NonCommercial 1.0 Generic</t>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>mark</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Public Domain Mark 1.0</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
+          <t>http://creativecommons.org/licenses/nc/1.0/</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
         <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>mark</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Public Domain Mark 1.0</t>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nc</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>NonCommercial 1.0 Generic</t>
         </is>
       </c>
     </row>
@@ -834,7 +834,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -904,7 +904,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -942,7 +942,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>You may find additional information about the copyright status of the Item on the website of the organization that has made the Item available.</t>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -992,6 +992,44 @@
       <c r="G4" t="inlineStr">
         <is>
           <t>This Rights Statement can be used only for copyrighted Items for which the organization making the Item available is the rights-holder or has been explicitly authorized by the rights-holder(s) to allow third parties to use their Work(s) for educational purposes without first obtaining permission.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>http://rightsstatements.org/vocab/NoC-US/1.0/</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>The organization that has made the Item available believes that the Item is in the Public Domain under the laws of the United States, but a determination was not made as to its copyright status under the copyright laws of other countries. The Item may not be in the Public Domain under the laws of other countries.
+  Please refer to the organization that has made the Item available for more information.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>This Rights Statement indicates that the Item is in the Public Domain under the laws of the United States, but that a determination was not made as to its copyright status under the copyright laws of other countries.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>NoC-US</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Unless expressly stated otherwise, the organization that has made this Item available makes no warranties about the Item and cannot guarantee the accuracy of this Rights Statement. You are responsible for your own use.</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>No Copyright - United States</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>This Rights Statement should be used for Items for which the organization that intends to make the Item available has determined are free of copyright under the laws of the United States. This Rights Statement should not be used for Orphan Works (which are assumed to be in-copyright) or for Items where the organization that intends to make the Item available has not undertaken an effort to ascertain the copyright status of the underlying Work.</t>
         </is>
       </c>
     </row>
@@ -1070,7 +1108,7 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image1</t>
+          <t>http://example.com/person0:Image0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1103,7 +1141,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>http://example.com/person0:Image1</t>
+          <t>http://example.com/person0:Image0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1192,7 +1230,7 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image1</t>
+          <t>http://example.com/person4:Image0</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1220,7 +1258,7 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>http://example.com/person4:Image1</t>
+          <t>http://example.com/person4:Image0</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1298,7 +1336,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image1</t>
+          <t>http://example.com/person1:Image0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1330,7 +1368,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://example.com/person1:Image1</t>
+          <t>http://example.com/person1:Image0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1712,7 +1750,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://example.com/exhibitionEvent0:Image0</t>
+          <t>http://example.com/exhibitionEvent0:Image1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1729,7 +1767,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://example.com/exhibitionEvent0:Image0</t>
+          <t>http://example.com/exhibitionEvent0:Image1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1746,7 +1784,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://example.com/exhibitionEvent1:Image1</t>
+          <t>http://example.com/exhibitionEvent1:Image0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1763,7 +1801,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://example.com/exhibitionEvent1:Image1</t>
+          <t>http://example.com/exhibitionEvent1:Image0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1780,7 +1818,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://example.com/exhibitionEvent2:Image0</t>
+          <t>http://example.com/exhibitionEvent2:Image1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1797,7 +1835,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>http://example.com/exhibitionEvent2:Image0</t>
+          <t>http://example.com/exhibitionEvent2:Image1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2065,7 +2103,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dcterms:description:Image0</t>
+          <t>dcterms:description:Image1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2097,7 +2135,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dcterms:description:Image0</t>
+          <t>dcterms:description:Image1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2129,7 +2167,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image1</t>
+          <t>dcterms:extent:Image0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2161,7 +2199,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dcterms:extent:Image1</t>
+          <t>dcterms:extent:Image0</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2257,7 +2295,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image1</t>
+          <t>dcterms:medium:Image0</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -2289,7 +2327,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>dcterms:medium:Image1</t>
+          <t>dcterms:medium:Image0</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2385,7 +2423,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>dcterms:source:Image1</t>
+          <t>dcterms:source:Image0</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -2417,7 +2455,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>dcterms:source:Image1</t>
+          <t>dcterms:source:Image0</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -2513,7 +2551,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image1</t>
+          <t>dcterms:subject:Image0</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -2545,7 +2583,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>dcterms:subject:Image1</t>
+          <t>dcterms:subject:Image0</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -2756,7 +2794,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>schema:description:Image1</t>
+          <t>schema:description:Image0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2788,7 +2826,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>schema:description:Image1</t>
+          <t>schema:description:Image0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2884,7 +2922,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>schema:spatial:Image1</t>
+          <t>schema:spatial:Image0</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2916,7 +2954,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>schema:spatial:Image1</t>
+          <t>schema:spatial:Image0</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3105,7 +3143,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -3127,7 +3165,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:1:Image1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3149,7 +3187,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -3171,7 +3209,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:2:Image1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3325,7 +3363,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -3347,7 +3385,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:6:Image1</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -3545,7 +3583,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -3567,7 +3605,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:11:Image0</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -3589,7 +3627,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -3611,7 +3649,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:12:Image1</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -3633,7 +3671,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -3655,7 +3693,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:13:Image0</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -3721,7 +3759,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -3743,7 +3781,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:15:Image1</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -3765,7 +3803,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -3787,7 +3825,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:16:Image0</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -3853,7 +3891,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -3875,7 +3913,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:18:Image0</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -3941,7 +3979,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -3963,7 +4001,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:20:Image1</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -4073,7 +4111,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -4095,7 +4133,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image1</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:23:Image0</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -4293,7 +4331,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -4315,7 +4353,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image0</t>
+          <t>urn:paradicms_etl:pipeline:synthetic_data:concept:28:Image1</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -4381,7 +4419,7 @@
      